<commit_message>
Added func to store quest, query and emb vector
</commit_message>
<xml_diff>
--- a/ChatGPT/Vector_DB/Question_Query_Embeddings.xlsx
+++ b/ChatGPT/Vector_DB/Question_Query_Embeddings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dovcohen/Documents/Projects/AI/NL2SQL/OpenAI/Vector_DB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dovcohen/Documents/Projects/AI/NL2SQL/ChatGPT/Vector_DB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75A98D3-69BB-524C-A1E0-C0C57F0C8599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDAA8FA2-88BD-2F45-BF41-7DB1A10ADD6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VDS" sheetId="1" r:id="rId1"/>
@@ -452,7 +452,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added two new embedding methods
</commit_message>
<xml_diff>
--- a/ChatGPT/Vector_DB/Question_Query_Embeddings.xlsx
+++ b/ChatGPT/Vector_DB/Question_Query_Embeddings.xlsx
@@ -1,115 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dovcohen/Documents/Projects/AI/NL2SQL/ChatGPT/Vector_DB/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDAA8FA2-88BD-2F45-BF41-7DB1A10ADD6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="VDS" sheetId="1" r:id="rId1"/>
+    <sheet name="VDS" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>Question</t>
-  </si>
-  <si>
-    <t>Query</t>
-  </si>
-  <si>
-    <t>Metadata</t>
-  </si>
-  <si>
-    <t>Embedding</t>
-  </si>
-  <si>
-    <t>What are Mary Spocks account balances on 10/10/2023?</t>
-  </si>
-  <si>
-    <t>SELECT account.acct_nbr, balance.balance, product.type, date.date FROM account INNER JOIN product ON account.product_id = product.id INNER JOIN balance ON account.id = balance.account_id INNER JOIN date ON balance.balance_dt_id = date.id  INNER JOIN relationship ON account.id = relationship.account_id  INNER JOIN client ON relationship.client_id = client.id WHERE client.name = 'Mary Spock' AND date.date = '2023-10-10' AND relationship.relationship_type = 'Primary';</t>
-  </si>
-  <si>
-    <t>[-0.006784611381590366, -0.02970653399825096, -0.010175181552767754, -0.033204685896635056, -0.020891744643449783, 0.005170880351215601, -0.04347703978419304, 0.005181291606277227, -0.014769977889955044, -0.00833587534725666, 0.032704949378967285, 0.004667673725634813, -0.01760181598365307, 0.012049192562699318, 0.016810566186904907, 0.029595481231808662, 0.01157721970230341, -0.0069754826836287975, 0.003761902218684554, -0.03389876335859299, -0.011486989445984364, 0.01638023927807808, -0.017157604917883873, 0.007149002514779568, -0.01000166218727827, -0.008960545994341373, 0.005170880351215601, -0.00580943189561367, 0.001872275141067803, -0.03589770942926407, 0.023570885881781578, -0.004067296627908945, -0.0017742366762831807, -0.027124565094709396, -0.019128786399960518, -0.011542515829205513, -0.014117544516921043, -0.011042779311537743, 0.006205056328326464, 0.00042794240289367735, -0.006201586220413446, 0.04333822429180145, -0.01470057014375925, -0.006926897447556257, -0.019864508882164955, 0.005198643542826176, -0.007537685800343752, -0.02851272001862526, -0.02962324395775795, -0.007121239323168993, 0.026014039292931557, -0.0008033951744437218, -0.012035311199724674, 0.0036786128766834736, 0.015630634501576424, -0.024209437891840935, 0.01394402515143156, 0.009682387113571167, -0.018046025186777115, 0.015644514933228493, 0.010119656100869179, 0.0012163715437054634, -0.012083896435797215, 0.023015623912215233, -0.017240894958376884, -0.002611468080431223, -0.011584159918129444, -0.01066103670746088, -0.016907738521695137, 0.019267601892352104, 0.005299284588545561, 0.011452285572886467, 0.005868428852409124, -0.011452285572886467, 0.009689327329397202, -0.027929695323109627, -0.0049626571126282215, -0.004632969852536917, 0.0008363638771697879, 0.0037063760682940483, 0.01768510416150093, 0.0042755198664963245, -0.0007947192061692476, -0.009189591743052006, 0.009682387113571167, -0.0035883828531950712, 0.013860736042261124, 0.005344399716705084, -0.021072205156087875, 0.018365301191806793, 0.029956402257084846, 0.023209964856505394, 0.025514302775263786, 0.021183257922530174, -0.021197138354182243, 0.006062770262360573, -0.028276734054088593, 0.014533990994095802, -0.012035311199724674, -0.020766811445355415, -0.014298005029559135, 0.008474690839648247, -0.03514810651540756, -0.012035311199724674, -0.01990615390241146, -0.013694156892597675, -0.0004036496684420854, 0.0031094690784811974, 0.017004908993840218, -0.0052506993524730206, -0.0017126372549682856, 0.0014835915062576532, 0.01799049973487854, -0.013465111143887043, -0.0018705399706959724, -0.01506149023771286, 0.01182708702981472, 0.006781141273677349, -0.015838857740163803, -0.005632441956549883, 0.030067455023527145, 0.010154359973967075, 0.0024847988970577717, -0.006840137764811516, 0.003623086726292968, -0.015186424367129803, -0.005830254405736923, -0.014395175501704216, -0.01324300654232502, -0.005299284588545561, 0.005854547023773193, -0.002271370030939579, -0.0011339497286826372, -0.009258999489247799, -0.00631957920268178, 0.02436213381588459, -0.029179034754633904, 0.007433574181050062, -0.012937611900269985, -0.03223297744989395, 0.003100793110206723, 0.031094690784811974, -0.0077389683574438095, -0.00823870487511158, -0.0030209741089493036, -0.0020978504326194525, 0.013832972384989262, 0.011993666179478168, -0.0036300274077802896, -0.01259057316929102, 0.014124485664069653, 0.014742214232683182, -0.005101472605019808, -0.008967486210167408, -0.0032378733158111572, 0.0039874776266515255, 0.019989443942904472, 0.02397345006465912, -0.004813430365175009, -0.015283595770597458, -0.03903494030237198, 0.007863902486860752, 0.013534518890082836, 0.016435764729976654, -0.003100793110206723, 0.022571412846446037, -0.008516335859894753, 0.01657458022236824, -0.007919428870081902, -0.0024431541096419096, -0.019364774227142334, 0.022071676328778267, -0.033204685896635056, 0.012035311199724674, -0.011563337408006191, 0.035425737500190735, 0.0032448142301291227, -0.023390425369143486, -0.013541460037231445, -0.014422939158976078, 0.01667175069451332, 0.02436213381588459, 0.007620975375175476, 0.03170548006892204, -0.0020371186546981335, -0.02811015583574772, 0.03326021134853363, -0.0245564766228199, 0.005531800910830498, -0.0021603174973279238, 0.015297477133572102, 0.0368138924241066, -0.02618061751127243, -0.017102079465985298, -0.6241148710250854, -0.02518114633858204, 0.005254169926047325, -0.029567718505859375, 0.024695292115211487, -0.004882838111370802, 0.024306608363986015, 0.013319354504346848, -0.03276047855615616, -0.0045705027878284454, 0.011008075438439846, 0.02576417103409767, -0.006409809459000826, -0.004386572167277336, 0.0015061490703374147, -0.020503060892224312, 0.007551567628979683, 0.00920347310602665, 0.0102654118090868, 0.007620975375175476, -0.020044969394803047, 0.028790351003408432, 0.01446458324790001, 0.011188535951077938, 0.039173755794763565, -0.014992082491517067, 0.018462471663951874, -0.047752559185028076, -0.01446458324790001, 0.005871898960322142, -0.00026374959270469844, 0.025042330846190453, 0.018143195658922195, -0.012958434410393238, 0.03281600400805473, 0.010890082456171513, -0.043921250849962234, 0.017657341435551643, -0.01585274003446102, 0.040589675307273865, -0.02293233387172222, -0.01182708702981472, -0.0015295741613954306, -0.02355700358748436, -0.013569222763180733, 0.023321017622947693, 0.010411168448626995, 0.01496431976556778, 0.013354058377444744, 0.004285931121557951, 0.0065798587165772915, 0.01575556769967079, 0.0012640893692150712, 0.004376161377876997, 0.007336403243243694, -0.0006211997242644429, 0.030900347977876663, 0.0021967566572129726, -0.013430407270789146, -0.016824448481202126, -0.013916261494159698, -0.016144251450896263, -0.016796685755252838, -0.007475219201296568, -0.024847988039255142, -0.005098002031445503, -0.007607094012200832, 0.03981230780482292, 0.020961152389645576, -0.03084482252597809, 0.023806871846318245, 0.029595481231808662, 0.001449755160138011, 0.00392153998836875, 0.01939253695309162, 0.008328935131430626, 0.03151113539934158, -0.002181139774620533, 0.021960625424981117, 0.016255304217338562, 0.007551567628979683, -0.01588050276041031, -0.022682465612888336, -0.007836139760911465, 0.005753905978053808, 0.008634328842163086, 0.0025403250474482775, -0.0031702008564025164, 0.013728860765695572, 0.008328935131430626, 0.03112245351076126, 0.02041977271437645, 0.03428744897246361, -0.03031732328236103, 0.007162883877754211, 0.0012805737787857652, -0.032593898475170135, -0.017421355471014977, -0.006156471092253923, -0.007863902486860752, -0.006968542002141476, 0.012319882400333881, 0.008925842121243477, 0.007648738566786051, 0.020392008125782013, -0.008932782337069511, 0.001795926596969366, 0.016296949237585068, 0.0073433443903923035, -0.042088884860277176, 0.017115961760282516, -0.012097777798771858, 0.02468140982091427, -0.010827614925801754, -0.016047080978751183, -0.0279852207750082, 0.0462811142206192, -0.0033732187002897263, -0.01575556769967079, -0.007981895469129086, 0.03367666155099869, 0.011299587786197662, 0.0073780482634902, -0.014589517377316952, -0.012208830565214157, 0.007183706387877464, 0.014561754651367664, -0.012500342912971973, -0.002059676218777895, -0.012021428905427456, -0.0026878167409449816, 0.0006368164904415607, -0.0009317995863966644, -0.018976090475916862, 0.025195028632879257, 0.007863902486860752, 0.005788609851151705, -0.03062271699309349, -0.00023490199237130582, -0.011063601821660995, 0.00409505981951952, 0.01567227952182293, 0.00416793767362833, -0.01597767323255539, -0.006985893938690424, -0.03928481042385101, 0.0008216146961785853, 0.008634328842163086, 0.006156471092253923, 0.012958434410393238, -0.019753456115722656, -0.012243534438312054, 0.012132481671869755, 0.005344399716705084, -0.012708566151559353, -0.012014488689601421, 0.0010862319031730294, -0.007947191596031189, 0.006628443952649832, -0.004997360985726118, -0.014436820521950722, 0.011924258433282375, -0.004303283058106899, 0.0006524331984110177, 0.0077528501860797405, -0.015575108118355274, 0.0003333742788527161, -0.008099889382719994, -0.018823392689228058, -0.013402644544839859, -0.01790720969438553, -0.01496431976556778, -0.00530622573569417, -0.014138367027044296, -0.0047370814718306065, -0.0007031876593828201, 0.02041977271437645, 0.008780085481703281, 0.004344927612692118, -0.010091892443597317, -0.008731500245630741, -0.010445872321724892, 0.007912487722933292, 0.01667175069451332, 0.04700295627117157, 0.02153029665350914, 0.012611395679414272, 0.02425108104944229, -0.004691966809332371, 0.014367412775754929, -0.007162883877754211, 0.008106829598546028, 0.002741607604548335, 0.01871233992278576, 0.009182650595903397, -0.014631162397563457, -0.0008879859233275056, -0.011507811956107616, 0.008884197100996971, 0.0008437384385615587, 0.027013512328267097, 0.01737971045076847, 0.007169824559241533, 0.011736857704818249, -0.018976090475916862, -0.002328631468117237, 0.01000860333442688, -0.02920679748058319, 0.02931785024702549, 0.010091892443597317, 0.0016067903488874435, -0.009890610352158546, -0.008793966844677925, -0.002051000250503421, 0.006309167947620153, 0.0026826111134141684, -0.007093476131558418, -0.008932782337069511, -0.0056359125301241875, 0.02416779287159443, 0.0022436068393290043, 0.0024917395785450935, 0.024042857810854912, -0.02819344401359558, -0.004390042740851641, -0.00030561117455363274, -0.005927425343543291, 0.01021682657301426, 0.022196611389517784, -0.00332289794459939, -0.0071420613676309586, 0.0015052814269438386, 0.011368995532393456, 0.027513248845934868, 0.0406174398958683, 0.007822257466614246, 0.022002268582582474, 0.00599336251616478, 0.03861849382519722, 0.009231235831975937, 0.0014697099104523659, 0.006035007536411285, 0.03939586132764816, 0.009689327329397202, -0.019156549125909805, 0.020905626937747, 0.015464055351912975, 0.019947798922657967, -0.0005799888167530298, 0.0035814419388771057, -0.033093634992837906, -0.03578665480017662, -0.007856962271034718, -0.002753754146397114, 0.018073787912726402, -0.030150743201375008, -0.014658925123512745, -0.004698907490819693, -0.0037723134737461805, 0.026305552572011948, 0.00371331674978137, 0.007697323802858591, 0.017629578709602356, -0.023321017622947693, 0.016616225242614746, 0.005781668704003096, -0.03023403324186802, 0.009397814981639385, 0.011709094047546387, -0.025944631546735764, -0.02629167027771473, -0.01668563298881054, 0.000759581511374563, 0.0036369680892676115, -0.01086925994604826, -0.017518525943160057, 0.0005357413901947439, 0.006763789337128401, 0.0011018486693501472, -0.0030903818551450968, -0.02597239427268505, -0.027416076511144638, 0.023612530902028084, 0.016310831531882286, -0.005871898960322142, -0.002722520614042878, 0.005441570654511452, 0.011410640552639961, 0.02495904080569744, 0.030095217749476433, 0.003545002778992057, -0.002510826801881194, -0.013173598796129227, 0.009606038220226765, -0.028276734054088593, -0.005708790849894285, 0.008634328842163086, -0.0024258021730929613, -0.007384988944977522, -0.011792383156716824, 0.016449647024273872, 0.007759790867567062, 0.004070766735821962, -0.020294837653636932, 0.012833500280976295, -0.004608677234500647, -0.01939253695309162, -0.043116118758916855, -0.010438931174576283, -0.02415391057729721, 0.017435237765312195, -0.0031302913557738066, -0.043615855276584625, 0.013874617405235767, 0.015339121222496033, 0.017407473176717758, -0.023515358567237854, -0.03550902381539345, 0.03023403324186802, 0.021780164912343025, 0.00247785821557045, 0.002340777777135372, -0.040173228830099106, 0.008009659126400948, 0.11166325211524963, 0.0323440283536911, 0.000544417358469218, -0.005625501275062561, -0.008356697857379913, 0.010883141309022903, 0.003970125690102577, -0.009987780824303627, 0.028360022231936455, -0.0034877413418143988, 0.01607484370470047, 0.0003789231413975358, -0.015588989481329918, -0.002120407996699214, 0.0010957755148410797, 0.006864430382847786, 0.004636440426111221, -0.0072531141340732574, -0.006524332333356142, -0.016199778765439987, -0.026430485770106316, 0.004580914042890072, -0.00042620720341801643, 0.03989559784531593, 0.005146587733179331, 0.01338876225054264, -0.0007691250648349524, -0.015644514933228493, 0.01440905686467886, -0.015241950750350952, -0.01414530724287033, 0.011979784816503525, -0.0019850628450512886, -0.0058476063422858715, -6.170786218717694e-05, 0.01172991655766964, 0.022474242374300957, -0.015089253894984722, -0.0006719541852362454, 0.007711205631494522, 0.0019364773761481047, 0.021877335384488106, 0.007995777763426304, -0.017365828156471252, 0.018143195658922195, -0.006545154377818108, -0.013020901009440422, 0.038174282759428024, 0.019128786399960518, -0.0036126754712313414, 0.0244454238563776, 0.0035484733525663614, -0.016824448481202126, -0.016602342948317528, 0.01649129018187523, 0.007516863755881786, -0.008266467601060867, -0.028484957292675972, -0.010341760702431202, -0.005986421834677458, -0.03903494030237198, -0.025139501318335533, 0.0017551494529470801, -0.0024553006514906883, 0.03487047553062439, -0.018642932176589966, -0.02568088285624981, 0.0016102606896311045, -0.02970653399825096, -0.008766204118728638, -0.011639686301350594, -0.010445872321724892, -0.028651535511016846, 0.0018653343431651592, 0.037646785378456116, 0.012215770781040192, 0.036591786891222, -0.01739359274506569, 0.01586662046611309, 0.017143724486231804, 0.00034226715797558427, -0.025833578780293465, 0.007516863755881786, -0.03384323790669441, 0.0005305358208715916, 0.02344595082104206, 0.0016744629247114062, 0.00365432002581656, -0.008065185509622097, 0.03156666457653046, 0.0012606190284714103, -0.0022488124668598175, 0.011181594803929329, -0.021377598866820335, 0.006493098568171263, -0.0053929854184389114, 0.0007305169710889459, 0.03273271396756172, 0.005670616403222084, 0.019795101135969162, 0.010494457557797432, 0.008349756710231304, -0.013180539011955261, -0.033121395856142044, 0.002030177740380168, 0.006000303663313389, -0.008058244362473488, 0.010841497220098972, -0.013312414288520813, -0.007711205631494522, 0.01596379093825817, -0.006382046267390251, 0.008259527385234833, -0.0008567523909732699, 0.00763485673815012, 0.01808767020702362, 0.02375134639441967, 0.0008632593671791255, -0.025139501318335533, 0.011813205666840076, 0.003164995228871703, -0.0025906458031386137, 0.03051166422665119, 0.0047509633004665375, -0.0054589225910604, 0.0030001518316566944, -0.01188261341303587, -0.00465379236266017, -0.00707612419500947, 0.025208909064531326, 0.015575108118355274, -0.016116488724946976, -0.011445344425737858, -0.03606428951025009, 0.0066874404437839985, -0.03731362894177437, -0.01778227649629116, 0.01061245147138834, 0.010022484697401524, 0.01461728010326624, 0.005285403225570917, 0.001202489947900176, -0.01379132829606533, -0.015824975445866585, 0.03001192770898342, -0.028054628521203995, -0.018670694902539253, -0.029651008546352386, 0.027957458049058914, 0.036564022302627563, -0.002738137263804674, 0.003647379344329238, -0.03295481950044632, 0.009897550567984581, -0.006378575693815947, -0.016824448481202126, 0.002935949480161071, -0.0023147498723119497, 0.043615855276584625, -0.005504037719219923, 0.025819698348641396, -0.003531121416017413, 0.03784112632274628, 0.013513696379959583, 0.013687215745449066, -0.01319442130625248, -0.005191702861338854, -0.003220521379262209, -0.014166129752993584, -0.016907738521695137, 0.01172991655766964, 0.0031788768246769905, 0.004986949730664492, -0.0017941914265975356, 0.011757679283618927, 0.006874841637909412, -0.024209437891840935, -0.011188535951077938, -0.03214968740940094, -0.02881811372935772, -0.012625277042388916, -0.01879562996327877, -0.012944553047418594, 0.009383933618664742, -0.045531511306762695, -0.008488573133945465, -0.003541532438248396, 0.03131679445505142, -0.0015052814269438386, 0.006447983905673027, 0.018642932176589966, -0.011285706423223019, 0.046447694301605225, -0.009494985453784466, -0.029179034754633904, 0.0003299039090052247, -0.007863902486860752, -0.022862926125526428, -0.014450701884925365, -0.011160772293806076, -0.018351418897509575, 0.032510608434677124, 0.016255304217338562, 0.009036893956363201, -0.004025651607662439, 0.007301699370145798, -0.010230707935988903, -0.015505700372159481, 0.00586495827883482, -0.018934445455670357, -0.010494457557797432, -0.009425577707588673, -0.008828670717775822, -0.003623086726292968, 0.027624299749732018, 0.012340704910457134, -0.023404307663440704, 0.021502533927559853, -0.023432070389389992, -0.006833197083324194, 0.005528330337256193, 0.01207001507282257, 0.005642853211611509, 0.03439849987626076, 0.03187205642461777, 0.034537315368652344, 0.005382574163377285, 0.0012120335595682263, 0.021155495196580887, -0.010459753684699535, -0.016199778765439987, 0.040895070880651474, 0.03820204734802246, -0.03414863348007202, -0.004226934630423784, 0.014062018133699894, 0.001214636373333633, -0.012868204154074192, -0.014811621978878975, 0.004594795871526003, -0.021169375628232956, 0.008349756710231304, 0.007260054815560579, -0.03162219002842903, -0.010667976923286915, 0.03384323790669441, -0.0080304816365242, 0.005389514844864607, -0.0038486619014292955, -0.008981367573142052, -0.008821730501949787, -0.01344428863376379, 0.012514224275946617, 0.011368995532393456, 0.002141230273991823, -0.01939253695309162, -0.005774728022515774, -0.016310831531882286, 0.0126877436414361, 0.01728253997862339, -0.027110682800412178, 0.04125599190592766, -0.01329159177839756, 0.017227012664079666, -0.008537158370018005, -0.007315581198781729, -0.012181066907942295, -0.0035068285651504993, 0.017421355471014977, 0.02669423632323742, -0.03170548006892204, 0.00014456341159529984, 0.011237121187150478, -0.02498680353164673, -0.0003895512199960649, 0.0008628256036899984, -0.020697403699159622, -0.004934893921017647, 0.0022540180943906307, 0.009640742093324661, 0.030650479719042778, -0.008106829598546028, -0.010230707935988903, -0.021377598866820335, 0.00038694843533448875, 0.00026656928821466863, -0.036536261439323425, -0.0055595641024410725, 0.010667976923286915, -0.005573445465415716, -0.024528713896870613, 0.008703736588358879, -0.00946028158068657, 0.029151272028684616, -0.01324300654232502, 0.011486989445984364, -0.0030660892371088266, 0.012000607326626778, -0.03842415288090706, 0.020752929151058197, 0.0013517166953533888, 0.009536630474030972, -0.034926000982522964, -0.0014367412077262998, -0.025500422343611717, -0.016852211207151413, 0.0009604303049854934, -0.01425636000931263, -0.032010871917009354, -0.009189591743052006, 0.02315443940460682, 0.005268051289021969, -0.011167713440954685, -0.0067464374005794525, -0.006364694330841303, 0.008405283093452454, 0.018046025186777115, -0.030400611460208893, -0.020891744643449783, -0.001255413400940597, 0.009363111108541489, -0.009376992471516132, -0.002222784562036395, -0.02942890301346779, 0.00940475519746542, -0.02738831378519535, 0.004105470608919859, -0.010647155344486237, 0.01243093516677618, -0.011389818042516708, 0.010806793347001076, -0.0078430799767375, -0.006288345903158188, -0.005580386146903038, -0.027166208252310753, 0.0028248969465494156, -0.007565448991954327, 0.015241950750350952, 0.019739575684070587, -0.0038278396241366863, 0.004337986931204796, 0.017213132232427597, 0.026055684313178062, 0.007641797885298729, 0.005316636525094509, -0.004112411756068468, -0.0036057347897440195, -0.027846405282616615, -0.02283516339957714, -0.023737464100122452, 0.007062242832034826, 0.023390425369143486, -0.003225727006793022, -0.016907738521695137, -0.016963263973593712, 0.007607094012200832, -0.0031580545473843813, -0.02973429672420025, -0.033621132373809814, 0.03409310802817345, 0.057580702006816864, 0.0038313099648803473, 0.01810155250132084, 0.005344399716705084, 0.010584687814116478, 0.017768394201993942, -0.0377856008708477, -0.008488573133945465, 0.03961796686053276, -0.02254365012049675, 0.005816372577100992, 0.001953829312697053, -0.03950691223144531, 0.0027468132320791483, 0.028484957292675972, 0.020669639110565186, 0.031400084495544434, 0.016727278009057045, -0.008793966844677925, -0.03231626749038696, 0.0006893061217851937, -0.005042476113885641, 0.003378424094989896, 0.0083844605833292, 0.0075723896734416485, -0.03981230780482292, 0.003482535947114229, -0.004844663664698601, 0.018420826643705368, -0.002677405485883355, -0.0030817058868706226, 0.005580386146903038, -0.00859962496906519, 0.005122295115143061, -0.029373377561569214, -0.0024847988970577717, -0.02264082059264183, 0.008578802458941936, 0.026833051815629005, 0.027416076511144638, 0.010667976923286915, 0.02001720666885376, 0.027235615998506546, -0.0133401770144701, 0.010779029689729214, 0.022057795897126198, -0.0033281035721302032, -0.024292726069688797, 0.00748215988278389, -0.008717618882656097, 0.0059690698981285095, 0.009036893956363201, -0.008120710961520672, 0.004650321789085865, -0.019795101135969162, -0.006482687778770924, -0.02071128413081169, 0.0018826862797141075, 0.012458697892725468, 0.003529386129230261, -0.024514831602573395, 0.006638855207711458, -0.03134455904364586, -0.0063230497762560844, 0.010466694831848145, -0.018073787912726402, 0.003217051038518548, -0.0077389683574438095, -0.02284904383122921, 0.030039692297577858, -0.031177978962659836, -0.037147048860788345, 0.01728253997862339, 0.02182180993258953, 0.02376522682607174, 0.03617534041404724, 0.2204391360282898, 0.01511701662093401, 0.005486685782670975, 0.0450873002409935, -0.006305697839707136, 0.004386572167277336, 0.013569222763180733, 0.01768510416150093, 0.008349756710231304, 0.018268130719661713, -0.037452444434165955, -0.016560697928071022, 0.008002717979252338, 0.0034061872866004705, -0.007433574181050062, -0.01167439017444849, -0.037535734474658966, -0.026014039292931557, -0.011965903453528881, -0.02032260037958622, 0.0009187856339849532, 0.010848437435925007, -0.0013308944180607796, -0.009765676222741604, 0.007121239323168993, 0.00037350066122598946, -0.001771633862517774, 0.016560697928071022, -0.015949910506606102, 0.01440905686467886, -0.006003773771226406, -0.00621546758338809, -0.019448062404990196, -0.007773672696202993, -0.0005088458419777453, -0.013881557621061802, 0.002453565364703536, -0.009029953740537167, 0.019239839166402817, 0.0023182202130556107, -0.02518114633858204, 0.013506756164133549, -0.0007443985668942332, -0.02212720364332199, -0.020378127694129944, 0.005045946221798658, -0.009134065359830856, -0.01293067168444395, 0.0015486612683162093, 0.015908265486359596, -0.04803019016981125, 0.0010775559348985553, 0.037952180951833725, -0.00565673504024744, -0.009265939705073833, -0.007822257466614246, 0.04653098061680794, -0.013423466123640537, -0.04400453716516495, 0.00730864005163312, -0.0023216905537992716, 0.008488573133945465, -0.02010049670934677, 0.0015582048799842596, -0.006288345903158188, 0.017365828156471252, 0.013437348417937756, 0.0122227119281888, 0.04111717641353607, -0.020975034683942795, 0.027860287576913834, -0.00023034709738567472, 0.008516335859894753, 0.01869845949113369, -0.01992003619670868, -0.02627778984606266, 0.015311358496546745, 0.017254777252674103, 0.03339902684092522, 0.020766811445355415, -0.024945160374045372, 0.011771561577916145, 0.00642369082197547, -0.020905626937747, -0.015172543004155159, -0.03911823034286499, 0.01608872599899769, 0.006340401712805033, -0.004056885372847319, 0.006833197083324194, 0.01329853292554617, -0.01440905686467886, -0.022765755653381348, -0.016421882435679436, 0.0057851392775774, 0.0023754816502332687, -0.002929008798673749, 0.035120341926813126, -0.017254777252674103, -0.011271825060248375, -0.01892056316137314, 0.022099440917372704, -0.0014879294903948903, -0.015838857740163803, 0.009335347451269627, -0.013465111143887043, -0.0167689211666584, 0.006114826072007418, 0.00044052256271243095, -0.03184429556131363, -0.013402644544839859, -0.0038903066888451576, -0.0007522069499827921, -0.009488045237958431, -0.013229125179350376, 0.03264942392706871, 0.003057413036003709, 0.004761374555528164, 0.02616673707962036, -0.016963263973593712, 0.009279821068048477, -0.021058322861790657, -0.025333844125270844, -0.013249946758151054, 0.01757405325770378, -0.025653118267655373, -0.011847909539937973, -0.015283595770597458, 0.010647155344486237, -0.04886308312416077, 0.023709701374173164, 0.0044420985504984856, 0.02012825943529606, -0.0010836290894076228, -0.01647740975022316, 0.008738440461456776, 0.016741158440709114, -0.005309695843607187, -0.02214108407497406, -0.012798796407878399, 0.0030660892371088266, -0.014381294138729572, -0.009786498732864857, -0.0026982277631759644, 0.0065347435884177685, -0.01729642041027546, 0.0246675293892622, -0.022210493683815002, -0.015686159953475, -0.02246036008000374, -0.006031536962836981, -0.03131679445505142, -0.02659706585109234, 0.015630634501576424, 0.027374431490898132, 0.023209964856505394, -0.012410112656652927, -0.02375134639441967, -0.009571334347128868, -0.0038278396241366863, -0.04192230477929115, 0.02283516339957714, 0.020364245399832726, -0.01669951342046261, -0.020600231364369392, 0.009543570689857006, -0.17846131324768066, 0.0009439459536224604, -0.014686688780784607, -0.031205741688609123, 0.01258363202214241, 0.015991555526852608, 0.009585215710103512, -0.04033980891108513, -0.013534518890082836, 0.007232291623950005, 0.009703208692371845, 0.018143195658922195, -0.013249946758151054, -0.02225213684141636, -0.003602264216169715, 0.02637496031820774, -0.024223318323493004, 0.03922928124666214, -0.008898078463971615, 0.0067013222724199295, 0.02051694318652153, -0.01768510416150093, -0.001384685398079455, -0.024320488795638084, 0.00823176372796297, 0.022293781861662865, -0.025597592815756798, 0.03206639736890793, -0.0016475673764944077, 0.0003283856203779578, -0.018226485699415207, -0.0025663529522717, 0.03667507693171501, 0.003945833072066307, 0.002550736302509904, 0.006441042758524418, -6.10029419476632e-05, -0.019489707425236702, -0.00147838587872684, 0.03628639131784439, -0.0007778010331094265, 0.008974427357316017, 0.016657870262861252, -0.006506980396807194, -0.035120341926813126, 0.010383405722677708, 0.012347646057605743, -0.002340777777135372, -0.0016909473342821002, -0.015047608874738216, -0.0030487370677292347, -0.020183784887194633, 0.016199778765439987, 0.012646099552512169, -0.012472580187022686, -0.011993666179478168, 0.011202417314052582, 0.03617534041404724, 0.018517998978495598, -0.018073787912726402, -0.016824448481202126, -0.014492346905171871, 0.010785970836877823, -0.017421355471014977, -0.010397287085652351, -0.0014714451972395182, 0.000319058948662132, -0.004074237309396267, -0.02072516642510891, 0.02587522380053997, 0.010959490202367306, -0.03911823034286499, 0.02162746712565422, 0.0024067151825875044, 0.005517919082194567, -0.010272352956235409, -0.01787944696843624, 0.03126126900315285, -0.0008511129999533296, 0.0009014336974360049, -0.0004045172827318311, 0.041589148342609406, -0.01769898645579815, -0.011327351443469524, 0.005972540471702814, -0.003914599306881428, -0.002552471589297056, 0.001547793741337955, 0.011868732050061226, -0.019600760191679, 0.006864430382847786, -0.006513921078294516, 0.019836746156215668, -0.01737971045076847, 0.005899662151932716, 0.017143724486231804, 0.008169297128915787, -0.0025403250474482775, 0.006198115646839142, -0.008974427357316017, -0.021072205156087875, 0.013104191049933434, -0.009432518854737282, 0.020364245399832726, 0.03262166306376457, 0.004022181499749422, -0.005150057841092348, -0.0029116568621248007, 0.0030036221724003553, -0.017546288669109344, -0.03439849987626076, -0.017365828156471252, 0.026250025257468224, 0.02164134941995144, 0.011001134291291237, 0.021807927638292313, -0.01490879338234663, -0.010071069933474064, -0.0031788768246769905, 0.007280877325683832, 0.050390057265758514, -0.009737912565469742, -0.01768510416150093, 0.01172991655766964, -0.013617807999253273, -0.018337538465857506, -0.09483880549669266, -0.020253192633390427, -0.005799020640552044, 0.033010344952344894, 0.03345455601811409, 0.03020627051591873, 0.008099889382719994, 0.011591101065278053, -9.38089651754126e-05, 0.004976538475602865, 0.008905019611120224, -0.03670283779501915, -0.00580943189561367, -0.005962129216641188, 0.011306528933346272, -0.033621132373809814, 0.014082840643823147, -0.016643987968564034, 0.018767867237329483, 0.02749936655163765, 0.013104191049933434, -0.010230707935988903, -0.011153832077980042, -0.02497292309999466, 0.004206112120300531, -0.027110682800412178, -0.019267601892352104, 0.035620078444480896, 0.025542067363858223, 0.005896191578358412, 0.005705320276319981, -0.02536160685122013, -0.007704264484345913, -0.021058322861790657, 0.006496569141745567, -0.0027572244871407747, -0.03878507390618324, -0.006798493210226297, -0.011244062334299088, -0.048779793083667755, -0.0005791212315671146, 0.02788805030286312, 0.0198228657245636, -0.02648601308465004, 0.023904042318463326, -0.0147560965269804, -0.01649129018187523, 0.024195555597543716, -0.006572917569428682, -0.019253721460700035, -0.008557980880141258, -0.0017803098307922482, 0.0015243685338646173, -0.017254777252674103, 0.011965903453528881, -0.0050390055403113365, 0.008051303215324879, 0.025403251871466637, 0.007614034693688154, -0.021058322861790657, -0.017823919653892517, 0.012604454532265663, -0.01147310808300972, -0.00459826597943902, 0.003041796386241913, -0.02323772758245468, 0.002710374305024743, -0.018323656171560287, 0.0004797813598997891, -0.02032260037958622, -0.019600760191679, 0.023015623912215233, -0.02283516339957714, 0.022085558623075485, -0.017115961760282516, 0.005910073406994343, -0.01758793368935585, -0.024431541562080383, -0.012111659161746502, -0.03339902684092522, 0.00168140372261405, -0.014881029725074768, -0.004511506296694279, 0.016324711963534355, 0.023501478135585785, 0.02426496334373951, -0.0126877436414361, 0.0061113559640944, 0.009141005575656891, -0.009807320311665535, 0.009328407235443592, 0.036341920495033264, -0.0020249723456799984, -0.007856962271034718, -0.037535734474658966, 0.01850411668419838, -0.020863981917500496, -0.002351188799366355, 0.001868804800324142, -0.007780613377690315, -0.0420333594083786, 0.019739575684070587, -0.06652042269706726, 0.03226074203848839, 0.014811621978878975, -0.007364166434854269, -0.009564393199980259, 0.00694771995767951, 0.03736915439367294, -0.02973429672420025, -0.019378654658794403, 0.04117270186543465, -0.029484428465366364, 0.01050833985209465, 0.0027155796997249126, 0.016741158440709114, -0.0210166797041893, -0.029678771272301674, 0.020850099623203278, -0.02062799595296383, 0.022210493683815002, 0.01172991655766964, -0.012868204154074192, -0.0010098833590745926, 0.017712868750095367, 0.021696874871850014, -0.0033124866895377636, 0.02981758676469326, -0.019600760191679, -0.0003396643733140081, -0.0063993982039391994, -0.036841653287410736, 0.009835083968937397, -0.01819872297346592, 0.0012155039003118873, 0.04478190466761589, 0.0012085631024092436, 0.002717314986512065, 0.006028066389262676, 0.0009890609653666615, 0.0068089039996266365, -0.018157077953219414, 0.001291852444410324, -0.019156549125909805, -0.02437601611018181, -0.010688799433410168, -0.013860736042261124, 0.011119128204882145, 0.0022887219674885273, 0.01758793368935585, 0.011105246841907501, 0.015824975445866585, 0.024723054841160774, 0.006274464074522257, -0.0019382125465199351, -0.010126596316695213, -0.007103887386620045, -0.020697403699159622, 0.03456507995724678, 0.003104263450950384, 0.0040152408182621, -0.003149378579109907, 0.02204391360282898, 0.00588925089687109, 0.0045392694883048534, -0.00829423125833273, 0.0009500191081315279, 0.0012909849174320698, 0.015575108118355274, 0.016019318252801895, 0.008877255953848362, -0.049168478697538376, -0.010355642065405846, 0.008745381608605385, -0.0006246701232157648, 0.040978360921144485, -0.013416525907814503, 0.006003773771226406, 0.0017907209694385529, 0.01006412971764803, -0.008856434375047684, 0.018073787912726402, 0.030900347977876663, -0.024320488795638084, -0.031594425439834595, 0.001494870288297534, 0.0052819326519966125, 0.02345983311533928, 0.004043003544211388, 0.021669112145900726, -0.003904188284650445, 0.011806265451014042, 0.011410640552639961, -0.019281484186649323, -0.017324184998869896, -0.02486187033355236, 0.03195534646511078, -0.005965599324554205, -0.003945833072066307, -0.014353531412780285, -0.0065659768879413605, 0.014658925123512745, 0.006350812967866659, 0.0058024912141263485, -0.0010350436205044389, -0.007183706387877464, -0.006395927630364895, 0.010515280067920685, -0.000479347538203001, -0.029762059450149536, 0.01177850179374218, 0.003984007053077221, 0.017934972420334816, 0.022807400673627853, -0.00946028158068657, 0.0022158436477184296, -0.0016831388929858804, 0.02226601</t>
-  </si>
-  <si>
-    <t>What are the names and addresses of clients that live in San Diego?</t>
-  </si>
-  <si>
-    <t>select  client.Name, address.Address, address.City, address.State, address.Zip FROM client INNER JOIN address ON client.Address_ID = address.ID  WHERE address.City = 'San Diego';</t>
-  </si>
-  <si>
-    <t>[0.007716412656009197, -0.008434999734163284, -0.0006514291162602603, -0.01908620074391365, -0.015338804572820663, 0.031241733580827713, -0.003586217761039734, 0.013512116856873035, -0.002928073052316904, -0.03220880404114723, 0.010805663652718067, 0.007911169901490211, 0.012168964371085167, 0.010167666710913181, -0.0128002455458045, 0.0036701648496091366, 0.010859389789402485, -0.019032474607229233, 0.023854393512010574, -0.020805437117815018, -0.03062388300895691, 0.018736980855464935, 0.01860266551375389, 0.0007047354592941701, -0.013001718558371067, -0.025694511830806732, 0.009039417840540409, 0.00371045945212245, -0.02796444110572338, -0.026621287688612938, -0.0020936394575983286, -0.028313660994172096, -0.026030300185084343, -0.016534211114048958, -0.029710538685321808, 0.005799062084406614, 0.007105278316885233, 0.00026107532903552055, 0.018804138526320457, 0.004314878024160862, 0.002795436652377248, -0.02060396410524845, 0.001495096948929131, -0.02541244961321354, 0.019972681999206543, -0.0038850693963468075, -0.0016327700577676296, -0.007763423025608063, -0.03553982079029083, 0.010597474873065948, 0.029710538685321808, 0.006544511765241623, 0.005449842195957899, -0.016547642648220062, -0.003925363998860121, -0.01004006713628769, -0.012095090933144093, -0.0036701648496091366, -0.013303928077220917, -5.3332609240897e-05, 0.00971099454909563, 0.010778800584375858, -0.010926547460258007, 0.004949518013745546, -0.01947571523487568, -0.012773382477462292, 0.007985043339431286, 0.01090640015900135, 0.0014564812881872058, -0.00781714916229248, 0.019878661260008812, 0.0148418378084898, -0.009543100371956825, -0.024243908002972603, 0.0009502805769443512, -0.01759530045092106, 0.005480063147842884, -0.029952306300401688, 0.006003892980515957, 0.02965681254863739, 0.0063766175881028175, -0.0274137482047081, -0.02511695586144924, 0.010429581627249718, 0.01472095400094986, -0.004966307431459427, 0.010167666710913181, 0.0025100167840719223, -0.023102227598428726, 0.0021675126627087593, 0.009818446822464466, 0.03365940973162651, 0.009717710316181183, 0.012007785961031914, -0.0052752322517335415, 0.005987103562802076, -0.00864990334957838, 0.036453165113925934, -0.006782921496778727, -0.003747396171092987, -0.00949609000235796, -0.0008495441288687289, -0.009825162589550018, -0.017528142780065536, -0.01220925897359848, 0.004694318864494562, 0.0016697067767381668, -0.031161144375801086, 0.0053692529909312725, -0.013599421828985214, -0.008703629486262798, 0.01814599335193634, 0.00830068439245224, -0.017460985109210014, -0.0039152903482317924, 0.0026544055435806513, 0.01638646423816681, -0.009482658468186855, 0.011853323318064213, -0.0192339476197958, 0.005490136798471212, 0.0009326516883447766, 0.023760372772812843, -0.02777639962732792, -0.01672225259244442, 0.0010526960249990225, -0.013196475803852081, -0.03449216112494469, -0.004949518013745546, 0.0011366429971531034, -0.01805197261273861, 0.010053498670458794, 0.025909416377544403, 0.0007655970985069871, -0.017823636531829834, -0.023975277319550514, 0.003801122307777405, 0.041637737303972244, -0.0024478959385305643, -0.006588164251297712, 0.0019945818930864334, 0.018159424886107445, -0.002281680703163147, 0.013028581626713276, 0.003945511300116777, 0.025828827172517776, 0.008347694762051105, 0.006598237901926041, 0.011839891783893108, -0.009019270539283752, -0.006128134671598673, 0.014465754851698875, 0.019516009837388992, 0.004717824049293995, -0.018911590799689293, 0.016856567934155464, 0.013821042142808437, 0.022591829299926758, -0.02359919436275959, -0.0075686657801270485, -0.02350517362356186, 0.015956655144691467, 0.03137604892253876, 0.002928073052316904, 0.017890794202685356, 0.026863055303692818, -0.01971748284995556, -0.009731141850352287, -0.010006488300859928, -0.009032702073454857, -0.0009024307364597917, 0.02244408242404461, -0.008851376362144947, 0.0026073954068124294, -0.00694409990683198, -0.014170262031257153, 0.010825810953974724, -0.008314115926623344, -0.0163596011698246, -0.022887323051691055, 0.022591829299926758, -0.025976574048399925, -0.012477888725697994, 0.030274663120508194, -0.013438243418931961, -0.011101157404482365, 0.0174206905066967, -0.02823307178914547, 0.00518792774528265, -0.01312931813299656, 0.01787736266851425, 0.013713589869439602, 0.03269233927130699, -0.011470524594187737, -0.653739333152771, -0.02417675033211708, 0.009341627359390259, -0.009966193698346615, 0.0021725494880229235, 0.0321013517677784, 0.019986113533377647, 0.022605260834097862, -0.010429581627249718, 0.02408272959291935, 0.0007928798440843821, 0.013538979925215244, -0.030785061419010162, -0.007400771602988243, -0.0031883087940514088, -0.022067999467253685, 0.0090125547721982, 0.02731972746551037, 0.021342696622014046, -0.006923952605575323, -0.01877727545797825, 0.023787235841155052, 0.007944748736917973, 0.01756843738257885, 0.026795897632837296, 0.01783706806600094, 0.011007136665284634, -0.03516373783349991, 0.0038917851634323597, 0.029065825045108795, -0.023102227598428726, 0.009845309890806675, 0.011853323318064213, -0.0060542612336575985, 0.028636015951633453, 0.010228108614683151, -0.0097714364528656, 0.03371313586831093, -0.021248675882816315, 0.02941504493355751, -0.020214449614286423, -0.0008562598959542811, 0.01978464052081108, 0.015916360542178154, 0.0008864808478392661, 0.01729980669915676, 0.019139926880598068, -0.013659863732755184, -0.002837410196661949, -0.0033024768345057964, 0.015150763094425201, -0.009079712443053722, -0.05651986971497536, -0.0006258252542465925, 0.026003437116742134, -0.0023370857816189528, 0.008367842063307762, 0.0012323426781222224, 0.009630405344069004, 0.004895791877061129, -0.0090125547721982, 0.0006044187466613948, -0.009784867987036705, -0.01602381281554699, -0.009247606620192528, 0.015674592927098274, -0.0016319305868819356, 0.004657382145524025, 0.0017511354526504874, 0.00528530590236187, 0.001189529662951827, 0.018831001594662666, -0.021208381280303, 0.02538558654487133, 0.010496738366782665, -0.0013221659464761615, 0.023585762828588486, -0.011544398032128811, -0.010026635602116585, 0.0009410463972017169, -0.00688365800306201, 0.009281185455620289, -0.01626558043062687, -0.012545046396553516, -0.004106689710170031, 0.00045499298721551895, -0.04314206540584564, -0.025828827172517776, -0.001642843708395958, -0.0274137482047081, 0.013633000664412975, 0.010953410528600216, 0.008495441637933254, -0.018696686252951622, -0.00048605340998619795, 0.005288663785904646, -0.010288550518453121, 0.00781714916229248, 0.0008071508491411805, -0.03110741823911667, 0.0029734044801443815, -0.01638646423816681, 0.023975277319550514, 0.010678064078092575, 0.011255620047450066, -0.006833289749920368, -0.018696686252951622, 0.030919376760721207, 0.0218128003180027, -0.03129545971751213, -0.009207312017679214, -0.009167017415165901, -0.017340101301670074, -0.021060634404420853, -0.0192339476197958, -0.022551534697413445, 0.01568802446126938, 0.009724426083266735, 0.0020650974474847317, 0.005752051714807749, 0.015607435256242752, -0.004623803310096264, 0.03489510715007782, -0.015567140653729439, 0.011410082690417767, 0.007259740494191647, 0.012350290082395077, -0.020577101036906242, 0.027225706726312637, -0.018468350172042847, 0.006826573982834816, -0.002400885568931699, 0.01090640015900135, -0.019408557564020157, 0.007306750863790512, 0.010241540148854256, 0.006897089537233114, -0.01592979207634926, -0.011195178143680096, -0.009569963440299034, -0.011880186386406422, -2.1891815777053125e-05, 0.000350688787875697, -0.013720305636525154, 0.006124776788055897, -0.016681957989931107, 0.0010535354958847165, -0.0015630939742550254, -0.027937578037381172, 0.0004235128581058234, -0.006222154945135117, -0.020617395639419556, -0.0036936700344085693, 0.009308048523962498, -0.0002379898796789348, -0.008253674022853374, -0.008690197952091694, -0.01370687410235405, 0.010913115926086903, -0.01554027758538723, 0.013424811884760857, 0.016829704865813255, -0.016681957989931107, -0.009334911592304707, 0.00784401223063469, -0.02050994336605072, 0.022605260834097862, 0.012665930204093456, 0.016413327306509018, -0.010006488300859928, 0.005530431400984526, -0.005919945891946554, -0.022914186120033264, 0.01019452977925539, -0.0066553219221532345, 0.008139505982398987, -0.01817285642027855, 0.012726372107863426, 0.007105278316885233, 0.002897852100431919, 0.007253024727106094, -0.005365895107388496, 0.0011290877591818571, 0.03599649295210838, 0.02613775245845318, -0.016856567934155464, 0.030006032437086105, 0.034330982714891434, -0.013968789018690586, 0.0055237156338989735, -0.008743924088776112, -5.9759804571513087e-05, -0.010839242488145828, -0.0003865761391352862, 0.0013011792907491326, 0.014788111671805382, 0.007588813081383705, 1.7956797819351777e-05, 0.01848178170621395, -0.0029398256447166204, 0.02507666125893593, -8.725246152607724e-05, 0.013203191570937634, -0.013075591996312141, 0.009214027784764767, -0.033337052911520004, 0.006477354094386101, -0.02753463201224804, 0.06049560010433197, 0.014680659398436546, 0.010973557829856873, -0.0430077500641346, 0.01422398816794157, -0.0031496931333094835, -0.013028581626713276, 0.01364643219858408, -0.014774680137634277, 0.01626558043062687, -0.010584043338894844, 0.024525970220565796, 0.005023391451686621, -0.007333613932132721, 0.03677552193403244, -0.02017415501177311, -0.011101157404482365, 0.0019291031640022993, 0.00010021178604802117, 0.008441715501248837, -0.0009805015288293362, 0.001248292624950409, -0.013324075378477573, -0.022739576175808907, 0.02338428981602192, 0.00468760309740901, -0.008569314144551754, -0.015620866790413857, 0.0030103411991149187, 0.0023656277917325497, 0.017675889655947685, 0.0007122906972654164, 1.8140432075597346e-05, 0.0074142031371593475, 0.019368262961506844, -0.003713817335665226, 0.013485253788530827, 0.01896531693637371, 0.013377801515161991, 0.026527266949415207, -0.00438539357855916, 0.01587606593966484, -0.03304155915975571, -0.008293968625366688, -0.0009863778250291944, 0.009160301648080349, -0.017152059823274612, -0.005849430337548256, 0.008925249800086021, 0.008340978994965553, -0.002224596682935953, 0.014895563945174217, 0.013485253788530827, -0.005496852565556765, 0.012484604492783546, -0.03328332677483559, 0.0118130287155509, -0.0022917543537914753, 0.008401420898735523, -0.007038120646029711, 0.008260389789938927, -0.007353761233389378, 0.007978327572345734, 0.007044836413115263, 0.0008512230706401169, 0.019274242222309113, 0.002798794535920024, 0.011551113799214363, -0.007716412656009197, -0.02193368412554264, -0.000547334726434201, -0.005446484312415123, -0.03137604892253876, -0.003253787523135543, -0.00010068398842122406, 0.026983939111232758, 0.014828406274318695, 0.003228603396564722, -0.0037641855888068676, -0.0012079980224370956, -0.05146961286664009, 0.019005611538887024, 0.009469226934015751, 0.0016352884704247117, -0.0005880490643903613, -0.004942802246659994, 0.007622391916811466, -0.011638418771326542, -0.0015454650856554508, -0.021302402019500732, -0.0027803261764347553, 0.015029879286885262, 0.011779449880123138, 0.013794179074466228, 0.019623462110757828, -0.010087077505886555, 0.03347136825323105, 0.004140268545597792, -0.005009959917515516, -0.005584157537668943, -0.0207517109811306, -0.0430077500641346, 0.010946694761514664, 0.01918022148311138, -0.03911260887980461, 0.02441851794719696, 0.019556304439902306, -0.009684131480753422, -0.03588904067873955, -0.00650421716272831, 0.04265853017568588, 0.0008680124883539975, -0.02314252220094204, -0.02850170247256756, -0.021248675882816315, 0.008280537091195583, 0.08929279446601868, 0.016775978729128838, -0.000304937653709203, 0.005678178276866674, 0.01048330683261156, 0.0023219753056764603, -0.022403787821531296, -0.002676231786608696, 0.001463197055272758, -0.00492937071248889, -0.008817797526717186, -0.0041671316139400005, -0.0033091926015913486, 0.00889167096465826, 0.009032702073454857, -0.0038817115128040314, 0.011013852432370186, -0.0009905751794576645, 0.005849430337548256, -0.010523601435124874, -0.031913310289382935, 0.007655970752239227, 0.019636893644928932, 0.03373999893665314, 0.012289848178625107, 0.0318058580160141, 0.046365633606910706, 0.012907697819173336, -0.0018820927944034338, 0.00650421716272831, 0.01469409093260765, 0.022430650889873505, -0.0010795589769259095, 0.011584692634642124, -0.00836112629622221, 0.017044609412550926, -0.002100355224683881, 0.005819209385663271, 0.032396845519542694, -0.008945397101342678, 0.015137331560254097, -0.007575381547212601, 0.005567368119955063, -0.024727441370487213, 0.029737401753664017, -0.008246958255767822, -0.019999545067548752, 0.022094862535595894, 0.012222690507769585, -0.002953257178887725, 0.019247379153966904, -0.016547642648220062, 0.016829704865813255, -0.04346442222595215, -0.0037608277052640915, -0.01226970087736845, -2.2718169930158183e-05, -0.005879651289433241, -0.023679783567786217, -0.009536384604871273, -0.04244362562894821, -0.011356356553733349, -0.019824935123324394, -0.024284202605485916, -0.013518832623958588, -0.041610874235630035, -0.03279979154467583, -0.009731141850352287, -0.010113940574228764, -0.02017415501177311, 0.03185958415269852, 0.012941276654601097, -0.027037665247917175, 0.018401192501187325, 0.02705109678208828, 0.021006908267736435, 0.02198741026222706, -0.01793108880519867, 0.008864807896316051, 0.02550647035241127, -0.0015160837210714817, -0.011557829566299915, 0.016037244349718094, -0.011537682265043259, -0.027561495080590248, 0.022256040945649147, 0.006658679805696011, -0.013518832623958588, 0.0020516659133136272, 0.02208143100142479, -0.01744755357503891, -0.00931476429104805, -0.0026090743485838175, 0.006128134671598673, 0.0003723051631823182, -0.009724426083266735, 0.005896440707147121, 0.016104402020573616, -0.0324237085878849, -0.006020682398229837, 0.018575802445411682, -0.010798947885632515, 0.012961423955857754, 0.008387989364564419, 0.007246308960020542, -0.009536384604871273, 0.002191017847508192, -0.0003443927562329918, -0.016184991225600243, -0.0006892052479088306, 0.007232877425849438, -0.020671121776103973, 0.000639676523860544, 0.00542297912761569, 0.004439119715243578, 0.03269233927130699, 0.01783706806600094, -0.0022934332955628633, 0.007823864929378033, 0.03293410688638687, 0.020456217229366302, -0.013666579499840736, 0.03462647646665573, 0.009059565141797066, -0.016440190374851227, 0.00341160804964602, -0.008965544402599335, -0.024673717096447945, 0.01799824647605419, -0.00010015931911766529, -0.005688251927495003, 0.00011028543667634949, 0.006782921496778727, -0.01172572374343872, -0.013780747540295124, -0.021826231852173805, -7.182719127740711e-05, 0.01621185429394245, 0.0017158776754513383, -0.0006275041960179806, -0.014949290081858635, -0.007367192767560482, -0.022618692368268967, -0.005419621244072914, -0.012457741424441338, -0.0277226734906435, -0.0003322204283904284, -0.01768932119011879, 0.032369982451200485, 0.0060240402817726135, -0.000943564809858799, 0.02217545174062252, -0.0016193385235965252, 0.010516885668039322, -0.003020414849743247, -0.005872935522347689, 0.0036097229458391666, 0.010960126295685768, 0.010416150093078613, 0.0293881818652153, 0.015956655144691467, 0.02174564264714718, 0.0014850232983008027, 0.008052201010286808, 0.0103758554905653, 0.016896862536668777, -0.020012976601719856, 0.011369788087904453, -0.005325600504875183, 0.004063037224113941, 0.014828406274318695, 0.004731255583465099, -0.0005834319745190442, 0.013847905211150646, -0.011215325444936752, 0.010026635602116585, 0.003285687416791916, -0.03132232278585434, 0.0021205025259405375, -0.05144274979829788, -0.011094441637396812, -0.017272943630814552, -0.015110468491911888, 0.009281185455620289, -0.013115886598825455, -0.014210556633770466, 0.020254744216799736, 0.01611783355474472, -0.004754760768264532, -0.039005156606435776, 0.004811844788491726, -0.0069038053043186665, 0.0134046645835042, -0.0031228300649672747, 5.1679900934686884e-05, -0.0074746450409293175, -0.018253445625305176, -0.021409854292869568, -0.007333613932132721, 0.005728546530008316, 0.015889497473835945, -0.01853550784289837, 0.018790706992149353, 0.01282710861414671, 0.001920708455145359, 0.010584043338894844, -0.011188462376594543, -0.0012944635236635804, -0.0072866035625338554, 0.004512993153184652, -0.020953182131052017, 0.0035526391584426165, -0.039676733314991, -0.005443126428872347, -0.014626933261752129, -0.013794179074466228, -0.015526846051216125, 0.017004314810037613, -0.031026829034090042, -0.019636893644928932, -0.014788111671805382, -0.0007219446124508977, 0.010301982052624226, 0.015016447752714157, 0.019072769209742546, 0.03390117734670639, -0.028179345652461052, -0.009825162589550018, -0.006621743086725473, -0.013418096117675304, -0.0029146415181457996, 0.005795704200863838, 0.040912434458732605, -0.02562735415995121, -0.02666158229112625, 0.025425881147384644, -0.0004629679606296122, 0.01334422267973423, -0.012215974740684032, 0.016399895772337914, 0.051389023661613464, 0.0018535507842898369, 0.0006350594339892268, 0.024136455729603767, -0.029334455728530884, 0.02323654294013977, 0.0061180610209703445, -0.011954059824347496, -0.00889167096465826, -0.013216623105108738, -0.028179345652461052, -0.0027820051182061434, -0.023370858281850815, 0.02092631906270981, 0.013874768279492855, 0.007716412656009197, -0.010731790214776993, -0.01971748284995556, 0.02008013427257538, 0.0070918467827141285, -0.026460109278559685, 0.009120007045567036, -0.006081124301999807, -0.02026817575097084, 0.0037272488698363304, 0.03172526881098747, -0.02335742674767971, 0.01811913028359413, 0.011685429140925407, 0.020523374900221825, -0.0010518565541133285, -0.004056321457028389, 0.012168964371085167, -0.023827530443668365, -0.016493916511535645, 0.018951885402202606, 0.014385165646672249, -0.009825162589550018, -0.015567140653729439, -0.018696686252951622, 0.0363457128405571, 0.00506704393774271, 0.01978464052081108, -0.019623462110757828, -0.01778334192931652, -0.032584886997938156, -0.009939330630004406, -0.0006216278998181224, -0.006269165314733982, -0.0023286910727620125, -0.006121418904513121, 0.009522953070700169, 0.0016084254020825028, -0.002112107817083597, 0.01398222055286169, -0.015164194628596306, 0.008139505982398987, -0.005809135735034943, -0.03328332677483559, 0.014385165646672249, -0.003646659664809704, -0.003047277918085456, -0.05463945493102074, -0.004637234844267368, -0.0042577944695949554, -0.03322960063815117, -0.0081798005849123, 0.0186295285820961, -0.03583531454205513, -0.01592979207634926, 0.00877078715711832, 0.007017973344773054, 0.009986340999603271, -0.011779449880123138, -0.0015891175717115402, 0.012847255915403366, 0.003231961280107498, -0.02335742674767971, -0.01001320406794548, 0.005913230124861002, -0.03841416910290718, -0.020980045199394226, -0.00500660203397274, -0.011121304705739021, 0.008925249800086021, 0.0042577944695949554, 0.012424162589013577, 0.018562370911240578, 0.010798947885632515, -0.024700580164790154, -0.0008965544402599335, 0.014170262031257153, -0.0067191217094659805, -0.004214141983538866, -0.0010904720984399319, 0.014344871044158936, -0.013747168704867363, 0.034787654876708984, 0.0028139050118625164, -0.009724426083266735, -0.006786279380321503, 0.024861756712198257, 0.014801543205976486, 0.014492617920041084, -0.009321480058133602, -0.030758198350667953, -0.013498685322701931, -0.015553709119558334, -0.05155020207166672, -0.003619796596467495, -0.0024915484245866537, 0.022215746343135834, 0.0023051858879625797, -0.022067999467253685, -0.013183044269680977, 0.005020033568143845, -0.027440611273050308, 0.007608960382640362, 0.009959477931261063, 0.008246958255767822, 0.022793302312493324, 0.017850499600172043, -0.012215974740684032, -0.009744573384523392, -0.005030107218772173, 0.05651986971497536, -0.006379975471645594, -0.008972260169684887, 0.027400316670536995, -0.04244362562894821, 0.012350290082395077, -0.01826687715947628, -0.02842111326754093, -0.007105278316885233, 0.006332965102046728, 0.006860152818262577, 0.0026930212043225765, 0.026379520073533058, -0.02678246609866619, -0.03105369210243225, -0.012934560887515545, 0.002839089138433337, -0.025103524327278137, 0.004318235907703638, 0.01942198909819126, -0.02114122360944748, -0.0044559091329574585, 6.605583621421829e-05, -0.0035492812748998404, 0.0029331098776310682, 0.006030756048858166, 0.012061512097716331, -0.020765142515301704, -0.013485253788530827, -0.006850079167634249, -0.009308048523962498, 0.007467929273843765, -0.0029347888194024563, 0.011235472746193409, -0.005641241557896137, -0.02535872347652912, 0.02823307178914547, 0.017152059823274612, -0.0073806243017315865, -0.012041364796459675, 0.014519480988383293, -0.00931476429104805, -0.006393407005816698, -0.007118709851056337, -0.026527266949415207, -0.016037244349718094, -0.01398222055286169, -0.0030321674421429634, -0.016950588673353195, 0.02844797633588314, -0.015674592927098274, -0.011638418771326542, -0.0017007671995088458, 0.016010381281375885, 0.01358599029481411, -0.034545887261629105, -0.009845309890806675, -0.003898500930517912, -0.019247379153966904, 0.018696686252951622, -0.0005993819213472307, -0.029280729591846466, -0.013122602365911007, 0.006487427745014429, 0.05106666684150696, -0.032611750066280365, -0.02326340600848198, 0.009690847247838974, -0.02145014889538288, 0.01054374873638153, -0.008032053709030151, 0.2232857197523117, -0.003932079765945673, -0.015043310821056366, 0.013713589869439602, -0.005621094256639481, 0.0236260574311018, 0.030973102897405624, -0.004408898763358593, 0.001035906607285142, 0.0230216383934021, -0.01911306381225586, -0.009321480058133602, 0.0035492812748998404, 0.010228108614683151, -0.00014585799362976104, -0.019260810688138008, -0.04486130177974701, -0.014452323317527771, -0.010127372108399868, 0.004650666378438473, -0.012612204067409039, 0.020832300186157227, 0.0019106348045170307, -0.0023270121309906244, 0.030677609145641327, 0.020563669502735138, -0.008717061020433903, 0.024042434990406036, 0.02717198058962822, 0.021826231852173805, -0.006480711977928877, 0.003623154480010271, 0.0067493426613509655, 0.0195428729057312, -0.012894266285002232, -0.01078551635146141, -0.0007928798440843821, -0.012968139722943306, 0.0336325466632843, 0.00811935868114233, -0.017581868916749954, -0.047064073383808136, -0.030462704598903656, -0.0074209189042449, -0.023303700610995293, -0.014949290081858635, -0.001094669452868402, -0.03086565062403679, -0.012061512097716331, 0.01699088327586651, -0.022699281573295593, -0.0169640202075243, 0.01648048497736454, 0.02920014038681984, -0.0025771744549274445, -0.01292112935334444, 0.0015152442501857877, 0.016319306567311287, -0.04077811911702156, -0.0025385587941855192, 0.016977451741695404, 0.031886447221040726, -0.015594003722071648, 0.04359873756766319, 0.027346590533852577, 0.007085131015628576, 0.007206014357507229, 0.012437594123184681, 0.030973102897405624, -0.024123024195432663, 0.024485675618052483, -7.471287244698033e-05, 0.01920708455145359, 0.010261687450110912, -0.02617804706096649, -0.012390583753585815, 0.01508360542356968, 0.022981343790888786, 0.009167017415165901, 0.028636015951633453, -0.024472244083881378, 0.00115679029840976, 0.01614469662308693, 0.019072769209742546, -0.0008113482035696507, -0.019851798191666603, 0.02026817575097084, -0.01674911566078663, -0.004781623836606741, -0.0006980196922086179, -0.002078528981655836, -0.02287389151751995, -0.0010610907338559628, -0.012726372107863426, 0.010160950943827629, 0.013518832623958588, 0.009932614862918854, 0.01838776096701622, 4.247195829520933e-05, -0.003653375431895256, -0.01169214490801096, 0.06307445466518402, 0.016171559691429138, -0.008804365992546082, -0.020523374900221825, -0.004052963573485613, 0.02183966338634491, 0.0277226734906435, -0.017917657271027565, -0.008985691703855991, -0.0020583816803991795, -0.02774953655898571, -0.0013968788553029299, -0.016735684126615524, 0.0064068385399878025, -0.00540618970990181, 0.01711176708340645, -0.01686999946832657, 0.003292403183877468, 0.02359919436275959, 0.016641663387417793, -0.035486094653606415, -0.028850920498371124, 0.04222872108221054, 0.024942345917224884, -0.00626244954764843, -0.014680659398436546, -0.003905216697603464, 0.008173084817826748, -0.01157126110047102, -0.0013162896502763033, -0.006064334884285927, 0.025103524327278137, -0.012551762163639069, -0.008703629486262798, 0.02435136027634144, 0.027346590533852577, 0.003478765720501542, 0.004936086479574442, -0.005631167907267809, 0.01425085123628378, 0.005792346317321062, 0.008085779845714569, -0.008126074448227882, -0.008112642914056778, -0.02714511752128601, -0.003102682763710618, -0.009569963440299034, 0.004170489497482777, -0.04349128529429436, -0.005033465102314949, -0.013693442568182945, 0.010268403217196465, -0.009704278782010078, 0.04324951767921448, -0.010926547460258007, 0.007911169901490211, -0.052785903215408325, 0.0058997985906898975, 0.002185981022194028, -0.01590292900800705, 0.010154235176742077, 0.024257339537143707, 0.005476705264300108, -0.03435784578323364, 0.009462511166930199, -0.17213845252990723, 0.04558660462498665, 0.024740872904658318, -0.022363493219017982, 0.008455147035419941, -0.007159003987908363, 0.021893389523029327, 0.009126722812652588, -0.019704051315784454, 0.036399438977241516, 0.0327192023396492, -0.0012558478629216552, -0.004758118651807308, -0.0010233145439997315, 0.0028827416244894266, 0.001855229726061225, -0.005567368119955063, 0.004365246277302504, 0.00034921971382573247, 0.032128214836120605, 0.014452323317527771, -0.0009620331693440676, 0.0006799710681661963, -0.0015437862602993846, 0.005043538752943277, -0.00883122906088829, -0.011222041212022305, 0.01358599029481411, -0.002182623138651252, -0.011551113799214363, -0.03134918585419655, 0.030435841530561447, 0.04443149268627167, 0.015849202871322632, -0.004831992089748383, -0.003653375431895256, 0.005459915846586227, 0.004976381082087755, 0.0011928875464946032, 0.019918955862522125, 0.004976381082087755, -0.0018518718425184488, 0.00237402250058949, -0.0009217385668307543, 0.0025788533966988325, -0.004120121244341135, 0.02108749747276306, 0.014022515155375004, -0.01978464052081108, -0.02523783966898918, 0.0053692529909312725, -0.05297394469380379, 0.011799597181379795, 0.006319533567875624, -0.00717915128916502, 0.012806961312890053, 0.020308470353484154, 0.025130387395620346, 0.009287901222705841, -0.011504103429615498, -0.028877783566713333, -0.03519060090184212, 0.0021792652551084757, -0.005100622773170471, 0.008233526721596718, -0.021665053442120552, -0.007770138792693615, -0.028877783566713333, -0.010704927146434784, 0.015016447752714157, -0.004418972413986921, -0.012759950943291187, 0.021074065938591957, -0.02535872347652912, 0.03183272108435631, -0.008985691703855991, -0.02251124009490013, -0.0041973525658249855, -0.008220095187425613, 0.0009494411060586572, -0.014989584684371948, 0.014532912522554398, -0.0081798005849123, 0.024767735973000526, -0.02572137489914894, -0.002412638161331415, -0.0026594423688948154, 0.009744573384523392, 0.007985043339431286, -0.0034619763027876616, 0.010422865860164165, -0.037608277052640915, 9.428303019376472e-05, 0.0036433017812669277, -0.0011677034199237823, 0.014465754851698875, 0.01754157431423664, 0.024405086413025856, -0.004358530510216951, 0.0015320336678996682, 0.006786279380321503, -0.026795897632837296, -0.01781020499765873, 0.023639488965272903, 0.017165491357445717, -0.0031245090067386627, -0.007642539218068123, 0.028662879019975662, 0.014022515155375004, 0.00040021754102781415, -0.02989858016371727, 0.030032895505428314, 0.009408785030245781, 0.01102728396654129, -0.00897897593677044, 0.006897089537233114, -0.015795476734638214, -0.016775978729128838, 0.008515588939189911, 0.011470524594187737, 0.050932351499795914, 0.025761669501662254, 0.005584157537668943, 0.00014365438255481422, 0.006302744150161743, 0.006722479593008757, -0.0914955660700798, 0.025372155010700226, -0.001009043538942933, -0.003102682763710618, -0.010704927146434784, 0.022309767082333565, 0.014868700876832008, 0.04080498218536377, 0.00103758554905653, 0.024069298058748245, -0.016681957989931107, -0.009240890853106976, -0.007790286093950272, -0.006816500332206488, 0.0033914607483893633, -0.020590532571077347, -0.012074943631887436, -0.02611088939011097, -0.000547334726434201, 0.014344871044158936, -0.005547220818698406, -0.019032474607229233, 0.007911169901490211, -0.00268126861192286, -0.02714511752128601, -0.011792881414294243, -0.010980273596942425, 0.0070918467827141285, 0.018978748470544815, 0.006836647633463144, 0.013297212310135365, -0.01793108880519867, 0.0013272027717903256, -0.002249780809506774, 0.00021700312208849937, 0.028394250199198723, -0.0375545509159565, -0.00854245200753212, 0.023666352033615112, -0.020886026322841644, 0.002073492156341672, 0.002807189244776964, 0.004288014955818653, -0.017944520339369774, -0.004778265953063965, -0.010382571257650852, -0.015580572187900543, 0.027440611273050308, 0.010530317202210426, -0.02825993485748768, -0.012370436452329159, -0.0057755568996071815, -0.005540505051612854, -0.0031496931333094835, 0.025587059557437897, -0.0032420349307358265, -0.006668753456324339, 0.023088796064257622, -0.03134918585419655, 0.012417446821928024, -0.0007542642415501177, 0.026486972346901894, -0.010396002791821957, -0.0030640673357993364, 0.03320273756980896, 0.006131492555141449, -0.02599000558257103, -0.01860266551375389, -6.55836338410154e-05, -0.00638333335518837, -0.03470706567168236, 0.00219269678927958, -0.038091812282800674, 0.0033645976800471544, -0.025493038818240166, -0.007864159531891346, -0.007891022600233555, -0.014613501727581024, -0.009146870113909245, -0.0017209145007655025, 0.0002805929980240762, -0.010825810953974724, -0.024673717096447945, -0.013021865859627724, 0.022014273330569267, -2.880433021346107e-05, -0.0011122983414679766, -0.01007364597171545, -0.008260389789938927, -0.02304850146174431, 0.03631884977221489, 0.019892092794179916, -0.012773382477462292, 0.0009234175086021423, -0.02005327120423317, -0.004036174155771732, -0.03470706567168236, 0.0013481895439326763, 0.006578090600669384, 0.007011257577687502, -0.023411152884364128, -0.008992407470941544, -0.07629107683897018, 0.01768932119011879, 0.004701034631580114, -0.005594231188297272, 0.0038615642115473747, -0.02666158229112625, -0.0028474838472902775, -0.02526470273733139, -0.010288550518453121, 0.02326340600848198, -0.003285687416791916, 0.026030300185084343, -0.007078415248543024, 0.023773804306983948, -0.038091812282800674, -0.00442904606461525, 0.034035492688417435, -0.0072866035625338554, 0.015567140653729439, 0.022766439244151115, 0.010798947885632515, 0.0012273058528080583, 0.006658679805696011, 0.013418096117675304, -0.0023673067335039377, 0.03398176655173302, -0.023088796064257622, 0.013498685322701931, -0.025493038818240166, -0.004052963573485613, 0.019610030576586723, -0.023223111405968666, -0.001008204068057239, 0.028824057430028915, -0.02316938526928425, -0.0029448624700307846, 0.005325600504875183, 0.016373032703995705, 0.002951578237116337, -0.000821421854197979, -0.0054632737301290035, -0.02707795985043049, -0.016225285828113556, -0.019610030576586723, 0.012437594123184681, 0.0009695884073153138, -0.0023656277917325497, -0.002506658900529146, 0.029522497206926346, -0.0245394017547369, 0.013821042142808437, 0.01226970087736845, -0.011342925019562244, -0.012323427014052868, -0.0039152903482317924, -0.024458812549710274, -0.003325982019305229, -0.001739382860250771, 0.017581868916749954, 0.004321593791246414, 0.020039839670062065, 0.02695707604289055, 0.018710117787122726, -0.004177205264568329, 0.03468020260334015, -0.008529020473361015, -0.0063128178007900715, 0.018334034830331802, 0.0015379099640995264, -0.031886447221040726, -0.015594003722071648, -0.0034267185255885124, -0.0022917543537914753, 0.003482123604044318, 0.015594003722071648, 0.010731790214776993, 0.02444538101553917, 0.029280729591846466, -0.00578563055023551, 0.031644679605960846, 0.009120007045567036, 0.004482772201299667, -0.006453848909586668, 0.018522076308727264, 0.004795055370777845, 0.0006833289517089725, 0.004298088606446981, 0.0011727402452379465, -0.016977451741695404, 0.0036668069660663605, -0.027883851900696754, -0.000442400953033939, -0.007978327572345734, -0.0277226734906435, 0.0030355253256857395, 0.017823636531829834, -0.004402182996273041, -0.0233305636793375, 0.007669402286410332, 0.02174564264714718, 0.0043316674418747425, 0.014640364795923233, -0.008267105557024479, -0.019193653017282486, -0.035700999200344086, 0.011712292209267616, -0.011732439510524273, -0.0174206905066967, -5.002719262847677e-05, -0.006171787157654762, 0.0005620254669338465, 0.014532912522554398, -0.006917236838489771, 0.</t>
-  </si>
-  <si>
-    <t>What is Angelica James portfolio summary on 10-11-2023?</t>
-  </si>
-  <si>
-    <t>SELECT product.type AS account_type,  COUNT(CASE WHEN account.status = 'Open' THEN 1 END) AS open_accounts, COUNT(CASE WHEN account.status = 'Closed' THEN 1 END) AS closed_accounts, SUM(balance.balance) AS total_balances, AVG(balance.balance) AS month_to_date_avg_balance FROM account INNER JOIN product ON account.product_id = product.id INNER JOIN balance ON account.id balance.account_id INNER JOIN date ON balance.balance_dt_id = date.id INNER JOIN relationship ON account.id = relationship.account_id INNER JOIN client ON relationship.client_id = client.id  WHERE client.name = 'Angelica James'  AND date.date = '2023-10-11'  AND relationship.relationship_type = 'Primary'  GROUP BY product.type;</t>
-  </si>
-  <si>
-    <t>[0.0025598574429750443, -0.02730967290699482, -0.008025866001844406, -0.0176406092941761, 0.010904856957495213, 0.005995634011924267, -0.051821835339069366, 0.02444426156580448, -0.01766776852309704, -0.0006594858132302761, 0.02827386185526848, 0.003106458345428109, -0.006161991041153669, 0.0025683450512588024, 0.012011638842523098, -0.010531403124332428, 0.027472633868455887, -0.011719665490090847, 0.008046235889196396, -0.026359062641859055, -0.006715381983667612, 0.028246702626347542, 0.002935008844360709, 0.0007490299176424742, -0.01913442462682724, -0.004169104620814323, 0.012106699869036674, -0.02111712656915188, 0.00866413302719593, -0.01719246432185173, 0.012622744776308537, 0.004223425406962633, 0.001414881437085569, -0.016106052324175835, -0.0062400768510997295, -0.010232639499008656, 0.004437312483787537, 0.007917224429547787, 0.026005977764725685, 0.021864034235477448, 0.01557642687112093, 0.011400531977415085, 0.004220030270516872, -0.016649257391691208, -0.012059168890118599, 0.0028348553460091352, -0.019025783985853195, -0.03126149624586105, -0.027649175375699997, 0.014028290286660194, 0.015454205684363842, 0.008827094919979572, -0.0002993997768498957, -0.012765336781740189, 0.01864553987979889, -0.028599785640835762, -0.010612883605062962, 0.02895287051796913, 0.002863713074475527, 0.010938807390630245, 0.046199653297662735, -0.002833157777786255, -0.005988844204694033, -0.010626464150846004, -0.009057956747710705, -0.019691210240125656, -0.03145161643624306, 0.01868627965450287, -0.013885698281228542, 0.037182439118623734, 0.02170107327401638, 0.02448500134050846, 0.018170233815908432, -0.01772208884358406, 0.006885133683681488, -0.006844393443316221, -0.018889982253313065, -0.002887478331103921, -0.01997639425098896, -0.014204831793904305, 0.011869046837091446, -0.005611995235085487, 0.011386952362954617, -0.015073961578309536, 0.01573938876390457, 0.02076404169201851, 0.001616886118426919, 0.009268449619412422, -0.015943091362714767, 0.004742865916341543, 0.021755393594503403, 0.0017450486775487661, 0.012649905867874622, 0.0062400768510997295, -0.038812056183815, -0.00028433429542928934, -0.02191835455596447, -0.0006934361881576478, -0.006324952933937311, -0.017260365188121796, -0.0028942686039954424, -0.013036939315497875, -0.04285893961787224, -0.004562928806990385, -0.018971463665366173, -0.02487882599234581, -0.0020489045418798923, 0.021592430770397186, 0.020913423970341682, 0.0012307006400078535, -0.012690645642578602, 0.0031658713705837727, 0.02170107327401638, -0.03164174035191536, 0.01469371747225523, -0.03357011824846268, 0.005903968121856451, 0.01000856701284647, 0.029686197638511658, -0.0022967420518398285, 0.021022064611315727, 0.03726391866803169, 0.008127717301249504, -0.019650470465421677, 0.006695011630654335, 0.007102415896952152, 0.0044678677804768085, -0.03905649855732918, -0.009533261880278587, -0.00854870118200779, 0.011251150630414486, 0.01740974560379982, 0.01927022635936737, 0.004437312483787537, 0.015359144657850266, 0.003907687030732632, -0.018659120425581932, 0.016689999029040337, -0.008677712641656399, -0.03419480472803116, -0.0030368599109351635, 0.018088754266500473, -0.0051400852389633656, -0.010001776739954948, -0.004274350591003895, 0.005540699232369661, 0.01917516440153122, -0.0006662759114988148, 0.018373936414718628, 0.014652976766228676, -0.005995634011924267, 0.016418395563960075, -0.01652703620493412, -0.005129899829626083, -0.001481084618717432, 0.02011219598352909, 0.00923449918627739, 0.007767843082547188, 0.003639478934928775, -0.007509820628911257, 0.010266589932143688, 0.01590234972536564, 0.011339421384036541, 0.01613321341574192, 0.016404815018177032, 0.03579726442694664, 0.00221016863361001, 0.0001378172601107508, 0.0006985287182033062, -0.004165709484368563, -0.02474302425980568, 0.02811090089380741, -0.030120762065052986, 0.009553632698953152, -0.0002348940761294216, 0.033923204988241196, 0.009906715713441372, -0.007523400709033012, -0.018238134682178497, -0.0006212916341610253, 0.01012399885803461, 0.02443068102002144, 0.010965967550873756, 0.006644085980951786, -0.011706084944307804, -0.01952824927866459, 0.031967662274837494, -0.03297259286046028, -0.005255516152828932, -0.013193110935389996, -0.0005033141351304948, 0.02987631969153881, 0.002551369834691286, -0.003921267110854387, -0.6331607103347778, -0.015399884432554245, 0.010673994198441505, -0.025910917669534683, 0.01962330937385559, -0.007075255736708641, 0.0001321942254435271, -0.012439412996172905, -0.01595667004585266, -0.005411687772721052, 0.0034900973550975323, 0.0013189716264605522, -0.008521541021764278, -0.004172499757260084, -0.01745048724114895, -0.027635596692562103, 0.0013503757072612643, 0.0085283312946558, -0.0018638749606907368, -0.005055209156125784, -0.031533095985651016, 0.01591593027114868, -0.0020964350551366806, -0.01630975492298603, 0.018713440746068954, -0.01027338020503521, 0.009370299987494946, -0.03346147760748863, 0.009186968207359314, 0.00821598805487156, -0.008779563941061497, 0.027920778840780258, 0.018754180520772934, -0.023222047835588455, 0.03840465098619461, -0.00998819712549448, -0.016024570912122726, 0.013749897480010986, 0.017029501497745514, 0.042668815702199936, -0.03376024216413498, 0.013580145314335823, 0.008915365673601627, -0.01956898905336857, -0.020750463008880615, 0.021266506984829903, 0.011943737976253033, -0.010443131439387798, -0.012758546508848667, -0.009397461079061031, 0.021049225702881813, 0.023317109793424606, -0.008738823235034943, -0.014625816605985165, 0.004562928806990385, -0.022787483409047127, 0.009682643227279186, -0.004787001293152571, -0.008643762208521366, -0.012595584616065025, -0.0063589029014110565, -0.020750463008880615, -0.038513291627168655, -0.009207339026033878, 0.003067415440455079, 0.0075301905162632465, 0.002352760173380375, 0.018835661932826042, 0.01762702874839306, -0.017002342268824577, -0.011061028577387333, 0.020261576399207115, -0.008344999514520168, 0.026318321004509926, 0.004817556589841843, -0.012425833381712437, -0.006742542143911123, 0.0010108720744028687, 0.012778916396200657, 0.018061593174934387, 0.011977688409388065, -0.028219541534781456, -0.008317839354276657, 0.008983266539871693, 0.001431007869541645, 0.010877696797251701, -0.008609811775386333, -0.024403521791100502, 0.0010032332502305508, -0.005707056261599064, 0.018048012629151344, 0.011040657758712769, -0.002298439620062709, -0.032103464007377625, 0.009302400052547455, 0.0038499711081385612, -0.036476269364356995, -0.011271520517766476, -0.021633172407746315, -0.013064099475741386, 0.006494704633951187, 0.006722171790897846, 0.022434400394558907, 0.008311049081385136, 0.01603815145790577, -0.002829762874171138, -0.001713644596748054, 0.0003683614486362785, 0.01308447029441595, -0.023710934445261955, -0.025693634524941444, 0.010375231504440308, -0.004715705290436745, -0.021089965477585793, -0.014625816605985165, -0.031098533421754837, 0.026752887293696404, 0.003687009448185563, -0.01635049469769001, -0.01670357957482338, 0.016934441402554512, 0.00810734648257494, 0.016459135338664055, -0.019677631556987762, -0.01736900582909584, 0.00928202923387289, 0.021062806248664856, -0.013919648714363575, -0.035688623785972595, -0.005920943338423967, 0.006365693174302578, 0.0030096997506916523, 0.003259234828874469, -0.019052943214774132, 0.02974051795899868, 0.005255516152828932, 0.010993127711117268, -0.018659120425581932, 0.011067818850278854, -0.02443068102002144, -0.0014208226930350065, -0.011848676949739456, -0.0031692665070295334, 0.004559533670544624, -0.02301834709942341, -0.024810925126075745, 0.006589765660464764, 0.01341039314866066, -0.011896206997334957, 0.010721525177359581, -0.025462772697210312, 0.0008305107476189733, -0.0145579157397151, 0.023887475952506065, 0.0017467462457716465, -0.016201114282011986, -0.003958612214773893, -0.01042955182492733, 0.0068376031704247, -0.009112277999520302, -0.0005945557495579123, 0.004895642399787903, -0.009119067341089249, 0.00033483546576462686, 0.013899278827011585, 0.0017272247932851315, 0.012446203269064426, 0.01974553056061268, -0.013797427527606487, -0.009736964479088783, -0.007034515496343374, 0.0015056986594572663, -0.0033780611120164394, -0.007727102842181921, -0.0026684985496103764, 0.020207256078720093, 0.0152912437915802, -0.0006879192660562694, 0.015250503085553646, 0.0027245166711509228, -0.0030113973189145327, -0.023765254765748978, 0.0024087782949209213, -0.0006212916341610253, 0.03538985922932625, 0.0035749732051044703, -0.004403362050652504, 0.03601454570889473, -0.009451781399548054, -0.013308542780578136, -0.01221534051001072, 0.022067736834287643, -0.008847464807331562, 0.009465361014008522, -0.027540534734725952, -0.004128364380449057, 0.005523724015802145, -0.0015634142328053713, 0.005004283506423235, -0.010178319178521633, 0.011543123982846737, 0.003982377704232931, 0.008270308375358582, 0.01542704552412033, -0.022393660619854927, 0.009764124639332294, 0.010415971279144287, -0.021755393594503403, 0.02166033163666725, -0.016119632869958878, 0.029550395905971527, -0.02231217920780182, -0.005191010423004627, 0.014897419139742851, -0.006610135547816753, 0.0049295928329229355, 0.012765336781740189, 0.004260770510882139, -0.0176406092941761, 0.008311049081385136, -0.01891714334487915, 0.0007027725223451853, -0.010402391664683819, -0.02819238230586052, 0.006888528820127249, 0.004274350591003895, -0.002829762874171138, 0.005924338474869728, 0.0003694223996717483, -0.009295609779655933, -0.016146792098879814, 0.0045187934301793575, 0.02625042013823986, 0.0029587741009891033, 0.01772208884358406, -0.017110982909798622, 0.026902267709374428, -0.013661626726388931, 0.02917015179991722, 0.010348070412874222, -0.0026837761979550123, -0.0025479746982455254, 0.031044213101267815, 0.030283724889159203, -9.787252929527313e-05, -7.235671364469454e-05, 0.02338501065969467, 0.04256017506122589, 0.0014827820705249906, 0.011848676949739456, -0.031397297978401184, -0.002256001578643918, 0.0229368656873703, 0.0007817071164026856, 0.027554115280508995, -0.02779855765402317, -0.011210409924387932, 0.010986337438225746, 0.007238217629492283, 0.035634301602840424, 0.017029501497745514, 0.03204914182424545, 0.013145580887794495, -0.004844716750085354, 0.013064099475741386, -6.954519631108269e-05, -0.01785789057612419, 0.006946244277060032, -0.01697518117725849, -0.014449275098741055, -0.010327700525522232, -0.029224472120404243, 0.025476353242993355, -0.008236357942223549, -0.00470552034676075, 0.010035727173089981, 0.01458507589995861, -0.008535121567547321, -0.003714169841259718, -0.0012222130317240953, -0.025435611605644226, -0.05269096419215202, 0.030908411368727684, 0.006508284714072943, 0.00611106539145112, -0.006504889577627182, 0.029441755264997482, 0.002953681629151106, -0.01268385536968708, 0.053369972854852676, 0.017654189839959145, 0.011434482410550117, -0.003737935097888112, 0.014503595419228077, -0.00185368990059942, 0.005696870852261782, 0.02615536004304886, -0.014883839525282383, -0.03107137233018875, -0.014748037792742252, 0.02987631969153881, -0.023004766553640366, 0.02395537681877613, -0.01825171522796154, 0.03066396899521351, 0.011957317590713501, -0.009750544093549252, -0.014041869901120663, -0.01590234972536564, -0.019460348412394524, 0.014218412339687347, -0.01518260221928358, -0.021972674876451492, 0.0024715864565223455, 0.0004137700598221272, 0.013159160502254963, -0.011305470950901508, -0.021361568942666054, 0.01312521006911993, 0.028572626411914825, 0.0038431810680776834, -0.02399611659348011, -0.029360273852944374, 0.016051732003688812, 0.11179175972938538, 0.015440625138580799, -0.01016473863273859, 0.004006142728030682, -0.019922073930501938, 0.007618461735546589, 0.006711986847221851, 0.008175247348845005, -0.007217847276479006, -0.0006951336981728673, 0.007795003242790699, -0.01613321341574192, -0.01639123633503914, -0.007564140949398279, 0.013193110935389996, -0.0014097888488322496, 0.0018384121358394623, -0.010151159018278122, 0.002330692484974861, -0.005870017688721418, -0.0021660332567989826, -0.023873895406723022, -0.01846899837255478, 0.02930595353245735, 0.004253980703651905, -0.015807289630174637, 0.023235628381371498, -0.013552985154092312, -0.013681996613740921, -0.010212269611656666, 0.00624347198754549, -0.014259153045713902, 0.021198606118559837, -0.0030453475192189217, -0.015630748122930527, -0.002678683726117015, 0.019080104306340218, 0.001023603486828506, 0.03615034744143486, -0.005160455126315355, 0.006470939144492149, 0.021089965477585793, 0.0012977526057511568, -0.017599867656826973, 0.01073510479182005, -0.008718453347682953, -0.01944676786661148, 0.042451534420251846, 0.023941796272993088, 0.022746743634343147, 0.022475140169262886, 0.009825235232710838, -0.01648629643023014, -0.004990703426301479, 0.0023731302935630083, 0.013946808874607086, -0.013206691481173038, -0.01746406778693199, -0.03481949120759964, 0.005615389905869961, -0.018441837280988693, -0.006633901037275791, -0.008311049081385136, -0.03615034744143486, 0.018767761066555977, -0.04709594324231148, -0.02444426156580448, -0.019514668732881546, -0.0094110406935215, -0.026752887293696404, -0.0029553791973739862, -0.0016890305560082197, -0.010945596732199192, 0.026847947388887405, 0.027459053322672844, 0.00826351810246706, 0.022067736834287643, -0.014490014873445034, 0.008555491454899311, 0.02138872817158699, -0.0023442725650966167, -0.034004684537649155, -0.027784977108240128, -0.038160208612680435, 0.0032150994520634413, 0.005214775912463665, -0.001458168146200478, -0.010836956091225147, 0.008331418968737125, 0.026318321004509926, -0.006674641277641058, 0.007713522762060165, 0.015169022604823112, -0.02686152793467045, 0.012609165161848068, -0.008365369401872158, -0.006104275584220886, 0.008732033893465996, 0.00470552034676075, 0.012711016461253166, 0.008596232160925865, -0.026522023603320122, -0.008623392321169376, -0.03557997941970825, 0.009064747020602226, 0.0035749732051044703, -0.003605528501793742, 0.005656130611896515, -0.031234335154294968, -0.013118420727550983, 0.008019075728952885, -0.005510143935680389, -0.007971545681357384, 0.005421873182058334, -0.008161667734384537, 0.025394871830940247, 0.0016058521578088403, 0.0020675770938396454, -0.033868882805109024, -0.0007906191167421639, 0.006610135547816753, -0.009553632698953152, 0.018061593174934387, 0.032538026571273804, -0.004461077973246574, 0.018849242478609085, -0.017206044867634773, -0.004532373510301113, 0.0076456218957901, 0.006986984983086586, 0.013505454175174236, -0.0060805100947618484, -0.013179531320929527, -0.007842534221708775, -0.001953843515366316, -0.014082610607147217, -0.014422114007174969, 0.0015999109018594027, -0.004294720944017172, -0.023873895406723022, 0.011169669218361378, 0.011237570084631443, 0.0018604799406602979, -0.022040575742721558, 0.010477081872522831, -0.03017508238554001, -0.01825171522796154, -0.005951498635113239, 0.01089127641171217, 0.022773904725909233, -0.005853042472153902, 0.00522496085613966, -0.0015472878003492951, -0.0034255916252732277, -0.019066523760557175, 0.0018927328055724502, 0.008575862273573875, -0.022067736834287643, 0.012520894408226013, 0.03663923218846321, 0.03544417768716812, -0.009458571672439575, 0.011509173549711704, 0.010789425112307072, 0.003578368341550231, 0.00462743453681469, -0.022638102993369102, -0.009472151286900043, -0.015657907351851463, 0.013016569428145885, -0.000705743208527565, 0.004478052724152803, -0.01237151212990284, -0.016499876976013184, 0.02134798839688301, 0.006813838146626949, -0.012106699869036674, -0.019650470465421677, -0.030528167262673378, -0.02629116177558899, -0.007319698575884104, -0.010646834038197994, -0.010375231504440308, -0.0005669710808433592, -0.040061429142951965, 0.0013741409638896585, 0.022420819848775864, 0.014299892820417881, 0.015046801418066025, -0.00923449918627739, 0.019025783985853195, 0.02779855765402317, 0.031180012971162796, -0.010443131439387798, -0.018835661932826042, 0.0037583052180707455, -0.016717158257961273, -0.019433187320828438, -0.0021881009452044964, 0.0068206279538571835, -0.006898713763803244, 0.02046527899801731, 0.015617167577147484, 0.021008484065532684, 0.009397461079061031, 0.00720426719635725, 0.0018231344874948263, -0.01482951920479536, 0.009377090260386467, -0.00954684242606163, 0.01652703620493412, -0.017260365188121796, -0.025286231189966202, -0.025164010003209114, 0.05220207944512367, -0.018808500841259956, -0.03283679112792015, 0.019052943214774132, -0.00967585388571024, 0.0070616756565868855, 0.007985125295817852, -0.009349930100142956, 0.03022940456867218, 0.02903435006737709, 0.030636807903647423, 0.041745368391275406, 0.025286231189966202, -0.009947456419467926, 0.010796215385198593, 0.010952387005090714, -0.002430845983326435, 0.016540616750717163, 0.029197312891483307, -0.015060381032526493, -0.0031539888586848974, 0.011916577816009521, 0.023004766553640366, -0.02965903840959072, -0.0008716755546629429, -0.004539163783192635, -0.002026836620643735, 0.011556703597307205, -0.0136752063408494, -0.014177671633660793, -0.007367229089140892, 0.008460430428385735, -0.0016839380841702223, -0.007849324494600296, -0.0043592266738414764, -0.0331355556845665, 0.00559162488207221, -0.010551773011684418, 0.001648290199227631, 0.01011720858514309, -0.00305383512750268, -0.0019742136355489492, -0.01089127641171217, -0.018414678052067757, 0.020220836624503136, 0.02178255282342434, -0.03596022352576256, 0.020655401051044464, -0.007625251542776823, 0.02656276524066925, -0.004074043594300747, 0.007469079922884703, -0.007428339682519436, 0.0022237487137317657, 0.033515799790620804, 0.024675123393535614, -0.03691083565354347, -0.007761053275316954, 0.02041095867753029, -0.017871471121907234, 0.009248078800737858, 0.026141779497265816, 0.003737935097888112, -0.022339338436722755, -0.013335702940821648, -0.009607953019440174, 0.008786354213953018, -0.012099909596145153, -0.011414112523198128, 0.0026379432529211044, 0.005126504693180323, -0.008806724101305008, -0.005968473851680756, -0.013573355041444302, 0.0006853729719296098, -0.029088672250509262, -0.0273504126816988, -0.00580211728811264, 0.005374342668801546, 0.024335620924830437, 0.017871471121907234, 0.002427451079711318, 0.02201341651380062, 0.008976476266980171, -0.011570284143090248, 0.004376201890408993, -0.00470552034676075, -0.003330530598759651, -0.030881250277161598, -0.0033475058153271675, -0.032456547021865845, -0.008093766868114471, 0.029088672250509262, -0.013451133854687214, -0.027689917013049126, -0.02965903840959072, 0.010823375545442104, 0.015250503085553646, -0.009628322906792164, -0.004647804889827967, -0.01032091025263071, -0.006284212227910757, -0.0024019882548600435, 0.0031862417235970497, -0.022081315517425537, 0.017138144001364708, 0.003527442691847682, 0.0019402633188292384, 0.006487914361059666, -0.02585659734904766, 0.02827386185526848, -0.011366581544280052, 0.0064811245538294315, -0.007374018896371126, 0.00943141058087349, -0.03183186054229736, -0.003147198585793376, 0.012649905867874622, 0.011162879876792431, 0.006525259930640459, -0.019894912838935852, -0.003945032134652138, -0.008888205513358116, 0.03680219501256943, 0.01542704552412033, -0.01572580821812153, 0.008460430428385735, 0.005418478045612574, 0.009397461079061031, 0.013444343581795692, -0.012167810462415218, -0.032538026571273804, -0.028572626411914825, -0.0431305430829525, -0.020343057811260223, 0.008623392321169376, 0.0028603181708604097, 0.013688786886632442, 0.022991186007857323, -0.040903396904468536, -0.020791202783584595, -0.007543770596385002, -0.037535522133111954, -0.03389604389667511, -0.03585158288478851, 0.03172321990132332, 0.009967826306819916, -0.003659849287942052, 0.019650470465421677, 0.019283806905150414, 0.014123351313173771, 0.0062400768510997295, -0.023493651300668716, -0.0028705033473670483, 0.024362780153751373, -0.016812220215797424, 0.009424621239304543, 0.013138790614902973, -0.03805156797170639, -0.01975911110639572, 0.003198124235495925, 0.019148005172610283, -0.009804865345358849, 0.008806724101305008, -0.0074419197626411915, -0.01497890055179596, -0.01413693092763424, 0.02333069033920765, 0.0009998382302001119, 0.020614661276340485, 0.005330207291990519, -0.030826929956674576, 0.0010830166283994913, 0.0048990375362336636, -0.005683290772140026, -0.0019080104539170861, 0.024417102336883545, 0.004966938402503729, -0.023588713258504868, -0.013566565699875355, -0.030745448544621468, 0.0022780694998800755, -0.004674965050071478, 0.02284180372953415, 0.022325759753584862, 0.0016678116517141461, 0.0025496722664684057, 0.02819238230586052, 0.016323335468769073, -0.010395601391792297, -0.00418607983738184, 0.004963543266057968, -0.02174181304872036, -0.027336832135915756, 0.032456547021865845, -0.009601162746548653, 0.017260365188121796, -0.016024570912122726, -0.004230215214192867, -0.0058802030980587006, -0.00883388426154852, 0.00176711636595428, -0.009472151286900043, -0.013396813534200191, 0.005836067255586386, -0.009709804318845272, -0.004040093161165714, -0.0069598243571817875, 0.0039178719744086266, -0.03340715914964676, -0.013050519861280918, -0.017165303230285645, 0.004009537864476442, -0.014204831793904305, -0.01599741168320179, 0.027689917013049126, -0.032945431768894196, -0.023303529247641563, 0.00418607983738184, -0.00590057298541069, 0.01208632905036211, 0.018971463665366173, 0.22238846123218536, 0.009200548753142357, -0.010497452691197395, 0.03169605880975723, -0.015522106550633907, 0.03221210464835167, 0.035552822053432465, 0.02805658057332039, 0.01909368485212326, 0.018170233815908432, -0.001453924342058599, -0.010823375545442104, 0.002887478331103921, -0.0078017935156822205, -0.0041385493241250515, -0.026657825335860252, -0.03536269813776016, -0.005078974179923534, -0.006766307633370161, -0.011210409924387932, 0.0049499631859362125, 0.005031443666666746, 0.006250261794775724, -0.017206044867634773, 0.04467867687344551, 0.0027228191029280424, -0.014680136926472187, 0.026128198951482773, -0.005992239341139793, 0.006338533014059067, -0.00795796513557434, 0.00923449918627739, 0.008148087188601494, 0.014340633526444435, -0.010633253492414951, -0.019718371331691742, -0.005785142071545124, 0.016255434602499008, 0.0015073961112648249, 0.019256645813584328, -0.019786272197961807, -0.004610459320247173, -0.001655080239288509, -0.018985042348504066, -0.003608923638239503, 0.03283679112792015, -0.004576508887112141, -0.021673912182450294, -0.021633172407746315, 0.020438117906451225, -0.03180469945073128, 0.007285748142749071, 0.034439247101545334, 0.001345283119007945, -0.01381100807338953, 0.008962895721197128, 0.0511699877679348, -0.016201114282011986, -0.0273504126816988, -0.0004659687401726842, -0.016676418483257294, 0.027010908350348473, -0.024688703939318657, 0.020275156944990158, 0.02713313139975071, 0.01772208884358406, 0.017925791442394257, 0.012147439643740654, 0.02037021890282631, -0.010592513717710972, 0.01935170777142048, 0.0005355670000426471, -0.006718777120113373, 0.0020336266607046127, -0.03381456062197685, -0.02280106395483017, 0.02876274846494198, 0.023792413994669914, 0.038431812077760696, 0.006854578386992216, 0.005954893771559, 0.00886104442179203, -0.004046883434057236, 0.014680136926472187, -0.0011933553032577038, -0.03644911199808121, 0.006195941474288702, -0.014748037792742252, 0.00042353078606538475, -0.004865087103098631, 0.008209197781980038, -0.02960471622645855, -0.04114783927798271, -0.02797509916126728, 0.010843746364116669, 0.024050436913967133, 0.013098049908876419, 0.04486880078911781, -0.017572708427906036, -0.015929510816931725, -0.024145498871803284, 0.026807207614183426, -0.002435938687995076, -0.013620886020362377, -0.02426772005856037, -0.0018010667990893126, -0.03009360283613205, -0.00013240642147138715, 0.009465361014008522, -0.021022064611315727, -0.00491601275280118, -0.01572580821812153, 0.008480801247060299, -0.01578012853860855, -0.0031268284656107426, 0.010246220044791698, 0.020383797585964203, -0.016948021948337555, 0.029333114624023438, -0.0008496078662574291, -0.039436742663383484, -0.032592348754405975, -0.0010320910951122642, -0.0027924173045903444, 0.01085053663700819, -0.0403873510658741, 0.0020607870537787676, -0.020098615437746048, 0.013946808874607086, -0.03101705200970173, 0.03191334009170532, -0.01413693092763424, 0.02889855019748211, -0.0008559735142625868, -0.0014123350847512484, 0.020207256078720093, -0.011529543437063694, 0.022570202127099037, -0.017436906695365906, -0.01409619115293026, -0.007102415896952152, -0.012412252835929394, 0.02550351247191429, -0.008093766868114471, 0.014951740391552448, -0.0205875001847744, 0.010626464150846004, -0.019813431426882744, -0.003608923638239503, -0.019188744947314262, -0.019161585718393326, -0.019894912838935852, -0.00863697286695242, 0.0305824875831604, 0.028083739802241325, 0.014503595419228077, -0.0008631880045868456, -0.02805658057332039, 0.023276370018720627, -0.012303612194955349, -0.017301104962825775, 0.01984059251844883, 0.012690645642578602, 0.011319051496684551, -0.019066523760557175, 0.023968957364559174, -0.1737172156572342, 0.02107638493180275, 0.015793709084391594, -0.03495529294013977, 0.027540534734725952, -0.009417830966413021, 0.031533095985651016, -0.012588794343173504, -0.019731951877474785, -0.0014157301047816873, 0.021266506984829903, -0.0015260688960552216, -0.026019558310508728, -0.03682935610413551, 0.0014352516736835241, 0.017124563455581665, -0.021320829167962074, 0.03085409104824066, 0.02064182050526142, 0.022882545366883278, 0.005886992905288935, -0.011543123982846737, 0.014490014873445034, -0.005737611558288336, 0.011862256564199924, 0.010171528905630112, -0.012609165161848068, 0.015698648989200592, 0.009961036965250969, 0.014951740391552448, -0.02995780110359192, -0.014775197952985764, 0.029088672250509262, -0.008935735560953617, 0.005778351798653603, 0.005761376582086086, -0.02364303357899189, 0.0067629124969244, -0.020804783329367638, 0.031180012971162796, 0.01666283793747425, 0.02846398390829563, 0.0023035320919007063, 0.0033712710719555616, -0.04910580441355705, 0.0022814644034951925, 0.011563493870198727, 0.005622180178761482, 0.01948750950396061, -0.037671323865652084, 0.016106052324175835, -0.04484163969755173, 0.030066441744565964, 0.0035647882614284754, 0.01798011176288128, 0.017572708427906036, 0.01011720858514309, 0.025707215070724487, 0.014815938659012318, -0.02770349569618702, -0.0023425749968737364, -0.00821598805487156, -0.011943737976253033, -0.018061593174934387, -0.0074419197626411915, -0.007374018896371126, -0.021619591861963272, 0.01204558927565813, -0.015209763310849667, 0.02011219598352909, 0.010348070412874222, -0.02005787566304207, 0.012629535049200058, -0.012446203269064426, 0.014490014873445034, -8.731608977541327e-05, -0.02995780110359192, 0.023575132712721825, 0.01842825673520565, 0.010395601391792297, -0.005061999429017305, 0.020872684195637703, -0.008779563941061497, -0.0018944302573800087, 0.0024715864565223455, 0.013777057640254498, 0.01856405846774578, 0.010843746364116669, 0.018170233815908432, -0.0007948628626763821, 0.012405462563037872, -0.02377883531153202, 0.01252768374979496, -0.019148005172610283, -0.010843746364116669, -0.003252444788813591, 0.012296821922063828, 0.00894931610673666, -0.012106699869036674, -0.016852959990501404, 0.009614743292331696, -0.004250585567206144, 0.00044262787560001016, -0.007054885383695364, 0.024987466633319855, 0.006094090174883604, 0.018536899238824844, 0.016160372644662857, 0.02068256214261055, -0.01842825673520565, -0.004810766316950321, 0.0012536172289401293, 0.00699377479031682, 0.0152912437915802, -0.01321348175406456, 0.026454122737050056, -0.011319051496684551, -0.007815374061465263, 0.015454205684363842, -0.020750463008880615, 0.04321202263236046, 0.01027338020503521, -0.01325422152876854, -0.002116805175319314, -0.030147923156619072, -0.02744547463953495, -0.0966363176703453, -0.008127717301249504, -0.00819561816751957, 0.019813431426882744, 0.00821598805487156, 0.002826367737725377, -0.001233246992342174, -0.013973969966173172, -0.007516610436141491, 0.020315896719694138, 0.005143479909747839, -0.02686152793467045, -0.005058604292571545, 0.0020438118372112513, 0.02271958254277706, -0.017423326149582863, -0.013267802074551582, -0.001511639915406704, 0.010415971279144287, 0.021225767210125923, -0.00018460510182194412, -0.017735669389367104, 0.0038669463247060776, -0.011570284143090248, -0.01578012853860855, -0.013138790614902973, -0.01599741168320179, 0.026617085561156273, 0.00958758220076561, 0.007312908302992582, 0.008283888921141624, -0.016201114282011986, 0.0003093726991210133, -0.023833155632019043, -0.009580792859196663, -0.03395036235451698, -0.025354132056236267, -0.012493733316659927, -0.005411687772721052, -0.04389103129506111, 0.01660851761698723, 0.021728232502937317, 0.021796133369207382, -0.02876274846494198, 0.00039594611735083163, -0.02236649952828884, 0.005265701562166214, 0.010694364085793495, -0.006175571121275425, -0.026725726202130318, -0.03172321990132332, 0.0034137091133743525, 0.003907687030732632, -0.006464149337261915, 0.01834677718579769, 0.017735669389367104, 0.003038557479158044, 0.011013497598469257, 0.003605528501793742, 0.0024410311598330736, -0.026888687163591385, 0.0012400370324030519, -0.02399611659348011, -0.009363510645925999, 0.025639314204454422, -0.0038907115813344717, -0.007285748142749071, 0.003442566841840744, 0.016228273510932922, -0.03981698676943779, -0.005442243069410324, 0.02995780110359192, -0.015793709084391594, 0.004766630940139294, -0.032592348754405975, -0.008609811775386333, -0.012310401536524296, -0.018143074586987495, 0.014924580231308937, -0.0029978170059621334, -0.02201341651380062, -0.02019367553293705, 0.00047318320139311254, 0.01723320409655571, 0.029360273852944374, 0.009641903452575207, -0.012493733316659927, -0.0185233186930418, 0.019148005172610283, -0.02572079561650753, 0.018401097506284714, 0.04011575132608414, 0.0036462689749896526, -0.011998058296740055, -0.02678004652261734, 0.005975264124572277, -0.01398754958063364, -0.011902997270226479, -0.011414112523198128, 0.026630664244294167, -0.02633190155029297, 0.0144085343927145, -0.08289320766925812, 0.040278710424900055, 0.004787001293152571, -0.0071499464102089405, -0.007795003242790699, 0.016581358388066292, 0.01692086085677147, -0.003322042990475893, -0.003663244191557169, 0.03536269813776016, -0.01354619488120079, -0.010035727173089981, -0.0032507472205907106, 0.023520812392234802, 0.014231991954147816, -0.02081836201250553, 0.027771396562457085, -0.016594937071204185, 0.01056535355746746, -0.013614095747470856, -0.01715172454714775, 0.010925226844847202, 0.020845523104071617, 0.011678924784064293, 0.0036530590150505304, 0.02350723184645176, -0.024634383618831635, -0.001914800493977964, -0.013919648714363575, -0.029414594173431396, 0.014775197952985764, -0.01148880273103714, 0.004488238133490086, 0.0378342866897583, -0.000822023197542876, -0.03517257794737816, -0.001972516067326069, 0.03359727934002876, -0.005707056261599064, -0.0017340148333460093, -0.014748037792742252, -0.0016839380841702223, 0.013736316934227943, -0.004671569913625717, 0.006036374717950821, 0.013715947046875954, -0.012364722788333893, -0.007815374061465263, 0.02338501065969467, 0.006688221823424101, 0.004736075643450022, 0.006966614630073309, -0.002926521236076951, -0.011672134511172771, -0.0006781585398130119, -0.005167245399206877, 0.0366663932800293, 0.002454611239954829, -0.012846817262470722, 0.003883921541273594, 0.01644555665552616, 0.0014038474764674902, -0.014340633526444435, -0.014503595419228077, -0.0031845441553741693, 0.0052589112892746925, -0.015793709084391594, 0.018143074586987495, 0.00943141058087349, -0.030555326491594315, -0.02987631969153881, -0.011923368088901043, 0.001058402587659657, 0.046688538044691086, 0.009804865345358849, 0.0006947093061171472, 0.012907927855849266, 0.011672134511172771, -0.014082610607147217, 0.022882545366883278, 0.024715865030884743, -0.012846817262470722, 0.010422761552035809, -0.00048591458471491933, 0.000414831010857597, 0.010191898792982101, -0.029360273852944374, 0.010307330638170242, -0.014204831793904305, 0.006874948740005493, -0.009533261880278587, -0.009669063612818718, -0.0037786755710840225, 0.0007167770527303219, 0.006521864794194698, -0.012378302402794361, -0.0007299327990040183, 0.004253980703651905, 0.009669063612818718, 0.0349009744822979, 0.008562281727790833, 0.002437636023387313, 0.00213208282366395, 0.0026311532128602266, -0.01927022635936737, 0.013865328393876553, 0.006678036414086819, -0.029088672250509262, 0.010348070412874222, -0.007767843082547188, -0.00020858253992628306, 0.012235711328685284, -0.007835743948817253, 0.0014369491254910827, -0.020003553479909897, 0.0154270455</t>
-  </si>
-  <si>
-    <t>Which clients are members of Angelica James household?</t>
-  </si>
-  <si>
-    <t>SELECT client.ID, client.Client_ID, client.Person_Org, client.Name, client.SSN, address.Address, address.City, address.State, address.Zip  FROM client INNER JOIN address ON client.Address_ID = address.ID  INNER JOIN HH ON client.HH_ID = HH.ID WHERE HH.Name = 'Angelica James';</t>
-  </si>
-  <si>
-    <t>[0.011297153308987617, -0.012586276046931744, 0.0033891459461301565, -0.015012044459581375, 0.007880283519625664, 0.026378504931926727, 0.014693229459226131, 0.012413006275892258, -0.0029421113431453705, -0.033794429153203964, -0.012939744628965855, -0.005814915057271719, -0.008462468162178993, 0.003642119001597166, -0.023758674040436745, 0.017812075093388557, 0.01387539878487587, -0.0041549960151314735, 0.02730722911655903, -0.026655735448002815, -0.01926753669977188, 0.03190925717353821, 0.010811999440193176, 0.007311961147934198, -0.03301818296313286, -0.0124476607888937, 0.0017950690817087889, -0.016176413744688034, -0.007104037795215845, -0.00507332244887948, -0.0018227921100333333, -0.015261552296578884, 0.00570055702701211, 0.0024257691111415625, -0.014831844717264175, 0.005974322557449341, 0.012253599241375923, 0.005007480271160603, 0.028097335249185562, 0.039727166295051575, 0.024022044613957405, -0.013508068397641182, 0.004567376337945461, -0.022774506360292435, -0.027293367311358452, 0.003922814968973398, -0.005336692091077566, -0.008871383965015411, -0.0210556760430336, 0.007478299550712109, 0.026198305189609528, 0.011484283953905106, -0.0019908633548766375, -0.027903273701667786, -0.0052777803502976894, 0.0013367719948291779, -0.004626288078725338, 0.019156644120812416, 0.015289275906980038, 0.01210805308073759, 0.03875685855746269, 0.017562568187713623, -0.016966521739959717, -0.013085290789604187, -0.014845706522464752, 0.007672361098229885, -0.005589664913713932, 0.00655650720000267, -0.004917380400002003, 0.018990306183695793, 0.0362340584397316, 0.009578322060406208, -0.0005765533423982561, -0.01904575154185295, -8.00287161837332e-05, -0.028582489117980003, -0.006663933862000704, -0.02413293719291687, -0.020806167274713516, 0.004778765141963959, 0.01530313678085804, -0.004886191803961992, -0.01904575154185295, 0.0035294939298182726, 0.027362674474716187, 0.0026856728363782167, -0.034154828637838364, 0.007201068568974733, -0.016703153029084206, 0.017950691282749176, 0.026794351637363434, 0.01530313678085804, 0.007977314293384552, 0.005728280171751976, -0.026932967826724052, -0.00253666122443974, -0.022109152749180794, 0.01673087477684021, -0.014665506780147552, -0.0026250286027789116, -0.019697245210409164, -0.0024378979578614235, -0.048515379428863525, -0.003725288202986121, -0.003380482317879796, 0.0015342988772317767, -0.01860218308866024, -0.010957545600831509, 0.014873429201543331, -0.01113081444054842, -0.026350783184170723, 0.01104071456938982, 0.026198305189609528, -0.03673307225108147, 0.02355075255036354, -0.019322983920574188, 0.014249660074710846, -0.006618883926421404, 0.0030374093912541866, 0.004279749467968941, 0.00838623009622097, 0.02765376679599285, 0.009183268062770367, -0.002309678588062525, 0.005894618574529886, 0.0033163728658109903, -0.005149560980498791, -0.026919106021523476, -0.030800335109233856, -0.002032447839155793, 0.01962793618440628, 0.003267857478931546, 0.02725178189575672, 0.003087657503783703, -0.007443645503371954, -0.0006995744770392776, -0.008157514967024326, 0.025934936478734016, -0.003335432382300496, -0.012724891304969788, -0.006071353331208229, 0.023897290229797363, 0.006182245444506407, 0.00783176813274622, 0.0008845393313094974, 0.017770491540431976, 0.014194213785231113, 0.006438684184104204, 0.010784275829792023, -0.00847632996737957, -0.019073475152254105, 0.004210441838949919, 0.004626288078725338, -0.021263597533106804, 0.018546737730503082, 0.008885245770215988, 0.005478772800415754, 0.02240024507045746, -0.0236061979085207, -0.012773406691849232, -0.03229738026857376, 0.029053783044219017, 0.011421906761825085, -0.0038535073399543762, 0.02827753685414791, 0.031216181814670563, 0.0007948725251480937, 0.0002891430049203336, -0.015621952712535858, 0.0021520035807043314, -0.012170429341495037, 0.010666453279554844, -0.00739513011649251, 0.021651720628142357, -0.007596122566610575, -0.012988260015845299, 0.003964399453252554, -0.020154675468802452, -0.0011323143262416124, -0.01842198334634304, 0.0020289826206862926, 0.017992274835705757, -0.0053956033661961555, 0.012218944728374481, -0.01037536095827818, 0.0017300931503996253, 0.0058287763968110085, -0.03573504462838173, 0.011276360601186752, -0.017867522314190865, 0.004123807419091463, 0.01815861463546753, 0.0008139321580529213, -0.03193698078393936, -0.6329732537269592, -0.018130891025066376, 0.02119429036974907, -0.004584703594446182, 0.02113884501159191, 0.018851689994335175, 0.016619984060525894, -0.00012951873941347003, -0.013535791076719761, 0.009003068320453167, 0.002768842037767172, 0.021152706816792488, 0.005589664913713932, -0.0038812304846942425, -0.019322983920574188, -0.03202015161514282, -0.00946049951016903, 0.008552568964660168, -0.01146349124610424, -0.013612030074000359, -0.023218074813485146, 0.0037148920819163322, 0.0074990917928516865, -0.017950691282749176, 0.023661645129323006, -0.010319914668798447, -0.008975345641374588, -0.02877655066549778, 0.006199572701007128, 0.01663384400308132, -0.023523028939962387, 0.03762021288275719, 0.03249144181609154, 0.002489878563210368, 0.04130738228559494, 0.006362445652484894, -0.016301168128848076, 0.02935873530805111, 0.010541698895394802, 0.027293367311358452, -0.05361642688512802, 0.01765959896147251, 0.04058657959103584, -0.0026146324817091227, 0.009141683578491211, 0.039283595979213715, 0.00651145726442337, 0.009730799123644829, -0.010507045313715935, 0.012038744986057281, 0.00047822302440181375, 0.01601007580757141, -0.039505381137132645, -0.003662911243736744, 0.020085368305444717, -0.019433874636888504, 0.010597145184874535, -0.0006952427211217582, -0.011962506920099258, 0.009855552576482296, -0.0009781047701835632, -0.015594229102134705, -0.02582404389977455, -0.024160658940672874, 0.009176338091492653, 0.018976444378495216, -0.021180428564548492, 0.013182321563363075, -0.0029542401898652315, -0.007152553182095289, 0.004830745980143547, 0.02899833582341671, -0.023703228682279587, 0.03689941391348839, -0.013736783526837826, 0.015677398070693016, -0.009425844997167587, 0.011331806890666485, 0.0031881534960120916, 0.018311090767383575, -0.02721019834280014, -0.02199826017022133, -0.012953606434166431, -0.004359453450888395, 0.018976444378495216, -0.004917380400002003, -0.018574459478259087, -0.029830029234290123, 0.019073475152254105, -0.04532722756266594, 0.017008107155561447, 0.0034082054626196623, -0.017202168703079224, -0.017742767930030823, 0.014956599101424217, -0.004283214919269085, -0.04003211855888367, 0.0020480421371757984, -0.006050561089068651, -0.01691107638180256, 0.026932967826724052, -0.01411797571927309, 0.01856059767305851, -0.0020705671049654484, -0.0004180119722150266, -0.0013428364181891084, -0.007478299550712109, 0.015206106007099152, 0.01860218308866024, -0.019697245210409164, 0.005454515106976032, 0.00939119141548872, 0.006996611133217812, -0.032408274710178375, -0.02801416628062725, -0.03301818296313286, 0.022760644555091858, 0.007672361098229885, -0.022330936044454575, -0.02885972149670124, 0.009647630155086517, 0.0017335584852844477, -0.01454075239598751, -0.026295335963368416, 0.018435845151543617, 0.0015247691189870238, -0.004969361238181591, -0.024590367451310158, -0.005198076367378235, -0.00284334784373641, 0.006123334169387817, 0.005017876625061035, 0.006251553539186716, -0.02551908977329731, 0.013729852624237537, 0.017299199476838112, 0.020002197474241257, -0.012863506563007832, 0.028180506080389023, -0.007554537616670132, 0.016037799417972565, -0.010562491603195667, 0.005381742026656866, 0.009287229739129543, -0.01030605286359787, -0.04094698280096054, -0.0010344171896576881, 0.006296603474766016, -0.036649905145168304, -0.010319914668798447, -0.008912968449294567, 0.010569422505795956, -0.012329837307333946, 0.020501213148236275, 0.01663384400308132, -0.007748599164187908, -0.013993222266435623, -0.020459629595279694, 0.011248637922108173, 0.005378276575356722, 9.0627918325481e-06, 0.014513029716908932, -0.0035762765910476446, -0.01077041495591402, 0.029719136655330658, 0.005911945831030607, 0.0047059920616447926, -0.006306999363005161, -0.00382578419521451, -0.008940691128373146, 0.015289275906980038, -0.0017777421744540334, -0.011186260730028152, 0.00045483169378712773, -0.004082222934812307, 0.03251916542649269, -0.019655659794807434, 0.0034203343093395233, -0.00382578419521451, 0.009425844997167587, 0.005918876267969608, -0.00820603035390377, -0.011151607148349285, 0.0039020227268338203, 0.030717166140675545, -0.006670864764600992, 0.004290145821869373, 0.03127162903547287, -0.0002936913224402815, -0.007131760939955711, -0.010111991316080093, 0.029192397370934486, -0.008240683935582638, 0.005437187850475311, -0.008393160998821259, -0.011629830114543438, 0.01820019818842411, 0.008510983549058437, 0.007734737824648619, -0.009217922575771809, 0.040392518043518066, -0.005198076367378235, 0.028360705822706223, -0.014305106364190578, 0.022455690428614616, -0.021984398365020752, 0.0086981151252985, -0.019336843863129616, 0.04435691982507706, -0.009529806673526764, 0.012205083854496479, -0.012565483339130878, -0.0017656133277341723, 0.004879261367022991, -0.0004951168084517121, -0.005839172750711441, 0.01222587563097477, 0.01454075239598751, -0.006275811232626438, 0.005253522656857967, -0.0059916493482887745, 0.0033839477691799402, 0.005409465171396732, 0.004511930514127016, 1.9425103801040677e-06, -0.00617878045886755, -0.00469559570774436, -0.0004258090921211988, 0.015247691422700882, 0.00863573793321848, -0.019821997731924057, -0.005180749576538801, 0.022538859397172928, 0.009599114768207073, 0.005617388058453798, -0.033212244510650635, 0.029331013560295105, -0.0023772537242621183, 0.01735464483499527, -0.01900416798889637, -0.013064499013125896, 0.0068787881173193455, 0.012080329470336437, 0.02787555195391178, 0.03969944268465042, 0.0010647393064573407, 0.01623186096549034, 0.02734881266951561, -0.003416868858039379, 0.013556583784520626, -0.004103015176951885, -0.001584546989761293, -0.007235722616314888, 0.03637267276644707, 0.023897290229797363, -0.017520982772111893, 0.01806158386170864, 0.007374337874352932, 0.011089229956269264, 0.03418255224823952, 0.021305182948708534, 0.005107976496219635, -0.0014364018570631742, -0.017507120966911316, 0.02002992108464241, 0.021610137075185776, -0.02256658300757408, -0.006362445652484894, -0.017950691282749176, -0.012163499370217323, -0.01476253755390644, -0.025727013126015663, 0.013404106721282005, -0.0024015114177018404, 0.025130966678261757, 0.0037841997109353542, -0.001116720144636929, -0.0006969754467718303, 0.00369063438847661, 0.015511060133576393, -0.006331257056444883, -0.03795288875699043, 0.016855629161000252, 0.009751591831445694, 0.0005453648627735674, -0.002067101653665304, 0.0010058277985081077, 0.0028935959562659264, -0.010943683795630932, 0.04094698280096054, 0.030994396656751633, 0.012821922078728676, -0.012974399141967297, 0.012620929628610611, -0.009405053220689297, 0.010777344927191734, -0.007880283519625664, -0.018089305609464645, 0.0009997633751481771, -0.007492160890251398, 0.006546110846102238, -0.010098129510879517, -0.007589191664010286, -0.0025418594013899565, 0.03739842772483826, -0.011789237149059772, -0.00635898020118475, -0.013126876205205917, -0.02051507495343685, -0.039006367325782776, 0.004466880578547716, -0.008517914451658726, -0.03202015161514282, 0.012745684012770653, 0.002841615118086338, -0.004709457512944937, -0.026697320863604546, -0.022913120687007904, 0.017964553087949753, -0.0017118998803198338, -0.029053783044219017, -0.023342829197645187, -0.03581821173429489, 0.013369453139603138, 0.1355103850364685, 0.017202168703079224, -0.010008029639720917, 0.003662911243736744, -0.0013549652649089694, -0.0006142393685877323, -0.007207999471575022, -0.00783176813274622, -0.012814991176128387, -0.005932738073170185, -0.002186657628044486, -0.0027324554976075888, -0.004924311302602291, -0.001595809473656118, 0.007956522516906261, 0.023231936618685722, 0.005516891833394766, -0.01438827533274889, -0.0031153804156929255, -0.005478772800415754, -0.004754507448524237, -0.026475535705685616, -0.0010032287100329995, 0.02212301269173622, 0.007686222437769175, -0.0054891686886549, 0.042000457644462585, 0.00862880703061819, -0.02194281294941902, -0.021346768364310265, 0.007686222437769175, -0.010604076087474823, 0.009093168191611767, 0.006851064972579479, -0.0022940845228731632, -0.01637047529220581, -0.008996137417852879, 0.02163786068558693, 0.044634148478507996, -0.018130891025066376, 0.02994091995060444, 0.009266437962651253, -0.006320861168205738, -0.009051583707332611, 0.004179253708571196, 0.0012839249102398753, -0.00655650720000267, 0.029996367171406746, 0.018214059993624687, 0.010902099311351776, 0.013826883397996426, 0.0018851690692827106, 0.020404182374477386, -0.014104113914072514, -0.009169407188892365, -0.000916594173759222, -0.032685503363609314, -0.0072495839558541775, -0.04158461093902588, 0.0232457984238863, -0.022247767075896263, 0.0022109150886535645, 0.0031032515689730644, -0.02779238298535347, -0.005243126302957535, -0.0527292862534523, -0.03310135006904602, -0.027736935764551163, -0.0030720632057636976, -0.04224996641278267, -0.0007493893499486148, 0.008531776256859303, -0.013667475432157516, 0.015109075233340263, 0.019336843863129616, 0.0332954116165638, 0.02662801370024681, -0.008011968806385994, 0.012821922078728676, 0.04125193506479263, -0.000716901384294033, -0.011290222406387329, 0.0035520188976079226, -0.03060627356171608, -0.009834760800004005, 0.005315899383276701, -0.0016512556467205286, -0.014859568327665329, -0.011920922435820103, -0.005953530315309763, -0.009716937318444252, 0.010936752893030643, 0.01362589094787836, -0.0232457984238863, 0.020376460626721382, 0.030190428718924522, -0.021124983206391335, 0.009314953349530697, -0.019475460052490234, 0.015275414101779461, 0.004210441838949919, -0.03398849070072174, 0.0006211701547726989, -0.023523028939962387, -0.004220838192850351, -0.005842638202011585, -0.0035624150186777115, 0.0030911227222532034, -0.04823815077543259, -0.023536890745162964, 0.02310718223452568, -0.01990516670048237, -0.02338441275060177, -0.02377253584563732, 0.006958491634577513, 0.013819952495396137, -0.0030356766656041145, 0.005939668510109186, -0.01709127612411976, -0.007533745374530554, 0.0018158614402636886, -0.02154082991182804, 0.031105289235711098, 0.023703228682279587, -0.03903409093618393, 0.027016136795282364, -0.0006987081142142415, -0.024770567193627357, 0.01820019818842411, 0.00269953440874815, 0.00538520747795701, -0.013480344787240028, -0.013487275689840317, -0.009550599381327629, -0.01396549865603447, 0.003967864904552698, -0.022829951718449593, 0.012662514112889767, -0.0025210671592503786, 0.0026163652073591948, -0.01037536095827818, 0.010673384182155132, 0.0009183268412016332, -0.0008966681780293584, -0.023703228682279587, -0.0358736589550972, 0.012274391017854214, 0.009384260512888432, 0.01140111405402422, 0.016023937612771988, -0.011241707019507885, -0.016051659360527992, 0.024521060287952423, -0.004598564933985472, -0.023190351203083992, 0.00748522998765111, 0.003683703485876322, -0.0027203266508877277, 0.027140889316797256, 0.0454103946685791, 0.024950766935944557, 0.0026510190218687057, 0.015608090907335281, 0.007942660711705685, -0.0019995267502963543, 0.01801999844610691, -0.02538047544658184, -0.0045257918536663055, 0.0014987786998972297, 0.019350705668330193, 0.00945356860756874, 0.015982352197170258, 0.006923838052898645, -0.004304007161408663, -0.0017240287270396948, 0.007866422645747662, -0.012856575660407543, -0.029053783044219017, -0.001853980589658022, -0.03337858244776726, 0.00112884899135679, -0.02391115203499794, -0.024992352351546288, -0.002301015192642808, -0.005683230236172676, -0.007058987859636545, 0.018810106441378593, 0.0035052362363785505, -0.0012362758861854672, -0.005132234189659357, 0.022857675328850746, 0.006851064972579479, 0.0265448447316885, 5.663737465511076e-05, -5.994032107992098e-05, -0.014901152811944485, -0.030661720782518387, -0.008608014322817326, 0.012336768209934235, 0.00957139115780592, -0.006442149635404348, 0.014485306106507778, -0.003404740011319518, 1.3543425666284747e-05, -0.010056545026600361, 0.01659226045012474, 0.013168460689485073, -0.020140813663601875, -0.002430967055261135, -0.00664660707116127, -0.04042024165391922, -0.020113090053200722, -0.013348660431802273, -0.027556736022233963, 0.03728753700852394, -0.012419937178492546, -0.022511135786771774, 0.003718357300385833, 0.006611953489482403, -0.0026319595053792, 0.004283214919269085, -0.0012830585474148393, 0.04549356549978256, 0.019128922373056412, 0.018505152314901352, 0.027778521180152893, 0.010319914668798447, -0.01278033759444952, -0.020043782889842987, -0.0068857185542583466, -0.005995114799588919, 0.01454075239598751, 0.035845935344696045, -0.006258483976125717, 0.007367406971752644, 0.018283367156982422, -0.005014411173760891, -0.037453874945640564, -0.017590289935469627, 0.006185710895806551, 0.0037634074687957764, -0.00474064564332366, -0.009439706802368164, -0.005281245801597834, -0.006317395716905594, 0.012253599241375923, -0.002488145837560296, 0.0033527594059705734, -0.006875322666019201, -0.019350705668330193, -0.015081352554261684, 0.009335745126008987, 0.007058987859636545, 0.01673087477684021, -0.003926280420273542, 0.008663460612297058, -0.0024015114177018404, -0.018186336383223534, 0.0030339439399540424, 0.01438827533274889, -0.030495382845401764, 0.015219967812299728, -0.010624868795275688, 0.018297228962183, 0.005035203415900469, 0.02302401326596737, -0.019780414178967476, 0.0053020380437374115, 0.007713945582509041, 0.028069613501429558, 0.001690241158939898, 0.01106150634586811, 0.038701411336660385, -0.008608014322817326, 0.020113090053200722, 0.0017864055698737502, 0.010555560700595379, -0.012031814083456993, -0.006306999363005161, -0.018588321283459663, 0.019239813089370728, -0.02079230546951294, 0.011678345501422882, -0.0014831845182925463, -0.01077041495591402, -0.018713075667619705, 0.007623845711350441, -0.038645967841148376, -7.374770939350128e-05, -0.013521929271519184, -0.018408121541142464, -0.0063797724433243275, 0.006175315007567406, 0.006636211182922125, 0.017326921224594116, -0.01619027554988861, 0.012655583210289478, -0.017299199476838112, -0.012101122178137302, -0.00047215860104188323, -0.025408197194337845, -0.01037536095827818, -0.029608244076371193, 0.0016859094612300396, -0.00317255943082273, -0.02515869028866291, 0.02592107467353344, 0.005953530315309763, -0.019336843863129616, -0.05023420974612236, 0.026059690862894058, 0.015081352554261684, 0.0003350593615323305, -0.001737890299409628, -0.01479026023298502, -0.002794832456856966, 0.0046817343682050705, -0.011338737793266773, 0.004685199819505215, 0.013868467882275581, -0.015469475649297237, -0.004882726352661848, 0.002890130504965782, 0.0013064498780295253, 0.03157658129930496, 0.009003068320453167, 0.025629982352256775, 0.0016001411713659763, 0.016938798129558563, -0.018394259735941887, 0.0016122700180858374, 0.010652591474354267, -0.009765452705323696, -0.001679845037870109, -0.024285413324832916, -0.010014960542321205, -0.014665506780147552, 0.029386458918452263, 0.0034740478731691837, -0.00439410749822855, -0.0018938325811177492, 0.012863506563007832, 0.012967468239367008, 0.010576353408396244, -0.021152706816792488, -0.01204567588865757, -0.03440433740615845, -0.036594457924366, -0.03243599832057953, -0.009640699252486229, -0.011110021732747555, -3.2650419598212466e-05, 0.012655583210289478, -0.03875685855746269, -0.015982352197170258, -0.008289199322462082, -0.056499626487493515, -0.01980813592672348, -0.016481367871165276, 0.017562568187713623, -0.0024240363854914904, 0.008427814580500126, 0.01222587563097477, 0.001971803605556488, 0.022954706102609634, 0.04973519593477249, -0.01681404560804367, -0.015012044459581375, 0.010818930342793465, -0.01122091431170702, 0.01354272197932005, 0.0003467550268396735, -0.03662218153476715, -0.012212014757096767, -0.011546660214662552, -0.003791130380704999, 0.01280112937092781, -0.005787191912531853, -0.015940768644213676, 0.0017526181181892753, -0.007079780101776123, 0.03279639780521393, -0.0038673689123243093, 0.019517045468091965, 0.015913045033812523, -0.01278033759444952, -0.017687320709228516, 0.007644637953490019, -0.009418915025889874, -0.019420014694333076, 0.006944630295038223, 0.007817907258868217, -0.030329043045639992, 0.0023547287564724684, -0.02952507510781288, 0.00829613022506237, 0.0014407335547730327, 0.021416075527668, 0.020362598821520805, -0.018768521025776863, -0.005125303287059069, 0.03326768800616264, -0.003943607211112976, -0.007083245553076267, 0.00265448447316885, 0.003333699656650424, -0.02511710487306118, -0.029164673760533333, 0.021360628306865692, -0.0314934141933918, -0.0029750324320048094, -0.025463644415140152, -0.012350630015134811, -0.019558629021048546, 0.0157467070966959, -0.005256988108158112, -0.0013003854546695948, 0.015178383328020573, 0.010028822347521782, -0.0197665523737669, -0.024160658940672874, 0.015178383328020573, -0.00199606129899621, 0.020487351343035698, -0.011366460472345352, -0.005908480379730463, -0.005191145930439234, -0.0024621556513011456, 0.002758445916697383, 0.027016136795282364, -0.02636464312672615, -0.003297313116490841, 0.01210805308073759, -0.0065426453948020935, 0.025006214156746864, 0.00814365316182375, 0.2181251496076584, 0.00664660707116127, -0.024119075387716293, 0.02149924449622631, -0.008836730383336544, 0.025311166420578957, 0.035263750702142715, 0.021804198622703552, 0.008219891227781773, 0.03199242800474167, 0.0014745210064575076, -0.011255567893385887, 0.0029906267300248146, 0.004151530563831329, -0.01188626792281866, -0.032269660383462906, -0.029913198202848434, -0.017451675608754158, 0.010389221832156181, -0.012066468596458435, -0.009654561057686806, 0.0055272881872951984, 0.013923914171755314, -0.02016853727400303, 0.04127965867519379, 0.017562568187713623, -0.0164675060659647, 0.021305182948708534, 0.006203038152307272, 0.004245095886290073, -0.00427281903102994, 0.01454075239598751, 0.011359529569745064, 0.029386458918452263, 0.004591634031385183, -0.02467353641986847, -0.0252557210624218, 0.008393160998821259, -0.0011782306246459484, 0.0197665523737669, -0.03559642657637596, -0.023121044039726257, -0.036206334829330444, -0.00669165700674057, -0.010188230313360691, 0.020625967532396317, 0.0012042210437357426, -0.016023937612771988, -0.007311961147934198, 0.02877655066549778, -0.022899258881807327, -0.001644324860535562, 0.012350630015134811, 0.02181806042790413, -0.03412710502743721, 0.006566903088241816, 0.025061659514904022, 0.0038812304846942425, -0.054087717086076736, 0.007235722616314888, -0.007838699035346508, 0.030439935624599457, -0.01691107638180256, 0.05652735009789467, 0.010312983766198158, 0.010118922218680382, 0.003534692106768489, 0.013466483913362026, 0.019392291083931923, -0.02057052217423916, 0.013799160718917847, 0.01402787584811449, 0.021984398365020752, 0.006050561089068651, -0.016425922513008118, -0.014194213785231113, 0.03118845820426941, 0.016606122255325317, 0.026960689574480057, 0.0060159070417284966, -0.004747576545923948, 0.026489397510886192, -0.007346614729613066, 0.040752921253442764, -0.011262498795986176, -0.018311090767383575, 0.008774353191256523, -0.00115137395914644, 0.007353545632213354, -0.018130891025066376, 0.006154522765427828, -0.032907288521528244, -0.018491290509700775, -0.0124476607888937, -0.005606991704553366, 0.02222004346549511, 0.00543025741353631, 0.011816960759460926, -0.015816014260053635, 0.003321570809930563, -0.043608397245407104, 0.036428119987249374, -0.0004968494758941233, 0.0055792685598134995, -0.04687971994280815, 0.025505227968096733, 0.001633928739465773, -0.00021117186406627297, 0.005582734011113644, -0.001104591297917068, -0.008275337517261505, -0.022635890170931816, -0.003732218872755766, -0.007658499293029308, 0.0053956033661961555, 0.0012588008539751172, 0.004598564933985472, -0.037315256893634796, 0.016758598387241364, 0.023633921518921852, -0.012329837307333946, -0.008601084351539612, -0.010472391732037067, 0.031022120267152786, 0.010257537476718426, -0.026170581579208374, -0.01454075239598751, -0.017368506640195847, 0.011345668695867062, -0.02787555195391178, 0.01119319163262844, -0.022511135786771774, 0.021513106301426888, -0.019863583147525787, 0.002756713191047311, 0.022954706102609634, 0.010992199182510376, 0.002902259351685643, 0.006785222329199314, -0.02793099731206894, -0.0003513033443596214, -0.005215403623878956, 0.037010304629802704, -0.017063552513718605, 0.014332829974591732, -0.027140889316797256, 0.0033181055914610624, -0.011269429698586464, -0.007450576405972242, -0.018657628446817398, -0.024562643840909004, 0.001761281630024314, 0.008330783806741238, 0.009654561057686806, 0.037537042051553726, -0.01984972134232521, 0.019295260310173035, -0.017118997871875763, 0.023439859971404076, 0.0030703304801136255, -0.028028028085827827, 0.020556660369038582, 0.0069307684898376465, -0.012648653239011765, -0.02913695201277733, 0.006088680122047663, -0.1787583827972412, 0.03831328824162483, 0.019433874636888504, -0.03556870296597481, 0.03165975213050842, -0.0073604765348136425, 0.020986367017030716, 0.0018713074969127774, -0.043968796730041504, 0.017590289935469627, 0.01699424535036087, 0.0072287917137146, -0.03238055109977722, -0.034792460501194, 0.022760644555091858, -0.0010586748830974102, -0.014513029716908932, 0.016883352771401405, 0.022774506360292435, 0.013882329687476158, 0.010493183508515358, 0.012073398567736149, 0.010749622248113155, 0.013549652881920338, 0.01113081444054842, -0.011255567893385887, -0.012676375918090343, -0.0038223189767450094, -0.003160430584102869, -0.006549576297402382, -0.025435920804739, 0.003839645767584443, 0.030301321297883987, 0.008136722259223461, 0.01900416798889637, 0.0060609569773077965, -0.008393160998821259, 0.00481688417494297, -0.003742614993825555, 0.015718983486294746, 0.007928798906505108, 0.02783396653831005, 0.010472391732037067, 0.006043630186468363, -0.004757972899824381, 0.014152629300951958, 0.018616044893860817, -0.004636684432625771, 0.013549652881920338, -0.0217764750123024, -0.007623845711350441, -0.03301818296313286, 0.040614303201436996, -0.005194610916078091, 0.01137339137494564, 0.003087657503783703, 0.010721899569034576, 0.038202397525310516, 0.008601084351539612, -0.020459629595279694, 0.015206106007099152, -0.04000439494848251, -0.0002241670445073396, -0.012607067823410034, 0.023980459198355675, -0.004979757126420736, -0.013771437108516693, 0.004868865013122559, -0.014720953069627285, 0.027847828343510628, -0.012814991176128387, -0.000939985504373908, 0.006580764893442392, -0.031382519751787186, 0.028527043759822845, 0.008871383965015411, -0.019115060567855835, 0.024368582293391228, 0.014887291006743908, 0.0019423479679971933, -0.014956599101424217, 0.014159560203552246, -0.01195557601749897, -0.008060484193265438, -0.007686222437769175, -0.005049064755439758, 0.0018609113758429885, -0.0033388978336006403, 0.014249660074710846, 0.0020878941286355257, 0.018227921798825264, -0.03889547288417816, 0.014443721622228622, -0.01614869013428688, 0.006733241956681013, 0.00026380238705314696, 0.01886555179953575, -0.006920372601598501, -0.008337714709341526, -0.00630006892606616, -0.009807037189602852, -0.003063399810343981, -0.0031881534960120916, 0.011435768567025661, 0.027667628601193428, -0.003999053500592709, 0.015414029359817505, 0.03531919792294502, 0.015039768069982529, -0.018172474578022957, -0.009855552576482296, 0.01177537627518177, 0.01807544380426407, 0.026669597253203392, -0.0047510419972240925, 0.01824178360402584, -0.004016380291432142, -0.00045006678556092083, 0.014887291006743908, -0.01164369098842144, 0.06126799434423447, 0.016051659360527992, 0.016578398644924164, -0.003908953629434109, -0.034792460501194, -0.016176413744688034, -0.08477716147899628, 0.004848072770982981, 0.0005128768971189857, -0.015289275906980038, 0.0055515458807349205, 0.0030027555767446756, 0.019018029794096947, 6.396070943992527e-07, -0.007048591505736113, 0.008102068677544594, 0.0013644950231537223, -0.016564536839723587, 0.002878001658245921, -0.0026718112640082836, -0.00022524998348671943, -0.014637783169746399, -0.01944773644208908, -0.009183268062770367, 0.0034324631560593843, 0.012704098597168922, -0.004948568996042013, -0.008309992030262947, -0.00023239733127411455, -0.012260530143976212, 0.015982352197170258, -0.02173488959670067, -0.018893275409936905, 0.00945356860756874, 0.024562643840909004, 0.020625967532396317, 0.01797841303050518, -0.010049614124000072, -0.0043386612087488174, -0.019018029794096947, -0.015219967812299728, -0.007436714600771666, -0.008594153448939323, -0.004910449497401714, 0.015871459618210793, -0.025089383125305176, 0.018491290509700775, 0.011588245630264282, 0.009363468736410141, -0.024146797135472298, 0.005329761188477278, -0.011983298696577549, -0.005215403623878956, 0.020861614495515823, 0.012516967952251434, -0.021402213722467422, -0.028804274275898933, -0.0003419901186134666, 0.012939744628965855, -0.0055515458807349205, 0.028748828917741776, 0.031077567487955093, 0.014000152237713337, 0.04435691982507706, -0.028831997886300087, -0.017881382256746292, -0.007665430195629597, -0.00880900677293539, -0.010174368508160114, 0.0002928249887190759, 0.024784428998827934, -0.009619906544685364, -0.005600061267614365, -0.01709127612411976, 0.004401037935167551, -0.0228853989392519, -0.005374811124056578, 0.02097250521183014, -0.019336843863129616, 0.0036351880989968777, -0.046325258910655975, 0.007201068568974733, -0.011408044956624508, -0.0063970996998250484, -0.003214143915101886, -0.006064422428607941, -0.012364490889012814, -0.021152706816792488, 0.00655650720000267, -0.0003099353052675724, 0.021041814237833023, 0.003874299582093954, 0.008739699609577656, 0.008885245770215988, -0.012246668338775635, -0.02833298221230507, 0.006840668618679047, 0.02167944423854351, -0.0013471681158989668, -0.004910449497401714, -0.026835937052965164, -0.014443721622228622, -0.03692713379859924, -0.0159269068390131, 0.00565550709143281, 0.014831844717264175, -0.012724891304969788, -0.0017214296385645866, -0.08544251322746277, 0.033212244510650635, -0.015913045033812523, -0.005256988108158112, -0.0048896572552621365, -0.02203984372317791, 0.011782307177782059, -0.026115136221051216, -0.004546584095805883, 0.02145765908062458, -0.021665582433342934, 0.017687320709228516, -0.013147667981684208, 0.021707167848944664, 0.005769865121692419, -0.01838039793074131, 0.03068944439291954, -0.01006347592920065, -0.0004964162944816053, -0.001609671046026051, 0.007901076227426529, 0.007311961147934198, 0.028721105307340622, 0.009252576157450676, 0.008614945225417614, 0.025283444672822952, -0.017742767930030823, 0.001244072918780148, -0.01659226045012474, -0.0038604382425546646, 0.01655067503452301, -0.02994091995060444, -0.01990516670048237, 0.017077414318919182, -0.004782230593264103, -0.017229890450835228, -0.021222013980150223, 0.019794275984168053, 0.013757576234638691, -0.011692206375300884, -0.02485373616218567, -0.015677398070693016, 0.008483260869979858, -0.010929821990430355, 0.010014960542321205, 0.010202091187238693, 0.008524845354259014, -0.014513029716908932, 0.015067490749061108, 0.00988327618688345, 0.002339134458452463, 0.00832385290414095, -0.005132234189659357, -0.021623998880386353, -0.0007437581080012023, -0.01735464483499527, 0.043525226414203644, -0.010340706445276737, -0.013916983269155025, -0.004213907290250063, 0.011491214856505394, 0.009093168191611767, 0.0045257918536663055, -0.0006844134186394513, 0.0024621556513011456, -0.005582734011113644, 0.01246845256537199, 0.006199572701007128, 0.018311090767383575, -0.036566734313964844, -0.017008107155561447, -0.003125776769593358, 0.007187207229435444, 0.0250755213201046, 0.009931791573762894, 0.008497122675180435, 0.013944706879556179, 0.01028526108711958, -0.010299121960997581, 0.02302401326596737, 0.0019458133028820157, -0.029968643561005592, 0.000739859533496201, -0.0011002594837918878, 0.012371421791613102, 0.006154522765427828, -0.04036479815840721, -0.015441752970218658, -0.014263521879911423, 0.009398122318089008, -0.016273444518446922, -0.002605969086289406, 0.002186657628044486, -0.0031188458669930696, 0.003111915197223425, -0.014776398427784443, -0.01820019818842411, 0.014007083140313625, -0.005482237786054611, 0.030938951298594475, 0.016093244776129723, 0.01327242236584425, 0.0030478055123239756, -0.005087184254080057, -0.02427155151963234, 0.01650909148156643, -0.01564967632293701, -0.022150736302137375, -0.015053629875183105, -0.010382291860878468, 0.0009824364678934216, 0.0018522479804232717, 0.014318968169391155, 0.01731305941939354, -0.0147486</t>
-  </si>
-  <si>
-    <t>Which clients are employed by a company similar to Stevens Valley School?</t>
-  </si>
-  <si>
-    <t>SELECT employer.name, client.ID, client.Client_ID, client.Person_Org, client.Name, client.SSN, address.Address, address.City,  address.State, address.Zip  FROM client INNER JOIN address ON client.Address_ID = address.ID INNER JOIN employer ON client.Employer_ID = employer.ID WHERE employer.Name LIKE '%Stevens Valley School%'</t>
-  </si>
-  <si>
-    <t>[0.012511341832578182, -0.01192118413746357, -0.008130289614200592, -0.02228713035583496, -0.009991021826863289, 0.038547709584236145, -0.01653829962015152, 0.0019405771745368838, 0.00014536971866618842, -0.018718412145972252, -0.023356357589364052, 0.0032233023084700108, 0.004353280644863844, -0.0023276512511074543, 0.0016793456161394715, -0.004988567903637886, 0.007873397320508957, -0.0275360606610775, 0.007547074928879738, 0.0008826328557915986, -0.010845014825463295, 0.029493996873497963, 0.003912398125976324, -0.019523803144693375, -0.004183176439255476, -0.008199719712138176, -0.001698439009487629, -0.005592611618340015, 0.003252810100093484, 0.016121719032526016, 0.03538168594241142, -0.011004704050719738, -0.02121790312230587, -0.0036867496091872454, 0.0005272364360280335, 0.003731879172846675, 0.011948956176638603, 0.006765983998775482, 0.018024109303951263, 0.012900152243673801, 0.0022946717217564583, -0.021148473024368286, -0.0033569554798305035, -0.015816224738955498, -0.014746998436748981, -0.015330213122069836, 0.0006400606944225729, 0.005957120563834906, -0.023675736039876938, 0.020468056201934814, 0.032410070300102234, 0.006765983998775482, -0.01735757850110531, -0.016940996050834656, 0.005314890295267105, 0.011386571452021599, 0.0051343715749681, -0.004492141306400299, -0.013073727488517761, -0.01910722255706787, 0.0012757820077240467, 0.003717993153259158, -0.0149275166913867, 0.003940170165151358, -0.011386571452021599, -0.0031642864923924208, -0.020495828241109848, 0.003235452575609088, -0.005512766540050507, 0.006342459004372358, 0.027994301170110703, 0.005391263868659735, -0.011900355108082294, -0.006141111254692078, 0.019232196733355522, -0.013649999164044857, -0.00040464854100719094, -0.023356357589364052, 0.007064534351229668, 0.0018867687322199345, -0.0071860370226204395, -0.03982522711157799, -0.03465961292386055, 0.011261596344411373, 0.013608341105282307, -0.023259153589606285, 0.005887690465897322, 0.006418832112103701, -0.018565665930509567, 0.0062278988771140575, 0.016816021874547005, 0.027119480073451996, 0.00705411983653903, 0.01920442469418049, -0.01795467920601368, 0.011837868019938469, 0.0043984102085232735, 0.02649460732936859, 0.019273854792118073, -0.023425787687301636, -0.006085566710680723, 0.030438248068094254, -0.023786824196577072, -0.013018183410167694, -0.03282665088772774, -0.0003829515480902046, -0.010761698707938194, -0.013198702596127987, 0.0011959371622651815, -0.02607802487909794, -0.030466020107269287, -0.014580365270376205, 0.00721380952745676, -0.01520523801445961, -0.006866657640784979, -0.004453954286873341, 0.02907741442322731, 0.007172151003032923, 0.016760477796196938, -0.017968565225601196, 0.02792487107217312, 0.011456001549959183, 0.02212049625813961, -0.028827466070652008, 0.028938554227352142, 0.003290996653959155, -0.01782970316708088, -0.002732082735747099, -0.018648982048034668, -0.012705747038125992, 0.007547074928879738, 0.010046565905213356, 0.01110190711915493, -0.021717801690101624, -0.01705208420753479, -0.011018590070307255, 0.016982654109597206, 0.02181500382721424, -0.019662663340568542, -0.003046254860237241, 0.010539521463215351, 0.016052287071943283, 0.006984689272940159, 0.017496438696980476, -0.011289368383586407, 0.022023294121026993, 0.015663478523492813, 0.027244454249739647, -0.010796413756906986, -0.00878293439745903, -0.0008075613295659423, -0.010004907846450806, -0.0018433748045936227, -0.023522989824414253, -0.010039622895419598, -0.012969582341611385, 0.004422710742801428, 0.0092967189848423, -0.027286112308502197, -0.018760070204734802, -0.04040843993425369, 0.022814800962805748, 9.606334788259119e-05, -0.0018451105570420623, 0.010921387933194637, 0.014483163133263588, 0.001799980876967311, -0.007477644365280867, 0.01011599600315094, -0.017815817147493362, -0.024328380823135376, 0.009074541740119457, -0.026189113035798073, 0.005099656525999308, 0.005832145921885967, -0.018024109303951263, 0.007199923507869244, 0.004953852854669094, 0.003700635628774762, -0.03715910390019417, 0.018607323989272118, 0.019870955497026443, -0.0026105795986950397, 0.04321342706680298, -0.007720650639384985, 0.0030549336224794388, -0.0037804804742336273, 0.0006938691949471831, -0.0040200152434408665, -0.007547074928879738, 0.039575278759002686, 0.01243496872484684, -0.0058182599022984505, -0.013094556517899036, -0.6412028074264526, -0.01774638704955578, -0.012636316940188408, 0.00882459245622158, 0.03604821860790253, 0.03507619351148605, 0.023772938176989555, 0.007137435954064131, -0.014871972613036633, 0.0013243831926956773, 0.015024719759821892, 0.013393106870353222, -0.011393514461815357, -0.004755976144224405, 0.00020894184126518667, -0.027633264660835266, -0.007727593649178743, 0.011976729147136211, 0.010081280954182148, -0.007831739261746407, -0.01400409359484911, 0.0229397751390934, -0.013781916350126266, -0.005700228735804558, 0.04804577678442001, 0.024328380823135376, -0.021287333220243454, -0.01576068066060543, 0.0029421094805002213, 0.0011594862444326282, -0.026702897623181343, 0.025244861841201782, 0.011483773589134216, 0.026008594781160355, 0.04399104416370392, 0.018287943676114082, -0.020454170182347298, 0.032187893986701965, -0.005328776314854622, 0.03793672099709511, -0.03774231672286987, 0.0012801213888451457, 0.021828889846801758, 0.002808456076309085, -0.00865101721137762, 0.039158694446086884, 0.009824388660490513, -0.004082502331584692, -0.008338580839335918, -0.015191351994872093, 0.0253420639783144, 0.00565857021138072, -0.019259968772530556, 9.129001409746706e-05, 0.035409457981586456, -0.02298143319785595, 0.0040477872826159, -0.003992242738604546, -0.01516357995569706, 0.019579347223043442, -0.004992039408534765, 0.008165004663169384, -0.005717586260288954, -0.017232602462172508, -0.018968360498547554, 0.006665309891104698, -0.011615690775215626, -0.003940170165151358, 0.0016724026063457131, -0.015871768817305565, 0.030854830518364906, 0.0182185135781765, -0.004169290419667959, 0.02203718014061451, 0.0012966110371053219, 0.014170726761221886, -0.010692267678678036, -0.0077484226785600185, -0.0013200438115745783, 0.02039862610399723, -0.018287943676114082, -0.026647353544831276, -0.004405353218317032, -0.0006708703585900366, -0.0033656342420727015, 0.0006383249419741333, -0.022023294121026993, -0.016177263110876083, 0.01803799532353878, -0.024453354999423027, 0.010386774316430092, 0.02039862610399723, -0.0010431904811412096, -0.045296333730220795, 0.002614051103591919, 0.020370854064822197, -0.009893819689750671, 0.00425260653719306, 0.011011647060513496, -0.023078635334968567, -0.001996121369302273, 0.008769048377871513, -0.009435579180717468, -0.0038290817756205797, -0.0040477872826159, 0.011476830579340458, -0.0057314722798764706, 0.009137028828263283, 0.019509917125105858, -0.026355745270848274, 0.022259358316659927, -0.022064952179789543, -0.021620599552989006, -0.008005314506590366, 0.005481522995978594, -0.03879765793681145, 0.00429426459595561, -0.012983468361198902, -0.02203718014061451, -0.013698600232601166, -0.0011386570986360312, -0.02259262278676033, 0.004186647944152355, 6.856243271613494e-05, -0.0010431904811412096, 0.003731879172846675, -0.01067143864929676, -0.026508493348956108, -6.113122071838006e-05, -0.0019128050189465284, -0.006575050298124552, -0.011810095980763435, 0.021273447200655937, -0.013851347379386425, -0.0002913903445005417, 0.01196284219622612, 0.0033274476882070303, -0.011858697049319744, -0.0015352778136730194, -0.03402085229754448, -0.00019321154104545712, -0.0015890862559899688, -0.0022599566727876663, -0.007956713438034058, -0.003077498637139797, 0.003933227155357599, -0.021939978003501892, 0.007755365688353777, -0.01657995767891407, -0.026689011603593826, -0.004443539772182703, -0.013177872635424137, -0.010122939012944698, -0.0016081795329228044, -0.003379520494490862, 0.0008691807161085308, -0.009359206072986126, -0.018954474478960037, 0.01363611314445734, -0.009845217689871788, 0.008859307505190372, 0.012816835194826126, -0.014899744652211666, -0.020495828241109848, -0.0028188705909997225, -0.005353076849132776, 0.02392568439245224, 0.00174530444201082, 0.012955696322023869, -0.005905047990381718, 0.04001963138580322, -0.0031694937497377396, 0.025050455704331398, 0.01885727234184742, 0.011969785206019878, 0.026897301897406578, -0.023606305941939354, 0.023078635334968567, -0.02169002965092659, -0.0008800291689112782, 0.002223505638539791, 0.006800699047744274, -0.005290589760988951, 0.016593843698501587, 0.034937333315610886, 0.004221362993121147, 0.007734536658972502, 0.02439781092107296, -0.017801931127905846, 0.0014337359461933374, 0.007970599457621574, 0.023953458294272423, -0.00882459245622158, -0.007651220075786114, 0.019232196733355522, 0.001799980876967311, 0.019037790596485138, 0.025911392644047737, 0.018926702439785004, 0.011761494912207127, 0.028799694031476974, -3.601697244448587e-05, 0.014538707211613655, -0.0017678693402558565, 0.011094964109361172, -0.041380465030670166, -0.008442725986242294, -0.03415971249341965, 0.02370350807905197, 0.02052360028028488, 0.009206458926200867, -0.010650609619915485, -0.015663478523492813, -0.011990615166723728, -0.006318158470094204, 0.004151932429522276, -0.009477237239480019, 0.008845421485602856, 0.01516357995569706, -0.004863593261688948, 0.0024387396406382322, -0.00541209289804101, 0.030049439519643784, -0.003624262288212776, 0.00734572671353817, -0.009199515916407108, -0.004526856355369091, 0.0024786621797829866, 0.008345523849129677, 0.008796820417046547, -0.0002939939731732011, 0.007998371496796608, 0.017774159088730812, -0.0022165626287460327, 0.007005518302321434, -0.0022044123616069555, 0.012032273225486279, -0.00994242075830698, 0.0208707507699728, -0.010095166973769665, -0.011247710324823856, 0.004044315777719021, 0.010942216962575912, -0.012178076431155205, 0.04329674318432808, 0.010365945287048817, 0.012171133421361446, 0.012205848470330238, -0.011254653334617615, 0.03679806366562843, -0.013032069429755211, 0.018107425421476364, 0.00489830831065774, -0.0006526448996737599, 0.029521768912672997, -0.0020846452098339796, 0.022259358316659927, 0.01058812253177166, 0.00709924940019846, 0.02246764861047268, -0.01103941909968853, -0.0024665119126439095, 0.00425260653719306, -0.03274333477020264, 0.024633875116705894, 0.007727593649178743, -0.02495325356721878, -0.01889893040060997, 0.006668781396001577, -0.019273854792118073, 0.0031070064287632704, 0.006710439454764128, 0.014038808643817902, 0.004471312277019024, 0.009095370769500732, 0.005103128030896187, 0.0028483786154538393, 0.0003723200352396816, -0.007692878600209951, 0.014385960064828396, -0.0027928343042731285, -0.033743131905794144, 0.021509509533643723, -0.006443133112043142, 0.006457019131630659, 0.02250930666923523, -0.0006752097979187965, -0.0005255006835795939, -0.027647150680422783, 0.02916073054075241, 0.009463351219892502, 0.0009607419488020241, -0.023856254294514656, 0.021537283435463905, -0.004204005468636751, 0.005512766540050507, -0.0014181140577420592, -0.014871972613036633, -0.003756179939955473, 0.0034836658742278814, 0.01170595083385706, 0.017107628285884857, 0.010615894570946693, 0.018621210008859634, 0.044046588242053986, -0.008199719712138176, -0.006967331748455763, -0.022925889119505882, -0.023606305941939354, -0.029882805421948433, 0.018246285617351532, -0.0026574451476335526, -0.013483365997672081, 0.0006795491790398955, 0.011615690775215626, -0.015816224738955498, -0.012080874294042587, -0.003473251359537244, 0.04238026216626167, 0.0007776194834150374, -0.01469145342707634, -0.02220381423830986, -0.025661442428827286, -0.00012909698125440627, 0.12897375226020813, 0.033520955592393875, -0.024286722764372826, 0.003264960367232561, 0.02495325356721878, -0.004596286453306675, -0.02924404665827751, -0.012441911734640598, 0.0017045141430571675, -0.005196858663111925, -0.005932820029556751, -0.0228564590215683, -0.016552185639739037, -0.00360690476372838, 0.006922202184796333, 0.02177334576845169, -0.0030983276665210724, -0.01906556263566017, -0.006436189636588097, -0.018801728263497353, -0.02560589835047722, -0.002108945744112134, 0.014441505074501038, 0.016871565952897072, 0.00822749175131321, 0.01641332544386387, 0.03749236837029457, 0.04746256023645401, 0.00469348905608058, -0.022953661158680916, 0.0026244658511132, 0.01594119891524315, -0.014510935172438622, 0.017551982775330544, -0.013177872635424137, 0.014663681387901306, -0.02169002965092659, -0.003382991999387741, 0.030132755637168884, 0.009185629896819592, 0.04065839201211929, 0.018662868067622185, -0.0029542597476392984, -0.014031865634024143, 0.01552461739629507, 0.0023102934937924147, 0.0011612219968810678, 0.009435579180717468, -0.00016967032570391893, -0.004658774007111788, 0.003082705894485116, -0.009581383317708969, 0.01614949107170105, -0.02809150330722332, -0.003506230656057596, -0.0004942570230923593, -0.0064813196659088135, 0.009095370769500732, -0.009400864131748676, -0.018315715715289116, -0.05854363739490509, -0.01351113896816969, -0.004662245512008667, -0.011761494912207127, 0.0010536049958318472, -0.009053712710738182, -0.0048948368057608604, -0.014219327829778194, 0.006835414096713066, -0.016121719032526016, -0.0053391908295452595, 0.009845217689871788, -0.034131940454244614, -0.010171541012823582, 0.04282461479306221, 0.01211558934301138, 0.009324491024017334, -0.006661838386207819, -0.010900558903813362, 0.029410680755972862, -0.010949159972369671, -0.015413529239594936, 0.011948956176638603, -0.011074135079979897, 0.001554371090605855, 0.0046900175511837006, -0.024939367547631264, 0.011157451197504997, -0.0028067203238606453, 0.00508924201130867, 0.0035340029280632734, 0.008470498025417328, -0.017343692481517792, -0.051267340779304504, 0.010726982727646828, 0.0027112537063658237, 0.007547074928879738, 0.01988484151661396, -0.0004755976260639727, -0.013261189684271812, 0.015052491798996925, -0.02675844170153141, 0.01086584385484457, -0.019523803144693375, 0.010969989001750946, -0.012219734489917755, -0.011094964109361172, -0.0013408728409558535, -0.03224343806505203, 0.005634269677102566, 0.04118606075644493, -0.011699007824063301, 0.005478051491081715, 0.026702897623181343, 0.003096591914072633, 0.017038198187947273, -0.004068616311997175, 0.018621210008859634, 0.009629984386265278, -0.0032094160560518503, 0.04685157537460327, -0.012643259949982166, 0.025022683665156364, 0.001639423193410039, -0.025619784370064735, -0.001354758976958692, 0.0252587478607893, -0.03490956127643585, 0.01544130127876997, -0.0038985118735581636, -0.022689824923872948, 0.02891078218817711, -0.007324897684156895, -0.0014007565332576632, -0.041852593421936035, -0.030743742361664772, -0.018787842243909836, 0.01764918491244316, 0.007036761846393347, -0.015746794641017914, 0.0053044757805764675, 0.020759662613272667, -0.0005849503795616329, -0.01984318345785141, -0.011282425373792648, -0.029132958501577377, -0.011546260677278042, -0.0021419250406324863, 0.003603433258831501, 0.0003202473162673414, -0.015774566680192947, -0.0006526448996737599, 0.01937105692923069, 0.00865101721137762, -0.0058668614365160465, -0.029049642384052277, -0.013337562792003155, 0.016246693208813667, 0.02868860401213169, 0.02632797323167324, 0.017815817147493362, 0.004408824723213911, 0.009532781317830086, -0.021273447200655937, 0.005262817721813917, 0.01224056351929903, -0.016691047698259354, -0.017107628285884857, 0.011914241127669811, 0.0034541580826044083, 0.015663478523492813, -0.00605779467150569, 0.02452278509736061, 0.001982235349714756, 0.005092713516205549, 0.015108035877346992, 0.01898224651813507, -0.02478662133216858, -0.0115532036870718, -0.05887690559029579, 0.0028987154364585876, -0.014316529966890812, -0.005863389931619167, 0.024508899077773094, -0.022967547178268433, -0.018787842243909836, 0.025050455704331398, -0.009886876679956913, -0.01535798516124487, -0.01649664156138897, 0.020690232515335083, -0.016816021874547005, 0.022453762590885162, -0.003638148307800293, 0.02749440260231495, -0.004769862163811922, -0.010872786864638329, -0.034298572689294815, -0.0060196081176400185, 0.005363491363823414, 0.0022373918909579515, 0.004356752149760723, 0.019857069477438927, -0.003150400472804904, -0.015788452699780464, 0.0013773237587884068, -0.014608137309551239, -0.008831535466015339, -0.011150508187711239, 0.0043636951595544815, 0.005668984726071358, -0.01705208420753479, -0.016302237287163734, 0.005047583486884832, 0.020801320672035217, 0.003908926621079445, -0.029993893578648567, -0.0007359613082371652, -0.010810299776494503, -0.01842680387198925, 0.01290709525346756, -0.029271818697452545, 0.029882805421948433, 0.020384740084409714, 0.038853202015161514, 0.025703100487589836, 0.005728000774979591, -0.0017687372164800763, -0.002692160429432988, -0.0030688196420669556, 0.01941271498799324, 0.014802542515099049, 0.02611968293786049, -0.020426398143172264, -0.002206148114055395, 0.023995116353034973, -0.0024474184028804302, -0.009275889955461025, -0.01524689607322216, 0.026480721309781075, 0.010657552629709244, -0.008456612005829811, -0.009324491024017334, 0.0042977361008524895, -0.028424769639968872, 0.016260579228401184, 0.0045754574239254, -0.00322677381336689, 0.008831535466015339, 0.0028518501203507185, -0.00642230361700058, 0.01118522323668003, -0.002664388157427311, 0.022967547178268433, 0.010407603345811367, 0.018357373774051666, 0.004731675609946251, -0.005436393432319164, 0.024078432470560074, 0.019121108576655388, -0.007887283340096474, 0.040047403424978256, -0.019121108576655388, -0.001418981933966279, 0.000273164885584265, 0.020648574456572533, -0.011164394207298756, 0.008574643172323704, -0.009741072542965412, 0.025966936722397804, -0.007602619007229805, 0.004169290419667959, 0.012691861018538475, -0.020370854064822197, 0.004054730292409658, -0.0024370038881897926, 0.0013860026374459267, -0.011886469088494778, 0.0025515640154480934, 0.005023282952606678, 0.04201922565698624, -0.0072693536058068275, 0.0007233770447783172, -0.001498826895840466, 0.012837664224207401, -0.010053508915007114, 0.0038811543490737677, -0.018648982048034668, -0.005172558128833771, -0.022412104532122612, -0.0182185135781765, -0.015385757200419903, 0.014094353653490543, 0.005599554628133774, 0.003960999194532633, -0.007769251707941294, 0.014219327829778194, 0.01834348775446415, -0.044907525181770325, 0.007116606924682856, -0.017024312168359756, 0.03032715991139412, -0.04771250858902931, 0.027119480073451996, -0.008289978839457035, -0.016899337992072105, 0.021245675161480904, 0.0050684125162661076, -0.0255086962133646, -0.059210170060396194, 0.0065889363177120686, 0.014316529966890812, -0.0006513430853374302, -0.004981624893844128, 0.0015873505035415292, -0.0081788906827569, -0.003464572597295046, -0.007290182635188103, -0.023481331765651703, 0.001808659639209509, -0.01980152539908886, -0.011504602618515491, -0.02232878841459751, -0.011178280226886272, 0.016732705757021904, -0.015996742993593216, -0.0031017991714179516, -0.0320490300655365, -0.011108850128948689, -0.034631840884685516, -0.014677567407488823, 0.008671846240758896, -0.015469073317945004, -0.02400900237262249, -0.02082909271121025, -0.0021662258077412844, -0.010345116257667542, -0.0025342062581330538, 0.004755976144224405, -0.02181500382721424, 0.015857882797718048, 0.014774770475924015, 0.03143804520368576, 0.03349318355321884, -0.029105186462402344, -0.023634077981114388, -0.003777008969336748, -0.043879956007003784, -0.014483163133263588, -0.0016446304507553577, -0.005099656525999308, 0.01544130127876997, 0.0017522474518045783, -0.02246764861047268, -0.01688545197248459, -0.005436393432319164, -0.04449094459414482, 0.0029369022231549025, 0.006370231043547392, 0.016302237287163734, 0.022870345041155815, 0.03638148307800293, 0.0015170522965490818, -0.008470498025417328, -0.010289572179317474, 0.010942216962575912, -0.02486993744969368, 0.01898224651813507, -0.01159486174583435, -0.015663478523492813, 0.019509917125105858, -0.0026539736427366734, -0.022134384140372276, 0.005922405514866114, 0.02121790312230587, -0.015927312895655632, 0.011254653334617615, -0.021190131083130836, -0.02328692562878132, -0.0015899541322141886, 0.024147862568497658, 0.0010874522849917412, -0.007790080737322569, 0.014719226397573948, -0.009907705709338188, -0.02185666188597679, -0.012289165519177914, 0.013295904733240604, -0.013531967997550964, -0.015094149857759476, -0.000588855822570622, -0.0035287956707179546, -0.012900152243673801, 0.0127543481066823, 0.011136622168123722, 0.019162766635417938, -0.006571578793227673, 0.014233213849365711, 0.01031040120869875, -0.011081078089773655, -0.0013617019867524505, 0.008630187250673771, 0.006727796979248524, -0.010345116257667542, 0.010254857130348682, -0.00582173140719533, -0.03104923479259014, -0.027175024151802063, -0.008963453583419323, -0.021870547905564308, 0.0015621819766238332, -0.004061673302203417, 0.0008418424986302853, -0.0016767419874668121, -0.0033343906980007887, -0.0011586183682084084, -0.0015257310587912798, -0.001186390407383442, 0.024286722764372826, -0.03354872763156891, -0.005051054991781712, 0.007005518302321434, -0.01544130127876997, 0.024925481528043747, -0.003409028286114335, -0.02289811708033085, -0.009949363768100739, -0.01400409359484911, -0.01099776104092598, 0.0026539736427366734, -0.02478662133216858, -0.02349521778523922, 0.00012399819388519973, 0.01524689607322216, 9.13442563614808e-05, -0.013490309938788414, 0.21140141785144806, 0.03682583570480347, -0.006286914460361004, 0.02702227793633938, 0.005582197103649378, 0.00758178997784853, 0.0371035598218441, 0.011692064814269543, -0.01834348775446415, 0.025453152135014534, 0.0013573626056313515, -0.010296515189111233, 0.0024890766944736242, 0.003134778467938304, 0.008206662721931934, -0.03738128021359444, -0.029605085030198097, -0.011268539354205132, -0.019037790596485138, 0.022662052884697914, 0.009789673611521721, 0.018787842243909836, 0.01752421073615551, -0.020176447927951813, 0.02160671353340149, 0.03049379214644432, -0.02899409830570221, 0.02757771871984005, 0.025675328448414803, 0.03199348598718643, -0.005925877019762993, 0.017288148403167725, 0.015857882797718048, 0.004044315777719021, -0.0037284076679497957, -0.017329806461930275, -0.011622633785009384, -0.005596083123236895, 0.016760477796196938, 0.03104923479259014, -0.005120485555380583, -0.024370038881897926, -0.03793672099709511, -0.0035687179770320654, -0.02482827939093113, -0.0159828569740057, -0.01914888061583042, -0.002614051103591919, 0.0056655132211744785, 0.012608544901013374, -0.02663346752524376, 0.00858852919191122, 0.011685121804475784, 0.03329877555370331, -0.0029837675392627716, -0.0014181140577420592, 0.006672252900898457, 0.010699210688471794, -0.042852386832237244, -0.013448650948703289, -0.016052287071943283, 0.016593843698501587, 0.0038811543490737677, 0.03602044656872749, 0.028633059933781624, -0.016677161678671837, 0.003219830570742488, 0.021676143631339073, 0.01262937393039465, -0.0069430312141776085, 0.014996946789324284, 0.020606916397809982, 0.02105127088725567, 0.007644277065992355, -0.024064546450972557, -0.026966731995344162, 0.00774147966876626, 0.039408646523952484, -0.0027338184881955385, 0.03088260255753994, -0.03127141296863556, 0.014066580682992935, -0.02224547229707241, 0.030993690714240074, 0.0008965188753791153, -0.009442522190511227, 0.011657348833978176, -0.021537283435463905, -0.012247506529092789, -0.00034606672124937177, 0.0013790595112368464, -0.006373702548444271, -0.013615284115076065, -0.020884636789560318, 0.012337766587734222, 0.027730466797947884, 0.00681805657222867, 0.025966936722397804, 0.006064737681299448, 0.005762715823948383, -0.02907741442322731, 0.06026551127433777, -0.005238517187535763, 0.027438858523964882, -0.01594119891524315, 0.005891161970794201, 0.013434764929115772, 0.018607323989272118, -0.010976932011544704, -0.0057835448533296585, -0.007769251707941294, -0.02220381423830986, -0.004801106173545122, -0.015774566680192947, 0.0049955109134316444, -0.006856243126094341, 0.004631001967936754, -0.02509211376309395, 0.02388402633368969, 0.003553096204996109, 0.015594047494232655, 0.002058608690276742, -0.005054526496678591, 0.016760477796196938, 0.01696876809000969, -0.004884422291070223, 0.00501633994281292, -0.01752421073615551, 0.0023623663000762463, -0.0052176876924932, 0.007755365688353777, 0.0007715443498454988, 0.02380071021616459, -0.02757771871984005, -0.0032163590658456087, -0.005974478088319302, -0.004172761924564838, -0.007276296615600586, 0.0047073750756680965, -0.012247506529092789, 0.023161951452493668, 0.0022755784448236227, 0.028202593326568604, 0.005505823530256748, 0.0026713311672210693, -0.02289811708033085, 0.010969989001750946, -0.004835821222513914, -0.009268946945667267, -0.021148473024368286, -0.008213605731725693, -0.026466835290193558, -0.010164598003029823, -0.01641332544386387, 0.027883213013410568, -0.008019200526177883, -0.007984485477209091, -0.03377090394496918, -0.004269964061677456, -0.002134982030838728, -0.047990232706069946, 0.03066042624413967, 0.030132755637168884, -0.02177334576845169, -0.03815889731049538, -0.007887283340096474, -0.17951901257038116, 0.01885727234184742, 0.009609155356884003, -0.006838885601609945, 0.02503656968474388, 0.005686342716217041, 0.022745370864868164, -0.015038605779409409, -0.03707578778266907, 0.011844811029732227, 0.011615690775215626, -0.004322037100791931, -0.017079856246709824, -0.008317750878632069, -0.002997653791680932, 0.002758119022473693, -0.0003443309396971017, -0.009289775975048542, 0.010511749424040318, 0.0004703903687186539, 0.025411494076251984, -0.006772927008569241, -0.011574032716453075, 0.004433125257492065, 0.009352263063192368, 0.013761087320744991, -0.025397608056664467, 0.00762344803661108, -0.002537677763029933, -0.012796006165444851, 0.002723403973504901, 0.025230975821614265, -0.007644277065992355, -0.019621005281805992, 0.008033087477087975, -0.024939367547631264, -0.0007168679730966687, -0.024383924901485443, 0.005790487863123417, 0.016552185639739037, 0.016010629013180733, 0.010143768042325974, 0.010289572179317474, 0.0076581635512411594, 0.006439661141484976, -0.004755976144224405, 0.026300201192498207, 0.00031655881321057677, 0.02134287729859352, -0.027938757091760635, 0.0066167088225483894, -0.041241604834795, 0.0022408633958548307, 0.008130289614200592, -0.016954882070422173, 0.007172151003032923, 0.013615284115076065, 0.013990207575261593, -0.008040030486881733, -0.000234978215303272, -0.020468056201934814, -0.031549133360385895, 0.010324287228286266, 0.0076303910464048386, -0.024425582960247993, -0.033187687397003174, -0.007935884408652782, -0.01782970316708088, -0.027772124856710434, 0.011518488638103008, 0.006509091705083847, -0.021828889846801758, 0.013754144310951233, -0.02212049625813961, 0.012740462087094784, 0.012178076431155205, 0.007123549934476614, 0.018440689891576767, -0.0003065782075282186, 0.003794366493821144, -0.012462740764021873, 0.043879956007003784, -0.015427415259182453, 0.004752504639327526, -0.01984318345785141, 0.01937105692923069, 0.011303254403173923, -0.0010917916661128402, 0.0318823978304863, 0.0007546207052655518, 0.011823982000350952, -0.042463578283786774, 0.002315500983968377, -0.022620394825935364, -0.00036407518200576305, 0.008894022554159164, 0.018648982048034668, -0.008456612005829811, 0.010963045991957188, -0.0025359420105814934, -0.00013549759751185775, -0.030771514400839806, -0.006804170552641153, 0.0023259154986590147, 0.02710559405386448, -0.010227085091173649, -0.006783341523259878, 0.04210254177451134, 0.018496235832571983, -0.02259262278676033, -0.01910722255706787, 0.0033274476882070303, 0.0161078330129385, -0.009685528464615345, -0.016566071659326553, 0.024578331038355827, -0.00942863617092371, -0.011303254403173923, 0.025841962546110153, 0.005276703741401434, 0.06743071973323822, 0.024453354999423027, 0.0006378910038620234, -0.012997354380786419, -0.0006687006680294871, 0.015705136582255363, -0.07498473674058914, 0.001482337131164968, 0.009373092092573643, -0.009088427759706974, -0.004565042909234762, 0.044296540319919586, 0.013205645605921745, 0.037992265075445175, -0.008366352878510952, 0.03471515700221062, 0.013941606506705284, -0.022148270159959793, 0.007998371496796608, -0.007262410596013069, -0.0038186670280992985, -0.022023294121026993, -0.001164693501777947, -0.016635501757264137, -0.027563832700252533, 0.022023294121026993, 0.003171229502186179, 0.008067802526056767, -0.008567700162529945, 0.0001568691077409312, -0.0025463567581027746, 0.028272023424506187, -0.027758238837122917, 0.012073931284248829, 0.02530040591955185, 0.018149083480238914, 0.032187893986701965, -0.011310197412967682, 0.012622430920600891, 0.013115385547280312, 0.00794282741844654, 0.004613643977791071, -0.07115218043327332, -0.030688198283314705, 0.03499287739396095, -0.025369836017489433, 0.0011473358608782291, 0.01050480641424656, -0.0020308366511017084, -0.03496510535478592, -0.0030688196420669556, -0.016940996050834656, -0.021828889846801758, 0.01178926695138216, 0.02507822774350643, -0.0025862790644168854, -0.01705208420753479, -0.007588732987642288, 0.006661838386207819, -0.012740462087094784, 0.016330009326338768, 0.031549133360385895, -0.006595879793167114, 0.037603456526994705, -0.020801320672035217, 0.011206052266061306, 0.003981828223913908, -0.0018138668965548277, -0.0009572704439051449, 0.00014244062185753137, 0.027091708034276962, -0.01539964322000742, -0.01123382430523634, -0.007151321973651648, -0.0029369022231549025, -0.012747405096888542, -0.007158264983445406, 0.008484384045004845, -0.03557609021663666, 0.025883620604872704, -0.02693895995616913, 0.011261596344411373, -0.005550953559577465, -0.0163577813655138, -0.017621412873268127, -0.03010498359799385, -0.02010701783001423, -0.012268335558474064, 0.002528999000787735, -0.014816428534686565, -0.006585464812815189, 0.006130696274340153, -0.005915462505072355, 0.013434764929115772, -0.0012471419759094715, -0.024286722764372826, 0.03504842147231102, 0.011740665882825851, 0.012525227852165699, -0.007324897684156895, -0.013774973340332508, -0.010706153698265553, -0.025592012330889702, -0.00013159213995095342, -0.015774566680192947, 0.0251754317432642, -0.0047247326001524925, -0.013525024987757206, -0.06759735196828842, 0.022398218512535095, -0.0158995408564806, -0.017774159088730812, 0.007727593649178743, -0.008657960221171379, 0.022009408101439476, -0.031854625791311264, -0.013629170134663582, 0.003832553280517459, -0.03396530821919441, 0.019857069477438927, -0.008519099093973637, 0.01988484151661396, -0.013101499527692795, -0.012546056881546974, 0.021801117807626724, -0.036353711038827896, 0.029743945226073265, 0.030771514400839806, 0.006047380156815052, -0.030354931950569153, 0.024300608783960342, -0.0073040686547756195, 0.007179094012826681, 0.0158995408564806, -0.017704728990793228, 0.01769084297120571, -0.019662663340568542, -0.025147657841444016, 0.010470091365277767, -0.026564037427306175, -0.008116403594613075, 0.022967547178268433, -0.008331636898219585, -0.006814585067331791, 0.005137843079864979, 0.02435615286231041, 0.014788656495511532, 0.017163172364234924, -0.03177130967378616, -0.027036163955926895, 0.006849300116300583, -0.02289811708033085, -0.022828686982393265, 0.011692064814269543, -0.004512970335781574, 0.00014612911036238074, 0.006113338749855757, 0.016691047698259354, 0.012782120145857334, -0.006141111254692078, -0.006620180327445269, -0.024619989097118378, -0.004422710742801428, -0.008630187250673771, -0.007192980032414198, -0.019995929673314095, 0.005793959368020296, 0.008498270064592361, 0.014156840741634369, 0.009782730601727962, 0.021759459748864174, 0.011497659608721733, 0.01606617495417595, 0.02005147375166416, -0.002537677763029933, 0.007720650639384985, 0.018996132537722588, 0.007491530384868383, -0.02237044647336006, 0.005502352025359869, 0.019732095301151276, 0.018621210008859634, -0.008352466858923435, -0.0036902211140841246, 0.014316529966890812, 0.014233213849365711, -0.012400253675878048, 0.03110477887094021, -0.009074541740119457, -0.004377581179141998, -0.025453152135014534, 0.004186647944152355, 0.011372685432434082, 0.004197062458842993, -0.0320490300655365, -0.006526449229568243, 0.0037631229497492313, 0.013018183410167694, -0.004221362993121147, 0.019315512850880623, -0.009949363768100739, -0.027688808739185333, -0.008220548741519451, 0.002541149500757456, -0.03365981578826904, -0.006606294307857752, -0.006995103787630796, 0.02066246047616005, 0.013851347379386425, 0.010969989001750946, -0.0032962041441351175, -0.017718615010380745, -0.0319657139480114, 0.014844200573861599, -0.006252199411392212, -0.006457019131630659, -0.008470498025417328, 0.007151321973651648, 0.022092724218964577, -0.013920777477324009, 0.00886</t>
-  </si>
-  <si>
-    <t>Which clients are employed by Stevens Valley School? Include Employer name, client name, client id, and their complete address</t>
-  </si>
-  <si>
-    <t>SELECT client.Name, client.ID, employer.Name, address.Address, address.City, address.State, address.Zip FROM client INNER JOIN employer ON client.Employer_ID = employer.ID INNER JOIN address ON client.Address_ID = address.ID WHERE employer.Name = 'Stevens Valley School';</t>
-  </si>
-  <si>
-    <t>[0.012723113410174847, 0.01613204926252365, -0.002328544622287154, -0.01813177950680256, -0.0155952088534832, 0.04493352770805359, -0.008146550506353378, -0.012065484188497066, -0.020064404234290123, -0.022708341479301453, -0.010307332500815392, 0.0060897814109921455, -0.011280355975031853, 0.01131390780210495, -0.019795984029769897, -0.009481940418481827, 0.005418731365352869, -0.033230412751436234, 0.016776258125901222, -0.009663124568760395, -0.009387994185090065, 0.013078770600259304, 0.011850748211145401, -0.0025416030548512936, -0.005435507278889418, -0.013696136884391308, -0.00011659498704830185, -0.012166141532361507, -0.002120519056916237, 0.00711313309147954, 0.0015576755395159125, -0.017098361626267433, -0.007488921284675598, -0.03843776136636734, -0.010199964977800846, 0.011293776333332062, -8.781321957940236e-05, 0.011340750381350517, 0.017621781677007675, 0.011998379603028297, 0.021929923444986343, -0.016118628904223442, -0.011441407725214958, -0.0005104176234453917, -0.003195876954123378, -0.006529319565743208, -0.005589848849922419, -0.015970997512340546, -0.03935039043426514, 0.013810215517878532, 0.02447991445660591, -0.003566632280126214, -0.010542199946939945, -0.02348676137626171, 0.011280355975031853, 0.004945640917867422, -0.00655951676890254, 0.004388669040054083, -0.02515096589922905, -0.01725941337645054, 0.00012372489436529577, 0.0015652248403057456, -0.008609575219452381, -0.002300024963915348, -0.011434697546064854, -0.007670104969292879, -0.004603405017405748, 0.011112593114376068, -0.0037075530271977186, 0.011448117904365063, 0.03951144218444824, 0.0077976044267416, -0.003616961184889078, 0.00868339091539383, -0.006260899361222982, -0.021151505410671234, 0.002107098000124097, -0.024251757189631462, 0.011542065069079399, 0.008421680890023708, -0.012105747126042843, -0.025768332183361053, -0.03143199533224106, 0.023540444672107697, 0.026533329859375954, -0.00790497288107872, 0.0033904816955327988, -0.0023469985462725163, -0.018534408882260323, -0.0030012724455446005, 0.0143336346372962, 0.015554945915937424, -0.017192307859659195, 0.012884166091680527, -0.015165736898779869, 0.013769952580332756, 0.01415916159749031, 0.01613204926252365, 0.018816251307725906, -0.02164808288216591, 0.001157561782747507, 0.02131255716085434, -0.016440732404589653, -0.017326518893241882, -0.026318592950701714, 0.004657089244574308, -0.01197824813425541, -0.02217150293290615, -9.908476931741461e-05, -0.021822554990649223, -0.025285175070166588, 0.004036367405205965, 0.003744460642337799, -0.009696677327156067, 0.012817060574889183, 0.007690236438065767, 0.022641237825155258, 0.002221176400780678, 0.01197824813425541, -0.014830212108790874, 0.02128571644425392, 0.017044678330421448, 0.02172860875725746, -0.022037291899323463, 0.018749145790934563, 0.004499392118304968, -0.014024951495230198, -0.012112458236515522, 0.002966042375192046, -0.0010342563036829233, -0.01735336147248745, 0.01487047504633665, 0.01032746396958828, -0.01801099069416523, -0.02065492793917656, -0.019245723262429237, 0.008643127977848053, 0.027217799797654152, -0.026278330013155937, -0.015259684063494205, 0.005928729195147753, 0.027043327689170837, 0.016105206683278084, 0.01634678617119789, -0.00022039808391127735, 0.01097167283296585, 0.027754640206694603, 0.02955305576324463, 0.007186948787420988, -0.013072059489786625, -0.01733993925154209, 0.0033233766444027424, 0.0022379527799785137, -0.015648892149329185, -0.007931814529001713, 0.0057878089137375355, 0.018588094040751457, 0.01197824813425541, -0.015970997512340546, -0.032344624400138855, -0.03467987850308418, 0.030009370297193527, 0.019943615421652794, -0.02294992096722126, 0.012568771839141846, 0.018977303057909012, -0.028720952570438385, -0.03347199037671089, 0.008005630224943161, -0.00013620224490296096, -0.015232841484248638, 0.001649106154218316, -0.027486220002174377, 0.012454693205654621, 3.3211748814210296e-05, -0.006750766187906265, 0.0010250293416902423, -0.007394974119961262, -0.00422761682420969, -0.033901460468769073, 0.01372968964278698, 0.00046889641089364886, -0.011850748211145401, 0.03580724447965622, -0.011354170739650726, -0.007743920665234327, 0.0007893228903412819, 0.0014259818708524108, 0.013823635876178741, -0.006304517388343811, 0.04592668265104294, 0.023204918950796127, 0.005576428025960922, -0.0029777856543660164, -0.6321830749511719, -0.023540444672107697, -0.006817871239036322, -0.020708613097667694, 0.021003874018788338, 0.02383570745587349, 0.02524491213262081, 0.015729419887065887, -0.007287606131285429, 0.017957305535674095, -0.012266799807548523, 0.041229330003261566, -0.012152721174061298, 0.00559655949473381, 0.006878265645354986, -0.026425961405038834, -0.010877725668251514, 0.01236074697226286, 0.003368672449141741, -0.005006035324186087, -0.010911277495324612, 0.02756674587726593, -0.002308413153514266, 0.009763781912624836, 0.04028986021876335, 0.027942534536123276, -0.007019186392426491, -0.0233928132802248, -0.0019091381691396236, 0.011864169500768185, -0.01725941337645054, 0.02317807823419571, -0.0034273893106728792, 0.016319943591952324, 0.034545671194791794, 0.016964152455329895, -0.023084130138158798, 0.041900381445884705, -0.007616420742124319, 0.040370386093854904, -0.018722303211688995, -0.03065357729792595, 0.008851153776049614, -0.013823635876178741, -0.004197419621050358, 0.02963358163833618, 0.00939470436424017, 0.006374977994710207, -0.0064085302874445915, -0.006492411717772484, 0.018843092024326324, -0.017058098688721657, -0.028801478445529938, 0.0005523582804016769, 0.029069898650050163, -0.033230412751436234, -0.0024912741500884295, -0.002437590155750513, 0.0006819548434577882, 0.009146415628492832, -0.007663394324481487, 0.01877598837018013, -0.01911151222884655, -0.016870204359292984, -0.024533599615097046, 0.014534949325025082, -0.0039759729988873005, -0.012756666168570518, 0.02065492793917656, -0.012944560497999191, 0.018400199711322784, 0.02437254786491394, 0.011521933600306511, 0.022533869370818138, 0.011797063983976841, 0.0014159161364659667, -0.0015006362227723002, -0.0030516013503074646, -0.005888466257601976, 0.009132994338870049, 0.0008509756880812347, -0.015769682824611664, -0.013957845978438854, -0.011126014403998852, -0.010636147111654282, 0.006311228033155203, -0.027271484956145287, -0.02250702679157257, 0.00708629097789526, -0.02351360209286213, 0.02152729406952858, 0.010548911057412624, 0.01615889184176922, -0.025983067229390144, -0.007012475747615099, 0.014508107677102089, 0.014065214432775974, -0.004006170202046633, 0.008321023546159267, -0.027419114485383034, -0.017715727910399437, 0.00025164385442622006, 0.002088644076138735, 0.015528104268014431, 0.007623131386935711, 0.010065754875540733, -0.02845253236591816, 0.010233516804873943, 0.0031757454853504896, -0.014977842569351196, 0.015581788495182991, -0.008260629139840603, -0.02810358628630638, 0.00010181091056438163, -0.02735201083123684, -0.038276709616184235, 0.011280355975031853, 0.015447578392922878, -0.020842822268605232, 0.003120383946225047, 0.028479374945163727, 0.003533079754561186, 0.021809134632349014, -0.02328544482588768, 0.007663394324481487, 0.016064943745732307, -0.000575006240978837, -0.030814629048109055, 0.004334984812885523, 0.002300024963915348, 0.005230837035924196, -0.01427995041012764, 0.03269357234239578, -0.014065214432775974, -0.00939470436424017, -0.007864709943532944, 0.020292561501264572, -0.011998379603028297, -0.015877049416303635, -0.02976779080927372, 0.002308413153514266, 0.015031526796519756, -0.004855048842728138, -0.00678431848064065, -0.005432152189314365, -0.010938120074570179, -0.007656684145331383, -0.007348001003265381, -0.016172312200069427, -0.011186408810317516, -0.011025356128811836, -0.0066433981992304325, 0.008267339318990707, 0.011454829014837742, 0.006009255535900593, 0.0012825449230149388, -0.003908867947757244, -0.02175545133650303, 0.004865114577114582, -0.017487570643424988, 0.0057710325345396996, 0.01648099534213543, -0.01042812131345272, -0.02217150293290615, -0.004435642622411251, -0.00928733590990305, 0.02810358628630638, -0.002935845172032714, 0.0053046527318656445, -0.0048047201707959175, 0.03612934798002243, 0.0004684769955929369, -0.004006170202046633, 0.011515223421156406, 0.005126824136823416, 0.032666727900505066, -0.03019726276397705, 0.006683661136776209, -0.01988993026316166, -0.015152315609157085, 0.009676544927060604, 0.0059253741055727005, -0.006421951577067375, 0.019245723262429237, 0.02515096589922905, 0.006884976290166378, 0.0033049227204173803, 0.012897586449980736, -0.013957845978438854, -0.025728069245815277, -0.0009361151605844498, 0.005730769596993923, 0.007488921284675598, -0.012944560497999191, 0.025312017649412155, 0.020722033455967903, 0.01405179314315319, 0.01214601006358862, 0.020480455830693245, 0.024345705285668373, 0.02909674122929573, -0.003303245175629854, 0.010770357213914394, 0.012072195298969746, 0.0377667099237442, -0.03167357295751572, -0.0018068029312416911, -0.019192038103938103, 0.02547306939959526, 0.02164808288216591, 0.006368267349898815, -0.025419386103749275, -0.018507568165659904, -0.011079040355980396, -0.014548370614647865, 0.005677085369825363, -0.005019456148147583, 0.02019861340522766, -0.011669564992189407, -0.0032965345308184624, 0.010361016727983952, -0.011495091952383518, 0.04117564484477043, -0.00977049209177494, 0.0026842011138796806, 0.006415240932255983, 0.01147496048361063, 0.025567015632987022, 0.010548911057412624, 0.005120113957673311, -0.010964961722493172, 0.005448928568512201, 0.02657359279692173, 0.00395248644053936, 0.003888736478984356, 0.011119303293526173, 0.015340209938585758, -0.013756531290709972, 0.028613584116101265, -0.016306523233652115, -0.013219690881669521, 0.006848068442195654, 0.013521663844585419, -0.006750766187906265, 0.03274725377559662, 0.025338860228657722, 0.011005224660038948, 0.018185462802648544, -0.00835457630455494, 0.04074617475271225, -0.0018437106627970934, 0.018427040427923203, -0.008374707773327827, 0.00524090277031064, 0.013434426859021187, 0.006556161679327488, 0.02207755483686924, 0.013152586296200752, 0.022574132308363914, 0.01580994576215744, -0.007361421827226877, -0.008428392000496387, 0.0018789408495649695, -0.01648099534213543, 0.028291480615735054, 0.019285986199975014, -0.03151252120733261, -0.008502207696437836, 0.011615880765020847, -0.024734914302825928, 0.003274725517258048, 0.007636552676558495, 0.007824446074664593, 0.016521258279681206, 0.019849667325615883, 0.009528914466500282, -0.015984417870640755, 0.005472415126860142, 0.008716943673789501, 0.011991668492555618, -0.019245723262429237, -0.006848068442195654, -0.0006966341170482337, 0.0143336346372962, 0.010897857137024403, 0.01724599301815033, 0.003590119071304798, 0.008763916790485382, -0.029177267104387283, 0.015568367205560207, 0.01329350657761097, -0.004046433139592409, -0.025432806462049484, 0.014696002006530762, 0.00028603518148884177, 8.398613863391802e-05, 0.00972351897507906, -0.03298883140087128, -0.0005297103198245168, 0.014951000921428204, -0.0035397903993725777, 0.01218627393245697, 0.023003604263067245, 0.021782292053103447, 0.05467717722058296, -0.013139165006577969, -0.006663529668003321, -0.017286255955696106, -0.011360881850123405, -0.01756809651851654, 0.015957575291395187, 0.016172312200069427, -0.01766204461455345, -0.0010879402980208397, 0.03591461107134819, -0.014964422211050987, -0.015877049416303635, -0.00845523364841938, 0.042678799480199814, -0.013850478455424309, -0.027097010985016823, -0.04818141087889671, -0.028613584116101265, 0.011783643625676632, 0.07558710873126984, 0.029069898650050163, -0.01230035163462162, 0.007978787645697594, 0.018937040120363235, -0.0036840662360191345, -0.035297244787216187, -0.00022081748466007411, -0.0070460280403494835, -0.020077824592590332, 0.002467787591740489, -0.032022520899772644, -0.017648622393608093, -0.009851018898189068, 0.012957981787621975, 0.009267204441130161, 0.010924698784947395, -0.021607819944620132, -0.005841492675244808, -0.013702847063541412, -0.031002523377537727, 0.0023168011102825403, -0.00023277057334780693, 0.0063816881738603115, 0.01614546962082386, 0.023352550342679024, 0.023862548172473907, 0.02987515926361084, 0.01866861991584301, -0.024184653535485268, 0.011991668492555618, 0.033552516251802444, -0.00846194475889206, 0.024251757189631462, -0.00939470436424017, 0.04088038578629494, -0.012179562821984291, 0.0026959446258842945, 0.019916772842407227, 0.012971402145922184, 0.030438842251896858, 0.009629571810364723, -0.008602865040302277, -0.019084671512246132, 0.029150424525141716, 0.0064890566281974316, 0.007307737600058317, 0.004710773006081581, 0.0028972597792744637, -0.0020114732906222343, 0.011602459475398064, -0.004079985897988081, 0.031593047082424164, -0.038384076207876205, -0.019272563979029655, -0.0015299946535378695, -0.0028335098177194595, 0.008066024631261826, -0.02239965833723545, -0.03019726276397705, -0.04152459278702736, -0.005405310075730085, 0.006898397114127874, -0.011864169500768185, -0.007891551591455936, -0.006958791520446539, -0.0014972810167819262, 0.0062172808684408665, 0.003590119071304798, 0.001441080472432077, 0.009622861631214619, 0.028640426695346832, -0.02603675238788128, 0.012018511071801186, 0.03688092529773712, 0.015165736898779869, 0.027164116501808167, -0.003303245175629854, 0.00015559978783130646, 0.01131390780210495, -0.0031975547317415476, -0.015675734728574753, 0.013541795313358307, -0.0023671300150454044, -0.012595614418387413, 0.010924698784947395, -0.019178617745637894, 0.007663394324481487, -0.005713993217796087, 0.017621781677007675, -0.011105882935225964, -0.004207485355436802, -0.01582336612045765, -0.03062673658132553, -0.0028267994057387114, 0.002940878039225936, -0.0032176862005144358, 0.0023570642806589603, -0.011414566077291965, -0.0006223991513252258, 0.018265988677740097, -0.020722033455967903, 0.002456044079735875, -0.0025751555804163218, 0.017286255955696106, -0.013058639131486416, -0.007093001622706652, -0.007549315690994263, -0.02406386472284794, 0.009193388745188713, 0.02634543552994728, -0.01791704259812832, 0.005576428025960922, 0.006378333084285259, -0.000502448936458677, 0.008240497671067715, -0.00999864935874939, 0.005885111168026924, 0.00802576169371605, 0.010978383012115955, 0.01799756847321987, -0.009374572895467281, 0.029902001842856407, 0.01660178415477276, -0.028801478445529938, 0.008757206611335278, 0.0178096741437912, -0.02834516391158104, 0.020292561501264572, 0.002244663191959262, -0.016011260449886322, 0.02362097054719925, -0.009535624645650387, 0.003724329173564911, -0.019165197387337685, -0.01978256367146969, -0.017957305535674095, 0.018051253631711006, 0.0003132966230623424, -0.01582336612045765, -0.01988993026316166, 0.018198885023593903, -0.010126149281859398, 0.0008237142465077341, 0.00450610276311636, -0.031002523377537727, 0.002221176400780678, -0.015514682978391647, 0.018749145790934563, 0.018614934757351875, -0.020010720938444138, 0.011011935770511627, 0.015460998751223087, 0.02241308055818081, -0.005388534162193537, -0.009267204441130161, -0.017876779660582542, 0.03392830491065979, 0.023218341171741486, 0.012716403231024742, 0.014749685302376747, 0.012038642540574074, 0.017178887501358986, -0.038679338991642, -0.0005045459256507456, 0.007871420122683048, -0.02109782211482525, -0.020695190876722336, -0.003761237021535635, -0.01236074697226286, 0.02481544017791748, -0.007059449329972267, 0.018641777336597443, -0.004975838121026754, 0.004798009525984526, 0.0025751555804163218, 0.0057710325345396996, 0.005542875733226538, -0.011823906563222408, -0.057817693799734116, 0.0042678797617554665, -0.013320348225533962, -0.010978383012115955, 0.041121963411569595, -0.03663934767246246, -0.009280625730752945, 0.010683121159672737, -0.028694111853837967, -0.011716538108885288, -0.026533329859375954, 0.01197824813425541, -0.02591596357524395, 0.027727797627449036, -0.0058985319919884205, -0.0028502861969172955, -0.0077372100204229355, -0.005056363996118307, -0.039940912276506424, -0.011434697546064854, 0.02019861340522766, 0.013877320103347301, 0.010179833509027958, 0.02600990980863571, -0.0008639772422611713, -0.020480455830693245, 0.006522608920931816, 0.016427312046289444, 0.0022044002544134855, -0.009575887583196163, -0.01005233358591795, 0.012119168415665627, -0.006703792605549097, -0.005351626314222813, -0.0007234761142171919, 0.009508782997727394, -0.01481679081916809, -0.01932624913752079, 0.013528374023735523, -0.019742300733923912, -0.024976491928100586, 0.0035532114561647177, -0.03484093025326729, 0.010548911057412624, 0.024439651519060135, 0.03953828290104866, 0.030143579468131065, -0.0064253066666424274, -0.014548370614647865, 0.007743920665234327, -0.011615880765020847, 0.016199154779314995, 0.019957035779953003, 0.023312287405133247, -0.013863898813724518, -0.02284255251288414, 0.04536300152540207, -0.00044750666711479425, -0.004331629723310471, -0.0033149884548038244, 0.028506217524409294, 0.03712250292301178, 0.0009109507664106786, -0.017742570489645004, 0.00824720785021782, -0.025432806462049484, 0.014360476285219193, -0.0035196589305996895, 0.007938524708151817, -0.00708629097789526, 0.006539385300129652, -0.019581247121095657, -0.006844712886959314, -0.025956226512789726, 0.022426500916481018, 0.017970727756619453, -0.00325459404848516, -0.014628896489739418, 0.005247613415122032, 0.02307070977985859, 0.005036232527345419, -0.02120518870651722, 0.02831832319498062, -0.011434697546064854, -0.000204670344828628, -0.012763376347720623, 0.03280093893408775, -0.01801099069416523, -0.002117163734510541, 0.01868204027414322, 0.028801478445529938, -0.017219150438904762, -0.015997840091586113, 0.01669573225080967, -0.009025626815855503, -0.0008329412085004151, 0.012266799807548523, 0.0009923155885189772, -0.014239687472581863, -0.016561521217226982, -0.0035297246649861336, 0.030841471627354622, 0.00868339091539383, -0.00024011018103919923, -0.02351360209286213, 0.009401414543390274, -0.02733858861029148, -0.007334579713642597, -0.009783913381397724, -0.006421951577067375, -0.02351360209286213, -0.03161989152431488, 0.0009143060306087136, 0.007616420742124319, 0.00354314548894763, 0.011810485273599625, 0.0015367051819339395, -0.00256844493560493, 0.025325438007712364, -0.042651958763599396, 0.006992344278842211, -0.006445438135415316, 0.026224646717309952, -0.05148297920823097, 0.011401144787669182, -0.012978113256394863, -0.03229093924164772, -0.006458858959376812, 0.016293101012706757, -0.04042407125234604, -0.04340353235602379, 0.014534949325025082, 0.018051253631711006, -0.01399810891598463, -0.004948996007442474, -0.027298325672745705, -0.018078094348311424, 0.0004240199050400406, 0.0001700693101156503, -0.025567015632987022, 0.009213520213961601, -0.015219421125948429, -0.019500721246004105, -0.018359936773777008, -0.017219150438904762, 0.0070997122675180435, -0.012642587535083294, 0.022372817620635033, -0.01323982235044241, -0.006156886462122202, -0.02141992561519146, -0.012971402145922184, 0.009636281989514828, -0.020359667018055916, -0.0010845850920304656, -0.006737344898283482, -0.016387049108743668, -0.012884166091680527, 0.010669699870049953, -0.0032176862005144358, -0.02316465601325035, -0.004680575802922249, 0.0018940394511446357, 0.04149775207042694, 0.030224105343222618, -0.013810215517878532, -0.028828321024775505, -0.0038719603326171637, -0.032881464809179306, -0.03231778368353844, -0.012447983026504517, -0.0028704176656901836, 0.011334039270877838, 0.011669564992189407, -0.01527310535311699, -0.014548370614647865, -0.022439921274781227, -0.042007748037576675, -0.005344915669411421, 0.02151387184858322, 0.01583678647875786, 0.013615611009299755, 0.03956512734293938, -0.0007905811653472483, -0.0085626021027565, -0.005703927483409643, 0.03645145148038864, -0.015622051432728767, 0.011743380688130856, 0.0002967300533782691, -0.020681770518422127, 0.007623131386935711, 0.0009059178992174566, -0.01692388951778412, -0.010320753790438175, 0.0008841087692417204, -0.0031606468837708235, -0.0011139435227960348, -0.013078770600259304, -0.02712385356426239, 0.0006333037163130939, 0.0238491278141737, -0.008703522384166718, -0.017299676313996315, 0.018359936773777008, -0.009347730316221714, -0.006442083045840263, -0.018158622086048126, 0.0017078230157494545, -0.009522203356027603, -0.011609170585870743, -0.005224126391112804, 0.0010158023796975613, -0.018400199711322784, 0.01703125610947609, 0.012434561736881733, 0.013387453742325306, -0.013608899898827076, 0.0020332823041826487, 0.010012070648372173, 0.0056334673427045345, -0.015863629058003426, 0.0316467322409153, 0.0017497636144980788, 0.011743380688130856, 0.026439381763339043, 0.014011530205607414, -0.028372006490826607, -0.002942555584013462, -0.016776258125901222, -0.01240772008895874, 0.001143301953561604, -0.005730769596993923, -0.00259528704918921, -0.012468114495277405, -0.0025416030548512936, -0.014467844739556313, -0.0012624133378267288, -0.0028351875953376293, 0.008052603341639042, -0.013702847063541412, -0.015783103182911873, -0.01691046729683876, -0.025513332337141037, 0.007482211105525494, 0.0003189585986547172, -0.01669573225080967, -0.020601244643330574, -0.016762835904955864, -0.0004663799481932074, 0.015179158188402653, -0.03263988718390465, -0.007220501080155373, 0.01136759202927351, 0.0025432805996388197, 0.0002271085832035169, -0.02217150293290615, 0.214950829744339, 0.009743650443851948, -0.0007872259011492133, 0.01790362223982811, 0.002283248584717512, 0.010045623406767845, 0.037068817764520645, 0.008529049344360828, 0.003070055041462183, 0.01646757498383522, -0.0030398578383028507, -0.009159836918115616, 0.0006106557557359338, 0.010226806625723839, 0.021003874018788338, -0.03250567615032196, -0.03688092529773712, -0.01470942236483097, -0.031995680183172226, 0.009300757199525833, 0.006022676359862089, 0.026157541200518608, 0.011542065069079399, -0.03744460642337799, 0.02545964904129505, 0.014696002006530762, -0.009153125807642937, 0.044987212866544724, 0.030143579468131065, 0.032908305525779724, -0.02238623797893524, 0.01015299092978239, 0.015742840245366096, -0.00428130105137825, -0.0029811409767717123, -0.007643262855708599, 0.005871690344065428, -0.010146280750632286, 0.012743244878947735, 0.049711406230926514, 0.0059522162191569805, -0.031995680183172226, -0.03988723084330559, -0.02614411897957325, -0.01010601781308651, -0.011119303293526173, -0.007153396029025316, -0.003090186743065715, -0.019192038103938103, 0.017836516723036766, -0.03194199502468109, -0.003593474393710494, 0.004375247750431299, 0.009461808949708939, 0.001773250405676663, 0.010407989844679832, 0.008414970710873604, 0.023419655859470367, -0.03269357234239578, -0.008166681975126266, 0.00650583254173398, 0.024023599922657013, -0.006284385919570923, 0.029392004013061523, 0.026748064905405045, -0.01225337851792574, 0.00557307293638587, 0.01005233358591795, 0.02120518870651722, -0.02042677067220211, 0.027311747893691063, 0.013535084202885628, 0.023459918797016144, 0.016078365966677666, -0.03642461076378822, -0.03097568266093731, 0.012085615657269955, 0.023137815296649933, -5.4365558753488585e-05, 0.034223563969135284, -0.03961880877614021, -0.003700842382386327, -0.014615475200116634, 0.0007779989391565323, -0.010354306548833847, -0.013837057165801525, 0.019728878512978554, -0.01218627393245697, -0.00927391555160284, 0.013226401060819626, -0.009267204441130161, 0.00038040164508856833, -0.006119978614151478, -0.014830212108790874, 0.018386777490377426, 0.03569987788796425, 0.011555486358702183, 0.02813042886555195, 0.01027377974241972, 0.012508377432823181, -0.020037561655044556, 0.07021870464086533, 0.00262212916277349, 0.014588633552193642, -0.022265449166297913, -0.00582471676170826, 0.014306792058050632, 0.009609440341591835, -0.021218610927462578, -0.010803909972310066, -0.006690371315926313, -0.025499911978840828, -0.006884976290166378, -0.011099171824753284, 0.0023268668446689844, -0.0003850150969810784, 0.00582136120647192, -0.03161989152431488, 0.01658836379647255, 0.009032336995005608, 0.01877598837018013, -0.010797199793159962, 0.0006387560279108584, 0.025083860382437706, 0.02183597721159458, -0.00045044251601211727, -0.008931679651141167, -0.0188833549618721, -0.0015534814447164536, -0.010119438171386719, 0.014360476285219193, 0.00977049209177494, 0.019312826916575432, -0.025540174916386604, -0.00999864935874939, -0.005609980318695307, 0.003209298010915518, 0.00949536170810461, -0.0006882459856569767, -0.01733993925154209, 0.01657494157552719, -0.00516373198479414, 0.021701766178011894, 0.00620386004447937, -0.016400469467043877, -0.020708613097667694, -0.0077640521340072155, -0.010797199793159962, 0.003264659782871604, -0.03427724912762642, -0.022654658183455467, -0.028962530195713043, -0.016400469467043877, -0.012213115580379963, 0.03680039942264557, -0.012286931276321411, -0.01065627858042717, -0.03280093893408775, -0.010072465054690838, -0.006193794310092926, -0.035404615104198456, 0.0327204130589962, 0.020037561655044556, -0.02767411433160305, -0.04973824694752693, 0.006160241551697254, -0.17082256078720093, 0.0064789908938109875, 0.01405179314315319, -0.018869934603571892, 0.01119311898946762, -0.008294181898236275, 0.006730634719133377, -0.01053548976778984, -0.05258350074291229, 0.02273518405854702, 0.015098631381988525, -0.007817735895514488, -0.021715188398957253, -0.004982548300176859, -0.002420814009383321, -0.012011799961328506, -0.005284521263092756, -0.012642587535083294, 0.02548648975789547, 0.01415916159749031, 0.028828321024775505, -0.006170307751744986, -0.012005089782178402, -0.00894510094076395, -0.007093001622706652, 0.018467305228114128, -0.023124393075704575, 0.014441002160310745, -0.015662314370274544, -0.012011799961328506, -0.012239957228302956, 0.02909674122929573, 0.001132397330366075, -0.010448252782225609, 0.006059584207832813, -0.023808864876627922, -0.001465406152419746, -0.010508648119866848, 0.001641556853428483, 0.02195676602423191, 0.012293641455471516, 0.012045352719724178, 0.008529049344360828, 0.00392564432695508, 0.005911953281611204, -0.0022094331216067076, 0.02128571644425392, 0.022238606587052345, 0.019702037796378136, -0.036505136638879776, 0.013421006500720978, -0.04753720387816429, 0.016199154779314995, 0.010119438171386719, -0.011132724583148956, 0.020359667018055916, 0.02131255716085434, 0.012984823435544968, -0.011427986435592175, 0.0011533676879480481, -0.017715727910399437, -0.034250408411026, 0.000980572309345007, -0.012280220165848732, -0.020252298563718796, -0.010770357213914394, -0.007475500460714102, -0.018910197541117668, -0.010569042526185513, 0.017729148268699646, -0.009797334671020508, -0.03548514097929001, 0.01427995041012764, -0.029392004013061523, 0.020359667018055916, -0.01098509319126606, -0.00021599431056529284, 0.008884705603122711, -0.006646753288805485, -0.0017212440725415945, -0.023459918797016144, 0.03435777500271797, -0.00488524604588747, 0.006331359501928091, -0.01318613812327385, 0.009924833662807941, 0.010824041441082954, 0.006707147695124149, 0.04960403963923454, 0.008710232563316822, 0.0031774232629686594, -0.04796667397022247, 0.020936770364642143, -0.014038372784852982, 0.005784453824162483, 0.004690641537308693, 0.036934610456228256, 0.0002742918150033802, 0.010716672986745834, 0.0027429182082414627, 0.0064789908938109875, -0.038491446524858475, -0.012823771685361862, 0.019017565995454788, 0.03438461571931839, -0.011461539193987846, -0.011501802131533623, 0.04018249362707138, 0.03170041739940643, -0.005942150484770536, -0.02799621783196926, 0.016749415546655655, 0.00845523364841938, -0.00028666428988799453, -0.00358340865932405, 0.012602324597537518, -0.03897460177540779, -0.027862008661031723, 0.01202522125095129, 0.022587552666664124, 0.04700036346912384, 0.02909674122929573, 0.008831022307276726, 0.0010493549052625895, 0.005885111168026924, 0.0044759055599570274, -0.07311764359474182, -0.007287606131285429, 0.00873036403208971, -0.005895176902413368, 0.008032471872866154, 0.04445037245750427, 0.0012422818690538406, 0.04581931605935097, 0.010736804455518723, 0.037068817764520645, -0.010374438017606735, -0.006740700453519821, 0.00425445893779397, -0.006210570689290762, -0.006187083665281534, -0.018413620069622993, -0.017407044768333435, -0.019178617745637894, -0.017098361626267433, 0.030250947922468185, -0.013132454827427864, -0.009971807710826397, 0.009837597608566284, 0.0018252568552270532, -0.01615889184176922, 0.02054755948483944, -0.020050983875989914, 0.012038642540574074, 0.023352550342679024, 0.014360476285219193, 0.025003334507346153, -0.008750495500862598, 0.006723924074321985, 0.021701766178011894, 0.005549585912376642, 0.01005233358591795, -0.06570924818515778, -0.023097550496459007, 0.023110972717404366, -0.023325707763433456, -0.004438997711986303, 0.00428130105137825, 0.010085886344313622, -0.027486220002174377, -0.0009218553313985467, 0.0030281145591288805, -0.017433887347579002, 0.024654388427734375, 0.027862008661031723, -0.014481265097856522, -0.02810358628630638, -0.0025130833964794874, -0.012763376347720623, -0.015152315609157085, 0.010421411134302616, 0.016668889671564102, -0.012756666168570518, 0.024412810802459717, -0.026184381917119026, 0.005653598811477423, 0.012414430268108845, -0.007515763398259878, 0.004925509449094534, -0.005099982488900423, 0.022668078541755676, -0.018413620069622993, -0.021473608911037445, -0.005405310075730085, 0.014347055926918983, -0.014494686387479305, -0.00043114981963299215, 0.012441272847354412, -0.04031670093536377, 0.017286255955696106, -0.036961451172828674, -0.01042812131345272, -0.02184939756989479, -0.005764321889728308, -0.016105206683278084, -0.02294992096722126, -0.00526774488389492, -0.015125473961234093, -0.025956226512789726, -0.00823378749191761, 0.0021758805960416794, 0.015608630143105984, -0.010662989690899849, 0.0011961471755057573, -0.011682985350489616, -0.02802306041121483, 0.035001982003450394, 0.014749685302376747, 0.01582336612045765, -0.017044678330421448, -0.008367997594177723, -0.02405044250190258, -0.037713028490543365, -0.00229163677431643, -0.0072808959521353245, 0.012729824520647526, 0.0006395948003046215, 0.0010325786424800754, -0.07655341923236847, 0.01009930670261383, -0.01932624913752079, -0.022493606433272362, -0.0036639347672462463, 0.002776470733806491, 0.02536570094525814, -0.025728069245815277, -0.011340750381350517, 0.022788867354393005, -0.01571599766612053, 0.01114614587277174, -0.0031858112197369337, 0.03148568049073219, -0.016333363950252533, -0.009481940418481827, 0.02963358163833618, -0.02284255251288414, 0.0026808460243046284, 0.024130968376994133, -0.006978922989219427, -0.021473608911037445, 0.008502207696437836, -0.010032202117145061, 0.007032607216387987, 0.03314988315105438, -0.020144930109381676, 0.010891146026551723, -0.01334047969430685, -0.013085480779409409, 0.01580994576215744, -0.022896235808730125, 0.005713993217796087, 0.04098775237798691, -0.012219825759530067, 0.010850883089005947, 0.0256878063082695, 0.025983067229390144, 0.01715204492211342, -0.021809134632349014, -0.02692253887653351, -0.013246532529592514, 0.005576428025960922, -0.016964152455329895, -0.016950730234384537, 0.012045352719724178, -0.01214601006358862, -0.011374302208423615, 0.008663259446620941, 0.020359667018055916, 0.021795714274048805, -0.00895852129906416, -0.006791029125452042, -0.015246262773871422, 0.0032915016636252403, -0.02799621783196926, -0.0022564067039638758, -0.011877590790390968, 0.011186408810317516, -0.008609575219452381, 0.05094613879919052, -0.0031774232629686594, 0.037954606115818024, 0.002773115411400795, 0.025083860382437706, 0.008005630224943161, -0.007394974119961262, 0.008482076227664948, 0.0005762644577771425, 0.008314313367009163, -0.026667539030313492, -0.015528104268014431, 0.007267474662512541, 0.008857863955199718, 0.020279139280319214, 0.010783778503537178, 0.015232841484248638, 0.02657359279692173, -0.004428931977599859, 0.02052071876823902, 0.02527175471186638, 0.013031796552240849, -0.017111781984567642, 0.014360476285219193, 0.010132859461009502, 0.01527310535311699, -0.045872997492551804, 0.003918933682143688, 0.004603405017405748, 0.00807944592088461, -0.024627545848488808, 0.028157271444797516, -0.02183597721159458, -0.019916772842407227, -0.0015677412739023566, 0.013984688557684422, -0.019916772842407227, 0.0016533001326024532, 0.020735453814268112, 0.0038216314278542995, -0.006569582503288984, 0.02053413912653923, -0.0025265044532716274, -0.01680309884250164, -0.03030463121831417, 0.015447578392922878, -0.024627545848488808, -0.018520988523960114, -0.010844172909855843, 0.02219834364950657, -0.007717078551650047, -0.00861628632992506, 0.010850883089005947, 0.016387049108743668, -0.006173662841320038, 0.001405850</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -124,43 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -448,93 +420,147 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Question</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Query</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Metadata</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Embedding</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>What are Mary Spocks account balances on 10/10/2023?</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>SELECT account.acct_nbr, balance.balance, product.type, date.date FROM account INNER JOIN product ON account.product_id = product.id INNER JOIN balance ON account.id = balance.account_id INNER JOIN date ON balance.balance_dt_id = date.id  INNER JOIN relationship ON account.id = relationship.account_id  INNER JOIN client ON relationship.client_id = client.id WHERE client.name = 'Mary Spock' AND date.date = '2023-10-10' AND relationship.relationship_type = 'Primary';</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>[-0.006811780855059624, -0.029691310599446297, -0.010255862027406693, -0.03327426314353943, -0.020845022052526474, 0.005402207374572754, -0.04346763342618942, 0.005169593263417482, -0.014845655299723148, -0.008235241286456585, 0.032774318009614944, 0.004593265242874622, -0.01749815233051777, 0.012193157337605953, 0.01687321811914444, 0.029552435502409935, 0.011582110077142715, -0.007086057215929031, 0.0036905824672430754, -0.033940862864255905, -0.011408518068492413, 0.01665101945400238, -0.017220403999090195, 0.007325615268200636, -0.010110043920576572, -0.0090198814868927, 0.00512445904314518, -0.005860492587089539, 0.001820988254621625, -0.03602397441864014, 0.02363639324903488, -0.003975274972617626, -0.0018522350583225489, -0.027219347655773163, -0.019275743514299393, -0.011776534840464592, -0.014144339598715305, -0.0110335573554039, 0.0061937905848026276, 0.0005290239932946861, -0.006245868280529976, 0.043106559664011, -0.014692893251776695, -0.007006204687058926, -0.01983124017715454, 0.005093212239444256, -0.007582532707601786, -0.02858031541109085, -0.029580211266875267, -0.0072006285190582275, 0.026108354330062866, -0.0008792474400252104, -0.011998733505606651, 0.0037496041040867567, 0.015595575794577599, -0.02426132746040821, 0.014061015099287033, 0.009728139266371727, -0.01801198720932007, 0.015692787244915962, 0.01013781875371933, 0.0011196734849363565, -0.012047339230775833, 0.022955909371376038, -0.017248179763555527, -0.0024771690368652344, -0.011589054018259048, -0.010734978131949902, -0.016928767785429955, 0.019039656966924667, 0.00519736809656024, 0.011568223126232624, 0.005860492587089539, -0.011616828851401806, 0.009533715434372425, -0.027983156964182854, -0.00512445904314518, -0.004645342938601971, 0.0008466988219879568, 0.0036871107295155525, 0.017664801329374313, 0.004471749998629093, -0.0007503547822125256, -0.009290685877203941, 0.009582322090864182, -0.0034857431892305613, 0.01385270431637764, 0.005200839601457119, -0.0210394449532032, 0.01826196163892746, 0.030135707929730415, 0.02320588380098343, 0.025372320786118507, 0.02108110673725605, -0.021136658266186714, 0.006162543781101704, -0.02833034284412861, 0.014512356370687485, -0.011852915398776531, -0.020581159740686417, -0.014248495921492577, 0.008464383892714977, -0.0351351797580719, -0.012033451348543167, -0.019859014078974724, -0.013811041601002216, -0.0005350997671484947, 0.003124670125544071, 0.01690099388360977, -0.005249445792287588, -0.0019060487393289804, 0.0014781425707042217, 0.017942549660801888, -0.013436081819236279, -0.0019112565787509084, -0.015026191249489784, 0.011727928183972836, 0.006690266076475382, -0.016053861007094383, -0.005721617955714464, 0.029996832832694054, 0.010130874812602997, 0.0024025242310017347, -0.006905520800501108, 0.0036142016761004925, -0.015317827463150024, -0.006027141585946083, -0.01445680670440197, -0.013324982486665249, -0.005169593263417482, 0.00583618925884366, -0.002320935484021902, -0.0012698312057182193, -0.009207361377775669, -0.0062180934473872185, 0.024566851556301117, -0.029135812073946, 0.007214515935629606, -0.012873641215264797, -0.03235769644379616, 0.003081271890550852, 0.03110782615840435, -0.007693632040172815, -0.00817969162017107, -0.002989267697557807, -0.0021473427768796682, 0.013901310041546822, 0.012095944955945015, -0.003520461730659008, -0.01270004827529192, 0.014054072089493275, 0.014720668084919453, -0.005235558375716209, -0.008867119438946247, -0.003319093957543373, 0.004138452000916004, 0.020011775195598602, 0.024164116010069847, -0.00490226037800312, -0.01537337712943554, -0.03913475573062897, 0.007874168455600739, 0.01351940631866455, 0.016914881765842438, -0.0031871635001152754, 0.022483738139271736, -0.008540765382349491, 0.016553808003664017, -0.007881112396717072, -0.0023782211355865, -0.019303517416119576, 0.021872689947485924, -0.03332981467247009, 0.012068170122802258, -0.011262699961662292, 0.03549625352025032, 0.0031107827089726925, -0.023233657702803612, -0.013311094604432583, -0.01452624425292015, 0.016595469787716866, 0.02437242679297924, 0.007790843956172466, 0.03177442401647568, -0.002197684720158577, -0.027941495180130005, 0.0331631638109684, -0.024677950888872147, 0.0056487093679606915, -0.0020240917801856995, 0.015303939580917358, 0.036801669746637344, -0.026177791878581047, -0.017067642882466316, -0.6239341497421265, -0.025052910670638084, 0.005214727018028498, -0.029524659737944603, 0.024830712005496025, -0.004964753519743681, 0.024247439578175545, 0.013206939212977886, -0.03282986581325531, -0.00454813102260232, 0.011019669473171234, 0.025775056332349777, -0.006315305363386869, -0.0042946855537593365, 0.0016829820815473795, -0.020414510741829872, 0.0076380823738873005, 0.009249023161828518, 0.010165593586862087, 0.007624194957315922, -0.01994233950972557, 0.02869141474366188, 0.014429031871259212, 0.011373799294233322, 0.03921808302402496, -0.014901204966008663, 0.018511934205889702, -0.047772735357284546, -0.014540131203830242, 0.005870908033102751, -0.00031941072666086257, 0.024969585239887238, 0.018136974424123764, -0.012963908724486828, 0.03282986581325531, 0.010978007689118385, -0.04396757856011391, 0.017845338210463524, -0.015859436243772507, 0.040495723485946655, -0.02280314825475216, -0.011970958672463894, -0.0015345602296292782, -0.0235669557005167, -0.013665223494172096, 0.02320588380098343, 0.010526666417717934, 0.015081740915775299, 0.013123614713549614, 0.004173170309513807, 0.0067944214679300785, 0.015789998695254326, 0.0011873745825141668, 0.004391897469758987, 0.007249234709888697, -0.0004660966224037111, 0.031135601922869682, 0.0022289312910288572, -0.013470799662172794, -0.016887106001377106, -0.013748548924922943, -0.01620662212371826, -0.01665101945400238, -0.007325615268200636, -0.024872373789548874, -0.005152233876287937, -0.007617251481860876, 0.03982912749052048, 0.0210394449532032, -0.03074675425887108, 0.02385859191417694, 0.02971908450126648, 0.001443424029275775, 0.0040585994720458984, 0.01942850463092327, 0.00836022850126028, 0.031496673822402954, -0.002150814514607191, 0.021914353594183922, 0.016164960339665413, 0.007658913731575012, -0.015942761674523354, -0.02294202148914337, -0.007860281504690647, 0.005659124813973904, 0.00858242716640234, 0.002655969699844718, -0.003199314931407571, 0.013692998327314854, 0.008374115452170372, 0.031163375824689865, 0.020358961075544357, 0.034385260194540024, -0.030357906594872475, 0.007158966269344091, 0.0012802467681467533, -0.03269099444150925, -0.017400940880179405, -0.006041029002517462, -0.007929718121886253, -0.006978429853916168, 0.012345918454229832, 0.008825456723570824, 0.0077352942898869514, 0.020525610074400902, -0.008922669105231762, 0.0017619667341932654, 0.016276059672236443, 0.007360334042459726, -0.04205111414194107, 0.01720651611685753, -0.012068170122802258, 0.024789050221443176, -0.010984951630234718, -0.016053861007094383, -0.028010930866003036, 0.046245116740465164, -0.0034718557726591825, -0.015928873792290688, -0.008006099611520767, 0.03371866047382355, 0.011193262413144112, 0.007367277517914772, -0.014484581537544727, -0.012227876111865044, 0.007263122126460075, 0.01445680670440197, -0.012422299943864346, -0.0020779056940227747, -0.01207511406391859, -0.0024806407745927572, 0.0005750260897912085, -0.0009174378355965018, -0.019081318750977516, 0.02528899721801281, 0.007853337563574314, 0.005832717753946781, -0.03063565492630005, -0.00016654057253617793, -0.010971063748002052, 0.004072486888617277, 0.015859436243772507, 0.004259966779500246, -0.01602608524262905, -0.006974957883358002, -0.03955138102173805, 0.0006414253148250282, 0.00865186471492052, 0.006176431197673082, 0.012818091548979282, -0.01972014084458351, -0.012234819121658802, 0.012082058005034924, 0.005304995458573103, -0.012623666785657406, -0.012061226181685925, 0.001147448318079114, -0.008019986562430859, 0.006843027658760548, -0.004971697460860014, -0.014317932538688183, 0.011984845623373985, -0.004496053326874971, 0.0005767620168626308, 0.007881112396717072, -0.015789998695254326, 0.0003348170721437782, -0.00797832477837801, -0.01884523220360279, -0.01337358821183443, -0.017873112112283707, -0.01504007913172245, -0.00533277029171586, -0.01410962175577879, -0.004680061247199774, -0.0005546289612539113, 0.020428398624062538, 0.00865880772471428, 0.004176642280071974, -0.010158649645745754, -0.008575483225286007, -0.010603046976029873, 0.007839449681341648, 0.01665101945400238, 0.0472172386944294, 0.02148384228348732, 0.012498680502176285, 0.024108566343784332, -0.004687005188316107, 0.014359595254063606, -0.007214515935629606, 0.008207466453313828, 0.0027358222287148237, 0.01888689398765564, 0.009179586544632912, -0.014595680870115757, -0.0008601522422395647, -0.011533504351973534, 0.00898516271263361, 0.0008241317118518054, 0.02696937508881092, 0.017262065783143044, 0.006929824128746986, 0.011776534840464592, -0.018970219418406487, -0.0024007882457226515, 0.009950337931513786, -0.029135812073946, 0.029135812073946, 0.01010309997946024, 0.001532824244350195, -0.009742027148604393, -0.008846288546919823, -0.0019650703761726618, 0.006280587054789066, 0.0026524977292865515, -0.007009676657617092, -0.008901838213205338, -0.005502891261130571, 0.024136340245604515, 0.002208100166171789, 0.0024580738972872496, 0.024178002029657364, -0.028260905295610428, -0.004235663916915655, -0.0005581008153967559, -0.005978535395115614, 0.010040606372058392, 0.02210877649486065, -0.0031871635001152754, -0.00699926121160388, 0.0015753544867038727, 0.011561279185116291, 0.027427660301327705, 0.04066237434744835, 0.007756125647574663, 0.022039338946342468, 0.005912570282816887, 0.038662586361169815, 0.009193473495543003, 0.0013679111143574119, 0.005992422811686993, 0.03927363082766533, 0.009832295589148998, -0.019192418083548546, 0.020803358405828476, 0.015526138246059418, 0.01994233950972557, -0.00026234210235998034, 0.0037808509077876806, -0.0330798402428627, -0.03571845218539238, -0.007797787897288799, -0.002577852923423052, 0.01819252409040928, -0.030274581164121628, -0.014720668084919453, -0.004711308050900698, -0.003680167021229863, 0.026288891211152077, 0.0035690676886588335, 0.007860281504690647, 0.01749815233051777, -0.023247545585036278, 0.016595469787716866, 0.005784111563116312, -0.030357906594872475, 0.009450390934944153, 0.011776534840464592, -0.025900043547153473, -0.026233341544866562, -0.016595469787716866, 0.0008688318775966763, 0.0037218292709439993, -0.01088773924857378, -0.017595363780856133, 0.0005489871837198734, 0.006718040909618139, 0.0011231453390792012, -0.003010098822414875, -0.025886155664920807, -0.02748320996761322, 0.023664169013500214, 0.01624828390777111, -0.005888267420232296, -0.0027201988268643618, 0.005402207374572754, 0.011484898626804352, 0.024761274456977844, 0.02994128316640854, 0.003766963491216302, -0.0024841127451509237, -0.01322777010500431, 0.009492053650319576, -0.028122030198574066, -0.005881323479115963, 0.00861714594066143, -0.0026160432025790215, -0.007554757874459028, -0.011873746290802956, 0.01647048257291317, 0.0077422382310032845, 0.0040585994720458984, -0.020470060408115387, 0.012748654000461102, -0.004641870968043804, -0.019456278532743454, -0.043051011860370636, -0.010589160025119781, -0.02401135303080082, 0.01723429188132286, -0.0030552330426871777, -0.04368983209133148, 0.013824929483234882, 0.015317827463150024, 0.01745649054646492, -0.0235669557005167, -0.03546847775578499, 0.03030235692858696, 0.021747704595327377, 0.0023955805227160454, 0.002319199498742819, -0.04021797701716423, 0.008054705336689949, 0.11187707632780075, 0.032302144914865494, 0.0005285900551825762, -0.005825773812830448, -0.00836022850126028, 0.010943288914859295, 0.004006521310657263, -0.009929507039487362, 0.028344228863716125, -0.0035430286079645157, 0.016276059672236443, 0.0001240103447344154, -0.015456701628863811, -0.0019997889176011086, 0.0010476324241608381, 0.006787477992475033, 0.0047008926048874855, -0.007263122126460075, -0.006613885052502155, -0.016151072457432747, -0.026483315974473953, 0.004461334552615881, -0.0004990792367607355, 0.03994022682309151, 0.00512445904314518, 0.013505518436431885, -0.0007451470009982586, -0.01577611267566681, 0.014317932538688183, -0.015206728130578995, -0.014276270754635334, 0.011748760007321835, -0.0019303517183288932, -0.0057632802054286, 0.00011500521941343322, 0.011714041233062744, 0.022567061707377434, -0.015109515748918056, -0.000644463230855763, 0.007818618789315224, 0.001959862420335412, 0.02202545292675495, 0.007929718121886253, -0.017192630097270012, 0.018053648993372917, -0.0065270885825157166, -0.013130557723343372, 0.037968214601278305, 0.01940072886645794, -0.0035725394263863564, 0.024400202557444572, 0.0035898988135159016, -0.016776006668806076, -0.01647048257291317, 0.016456596553325653, 0.007381164934486151, -0.008304678834974766, -0.028552541509270668, -0.010464172810316086, -0.005961176007986069, -0.03905143216252327, -0.025150122120976448, 0.0018261960940435529, -0.002459809649735689, 0.034857429563999176, -0.018873007968068123, -0.025900043547153473, 0.0016621509566903114, -0.02983018383383751, -0.008881006389856339, -0.011589054018259048, -0.010130874812602997, -0.028719190508127213, 0.0018053649691864848, 0.03782933950424194, 0.012304256670176983, 0.03655169531702995, -0.017331503331661224, 0.015817774459719658, 0.017262065783143044, 0.0003005324979312718, -0.025844493880867958, 0.0075408704578876495, -0.03388531133532524, 0.00033655299921520054, 0.02349752001464367, 0.0016361119924113154, 0.003617673646658659, -0.008006099611520767, 0.03155222535133362, 0.001281114760786295, -0.0023799571208655834, 0.011047444306313992, -0.021567167714238167, 0.0062840585596859455, -0.005384847987443209, 0.0006626904360018671, 0.03263544291257858, 0.005749392788857222, 0.019775690510869026, 0.010401679202914238, 0.00836022850126028, -0.013019458390772343, -0.033135391771793365, 0.002166437916457653, 0.005971591919660568, -0.00810331106185913, 0.010991894640028477, -0.013554124161601067, -0.007804731372743845, 0.015928873792290688, -0.006308361887931824, 0.0082907909527421, -0.0007768276846036315, 0.007783900480717421, 0.018275847658514977, 0.023691942915320396, 0.0008449628949165344, -0.02506679855287075, 0.011908465065062046, 0.003237505443394184, -0.0024216193705797195, 0.03041345626115799, 0.004725195467472076, -0.0057146744802594185, 0.0028486575465649366, -0.011998733505606651, -0.004746026825159788, -0.006957598961889744, 0.025302883237600327, 0.015873324126005173, -0.015970535576343536, -0.011471010744571686, -0.036329496651887894, 0.006645131856203079, -0.03744048997759819, -0.01785922609269619, 0.010637765750288963, 0.00995728187263012, 0.014595680870115757, 0.005291108042001724, 0.001157863880507648, -0.0137763237580657, -0.015942761674523354, 0.030024608597159386, -0.02803870663046837, -0.018748020753264427, -0.02960798516869545, 0.028052594512701035, 0.03652392327785492, -0.0027879001572728157, 0.00349963060580194, -0.032913193106651306, 0.009936450980603695, -0.006603469606488943, -0.016859330236911774, 0.002855601254850626, -0.002459809649735689, 0.04366205632686615, -0.0056105186231434345, 0.025816718116402626, -0.0033989467192441225, 0.03777378797531128, 0.01348468754440546, 0.013637448661029339, -0.013206939212977886, -0.005120987072587013, -0.0034024184569716454, -0.01423460803925991, -0.016817668452858925, 0.011616828851401806, 0.0033364533446729183, 0.005037662573158741, -0.001705549075268209, 0.011936239898204803, 0.006836083717644215, -0.024108566343784332, -0.011158544570207596, -0.03227436915040016, -0.02869141474366188, -0.012623666785657406, -0.018817458301782608, -0.012984740547835827, 0.00935317948460579, -0.045689620077610016, -0.008443553000688553, -0.0036037862300872803, 0.031163375824689865, -0.00160312931984663, 0.006325720809400082, 0.018678583204746246, -0.011262699961662292, 0.04641176760196686, -0.009540659375488758, -0.029219137504696846, 0.00042920815758407116, -0.007811675313860178, -0.02287258580327034, -0.014540131203830242, -0.01121409423649311, -0.018164748325943947, 0.03257989510893822, 0.01620662212371826, 0.009075431153178215, -0.004069014918059111, 0.0072075724601745605, -0.010408623144030571, -0.015540026128292084, 0.005929929669946432, -0.01877579465508461, -0.010401679202914238, -0.009380954317748547, -0.008790738880634308, -0.003562123980373144, 0.027566533535718918, 0.012304256670176983, -0.023511406034231186, 0.02166437916457653, -0.02345585636794567, -0.006617357023060322, 0.0055445535108447075, 0.012089001014828682, 0.005596631206572056, 0.03446858376264572, 0.03177442401647568, 0.03452413156628609, 0.005433454178273678, 0.0012437922414392233, 0.02115054428577423, -0.010512778535485268, -0.01620662212371826, 0.04088457301259041, 0.03838483616709709, -0.03413528576493263, -0.004204417113214731, 0.014213777147233486, 0.001147448318079114, -0.012797259725630283, -0.014831767417490482, 0.0046939486637711525, -0.02108110673725605, 0.008269960060715675, 0.0072006285190582275, -0.031746648252010345, -0.010700259357690811, 0.03374643623828888, -0.008110255002975464, 0.00558968773111701, -0.003850287990644574, -0.00898516271263361, -0.008999049663543701, -0.013644392602145672, 0.0125542301684618, 0.01136685535311699, 0.0022914246656000614, -0.01924796774983406, -0.0058188303373754025, -0.016401046887040138, 0.012630610726773739, 0.01730372942984104, -0.0270388126373291, 0.04102344810962677, -0.01322777010500431, 0.017331503331661224, -0.00836022850126028, -0.0072075724601745605, -0.01222093217074871, -0.0034857431892305613, 0.01734539121389389, 0.026691626757383347, -0.03171887248754501, 9.69407192314975e-05, 0.011102994903922081, -0.025080684572458267, -0.0003213636518921703, 0.0009243816020898521, -0.02072003483772278, -0.004999472294002771, 0.0020449229050427675, 0.00965870264917612, 0.030830077826976776, -0.008138029836118221, -0.009998944588005543, -0.021178320050239563, 0.0004509072459768504, 0.00031116505851969123, -0.03660724684596062, -0.005527194123715162, 0.010457228869199753, -0.005732033867388964, -0.024511301890015602, 0.008589371107518673, -0.009498996660113335, 0.029135812073946, -0.013401363044977188, 0.011464067734777927, -0.002999683376401663, 0.012019564397633076, -0.03838483616709709, 0.02072003483772278, 0.0013817985309287906, 0.00936706643551588, -0.034746330231428146, -0.001409573364071548, -0.025525083765387535, -0.016845444217324257, 0.0008931348565965891, -0.014262382872402668, -0.03182997182011604, -0.009158755652606487, 0.0230531208217144, 0.005169593263417482, -0.011061332188546658, -0.006943711545318365, -0.006381270941346884, 0.008263016119599342, 0.018067536875605583, -0.030552329495549202, -0.020817246288061142, -0.0013574955519288778, 0.00922124832868576, -0.00936706643551588, -0.0021334553603082895, -0.029580211266875267, 0.009575378149747849, -0.027177685871720314, 0.004148867446929216, -0.010609990917146206, 0.012352862395346165, -0.011394630186259747, 0.010866908356547356, -0.007985267788171768, -0.006304889917373657, -0.005565384868532419, -0.02719157375395298, 0.0029962114058434963, -0.00746448989957571, 0.015359489247202873, 0.01965070329606533, -0.003853759728372097, 0.004284270107746124, 0.01730372942984104, 0.025969481095671654, 0.007693632040172815, 0.005117515102028847, -0.004187057726085186, -0.003525669453665614, -0.027844281867146492, -0.02276148647069931, -0.02378915436565876, 0.007006204687058926, 0.02338642068207264, -0.003148972988128662, -0.016956543549895287, -0.016998205333948135, 0.007700575981289148, -0.0033972107339650393, -0.029802409932017326, -0.03366311267018318, 0.034051962196826935, 0.057549480348825455, 0.003919724840670824, 0.01826196163892746, 0.0052841645665466785, 0.010734978131949902, 0.017706463113427162, -0.03799598664045334, -0.008297734893858433, 0.03960692882537842, -0.022705936804413795, 0.005912570282816887, 0.001975485822185874, -0.03955138102173805, 0.002829562406986952, 0.028427554294466972, 0.02074780873954296, 0.031385574489831924, 0.016887106001377106, -0.008894894272089005, -0.032329920679330826, 0.0007525247056037188, -0.0050411345437169075, 0.0034978946205228567, 0.008540765382349491, 0.007568645291030407, -0.039801351726055145, 0.003503102343529463, -0.0048050484620034695, 0.018386946991086006, -0.002682008547708392, -0.0028937917668372393, 0.005520250648260117, -0.008492158725857735, 0.005089740268886089, -0.02935801073908806, -0.002475433051586151, -0.02273371070623398, 0.008742132224142551, 0.026774950325489044, 0.027469322085380554, 0.010575272142887115, 0.01991456374526024, 0.027108248323202133, -0.013290263712406158, 0.010894683189690113, 0.02217821404337883, -0.0033468687906861305, -0.02444186434149742, 0.007499208208173513, -0.008846288546919823, 0.005870908033102751, 0.009026824496686459, -0.008138029836118221, 0.004815463908016682, -0.019956225529313087, -0.006409045774489641, -0.020664485171437263, 0.0020292997360229492, 0.012575061060488224, 0.0034770634956657887, -0.02426132746040821, 0.006613885052502155, -0.03146889805793762, -0.00648542633280158, 0.010471116751432419, -0.018053648993372917, 0.0031941072084009647, -0.007790843956172466, -0.022775372490286827, 0.030024608597159386, -0.03130225092172623, -0.0371071919798851, 0.01727595366537571, 0.02170604094862938, 0.023803042247891426, 0.036135073751211166, 0.22019897401332855, 0.015165065415203571, 0.005377904511988163, 0.045106347650289536, -0.006148656364530325, 0.0044335597194731236, 0.013512462377548218, 0.017817562445998192, 0.008353284560143948, 0.018275847658514977, -0.03735716640949249, -0.016498258337378502, 0.008026930503547192, 0.0034753275103867054, -0.007290896959602833, -0.011519617401063442, -0.03744048997759819, -0.02620556578040123, -0.011984845623373985, -0.020358961075544357, 0.0008466988219879568, 0.010839133523404598, -0.0012299048248678446, -0.00980452075600624, 0.007131191436201334, 0.0006032349192537367, -0.0020049966406077147, 0.0165815819054842, -0.01584554836153984, 0.014290157705545425, -0.005975063424557447, -0.006231980863958597, -0.019442392513155937, -0.007797787897288799, -0.0006336136721074581, -0.013956859707832336, 0.002392108552157879, -0.00898516271263361, 0.01924796774983406, 0.002334822900593281, -0.02517789788544178, 0.013665223494172096, -0.0006770118488930166, -0.02221987582743168, -0.02038673684000969, 0.005006415769457817, -0.009186530485749245, -0.012929190881550312, 0.0014703308697789907, 0.015706675127148628, -0.047883834689855576, 0.0011847707210108638, 0.037968214601278305, -0.005704259034246206, -0.009450390934944153, -0.007825562730431557, 0.04668951407074928, -0.013408306986093521, -0.044078677892684937, 0.007242290768772364, -0.0023296151775866747, 0.008367172442376614, -0.020220087841153145, 0.001492897979915142, -0.0063951583579182625, 0.01734539121389389, 0.013443024829030037, 0.01218621339648962, 0.04080124944448471, -0.02090057171881199, 0.028024818748235703, -9.932761895470321e-05, 0.008533821441233158, 0.01866469532251358, -0.019956225529313087, -0.026261115446686745, 0.015415038913488388, 0.017442602664232254, 0.033468689769506454, 0.020733922719955444, -0.02503902278840542, 0.011970958672463894, 0.006440292112529278, -0.020775584504008293, -0.015248389914631844, -0.0392458550632, 0.016095522791147232, 0.006409045774489641, -0.0039301407523453236, 0.006915936712175608, 0.01330415066331625, -0.014359595254063606, -0.022747598588466644, -0.016498258337378502, 0.005912570282816887, 0.002459809649735689, -0.002871224656701088, 0.03532960265874863, -0.017373165115714073, -0.011207150295376778, -0.018831344321370125, 0.022053226828575134, -0.0016361119924113154, -0.015803886577486992, 0.009394841268658638, -0.013581898994743824, -0.016664907336235046, 0.006346552167087793, 0.0005147025804035366, -0.03188552334904671, -0.013491631485521793, -0.0038468160200864077, -0.000872303731739521, -0.009554547257721424, -0.012852809391915798, 0.03263544291257858, 0.0030500253196805716, 0.004732139408588409, 0.0260944664478302, -0.01690099388360977, 0.00922124832868576, -0.02092834562063217, -0.02517789788544178, -0.01315833255648613, 0.017692577093839645, -0.025538969784975052, -0.011915409006178379, -0.015303939580917358, 0.010825245641171932, -0.04893927648663521, 0.023775268346071243, 0.004492581356316805, 0.020039550960063934, -0.0009946866193786263, -0.016442708671092987, 0.008860175497829914, 0.01680378057062626, -0.005245973821729422, -0.022039338946342468, -0.012720879167318344, 0.003025722224265337, -0.014415144920349121, -0.009790632873773575, -0.00259347609244287, 0.006297945976257324, -0.01730372942984104, 0.02473350055515766, -0.022275425493717194, -0.015567800961434841, -0.02246985025703907, -0.006030613090842962, -0.03144112601876259, -0.026691626757383347, 0.01566501334309578, 0.027441546320915222, 0.023289207369089127, -0.012512567453086376, -0.023803042247891426, -0.009485109709203243, -0.0038815345615148544, -0.041773367673158646, 0.02298368513584137, 0.0205672737210989, -0.01669268123805523, -0.02063670940697193, 0.009498996660113335, -0.17853671312332153, 0.0008827192941680551, -0.014609568752348423, -0.03144112601876259, 0.012616723775863647, 0.01613718457520008, 0.00947816576808691, -0.040273524820804596, -0.01367216743528843, 0.007325615268200636, 0.009637871757149696, 0.018123086541891098, -0.013116670772433281, -0.022192101925611496, -0.0037634915206581354, 0.026288891211152077, -0.024247439578175545, 0.03921808302402496, -0.00887406338006258, 0.006881217937916517, 0.020483948290348053, -0.017664801329374313, -0.0014581794384866953, -0.024344652891159058, 0.008297734893858433, 0.02228931337594986, -0.025663956999778748, 0.032107722014188766, -0.0016204885905608535, 0.0002250196412205696, -0.018234185874462128, -0.0026212509255856276, 0.03660724684596062, 0.003933612257242203, 0.0025795886758714914, 0.006478482857346535, 0.00010513213055673987, -0.019497942179441452, -0.0014182530576363206, 0.03619062528014183, -0.0006644263630732894, 0.009026824496686459, 0.016734344884753227, -0.006481954362243414, -0.0352185033261776, 0.01050583552569151, 0.012359806336462498, -0.0024632816202938557, -0.0016907936660572886, -0.014915091916918755, -0.002994475420564413, -0.020220087841153145, 0.01617884822189808, 0.01258894894272089, -0.01244313083589077, -0.011950126849114895, 0.01121409423649311, 0.03605175018310547, 0.018414722755551338, -0.017873112112283707, -0.01680378057062626, -0.014442919753491879, 0.010839133523404598, -0.017331503331661224, -0.01039473619312048, -0.0015250126598402858, 0.00033394910860806704, -0.0039544436149299145, -0.02072003483772278, 0.025788944214582443, 0.010908570140600204, -0.03927363082766533, 0.0215532798320055, 0.0024112036917358637, 0.00558968773111701, -0.010269748978316784, -0.017762012779712677, 0.031413350254297256, -0.0008714357973076403, 0.0011040500830858946, -0.000370620604371652, 0.041634492576122284, -0.01763702742755413, -0.011373799294233322, 0.005853548645973206, -0.003766963491216302, -0.0025500780902802944, 0.0014833502937108278, 0.011887634173035622, -0.0195396039634943, 0.0067944214679300785, -0.006457651499658823, 0.01983124017715454, -0.017484264448285103, 0.006009782198816538, 0.017109304666519165, 0.008158860728144646, -0.0025240390095859766, 0.006086163222789764, -0.009137923829257488, -0.021108882501721382, 0.012943077832460403, -0.009422616101801395, 0.020261749625205994, 0.03263544291257858, 0.004138452000916004, -0.005061965435743332, -0.00310210301540792, 0.0031507089734077454, -0.017664801329374313, -0.03441303223371506, -0.0175259280949831, 0.026066692546010017, 0.021581055596470833, 0.01092245802283287, 0.021969903260469437, -0.01474844291806221, -0.01006143819540739, -0.0031211981549859047, 0.007158966269344091, 0.05032802000641823, -0.009519828483462334, -0.017581477761268616, 0.011734872125089169, -0.013609673827886581, -0.018275847658514977, -0.09498997032642365, -0.020261749625205994, -0.0057632802054286, 0.03294096514582634, 0.03355201333761215, 0.030219031497836113, 0.007992211729288101, 0.0115473922342062, -7.741153240203857e-05, 0.005120987072587013, 0.008901838213205338, -0.03677389398217201, -0.005797998979687691, -0.006044500507414341, 0.011352968402206898, -0.03366311267018318, 0.01396380364894867, -0.016914881765842438, 0.01873413287103176, 0.027566533535718918, 0.012998627498745918, -0.010144762694835663, -0.011165487580001354, -0.024969585239887238, 0.004235663916915655, -0.027136024087667465, -0.019192418083548546, 0.035551801323890686, 0.02546953409910202, 0.005898682866245508, 0.006037557031959295, -0.02533065900206566, -0.007513095624744892, -0.021122770383954048, 0.006502785719931126, -0.0027809564489871264, -0.03882923349738121, -0.006825668271631002, -0.011234925128519535, -0.04882817715406418, -0.0005498551181517541, 0.027830395847558975, 0.019747914746403694, -0.026441652327775955, 0.024094678461551666, -0.01485954225063324, -0.01647048257291317, 0.024289101362228394, -0.006565278861671686, -0.018984107300639153, -0.008457440882921219, -0.0016517353942617774, 0.0016335081309080124, -0.01727595366537571, 0.011866802349686623, -0.005117515102028847, 0.008047761395573616, 0.02517789788544178, 0.0076380823738873005, -0.020956121385097504, -0.01785922609269619, 0.01244313083589077, -0.011609884910285473, -0.004669645801186562, 0.0029927396681159735, -0.023303095251321793, 0.002836506115272641, -0.01826196163892746, 0.0004198775568511337, -0.02031729929149151, -0.019734026864171028, 0.023122558370232582, -0.022900359705090523, 0.02213655225932598, -0.017109304666519165, 0.0059577045030891895, -0.01756758987903595, -0.024427976459264755, -0.012207044288516045, -0.03319093957543373, 0.0017124927835538983, -0.014803992584347725, -0.004555074498057365, 0.016345497220754623, 0.023511406034231186, 0.024344652891159058, -0.012748654000461102, 0.006061859894543886, 0.009144867770373821, -0.009797576814889908, 0.009374010376632214, 0.03638504818081856, -0.001831403817050159, -0.007874168455600739, -0.03741271793842316, 0.01837306097149849, -0.020803358405828476, -0.0023747491650283337, 0.001992845209315419, -0.007679744623601437, -0.0421622134745121, 0.01969236508011818, -0.06660407781600952, 0.032191045582294464, 0.01474844291806221, -0.007214515935629606, -0.009533715434372425, 0.007075641769915819, 0.03741271793842316, -0.029524659737944603, -0.019303517416119576, 0.041078995913267136, -0.02960798516869545, 0.010540553368628025, 0.0028469215612858534, 0.01676211878657341, -0.02092834562063217, -0.029441336169838905, 0.020664485171437263, -0.020622823387384415, 0.022081002593040466, 0.011575167067348957, -0.012901416048407555, -0.0011543920263648033, 0.017595363780856133, 0.0215532798320055, -0.0033729078713804483, 0.029663534834980965, -0.0195396039634943, -0.0003302602854091674, -0.0063639115542173386, -0.03674612194299698, 0.009582322090864182, -0.018123086541891098, 0.0012923983158543706, 0.04491192474961281, 0.0011543920263648033, 0.002546606119722128, 0.006100050639361143, 0.0008280375623144209, 0.006711096968501806, -0.01826196163892746, 0.0013436081353574991, -0.019039656966924667, -0.024358538910746574, -0.010866908356547356, -0.013734661042690277, 0.01096411980688572, 0.0024806407745927572, 0.017720350995659828, 0.01110993791371584, 0.015762224793434143, 0.024830712005496025, 0.006141712889075279, -0.00205360259860754, -0.01028363686054945, -0.0073047843761742115, -0.020761696621775627, 0.03449635952711105, 0.003030929947271943, 0.004062070976942778, -0.0032079946249723434, 0.021969903260469437, 0.006013254169374704, 0.004419672302901745, -0.008221354335546494, 0.0008666619542054832, 0.0012689632130786777, 0.01566501334309578, 0.016123298555612564, 0.008929613046348095, -0.04907815158367157, -0.010457228869199753, 0.008686582557857037, -0.0005602706805802882, 0.04110677167773247, -0.013422193937003613, 0.005940345115959644, 0.001820988254621625, 0.010054494254291058, -0.00887406338006258, 0.018178636208176613, 0.03088562749326229, -0.024344652891159058, -0.031413350254297256, 0.001577090471982956, 0.005263333208858967, 0.023525293916463852, 0.0038225131575018167, 0.021581055596470833, -0.003978746477514505, 0.012019564397633076, 0.01140157412737608, -0.019386842846870422, -0.01738705299794674, -0.024969585239887238, 0.031857747584581375, -0.005888267420232296, -0.004065542947500944, -0.014387370087206364, -0.006593053694814444, 0.014692893251776695, 0.006270171143114567, 0.005839661229401827, -0.001032009138725698, -0.007360334042459726, -0.006315305363386869, 0.010491947643458843, -0.00042400037636980414, -0.02996905893087387, 0.011776534840464592, 0.0039301407523453236, 0.017984213307499886, 0.022900359705090523, -0.009346235543489456, 0.002176853595301509, -0.0016786422347649932, 0.022428188472986</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>What are the names and addresses of clients that live in San Diego?</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>select  client.Name, address.Address, address.City, address.State, address.Zip FROM client INNER JOIN address ON client.Address_ID = address.ID  WHERE address.City = 'San Diego';</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>[0.007716412656009197, -0.008434999734163284, -0.0006514291162602603, -0.01908620074391365, -0.015338804572820663, 0.031241733580827713, -0.003586217761039734, 0.013512116856873035, -0.002928073052316904, -0.03220880404114723, 0.010805663652718067, 0.007911169901490211, 0.012168964371085167, 0.010167666710913181, -0.0128002455458045, 0.0036701648496091366, 0.010859389789402485, -0.019032474607229233, 0.023854393512010574, -0.020805437117815018, -0.03062388300895691, 0.018736980855464935, 0.01860266551375389, 0.0007047354592941701, -0.013001718558371067, -0.025694511830806732, 0.009039417840540409, 0.00371045945212245, -0.02796444110572338, -0.026621287688612938, -0.0020936394575983286, -0.028313660994172096, -0.026030300185084343, -0.016534211114048958, -0.029710538685321808, 0.005799062084406614, 0.007105278316885233, 0.00026107532903552055, 0.018804138526320457, 0.004314878024160862, 0.002795436652377248, -0.02060396410524845, 0.001495096948929131, -0.02541244961321354, 0.019972681999206543, -0.0038850693963468075, -0.0016327700577676296, -0.007763423025608063, -0.03553982079029083, 0.010597474873065948, 0.029710538685321808, 0.006544511765241623, 0.005449842195957899, -0.016547642648220062, -0.003925363998860121, -0.01004006713628769, -0.012095090933144093, -0.0036701648496091366, -0.013303928077220917, -5.3332609240897e-05, 0.00971099454909563, 0.010778800584375858, -0.010926547460258007, 0.004949518013745546, -0.01947571523487568, -0.012773382477462292, 0.007985043339431286, 0.01090640015900135, 0.0014564812881872058, -0.00781714916229248, 0.019878661260008812, 0.0148418378084898, -0.009543100371956825, -0.024243908002972603, 0.0009502805769443512, -0.01759530045092106, 0.005480063147842884, -0.029952306300401688, 0.006003892980515957, 0.02965681254863739, 0.0063766175881028175, -0.0274137482047081, -0.02511695586144924, 0.010429581627249718, 0.01472095400094986, -0.004966307431459427, 0.010167666710913181, 0.0025100167840719223, -0.023102227598428726, 0.0021675126627087593, 0.009818446822464466, 0.03365940973162651, 0.009717710316181183, 0.012007785961031914, -0.0052752322517335415, 0.005987103562802076, -0.00864990334957838, 0.036453165113925934, -0.006782921496778727, -0.003747396171092987, -0.00949609000235796, -0.0008495441288687289, -0.009825162589550018, -0.017528142780065536, -0.01220925897359848, 0.004694318864494562, 0.0016697067767381668, -0.031161144375801086, 0.0053692529909312725, -0.013599421828985214, -0.008703629486262798, 0.01814599335193634, 0.00830068439245224, -0.017460985109210014, -0.0039152903482317924, 0.0026544055435806513, 0.01638646423816681, -0.009482658468186855, 0.011853323318064213, -0.0192339476197958, 0.005490136798471212, 0.0009326516883447766, 0.023760372772812843, -0.02777639962732792, -0.01672225259244442, 0.0010526960249990225, -0.013196475803852081, -0.03449216112494469, -0.004949518013745546, 0.0011366429971531034, -0.01805197261273861, 0.010053498670458794, 0.025909416377544403, 0.0007655970985069871, -0.017823636531829834, -0.023975277319550514, 0.003801122307777405, 0.041637737303972244, -0.0024478959385305643, -0.006588164251297712, 0.0019945818930864334, 0.018159424886107445, -0.002281680703163147, 0.013028581626713276, 0.003945511300116777, 0.025828827172517776, 0.008347694762051105, 0.006598237901926041, 0.011839891783893108, -0.009019270539283752, -0.006128134671598673, 0.014465754851698875, 0.019516009837388992, 0.004717824049293995, -0.018911590799689293, 0.016856567934155464, 0.013821042142808437, 0.022591829299926758, -0.02359919436275959, -0.0075686657801270485, -0.02350517362356186, 0.015956655144691467, 0.03137604892253876, 0.002928073052316904, 0.017890794202685356, 0.026863055303692818, -0.01971748284995556, -0.009731141850352287, -0.010006488300859928, -0.009032702073454857, -0.0009024307364597917, 0.02244408242404461, -0.008851376362144947, 0.0026073954068124294, -0.00694409990683198, -0.014170262031257153, 0.010825810953974724, -0.008314115926623344, -0.0163596011698246, -0.022887323051691055, 0.022591829299926758, -0.025976574048399925, -0.012477888725697994, 0.030274663120508194, -0.013438243418931961, -0.011101157404482365, 0.0174206905066967, -0.02823307178914547, 0.00518792774528265, -0.01312931813299656, 0.01787736266851425, 0.013713589869439602, 0.03269233927130699, -0.011470524594187737, -0.653739333152771, -0.02417675033211708, 0.009341627359390259, -0.009966193698346615, 0.0021725494880229235, 0.0321013517677784, 0.019986113533377647, 0.022605260834097862, -0.010429581627249718, 0.02408272959291935, 0.0007928798440843821, 0.013538979925215244, -0.030785061419010162, -0.007400771602988243, -0.0031883087940514088, -0.022067999467253685, 0.0090125547721982, 0.02731972746551037, 0.021342696622014046, -0.006923952605575323, -0.01877727545797825, 0.023787235841155052, 0.007944748736917973, 0.01756843738257885, 0.026795897632837296, 0.01783706806600094, 0.011007136665284634, -0.03516373783349991, 0.0038917851634323597, 0.029065825045108795, -0.023102227598428726, 0.009845309890806675, 0.011853323318064213, -0.0060542612336575985, 0.028636015951633453, 0.010228108614683151, -0.0097714364528656, 0.03371313586831093, -0.021248675882816315, 0.02941504493355751, -0.020214449614286423, -0.0008562598959542811, 0.01978464052081108, 0.015916360542178154, 0.0008864808478392661, 0.01729980669915676, 0.019139926880598068, -0.013659863732755184, -0.002837410196661949, -0.0033024768345057964, 0.015150763094425201, -0.009079712443053722, -0.05651986971497536, -0.0006258252542465925, 0.026003437116742134, -0.0023370857816189528, 0.008367842063307762, 0.0012323426781222224, 0.009630405344069004, 0.004895791877061129, -0.0090125547721982, 0.0006044187466613948, -0.009784867987036705, -0.01602381281554699, -0.009247606620192528, 0.015674592927098274, -0.0016319305868819356, 0.004657382145524025, 0.0017511354526504874, 0.00528530590236187, 0.001189529662951827, 0.018831001594662666, -0.021208381280303, 0.02538558654487133, 0.010496738366782665, -0.0013221659464761615, 0.023585762828588486, -0.011544398032128811, -0.010026635602116585, 0.0009410463972017169, -0.00688365800306201, 0.009281185455620289, -0.01626558043062687, -0.012545046396553516, -0.004106689710170031, 0.00045499298721551895, -0.04314206540584564, -0.025828827172517776, -0.001642843708395958, -0.0274137482047081, 0.013633000664412975, 0.010953410528600216, 0.008495441637933254, -0.018696686252951622, -0.00048605340998619795, 0.005288663785904646, -0.010288550518453121, 0.00781714916229248, 0.0008071508491411805, -0.03110741823911667, 0.0029734044801443815, -0.01638646423816681, 0.023975277319550514, 0.010678064078092575, 0.011255620047450066, -0.006833289749920368, -0.018696686252951622, 0.030919376760721207, 0.0218128003180027, -0.03129545971751213, -0.009207312017679214, -0.009167017415165901, -0.017340101301670074, -0.021060634404420853, -0.0192339476197958, -0.022551534697413445, 0.01568802446126938, 0.009724426083266735, 0.0020650974474847317, 0.005752051714807749, 0.015607435256242752, -0.004623803310096264, 0.03489510715007782, -0.015567140653729439, 0.011410082690417767, 0.007259740494191647, 0.012350290082395077, -0.020577101036906242, 0.027225706726312637, -0.018468350172042847, 0.006826573982834816, -0.002400885568931699, 0.01090640015900135, -0.019408557564020157, 0.007306750863790512, 0.010241540148854256, 0.006897089537233114, -0.01592979207634926, -0.011195178143680096, -0.009569963440299034, -0.011880186386406422, -2.1891815777053125e-05, 0.000350688787875697, -0.013720305636525154, 0.006124776788055897, -0.016681957989931107, 0.0010535354958847165, -0.0015630939742550254, -0.027937578037381172, 0.0004235128581058234, -0.006222154945135117, -0.020617395639419556, -0.0036936700344085693, 0.009308048523962498, -0.0002379898796789348, -0.008253674022853374, -0.008690197952091694, -0.01370687410235405, 0.010913115926086903, -0.01554027758538723, 0.013424811884760857, 0.016829704865813255, -0.016681957989931107, -0.009334911592304707, 0.00784401223063469, -0.02050994336605072, 0.022605260834097862, 0.012665930204093456, 0.016413327306509018, -0.010006488300859928, 0.005530431400984526, -0.005919945891946554, -0.022914186120033264, 0.01019452977925539, -0.0066553219221532345, 0.008139505982398987, -0.01817285642027855, 0.012726372107863426, 0.007105278316885233, 0.002897852100431919, 0.007253024727106094, -0.005365895107388496, 0.0011290877591818571, 0.03599649295210838, 0.02613775245845318, -0.016856567934155464, 0.030006032437086105, 0.034330982714891434, -0.013968789018690586, 0.0055237156338989735, -0.008743924088776112, -5.9759804571513087e-05, -0.010839242488145828, -0.0003865761391352862, 0.0013011792907491326, 0.014788111671805382, 0.007588813081383705, 1.7956797819351777e-05, 0.01848178170621395, -0.0029398256447166204, 0.02507666125893593, -8.725246152607724e-05, 0.013203191570937634, -0.013075591996312141, 0.009214027784764767, -0.033337052911520004, 0.006477354094386101, -0.02753463201224804, 0.06049560010433197, 0.014680659398436546, 0.010973557829856873, -0.0430077500641346, 0.01422398816794157, -0.0031496931333094835, -0.013028581626713276, 0.01364643219858408, -0.014774680137634277, 0.01626558043062687, -0.010584043338894844, 0.024525970220565796, 0.005023391451686621, -0.007333613932132721, 0.03677552193403244, -0.02017415501177311, -0.011101157404482365, 0.0019291031640022993, 0.00010021178604802117, 0.008441715501248837, -0.0009805015288293362, 0.001248292624950409, -0.013324075378477573, -0.022739576175808907, 0.02338428981602192, 0.00468760309740901, -0.008569314144551754, -0.015620866790413857, 0.0030103411991149187, 0.0023656277917325497, 0.017675889655947685, 0.0007122906972654164, 1.8140432075597346e-05, 0.0074142031371593475, 0.019368262961506844, -0.003713817335665226, 0.013485253788530827, 0.01896531693637371, 0.013377801515161991, 0.026527266949415207, -0.00438539357855916, 0.01587606593966484, -0.03304155915975571, -0.008293968625366688, -0.0009863778250291944, 0.009160301648080349, -0.017152059823274612, -0.005849430337548256, 0.008925249800086021, 0.008340978994965553, -0.002224596682935953, 0.014895563945174217, 0.013485253788530827, -0.005496852565556765, 0.012484604492783546, -0.03328332677483559, 0.0118130287155509, -0.0022917543537914753, 0.008401420898735523, -0.007038120646029711, 0.008260389789938927, -0.007353761233389378, 0.007978327572345734, 0.007044836413115263, 0.0008512230706401169, 0.019274242222309113, 0.002798794535920024, 0.011551113799214363, -0.007716412656009197, -0.02193368412554264, -0.000547334726434201, -0.005446484312415123, -0.03137604892253876, -0.003253787523135543, -0.00010068398842122406, 0.026983939111232758, 0.014828406274318695, 0.003228603396564722, -0.0037641855888068676, -0.0012079980224370956, -0.05146961286664009, 0.019005611538887024, 0.009469226934015751, 0.0016352884704247117, -0.0005880490643903613, -0.004942802246659994, 0.007622391916811466, -0.011638418771326542, -0.0015454650856554508, -0.021302402019500732, -0.0027803261764347553, 0.015029879286885262, 0.011779449880123138, 0.013794179074466228, 0.019623462110757828, -0.010087077505886555, 0.03347136825323105, 0.004140268545597792, -0.005009959917515516, -0.005584157537668943, -0.0207517109811306, -0.0430077500641346, 0.010946694761514664, 0.01918022148311138, -0.03911260887980461, 0.02441851794719696, 0.019556304439902306, -0.009684131480753422, -0.03588904067873955, -0.00650421716272831, 0.04265853017568588, 0.0008680124883539975, -0.02314252220094204, -0.02850170247256756, -0.021248675882816315, 0.008280537091195583, 0.08929279446601868, 0.016775978729128838, -0.000304937653709203, 0.005678178276866674, 0.01048330683261156, 0.0023219753056764603, -0.022403787821531296, -0.002676231786608696, 0.001463197055272758, -0.00492937071248889, -0.008817797526717186, -0.0041671316139400005, -0.0033091926015913486, 0.00889167096465826, 0.009032702073454857, -0.0038817115128040314, 0.011013852432370186, -0.0009905751794576645, 0.005849430337548256, -0.010523601435124874, -0.031913310289382935, 0.007655970752239227, 0.019636893644928932, 0.03373999893665314, 0.012289848178625107, 0.0318058580160141, 0.046365633606910706, 0.012907697819173336, -0.0018820927944034338, 0.00650421716272831, 0.01469409093260765, 0.022430650889873505, -0.0010795589769259095, 0.011584692634642124, -0.00836112629622221, 0.017044609412550926, -0.002100355224683881, 0.005819209385663271, 0.032396845519542694, -0.008945397101342678, 0.015137331560254097, -0.007575381547212601, 0.005567368119955063, -0.024727441370487213, 0.029737401753664017, -0.008246958255767822, -0.019999545067548752, 0.022094862535595894, 0.012222690507769585, -0.002953257178887725, 0.019247379153966904, -0.016547642648220062, 0.016829704865813255, -0.04346442222595215, -0.0037608277052640915, -0.01226970087736845, -2.2718169930158183e-05, -0.005879651289433241, -0.023679783567786217, -0.009536384604871273, -0.04244362562894821, -0.011356356553733349, -0.019824935123324394, -0.024284202605485916, -0.013518832623958588, -0.041610874235630035, -0.03279979154467583, -0.009731141850352287, -0.010113940574228764, -0.02017415501177311, 0.03185958415269852, 0.012941276654601097, -0.027037665247917175, 0.018401192501187325, 0.02705109678208828, 0.021006908267736435, 0.02198741026222706, -0.01793108880519867, 0.008864807896316051, 0.02550647035241127, -0.0015160837210714817, -0.011557829566299915, 0.016037244349718094, -0.011537682265043259, -0.027561495080590248, 0.022256040945649147, 0.006658679805696011, -0.013518832623958588, 0.0020516659133136272, 0.02208143100142479, -0.01744755357503891, -0.00931476429104805, -0.0026090743485838175, 0.006128134671598673, 0.0003723051631823182, -0.009724426083266735, 0.005896440707147121, 0.016104402020573616, -0.0324237085878849, -0.006020682398229837, 0.018575802445411682, -0.010798947885632515, 0.012961423955857754, 0.008387989364564419, 0.007246308960020542, -0.009536384604871273, 0.002191017847508192, -0.0003443927562329918, -0.016184991225600243, -0.0006892052479088306, 0.007232877425849438, -0.020671121776103973, 0.000639676523860544, 0.00542297912761569, 0.004439119715243578, 0.03269233927130699, 0.01783706806600094, -0.0022934332955628633, 0.007823864929378033, 0.03293410688638687, 0.020456217229366302, -0.013666579499840736, 0.03462647646665573, 0.009059565141797066, -0.016440190374851227, 0.00341160804964602, -0.008965544402599335, -0.024673717096447945, 0.01799824647605419, -0.00010015931911766529, -0.005688251927495003, 0.00011028543667634949, 0.006782921496778727, -0.01172572374343872, -0.013780747540295124, -0.021826231852173805, -7.182719127740711e-05, 0.01621185429394245, 0.0017158776754513383, -0.0006275041960179806, -0.014949290081858635, -0.007367192767560482, -0.022618692368268967, -0.005419621244072914, -0.012457741424441338, -0.0277226734906435, -0.0003322204283904284, -0.01768932119011879, 0.032369982451200485, 0.0060240402817726135, -0.000943564809858799, 0.02217545174062252, -0.0016193385235965252, 0.010516885668039322, -0.003020414849743247, -0.005872935522347689, 0.0036097229458391666, 0.010960126295685768, 0.010416150093078613, 0.0293881818652153, 0.015956655144691467, 0.02174564264714718, 0.0014850232983008027, 0.008052201010286808, 0.0103758554905653, 0.016896862536668777, -0.020012976601719856, 0.011369788087904453, -0.005325600504875183, 0.004063037224113941, 0.014828406274318695, 0.004731255583465099, -0.0005834319745190442, 0.013847905211150646, -0.011215325444936752, 0.010026635602116585, 0.003285687416791916, -0.03132232278585434, 0.0021205025259405375, -0.05144274979829788, -0.011094441637396812, -0.017272943630814552, -0.015110468491911888, 0.009281185455620289, -0.013115886598825455, -0.014210556633770466, 0.020254744216799736, 0.01611783355474472, -0.004754760768264532, -0.039005156606435776, 0.004811844788491726, -0.0069038053043186665, 0.0134046645835042, -0.0031228300649672747, 5.1679900934686884e-05, -0.0074746450409293175, -0.018253445625305176, -0.021409854292869568, -0.007333613932132721, 0.005728546530008316, 0.015889497473835945, -0.01853550784289837, 0.018790706992149353, 0.01282710861414671, 0.001920708455145359, 0.010584043338894844, -0.011188462376594543, -0.0012944635236635804, -0.0072866035625338554, 0.004512993153184652, -0.020953182131052017, 0.0035526391584426165, -0.039676733314991, -0.005443126428872347, -0.014626933261752129, -0.013794179074466228, -0.015526846051216125, 0.017004314810037613, -0.031026829034090042, -0.019636893644928932, -0.014788111671805382, -0.0007219446124508977, 0.010301982052624226, 0.015016447752714157, 0.019072769209742546, 0.03390117734670639, -0.028179345652461052, -0.009825162589550018, -0.006621743086725473, -0.013418096117675304, -0.0029146415181457996, 0.005795704200863838, 0.040912434458732605, -0.02562735415995121, -0.02666158229112625, 0.025425881147384644, -0.0004629679606296122, 0.01334422267973423, -0.012215974740684032, 0.016399895772337914, 0.051389023661613464, 0.0018535507842898369, 0.0006350594339892268, 0.024136455729603767, -0.029334455728530884, 0.02323654294013977, 0.0061180610209703445, -0.011954059824347496, -0.00889167096465826, -0.013216623105108738, -0.028179345652461052, -0.0027820051182061434, -0.023370858281850815, 0.02092631906270981, 0.013874768279492855, 0.007716412656009197, -0.010731790214776993, -0.01971748284995556, 0.02008013427257538, 0.0070918467827141285, -0.026460109278559685, 0.009120007045567036, -0.006081124301999807, -0.02026817575097084, 0.0037272488698363304, 0.03172526881098747, -0.02335742674767971, 0.01811913028359413, 0.011685429140925407, 0.020523374900221825, -0.0010518565541133285, -0.004056321457028389, 0.012168964371085167, -0.023827530443668365, -0.016493916511535645, 0.018951885402202606, 0.014385165646672249, -0.009825162589550018, -0.015567140653729439, -0.018696686252951622, 0.0363457128405571, 0.00506704393774271, 0.01978464052081108, -0.019623462110757828, -0.01778334192931652, -0.032584886997938156, -0.009939330630004406, -0.0006216278998181224, -0.006269165314733982, -0.0023286910727620125, -0.006121418904513121, 0.009522953070700169, 0.0016084254020825028, -0.002112107817083597, 0.01398222055286169, -0.015164194628596306, 0.008139505982398987, -0.005809135735034943, -0.03328332677483559, 0.014385165646672249, -0.003646659664809704, -0.003047277918085456, -0.05463945493102074, -0.004637234844267368, -0.0042577944695949554, -0.03322960063815117, -0.0081798005849123, 0.0186295285820961, -0.03583531454205513, -0.01592979207634926, 0.00877078715711832, 0.007017973344773054, 0.009986340999603271, -0.011779449880123138, -0.0015891175717115402, 0.012847255915403366, 0.003231961280107498, -0.02335742674767971, -0.01001320406794548, 0.005913230124861002, -0.03841416910290718, -0.020980045199394226, -0.00500660203397274, -0.011121304705739021, 0.008925249800086021, 0.0042577944695949554, 0.012424162589013577, 0.018562370911240578, 0.010798947885632515, -0.024700580164790154, -0.0008965544402599335, 0.014170262031257153, -0.0067191217094659805, -0.004214141983538866, -0.0010904720984399319, 0.014344871044158936, -0.013747168704867363, 0.034787654876708984, 0.0028139050118625164, -0.009724426083266735, -0.006786279380321503, 0.024861756712198257, 0.014801543205976486, 0.014492617920041084, -0.009321480058133602, -0.030758198350667953, -0.013498685322701931, -0.015553709119558334, -0.05155020207166672, -0.003619796596467495, -0.0024915484245866537, 0.022215746343135834, 0.0023051858879625797, -0.022067999467253685, -0.013183044269680977, 0.005020033568143845, -0.027440611273050308, 0.007608960382640362, 0.009959477931261063, 0.008246958255767822, 0.022793302312493324, 0.017850499600172043, -0.012215974740684032, -0.009744573384523392, -0.005030107218772173, 0.05651986971497536, -0.006379975471645594, -0.008972260169684887, 0.027400316670536995, -0.04244362562894821, 0.012350290082395077, -0.01826687715947628, -0.02842111326754093, -0.007105278316885233, 0.006332965102046728, 0.006860152818262577, 0.0026930212043225765, 0.026379520073533058, -0.02678246609866619, -0.03105369210243225, -0.012934560887515545, 0.002839089138433337, -0.025103524327278137, 0.004318235907703638, 0.01942198909819126, -0.02114122360944748, -0.0044559091329574585, 6.605583621421829e-05, -0.0035492812748998404, 0.0029331098776310682, 0.006030756048858166, 0.012061512097716331, -0.020765142515301704, -0.013485253788530827, -0.006850079167634249, -0.009308048523962498, 0.007467929273843765, -0.0029347888194024563, 0.011235472746193409, -0.005641241557896137, -0.02535872347652912, 0.02823307178914547, 0.017152059823274612, -0.0073806243017315865, -0.012041364796459675, 0.014519480988383293, -0.00931476429104805, -0.006393407005816698, -0.007118709851056337, -0.026527266949415207, -0.016037244349718094, -0.01398222055286169, -0.0030321674421429634, -0.016950588673353195, 0.02844797633588314, -0.015674592927098274, -0.011638418771326542, -0.0017007671995088458, 0.016010381281375885, 0.01358599029481411, -0.034545887261629105, -0.009845309890806675, -0.003898500930517912, -0.019247379153966904, 0.018696686252951622, -0.0005993819213472307, -0.029280729591846466, -0.013122602365911007, 0.006487427745014429, 0.05106666684150696, -0.032611750066280365, -0.02326340600848198, 0.009690847247838974, -0.02145014889538288, 0.01054374873638153, -0.008032053709030151, 0.2232857197523117, -0.003932079765945673, -0.015043310821056366, 0.013713589869439602, -0.005621094256639481, 0.0236260574311018, 0.030973102897405624, -0.004408898763358593, 0.001035906607285142, 0.0230216383934021, -0.01911306381225586, -0.009321480058133602, 0.0035492812748998404, 0.010228108614683151, -0.00014585799362976104, -0.019260810688138008, -0.04486130177974701, -0.014452323317527771, -0.010127372108399868, 0.004650666378438473, -0.012612204067409039, 0.020832300186157227, 0.0019106348045170307, -0.0023270121309906244, 0.030677609145641327, 0.020563669502735138, -0.008717061020433903, 0.024042434990406036, 0.02717198058962822, 0.021826231852173805, -0.006480711977928877, 0.003623154480010271, 0.0067493426613509655, 0.0195428729057312, -0.012894266285002232, -0.01078551635146141, -0.0007928798440843821, -0.012968139722943306, 0.0336325466632843, 0.00811935868114233, -0.017581868916749954, -0.047064073383808136, -0.030462704598903656, -0.0074209189042449, -0.023303700610995293, -0.014949290081858635, -0.001094669452868402, -0.03086565062403679, -0.012061512097716331, 0.01699088327586651, -0.022699281573295593, -0.0169640202075243, 0.01648048497736454, 0.02920014038681984, -0.0025771744549274445, -0.01292112935334444, 0.0015152442501857877, 0.016319306567311287, -0.04077811911702156, -0.0025385587941855192, 0.016977451741695404, 0.031886447221040726, -0.015594003722071648, 0.04359873756766319, 0.027346590533852577, 0.007085131015628576, 0.007206014357507229, 0.012437594123184681, 0.030973102897405624, -0.024123024195432663, 0.024485675618052483, -7.471287244698033e-05, 0.01920708455145359, 0.010261687450110912, -0.02617804706096649, -0.012390583753585815, 0.01508360542356968, 0.022981343790888786, 0.009167017415165901, 0.028636015951633453, -0.024472244083881378, 0.00115679029840976, 0.01614469662308693, 0.019072769209742546, -0.0008113482035696507, -0.019851798191666603, 0.02026817575097084, -0.01674911566078663, -0.004781623836606741, -0.0006980196922086179, -0.002078528981655836, -0.02287389151751995, -0.0010610907338559628, -0.012726372107863426, 0.010160950943827629, 0.013518832623958588, 0.009932614862918854, 0.01838776096701622, 4.247195829520933e-05, -0.003653375431895256, -0.01169214490801096, 0.06307445466518402, 0.016171559691429138, -0.008804365992546082, -0.020523374900221825, -0.004052963573485613, 0.02183966338634491, 0.0277226734906435, -0.017917657271027565, -0.008985691703855991, -0.0020583816803991795, -0.02774953655898571, -0.0013968788553029299, -0.016735684126615524, 0.0064068385399878025, -0.00540618970990181, 0.01711176708340645, -0.01686999946832657, 0.003292403183877468, 0.02359919436275959, 0.016641663387417793, -0.035486094653606415, -0.028850920498371124, 0.04222872108221054, 0.024942345917224884, -0.00626244954764843, -0.014680659398436546, -0.003905216697603464, 0.008173084817826748, -0.01157126110047102, -0.0013162896502763033, -0.006064334884285927, 0.025103524327278137, -0.012551762163639069, -0.008703629486262798, 0.02435136027634144, 0.027346590533852577, 0.003478765720501542, 0.004936086479574442, -0.005631167907267809, 0.01425085123628378, 0.005792346317321062, 0.008085779845714569, -0.008126074448227882, -0.008112642914056778, -0.02714511752128601, -0.003102682763710618, -0.009569963440299034, 0.004170489497482777, -0.04349128529429436, -0.005033465102314949, -0.013693442568182945, 0.010268403217196465, -0.009704278782010078, 0.04324951767921448, -0.010926547460258007, 0.007911169901490211, -0.052785903215408325, 0.0058997985906898975, 0.002185981022194028, -0.01590292900800705, 0.010154235176742077, 0.024257339537143707, 0.005476705264300108, -0.03435784578323364, 0.009462511166930199, -0.17213845252990723, 0.04558660462498665, 0.024740872904658318, -0.022363493219017982, 0.008455147035419941, -0.007159003987908363, 0.021893389523029327, 0.009126722812652588, -0.019704051315784454, 0.036399438977241516, 0.0327192023396492, -0.0012558478629216552, -0.004758118651807308, -0.0010233145439997315, 0.0028827416244894266, 0.001855229726061225, -0.005567368119955063, 0.004365246277302504, 0.00034921971382573247, 0.032128214836120605, 0.014452323317527771, -0.0009620331693440676, 0.0006799710681661963, -0.0015437862602993846, 0.005043538752943277, -0.00883122906088829, -0.011222041212022305, 0.01358599029481411, -0.002182623138651252, -0.011551113799214363, -0.03134918585419655, 0.030435841530561447, 0.04443149268627167, 0.015849202871322632, -0.004831992089748383, -0.003653375431895256, 0.005459915846586227, 0.004976381082087755, 0.0011928875464946032, 0.019918955862522125, 0.004976381082087755, -0.0018518718425184488, 0.00237402250058949, -0.0009217385668307543, 0.0025788533966988325, -0.004120121244341135, 0.02108749747276306, 0.014022515155375004, -0.01978464052081108, -0.02523783966898918, 0.0053692529909312725, -0.05297394469380379, 0.011799597181379795, 0.006319533567875624, -0.00717915128916502, 0.012806961312890053, 0.020308470353484154, 0.025130387395620346, 0.009287901222705841, -0.011504103429615498, -0.028877783566713333, -0.03519060090184212, 0.0021792652551084757, -0.005100622773170471, 0.008233526721596718, -0.021665053442120552, -0.007770138792693615, -0.028877783566713333, -0.010704927146434784, 0.015016447752714157, -0.004418972413986921, -0.012759950943291187, 0.021074065938591957, -0.02535872347652912, 0.03183272108435631, -0.008985691703855991, -0.02251124009490013, -0.0041973525658249855, -0.008220095187425613, 0.0009494411060586572, -0.014989584684371948, 0.014532912522554398, -0.0081798005849123, 0.024767735973000526, -0.02572137489914894, -0.002412638161331415, -0.0026594423688948154, 0.009744573384523392, 0.007985043339431286, -0.0034619763027876616, 0.010422865860164165, -0.037608277052640915, 9.428303019376472e-05, 0.0036433017812669277, -0.0011677034199237823, 0.014465754851698875, 0.01754157431423664, 0.024405086413025856, -0.004358530510216951, 0.0015320336678996682, 0.006786279380321503, -0.026795897632837296, -0.01781020499765873, 0.023639488965272903, 0.017165491357445717, -0.0031245090067386627, -0.007642539218068123, 0.028662879019975662, 0.014022515155375004, 0.00040021754102781415, -0.02989858016371727, 0.030032895505428314, 0.009408785030245781, 0.01102728396654129, -0.00897897593677044, 0.006897089537233114, -0.015795476734638214, -0.016775978729128838, 0.008515588939189911, 0.011470524594187737, 0.050932351499795914, 0.025761669501662254, 0.005584157537668943, 0.00014365438255481422, 0.006302744150161743, 0.006722479593008757, -0.0914955660700798, 0.025372155010700226, -0.001009043538942933, -0.003102682763710618, -0.010704927146434784, 0.022309767082333565, 0.014868700876832008, 0.04080498218536377, 0.00103758554905653, 0.024069298058748245, -0.016681957989931107, -0.009240890853106976, -0.007790286093950272, -0.006816500332206488, 0.0033914607483893633, -0.020590532571077347, -0.012074943631887436, -0.02611088939011097, -0.000547334726434201, 0.014344871044158936, -0.005547220818698406, -0.019032474607229233, 0.007911169901490211, -0.00268126861192286, -0.02714511752128601, -0.011792881414294243, -0.010980273596942425, 0.0070918467827141285, 0.018978748470544815, 0.006836647633463144, 0.013297212310135365, -0.01793108880519867, 0.0013272027717903256, -0.002249780809506774, 0.00021700312208849937, 0.028394250199198723, -0.0375545509159565, -0.00854245200753212, 0.023666352033615112, -0.020886026322841644, 0.002073492156341672, 0.002807189244776964, 0.004288014955818653, -0.017944520339369774, -0.004778265953063965, -0.010382571257650852, -0.015580572187900543, 0.027440611273050308, 0.010530317202210426, -0.02825993485748768, -0.012370436452329159, -0.0057755568996071815, -0.005540505051612854, -0.0031496931333094835, 0.025587059557437897, -0.0032420349307358265, -0.006668753456324339, 0.023088796064257622, -0.03134918585419655, 0.012417446821928024, -0.0007542642415501177, 0.026486972346901894, -0.010396002791821957, -0.0030640673357993364, 0.03320273756980896, 0.006131492555141449, -0.02599000558257103, -0.01860266551375389, -6.55836338410154e-05, -0.00638333335518837, -0.03470706567168236, 0.00219269678927958, -0.038091812282800674, 0.0033645976800471544, -0.025493038818240166, -0.007864159531891346, -0.007891022600233555, -0.014613501727581024, -0.009146870113909245, -0.0017209145007655025, 0.0002805929980240762, -0.010825810953974724, -0.024673717096447945, -0.013021865859627724, 0.022014273330569267, -2.880433021346107e-05, -0.0011122983414679766, -0.01007364597171545, -0.008260389789938927, -0.02304850146174431, 0.03631884977221489, 0.019892092794179916, -0.012773382477462292, 0.0009234175086021423, -0.02005327120423317, -0.004036174155771732, -0.03470706567168236, 0.0013481895439326763, 0.006578090600669384, 0.007011257577687502, -0.023411152884364128, -0.008992407470941544, -0.07629107683897018, 0.01768932119011879, 0.004701034631580114, -0.005594231188297272, 0.0038615642115473747, -0.02666158229112625, -0.0028474838472902775, -0.02526470273733139, -0.010288550518453121, 0.02326340600848198, -0.003285687416791916, 0.026030300185084343, -0.007078415248543024, 0.023773804306983948, -0.038091812282800674, -0.00442904606461525, 0.034035492688417435, -0.0072866035625338554, 0.015567140653729439, 0.022766439244151115, 0.010798947885632515, 0.0012273058528080583, 0.006658679805696011, 0.013418096117675304, -0.0023673067335039377, 0.03398176655173302, -0.023088796064257622, 0.013498685322701931, -0.025493038818240166, -0.004052963573485613, 0.019610030576586723, -0.023223111405968666, -0.001008204068057239, 0.028824057430028915, -0.02316938526928425, -0.0029448624700307846, 0.005325600504875183, 0.016373032703995705, 0.002951578237116337, -0.000821421854197979, -0.0054632737301290035, -0.02707795985043049, -0.016225285828113556, -0.019610030576586723, 0.012437594123184681, 0.0009695884073153138, -0.0023656277917325497, -0.002506658900529146, 0.029522497206926346, -0.0245394017547369, 0.013821042142808437, 0.01226970087736845, -0.011342925019562244, -0.012323427014052868, -0.0039152903482317924, -0.024458812549710274, -0.003325982019305229, -0.001739382860250771, 0.017581868916749954, 0.004321593791246414, 0.020039839670062065, 0.02695707604289055, 0.018710117787122726, -0.004177205264568329, 0.03468020260334015, -0.008529020473361015, -0.0063128178007900715, 0.018334034830331802, 0.0015379099640995264, -0.031886447221040726, -0.015594003722071648, -0.0034267185255885124, -0.0022917543537914753, 0.003482123604044318, 0.015594003722071648, 0.010731790214776993, 0.02444538101553917, 0.029280729591846466, -0.00578563055023551, 0.031644679605960846, 0.009120007045567036, 0.004482772201299667, -0.006453848909586668, 0.018522076308727264, 0.004795055370777845, 0.0006833289517089725, 0.004298088606446981, 0.0011727402452379465, -0.016977451741695404, 0.0036668069660663605, -0.027883851900696754, -0.000442400953033939, -0.007978327572345734, -0.0277226734906435, 0.0030355253256857395, 0.017823636531829834, -0.004402182996273041, -0.0233305636793375, 0.007669402286410332, 0.02174564264714718, 0.0043316674418747425, 0.014640364795923233, -0.008267105557024479, -0.019193653017282486, -0.035700999200344086, 0.011712292209267616, -0.011732439510524273, -0.0174206905066967, -5.002719262847677e-05, -0.006171787157654762, 0.0005620254669338465, 0.014532912522554398, -0.006917236838489771, 0.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>What is Angelica James portfolio summary on 10-11-2023?</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>SELECT product.type AS account_type,  COUNT(CASE WHEN account.status = 'Open' THEN 1 END) AS open_accounts, COUNT(CASE WHEN account.status = 'Closed' THEN 1 END) AS closed_accounts, SUM(balance.balance) AS total_balances, AVG(balance.balance) AS month_to_date_avg_balance FROM account INNER JOIN product ON account.product_id = product.id INNER JOIN balance ON account.id balance.account_id INNER JOIN date ON balance.balance_dt_id = date.id INNER JOIN relationship ON account.id = relationship.account_id INNER JOIN client ON relationship.client_id = client.id  WHERE client.name = 'Angelica James'  AND date.date = '2023-10-11'  AND relationship.relationship_type = 'Primary'  GROUP BY product.type;</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>[0.0025598574429750443, -0.02730967290699482, -0.008025866001844406, -0.0176406092941761, 0.010904856957495213, 0.005995634011924267, -0.051821835339069366, 0.02444426156580448, -0.01766776852309704, -0.0006594858132302761, 0.02827386185526848, 0.003106458345428109, -0.006161991041153669, 0.0025683450512588024, 0.012011638842523098, -0.010531403124332428, 0.027472633868455887, -0.011719665490090847, 0.008046235889196396, -0.026359062641859055, -0.006715381983667612, 0.028246702626347542, 0.002935008844360709, 0.0007490299176424742, -0.01913442462682724, -0.004169104620814323, 0.012106699869036674, -0.02111712656915188, 0.00866413302719593, -0.01719246432185173, 0.012622744776308537, 0.004223425406962633, 0.001414881437085569, -0.016106052324175835, -0.0062400768510997295, -0.010232639499008656, 0.004437312483787537, 0.007917224429547787, 0.026005977764725685, 0.021864034235477448, 0.01557642687112093, 0.011400531977415085, 0.004220030270516872, -0.016649257391691208, -0.012059168890118599, 0.0028348553460091352, -0.019025783985853195, -0.03126149624586105, -0.027649175375699997, 0.014028290286660194, 0.015454205684363842, 0.008827094919979572, -0.0002993997768498957, -0.012765336781740189, 0.01864553987979889, -0.028599785640835762, -0.010612883605062962, 0.02895287051796913, 0.002863713074475527, 0.010938807390630245, 0.046199653297662735, -0.002833157777786255, -0.005988844204694033, -0.010626464150846004, -0.009057956747710705, -0.019691210240125656, -0.03145161643624306, 0.01868627965450287, -0.013885698281228542, 0.037182439118623734, 0.02170107327401638, 0.02448500134050846, 0.018170233815908432, -0.01772208884358406, 0.006885133683681488, -0.006844393443316221, -0.018889982253313065, -0.002887478331103921, -0.01997639425098896, -0.014204831793904305, 0.011869046837091446, -0.005611995235085487, 0.011386952362954617, -0.015073961578309536, 0.01573938876390457, 0.02076404169201851, 0.001616886118426919, 0.009268449619412422, -0.015943091362714767, 0.004742865916341543, 0.021755393594503403, 0.0017450486775487661, 0.012649905867874622, 0.0062400768510997295, -0.038812056183815, -0.00028433429542928934, -0.02191835455596447, -0.0006934361881576478, -0.006324952933937311, -0.017260365188121796, -0.0028942686039954424, -0.013036939315497875, -0.04285893961787224, -0.004562928806990385, -0.018971463665366173, -0.02487882599234581, -0.0020489045418798923, 0.021592430770397186, 0.020913423970341682, 0.0012307006400078535, -0.012690645642578602, 0.0031658713705837727, 0.02170107327401638, -0.03164174035191536, 0.01469371747225523, -0.03357011824846268, 0.005903968121856451, 0.01000856701284647, 0.029686197638511658, -0.0022967420518398285, 0.021022064611315727, 0.03726391866803169, 0.008127717301249504, -0.019650470465421677, 0.006695011630654335, 0.007102415896952152, 0.0044678677804768085, -0.03905649855732918, -0.009533261880278587, -0.00854870118200779, 0.011251150630414486, 0.01740974560379982, 0.01927022635936737, 0.004437312483787537, 0.015359144657850266, 0.003907687030732632, -0.018659120425581932, 0.016689999029040337, -0.008677712641656399, -0.03419480472803116, -0.0030368599109351635, 0.018088754266500473, -0.0051400852389633656, -0.010001776739954948, -0.004274350591003895, 0.005540699232369661, 0.01917516440153122, -0.0006662759114988148, 0.018373936414718628, 0.014652976766228676, -0.005995634011924267, 0.016418395563960075, -0.01652703620493412, -0.005129899829626083, -0.001481084618717432, 0.02011219598352909, 0.00923449918627739, 0.007767843082547188, 0.003639478934928775, -0.007509820628911257, 0.010266589932143688, 0.01590234972536564, 0.011339421384036541, 0.01613321341574192, 0.016404815018177032, 0.03579726442694664, 0.00221016863361001, 0.0001378172601107508, 0.0006985287182033062, -0.004165709484368563, -0.02474302425980568, 0.02811090089380741, -0.030120762065052986, 0.009553632698953152, -0.0002348940761294216, 0.033923204988241196, 0.009906715713441372, -0.007523400709033012, -0.018238134682178497, -0.0006212916341610253, 0.01012399885803461, 0.02443068102002144, 0.010965967550873756, 0.006644085980951786, -0.011706084944307804, -0.01952824927866459, 0.031967662274837494, -0.03297259286046028, -0.005255516152828932, -0.013193110935389996, -0.0005033141351304948, 0.02987631969153881, 0.002551369834691286, -0.003921267110854387, -0.6331607103347778, -0.015399884432554245, 0.010673994198441505, -0.025910917669534683, 0.01962330937385559, -0.007075255736708641, 0.0001321942254435271, -0.012439412996172905, -0.01595667004585266, -0.005411687772721052, 0.0034900973550975323, 0.0013189716264605522, -0.008521541021764278, -0.004172499757260084, -0.01745048724114895, -0.027635596692562103, 0.0013503757072612643, 0.0085283312946558, -0.0018638749606907368, -0.005055209156125784, -0.031533095985651016, 0.01591593027114868, -0.0020964350551366806, -0.01630975492298603, 0.018713440746068954, -0.01027338020503521, 0.009370299987494946, -0.03346147760748863, 0.009186968207359314, 0.00821598805487156, -0.008779563941061497, 0.027920778840780258, 0.018754180520772934, -0.023222047835588455, 0.03840465098619461, -0.00998819712549448, -0.016024570912122726, 0.013749897480010986, 0.017029501497745514, 0.042668815702199936, -0.03376024216413498, 0.013580145314335823, 0.008915365673601627, -0.01956898905336857, -0.020750463008880615, 0.021266506984829903, 0.011943737976253033, -0.010443131439387798, -0.012758546508848667, -0.009397461079061031, 0.021049225702881813, 0.023317109793424606, -0.008738823235034943, -0.014625816605985165, 0.004562928806990385, -0.022787483409047127, 0.009682643227279186, -0.004787001293152571, -0.008643762208521366, -0.012595584616065025, -0.0063589029014110565, -0.020750463008880615, -0.038513291627168655, -0.009207339026033878, 0.003067415440455079, 0.0075301905162632465, 0.002352760173380375, 0.018835661932826042, 0.01762702874839306, -0.017002342268824577, -0.011061028577387333, 0.020261576399207115, -0.008344999514520168, 0.026318321004509926, 0.004817556589841843, -0.012425833381712437, -0.006742542143911123, 0.0010108720744028687, 0.012778916396200657, 0.018061593174934387, 0.011977688409388065, -0.028219541534781456, -0.008317839354276657, 0.008983266539871693, 0.001431007869541645, 0.010877696797251701, -0.008609811775386333, -0.024403521791100502, 0.0010032332502305508, -0.005707056261599064, 0.018048012629151344, 0.011040657758712769, -0.002298439620062709, -0.032103464007377625, 0.009302400052547455, 0.0038499711081385612, -0.036476269364356995, -0.011271520517766476, -0.021633172407746315, -0.013064099475741386, 0.006494704633951187, 0.006722171790897846, 0.022434400394558907, 0.008311049081385136, 0.01603815145790577, -0.002829762874171138, -0.001713644596748054, 0.0003683614486362785, 0.01308447029441595, -0.023710934445261955, -0.025693634524941444, 0.010375231504440308, -0.004715705290436745, -0.021089965477585793, -0.014625816605985165, -0.031098533421754837, 0.026752887293696404, 0.003687009448185563, -0.01635049469769001, -0.01670357957482338, 0.016934441402554512, 0.00810734648257494, 0.016459135338664055, -0.019677631556987762, -0.01736900582909584, 0.00928202923387289, 0.021062806248664856, -0.013919648714363575, -0.035688623785972595, -0.005920943338423967, 0.006365693174302578, 0.0030096997506916523, 0.003259234828874469, -0.019052943214774132, 0.02974051795899868, 0.005255516152828932, 0.010993127711117268, -0.018659120425581932, 0.011067818850278854, -0.02443068102002144, -0.0014208226930350065, -0.011848676949739456, -0.0031692665070295334, 0.004559533670544624, -0.02301834709942341, -0.024810925126075745, 0.006589765660464764, 0.01341039314866066, -0.011896206997334957, 0.010721525177359581, -0.025462772697210312, 0.0008305107476189733, -0.0145579157397151, 0.023887475952506065, 0.0017467462457716465, -0.016201114282011986, -0.003958612214773893, -0.01042955182492733, 0.0068376031704247, -0.009112277999520302, -0.0005945557495579123, 0.004895642399787903, -0.009119067341089249, 0.00033483546576462686, 0.013899278827011585, 0.0017272247932851315, 0.012446203269064426, 0.01974553056061268, -0.013797427527606487, -0.009736964479088783, -0.007034515496343374, 0.0015056986594572663, -0.0033780611120164394, -0.007727102842181921, -0.0026684985496103764, 0.020207256078720093, 0.0152912437915802, -0.0006879192660562694, 0.015250503085553646, 0.0027245166711509228, -0.0030113973189145327, -0.023765254765748978, 0.0024087782949209213, -0.0006212916341610253, 0.03538985922932625, 0.0035749732051044703, -0.004403362050652504, 0.03601454570889473, -0.009451781399548054, -0.013308542780578136, -0.01221534051001072, 0.022067736834287643, -0.008847464807331562, 0.009465361014008522, -0.027540534734725952, -0.004128364380449057, 0.005523724015802145, -0.0015634142328053713, 0.005004283506423235, -0.010178319178521633, 0.011543123982846737, 0.003982377704232931, 0.008270308375358582, 0.01542704552412033, -0.022393660619854927, 0.009764124639332294, 0.010415971279144287, -0.021755393594503403, 0.02166033163666725, -0.016119632869958878, 0.029550395905971527, -0.02231217920780182, -0.005191010423004627, 0.014897419139742851, -0.006610135547816753, 0.0049295928329229355, 0.012765336781740189, 0.004260770510882139, -0.0176406092941761, 0.008311049081385136, -0.01891714334487915, 0.0007027725223451853, -0.010402391664683819, -0.02819238230586052, 0.006888528820127249, 0.004274350591003895, -0.002829762874171138, 0.005924338474869728, 0.0003694223996717483, -0.009295609779655933, -0.016146792098879814, 0.0045187934301793575, 0.02625042013823986, 0.0029587741009891033, 0.01772208884358406, -0.017110982909798622, 0.026902267709374428, -0.013661626726388931, 0.02917015179991722, 0.010348070412874222, -0.0026837761979550123, -0.0025479746982455254, 0.031044213101267815, 0.030283724889159203, -9.787252929527313e-05, -7.235671364469454e-05, 0.02338501065969467, 0.04256017506122589, 0.0014827820705249906, 0.011848676949739456, -0.031397297978401184, -0.002256001578643918, 0.0229368656873703, 0.0007817071164026856, 0.027554115280508995, -0.02779855765402317, -0.011210409924387932, 0.010986337438225746, 0.007238217629492283, 0.035634301602840424, 0.017029501497745514, 0.03204914182424545, 0.013145580887794495, -0.004844716750085354, 0.013064099475741386, -6.954519631108269e-05, -0.01785789057612419, 0.006946244277060032, -0.01697518117725849, -0.014449275098741055, -0.010327700525522232, -0.029224472120404243, 0.025476353242993355, -0.008236357942223549, -0.00470552034676075, 0.010035727173089981, 0.01458507589995861, -0.008535121567547321, -0.003714169841259718, -0.0012222130317240953, -0.025435611605644226, -0.05269096419215202, 0.030908411368727684, 0.006508284714072943, 0.00611106539145112, -0.006504889577627182, 0.029441755264997482, 0.002953681629151106, -0.01268385536968708, 0.053369972854852676, 0.017654189839959145, 0.011434482410550117, -0.003737935097888112, 0.014503595419228077, -0.00185368990059942, 0.005696870852261782, 0.02615536004304886, -0.014883839525282383, -0.03107137233018875, -0.014748037792742252, 0.02987631969153881, -0.023004766553640366, 0.02395537681877613, -0.01825171522796154, 0.03066396899521351, 0.011957317590713501, -0.009750544093549252, -0.014041869901120663, -0.01590234972536564, -0.019460348412394524, 0.014218412339687347, -0.01518260221928358, -0.021972674876451492, 0.0024715864565223455, 0.0004137700598221272, 0.013159160502254963, -0.011305470950901508, -0.021361568942666054, 0.01312521006911993, 0.028572626411914825, 0.0038431810680776834, -0.02399611659348011, -0.029360273852944374, 0.016051732003688812, 0.11179175972938538, 0.015440625138580799, -0.01016473863273859, 0.004006142728030682, -0.019922073930501938, 0.007618461735546589, 0.006711986847221851, 0.008175247348845005, -0.007217847276479006, -0.0006951336981728673, 0.007795003242790699, -0.01613321341574192, -0.01639123633503914, -0.007564140949398279, 0.013193110935389996, -0.0014097888488322496, 0.0018384121358394623, -0.010151159018278122, 0.002330692484974861, -0.005870017688721418, -0.0021660332567989826, -0.023873895406723022, -0.01846899837255478, 0.02930595353245735, 0.004253980703651905, -0.015807289630174637, 0.023235628381371498, -0.013552985154092312, -0.013681996613740921, -0.010212269611656666, 0.00624347198754549, -0.014259153045713902, 0.021198606118559837, -0.0030453475192189217, -0.015630748122930527, -0.002678683726117015, 0.019080104306340218, 0.001023603486828506, 0.03615034744143486, -0.005160455126315355, 0.006470939144492149, 0.021089965477585793, 0.0012977526057511568, -0.017599867656826973, 0.01073510479182005, -0.008718453347682953, -0.01944676786661148, 0.042451534420251846, 0.023941796272993088, 0.022746743634343147, 0.022475140169262886, 0.009825235232710838, -0.01648629643023014, -0.004990703426301479, 0.0023731302935630083, 0.013946808874607086, -0.013206691481173038, -0.01746406778693199, -0.03481949120759964, 0.005615389905869961, -0.018441837280988693, -0.006633901037275791, -0.008311049081385136, -0.03615034744143486, 0.018767761066555977, -0.04709594324231148, -0.02444426156580448, -0.019514668732881546, -0.0094110406935215, -0.026752887293696404, -0.0029553791973739862, -0.0016890305560082197, -0.010945596732199192, 0.026847947388887405, 0.027459053322672844, 0.00826351810246706, 0.022067736834287643, -0.014490014873445034, 0.008555491454899311, 0.02138872817158699, -0.0023442725650966167, -0.034004684537649155, -0.027784977108240128, -0.038160208612680435, 0.0032150994520634413, 0.005214775912463665, -0.001458168146200478, -0.010836956091225147, 0.008331418968737125, 0.026318321004509926, -0.006674641277641058, 0.007713522762060165, 0.015169022604823112, -0.02686152793467045, 0.012609165161848068, -0.008365369401872158, -0.006104275584220886, 0.008732033893465996, 0.00470552034676075, 0.012711016461253166, 0.008596232160925865, -0.026522023603320122, -0.008623392321169376, -0.03557997941970825, 0.009064747020602226, 0.0035749732051044703, -0.003605528501793742, 0.005656130611896515, -0.031234335154294968, -0.013118420727550983, 0.008019075728952885, -0.005510143935680389, -0.007971545681357384, 0.005421873182058334, -0.008161667734384537, 0.025394871830940247, 0.0016058521578088403, 0.0020675770938396454, -0.033868882805109024, -0.0007906191167421639, 0.006610135547816753, -0.009553632698953152, 0.018061593174934387, 0.032538026571273804, -0.004461077973246574, 0.018849242478609085, -0.017206044867634773, -0.004532373510301113, 0.0076456218957901, 0.006986984983086586, 0.013505454175174236, -0.0060805100947618484, -0.013179531320929527, -0.007842534221708775, -0.001953843515366316, -0.014082610607147217, -0.014422114007174969, 0.0015999109018594027, -0.004294720944017172, -0.023873895406723022, 0.011169669218361378, 0.011237570084631443, 0.0018604799406602979, -0.022040575742721558, 0.010477081872522831, -0.03017508238554001, -0.01825171522796154, -0.005951498635113239, 0.01089127641171217, 0.022773904725909233, -0.005853042472153902, 0.00522496085613966, -0.0015472878003492951, -0.0034255916252732277, -0.019066523760557175, 0.0018927328055724502, 0.008575862273573875, -0.022067736834287643, 0.012520894408226013, 0.03663923218846321, 0.03544417768716812, -0.009458571672439575, 0.011509173549711704, 0.010789425112307072, 0.003578368341550231, 0.00462743453681469, -0.022638102993369102, -0.009472151286900043, -0.015657907351851463, 0.013016569428145885, -0.000705743208527565, 0.004478052724152803, -0.01237151212990284, -0.016499876976013184, 0.02134798839688301, 0.006813838146626949, -0.012106699869036674, -0.019650470465421677, -0.030528167262673378, -0.02629116177558899, -0.007319698575884104, -0.010646834038197994, -0.010375231504440308, -0.0005669710808433592, -0.040061429142951965, 0.0013741409638896585, 0.022420819848775864, 0.014299892820417881, 0.015046801418066025, -0.00923449918627739, 0.019025783985853195, 0.02779855765402317, 0.031180012971162796, -0.010443131439387798, -0.018835661932826042, 0.0037583052180707455, -0.016717158257961273, -0.019433187320828438, -0.0021881009452044964, 0.0068206279538571835, -0.006898713763803244, 0.02046527899801731, 0.015617167577147484, 0.021008484065532684, 0.009397461079061031, 0.00720426719635725, 0.0018231344874948263, -0.01482951920479536, 0.009377090260386467, -0.00954684242606163, 0.01652703620493412, -0.017260365188121796, -0.025286231189966202, -0.025164010003209114, 0.05220207944512367, -0.018808500841259956, -0.03283679112792015, 0.019052943214774132, -0.00967585388571024, 0.0070616756565868855, 0.007985125295817852, -0.009349930100142956, 0.03022940456867218, 0.02903435006737709, 0.030636807903647423, 0.041745368391275406, 0.025286231189966202, -0.009947456419467926, 0.010796215385198593, 0.010952387005090714, -0.002430845983326435, 0.016540616750717163, 0.029197312891483307, -0.015060381032526493, -0.0031539888586848974, 0.011916577816009521, 0.023004766553640366, -0.02965903840959072, -0.0008716755546629429, -0.004539163783192635, -0.002026836620643735, 0.011556703597307205, -0.0136752063408494, -0.014177671633660793, -0.007367229089140892, 0.008460430428385735, -0.0016839380841702223, -0.007849324494600296, -0.0043592266738414764, -0.0331355556845665, 0.00559162488207221, -0.010551773011684418, 0.001648290199227631, 0.01011720858514309, -0.00305383512750268, -0.0019742136355489492, -0.01089127641171217, -0.018414678052067757, 0.020220836624503136, 0.02178255282342434, -0.03596022352576256, 0.020655401051044464, -0.007625251542776823, 0.02656276524066925, -0.004074043594300747, 0.007469079922884703, -0.007428339682519436, 0.0022237487137317657, 0.033515799790620804, 0.024675123393535614, -0.03691083565354347, -0.007761053275316954, 0.02041095867753029, -0.017871471121907234, 0.009248078800737858, 0.026141779497265816, 0.003737935097888112, -0.022339338436722755, -0.013335702940821648, -0.009607953019440174, 0.008786354213953018, -0.012099909596145153, -0.011414112523198128, 0.0026379432529211044, 0.005126504693180323, -0.008806724101305008, -0.005968473851680756, -0.013573355041444302, 0.0006853729719296098, -0.029088672250509262, -0.0273504126816988, -0.00580211728811264, 0.005374342668801546, 0.024335620924830437, 0.017871471121907234, 0.002427451079711318, 0.02201341651380062, 0.008976476266980171, -0.011570284143090248, 0.004376201890408993, -0.00470552034676075, -0.003330530598759651, -0.030881250277161598, -0.0033475058153271675, -0.032456547021865845, -0.008093766868114471, 0.029088672250509262, -0.013451133854687214, -0.027689917013049126, -0.02965903840959072, 0.010823375545442104, 0.015250503085553646, -0.009628322906792164, -0.004647804889827967, -0.01032091025263071, -0.006284212227910757, -0.0024019882548600435, 0.0031862417235970497, -0.022081315517425537, 0.017138144001364708, 0.003527442691847682, 0.0019402633188292384, 0.006487914361059666, -0.02585659734904766, 0.02827386185526848, -0.011366581544280052, 0.0064811245538294315, -0.007374018896371126, 0.00943141058087349, -0.03183186054229736, -0.003147198585793376, 0.012649905867874622, 0.011162879876792431, 0.006525259930640459, -0.019894912838935852, -0.003945032134652138, -0.008888205513358116, 0.03680219501256943, 0.01542704552412033, -0.01572580821812153, 0.008460430428385735, 0.005418478045612574, 0.009397461079061031, 0.013444343581795692, -0.012167810462415218, -0.032538026571273804, -0.028572626411914825, -0.0431305430829525, -0.020343057811260223, 0.008623392321169376, 0.0028603181708604097, 0.013688786886632442, 0.022991186007857323, -0.040903396904468536, -0.020791202783584595, -0.007543770596385002, -0.037535522133111954, -0.03389604389667511, -0.03585158288478851, 0.03172321990132332, 0.009967826306819916, -0.003659849287942052, 0.019650470465421677, 0.019283806905150414, 0.014123351313173771, 0.0062400768510997295, -0.023493651300668716, -0.0028705033473670483, 0.024362780153751373, -0.016812220215797424, 0.009424621239304543, 0.013138790614902973, -0.03805156797170639, -0.01975911110639572, 0.003198124235495925, 0.019148005172610283, -0.009804865345358849, 0.008806724101305008, -0.0074419197626411915, -0.01497890055179596, -0.01413693092763424, 0.02333069033920765, 0.0009998382302001119, 0.020614661276340485, 0.005330207291990519, -0.030826929956674576, 0.0010830166283994913, 0.0048990375362336636, -0.005683290772140026, -0.0019080104539170861, 0.024417102336883545, 0.004966938402503729, -0.023588713258504868, -0.013566565699875355, -0.030745448544621468, 0.0022780694998800755, -0.004674965050071478, 0.02284180372953415, 0.022325759753584862, 0.0016678116517141461, 0.0025496722664684057, 0.02819238230586052, 0.016323335468769073, -0.010395601391792297, -0.00418607983738184, 0.004963543266057968, -0.02174181304872036, -0.027336832135915756, 0.032456547021865845, -0.009601162746548653, 0.017260365188121796, -0.016024570912122726, -0.004230215214192867, -0.0058802030980587006, -0.00883388426154852, 0.00176711636595428, -0.009472151286900043, -0.013396813534200191, 0.005836067255586386, -0.009709804318845272, -0.004040093161165714, -0.0069598243571817875, 0.0039178719744086266, -0.03340715914964676, -0.013050519861280918, -0.017165303230285645, 0.004009537864476442, -0.014204831793904305, -0.01599741168320179, 0.027689917013049126, -0.032945431768894196, -0.023303529247641563, 0.00418607983738184, -0.00590057298541069, 0.01208632905036211, 0.018971463665366173, 0.22238846123218536, 0.009200548753142357, -0.010497452691197395, 0.03169605880975723, -0.015522106550633907, 0.03221210464835167, 0.035552822053432465, 0.02805658057332039, 0.01909368485212326, 0.018170233815908432, -0.001453924342058599, -0.010823375545442104, 0.002887478331103921, -0.0078017935156822205, -0.0041385493241250515, -0.026657825335860252, -0.03536269813776016, -0.005078974179923534, -0.006766307633370161, -0.011210409924387932, 0.0049499631859362125, 0.005031443666666746, 0.006250261794775724, -0.017206044867634773, 0.04467867687344551, 0.0027228191029280424, -0.014680136926472187, 0.026128198951482773, -0.005992239341139793, 0.006338533014059067, -0.00795796513557434, 0.00923449918627739, 0.008148087188601494, 0.014340633526444435, -0.010633253492414951, -0.019718371331691742, -0.005785142071545124, 0.016255434602499008, 0.0015073961112648249, 0.019256645813584328, -0.019786272197961807, -0.004610459320247173, -0.001655080239288509, -0.018985042348504066, -0.003608923638239503, 0.03283679112792015, -0.004576508887112141, -0.021673912182450294, -0.021633172407746315, 0.020438117906451225, -0.03180469945073128, 0.007285748142749071, 0.034439247101545334, 0.001345283119007945, -0.01381100807338953, 0.008962895721197128, 0.0511699877679348, -0.016201114282011986, -0.0273504126816988, -0.0004659687401726842, -0.016676418483257294, 0.027010908350348473, -0.024688703939318657, 0.020275156944990158, 0.02713313139975071, 0.01772208884358406, 0.017925791442394257, 0.012147439643740654, 0.02037021890282631, -0.010592513717710972, 0.01935170777142048, 0.0005355670000426471, -0.006718777120113373, 0.0020336266607046127, -0.03381456062197685, -0.02280106395483017, 0.02876274846494198, 0.023792413994669914, 0.038431812077760696, 0.006854578386992216, 0.005954893771559, 0.00886104442179203, -0.004046883434057236, 0.014680136926472187, -0.0011933553032577038, -0.03644911199808121, 0.006195941474288702, -0.014748037792742252, 0.00042353078606538475, -0.004865087103098631, 0.008209197781980038, -0.02960471622645855, -0.04114783927798271, -0.02797509916126728, 0.010843746364116669, 0.024050436913967133, 0.013098049908876419, 0.04486880078911781, -0.017572708427906036, -0.015929510816931725, -0.024145498871803284, 0.026807207614183426, -0.002435938687995076, -0.013620886020362377, -0.02426772005856037, -0.0018010667990893126, -0.03009360283613205, -0.00013240642147138715, 0.009465361014008522, -0.021022064611315727, -0.00491601275280118, -0.01572580821812153, 0.008480801247060299, -0.01578012853860855, -0.0031268284656107426, 0.010246220044791698, 0.020383797585964203, -0.016948021948337555, 0.029333114624023438, -0.0008496078662574291, -0.039436742663383484, -0.032592348754405975, -0.0010320910951122642, -0.0027924173045903444, 0.01085053663700819, -0.0403873510658741, 0.0020607870537787676, -0.020098615437746048, 0.013946808874607086, -0.03101705200970173, 0.03191334009170532, -0.01413693092763424, 0.02889855019748211, -0.0008559735142625868, -0.0014123350847512484, 0.020207256078720093, -0.011529543437063694, 0.022570202127099037, -0.017436906695365906, -0.01409619115293026, -0.007102415896952152, -0.012412252835929394, 0.02550351247191429, -0.008093766868114471, 0.014951740391552448, -0.0205875001847744, 0.010626464150846004, -0.019813431426882744, -0.003608923638239503, -0.019188744947314262, -0.019161585718393326, -0.019894912838935852, -0.00863697286695242, 0.0305824875831604, 0.028083739802241325, 0.014503595419228077, -0.0008631880045868456, -0.02805658057332039, 0.023276370018720627, -0.012303612194955349, -0.017301104962825775, 0.01984059251844883, 0.012690645642578602, 0.011319051496684551, -0.019066523760557175, 0.023968957364559174, -0.1737172156572342, 0.02107638493180275, 0.015793709084391594, -0.03495529294013977, 0.027540534734725952, -0.009417830966413021, 0.031533095985651016, -0.012588794343173504, -0.019731951877474785, -0.0014157301047816873, 0.021266506984829903, -0.0015260688960552216, -0.026019558310508728, -0.03682935610413551, 0.0014352516736835241, 0.017124563455581665, -0.021320829167962074, 0.03085409104824066, 0.02064182050526142, 0.022882545366883278, 0.005886992905288935, -0.011543123982846737, 0.014490014873445034, -0.005737611558288336, 0.011862256564199924, 0.010171528905630112, -0.012609165161848068, 0.015698648989200592, 0.009961036965250969, 0.014951740391552448, -0.02995780110359192, -0.014775197952985764, 0.029088672250509262, -0.008935735560953617, 0.005778351798653603, 0.005761376582086086, -0.02364303357899189, 0.0067629124969244, -0.020804783329367638, 0.031180012971162796, 0.01666283793747425, 0.02846398390829563, 0.0023035320919007063, 0.0033712710719555616, -0.04910580441355705, 0.0022814644034951925, 0.011563493870198727, 0.005622180178761482, 0.01948750950396061, -0.037671323865652084, 0.016106052324175835, -0.04484163969755173, 0.030066441744565964, 0.0035647882614284754, 0.01798011176288128, 0.017572708427906036, 0.01011720858514309, 0.025707215070724487, 0.014815938659012318, -0.02770349569618702, -0.0023425749968737364, -0.00821598805487156, -0.011943737976253033, -0.018061593174934387, -0.0074419197626411915, -0.007374018896371126, -0.021619591861963272, 0.01204558927565813, -0.015209763310849667, 0.02011219598352909, 0.010348070412874222, -0.02005787566304207, 0.012629535049200058, -0.012446203269064426, 0.014490014873445034, -8.731608977541327e-05, -0.02995780110359192, 0.023575132712721825, 0.01842825673520565, 0.010395601391792297, -0.005061999429017305, 0.020872684195637703, -0.008779563941061497, -0.0018944302573800087, 0.0024715864565223455, 0.013777057640254498, 0.01856405846774578, 0.010843746364116669, 0.018170233815908432, -0.0007948628626763821, 0.012405462563037872, -0.02377883531153202, 0.01252768374979496, -0.019148005172610283, -0.010843746364116669, -0.003252444788813591, 0.012296821922063828, 0.00894931610673666, -0.012106699869036674, -0.016852959990501404, 0.009614743292331696, -0.004250585567206144, 0.00044262787560001016, -0.007054885383695364, 0.024987466633319855, 0.006094090174883604, 0.018536899238824844, 0.016160372644662857, 0.02068256214261055, -0.01842825673520565, -0.004810766316950321, 0.0012536172289401293, 0.00699377479031682, 0.0152912437915802, -0.01321348175406456, 0.026454122737050056, -0.011319051496684551, -0.007815374061465263, 0.015454205684363842, -0.020750463008880615, 0.04321202263236046, 0.01027338020503521, -0.01325422152876854, -0.002116805175319314, -0.030147923156619072, -0.02744547463953495, -0.0966363176703453, -0.008127717301249504, -0.00819561816751957, 0.019813431426882744, 0.00821598805487156, 0.002826367737725377, -0.001233246992342174, -0.013973969966173172, -0.007516610436141491, 0.020315896719694138, 0.005143479909747839, -0.02686152793467045, -0.005058604292571545, 0.0020438118372112513, 0.02271958254277706, -0.017423326149582863, -0.013267802074551582, -0.001511639915406704, 0.010415971279144287, 0.021225767210125923, -0.00018460510182194412, -0.017735669389367104, 0.0038669463247060776, -0.011570284143090248, -0.01578012853860855, -0.013138790614902973, -0.01599741168320179, 0.026617085561156273, 0.00958758220076561, 0.007312908302992582, 0.008283888921141624, -0.016201114282011986, 0.0003093726991210133, -0.023833155632019043, -0.009580792859196663, -0.03395036235451698, -0.025354132056236267, -0.012493733316659927, -0.005411687772721052, -0.04389103129506111, 0.01660851761698723, 0.021728232502937317, 0.021796133369207382, -0.02876274846494198, 0.00039594611735083163, -0.02236649952828884, 0.005265701562166214, 0.010694364085793495, -0.006175571121275425, -0.026725726202130318, -0.03172321990132332, 0.0034137091133743525, 0.003907687030732632, -0.006464149337261915, 0.01834677718579769, 0.017735669389367104, 0.003038557479158044, 0.011013497598469257, 0.003605528501793742, 0.0024410311598330736, -0.026888687163591385, 0.0012400370324030519, -0.02399611659348011, -0.009363510645925999, 0.025639314204454422, -0.0038907115813344717, -0.007285748142749071, 0.003442566841840744, 0.016228273510932922, -0.03981698676943779, -0.005442243069410324, 0.02995780110359192, -0.015793709084391594, 0.004766630940139294, -0.032592348754405975, -0.008609811775386333, -0.012310401536524296, -0.018143074586987495, 0.014924580231308937, -0.0029978170059621334, -0.02201341651380062, -0.02019367553293705, 0.00047318320139311254, 0.01723320409655571, 0.029360273852944374, 0.009641903452575207, -0.012493733316659927, -0.0185233186930418, 0.019148005172610283, -0.02572079561650753, 0.018401097506284714, 0.04011575132608414, 0.0036462689749896526, -0.011998058296740055, -0.02678004652261734, 0.005975264124572277, -0.01398754958063364, -0.011902997270226479, -0.011414112523198128, 0.026630664244294167, -0.02633190155029297, 0.0144085343927145, -0.08289320766925812, 0.040278710424900055, 0.004787001293152571, -0.0071499464102089405, -0.007795003242790699, 0.016581358388066292, 0.01692086085677147, -0.003322042990475893, -0.003663244191557169, 0.03536269813776016, -0.01354619488120079, -0.010035727173089981, -0.0032507472205907106, 0.023520812392234802, 0.014231991954147816, -0.02081836201250553, 0.027771396562457085, -0.016594937071204185, 0.01056535355746746, -0.013614095747470856, -0.01715172454714775, 0.010925226844847202, 0.020845523104071617, 0.011678924784064293, 0.0036530590150505304, 0.02350723184645176, -0.024634383618831635, -0.001914800493977964, -0.013919648714363575, -0.029414594173431396, 0.014775197952985764, -0.01148880273103714, 0.004488238133490086, 0.0378342866897583, -0.000822023197542876, -0.03517257794737816, -0.001972516067326069, 0.03359727934002876, -0.005707056261599064, -0.0017340148333460093, -0.014748037792742252, -0.0016839380841702223, 0.013736316934227943, -0.004671569913625717, 0.006036374717950821, 0.013715947046875954, -0.012364722788333893, -0.007815374061465263, 0.02338501065969467, 0.006688221823424101, 0.004736075643450022, 0.006966614630073309, -0.002926521236076951, -0.011672134511172771, -0.0006781585398130119, -0.005167245399206877, 0.0366663932800293, 0.002454611239954829, -0.012846817262470722, 0.003883921541273594, 0.01644555665552616, 0.0014038474764674902, -0.014340633526444435, -0.014503595419228077, -0.0031845441553741693, 0.0052589112892746925, -0.015793709084391594, 0.018143074586987495, 0.00943141058087349, -0.030555326491594315, -0.02987631969153881, -0.011923368088901043, 0.001058402587659657, 0.046688538044691086, 0.009804865345358849, 0.0006947093061171472, 0.012907927855849266, 0.011672134511172771, -0.014082610607147217, 0.022882545366883278, 0.024715865030884743, -0.012846817262470722, 0.010422761552035809, -0.00048591458471491933, 0.000414831010857597, 0.010191898792982101, -0.029360273852944374, 0.010307330638170242, -0.014204831793904305, 0.006874948740005493, -0.009533261880278587, -0.009669063612818718, -0.0037786755710840225, 0.0007167770527303219, 0.006521864794194698, -0.012378302402794361, -0.0007299327990040183, 0.004253980703651905, 0.009669063612818718, 0.0349009744822979, 0.008562281727790833, 0.002437636023387313, 0.00213208282366395, 0.0026311532128602266, -0.01927022635936737, 0.013865328393876553, 0.006678036414086819, -0.029088672250509262, 0.010348070412874222, -0.007767843082547188, -0.00020858253992628306, 0.012235711328685284, -0.007835743948817253, 0.0014369491254910827, -0.020003553479909897, 0.0154270455</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Which clients are members of Angelica James household?</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>SELECT client.ID, client.Client_ID, client.Person_Org, client.Name, client.SSN, address.Address, address.City, address.State, address.Zip  FROM client INNER JOIN address ON client.Address_ID = address.ID  INNER JOIN HH ON client.HH_ID = HH.ID WHERE HH.Name = 'Angelica James';</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>[0.011336488649249077, -0.012508273124694824, 0.0034737498499453068, -0.015059849247336388, 0.007883540354669094, 0.02640327252447605, 0.014685433357954025, 0.012473604641854763, -0.002854923252016306, -0.0338083915412426, -0.012945091351866722, -0.005768781993538141, -0.008403562940657139, 0.0036540243308991194, -0.023782359436154366, 0.017861036583781242, 0.013888065703213215, -0.0042052483186125755, 0.027332378551363945, -0.026597414165735245, -0.019330967217683792, 0.03195017948746681, 0.010878869332373142, 0.007266446948051453, -0.03297635540366173, -0.01239040121436119, 0.001809678040444851, -0.016183098778128624, -0.0071277739480137825, -0.004992215428501368, -0.0019015487050637603, -0.015295593068003654, 0.005612775683403015, 0.0024718400090932846, -0.014879574999213219, 0.006028793286532164, 0.012196259573101997, 0.004964480642229319, 0.028095079585909843, 0.03966037929058075, 0.024115173146128654, -0.013631521724164486, 0.004579664207994938, -0.02278391644358635, -0.027263043448328972, 0.004045774694532156, -0.005283427890390158, -0.008868115954101086, -0.02106437459588051, 0.007439787499606609, 0.026098191738128662, 0.01155836507678032, -0.002038487931713462, -0.02790093794465065, -0.005227958783507347, 0.00127838843036443, -0.00454846303910017, 0.01923389732837677, 0.015337195247411728, 0.012078387662768364, 0.03868966922163963, 0.017694629728794098, -0.017098337411880493, -0.01300056092441082, -0.014851841144263744, 0.007647796534001827, -0.005519171245396137, 0.006580017041414976, -0.005009549669921398, 0.01892881654202938, 0.03638770431280136, 0.009714019484817982, -0.0006006259354762733, -0.019178427755832672, -0.0001292472443310544, -0.028566565364599228, -0.006580017041414976, -0.02412904053926468, -0.020787030458450317, 0.004791140090674162, 0.015295593068003654, -0.004773805849254131, -0.019150692969560623, 0.003640156937763095, 0.02734624594449997, 0.002688515931367874, -0.03414120525121689, 0.007238712161779404, -0.016696186736226082, 0.017999710515141487, 0.026749953627586365, 0.015253991819918156, 0.00794594269245863, 0.005727180279791355, -0.026957962661981583, -0.0025533102452754974, -0.022104419767856598, 0.016668451949954033, -0.014713168144226074, -0.0026538479141891003, -0.019608313217759132, -0.002291565528139472, -0.0485076941549778, -0.003688692580908537, -0.0034650827292352915, 0.0014205279294401407, -0.01852666586637497, -0.01094820536673069, 0.014935044571757317, -0.011107679456472397, -0.026347802951931953, 0.011038342490792274, 0.026222998276352882, -0.036859191954135895, 0.02361595258116722, -0.019372569397091866, 0.014158477075397968, -0.006469079293310642, 0.002995329210534692, 0.004104710649698973, 0.008521433919668198, 0.027637459337711334, 0.009187063202261925, -0.0022308961488306522, 0.005831184796988964, 0.0032952087931334972, -0.005106620490550995, -0.02698569744825363, -0.030757592990994453, -0.0020974238868802786, 0.019746985286474228, 0.0031894708517938852, 0.027207573875784874, 0.002997062634676695, -0.007529924623668194, -0.0007375651621259749, -0.008209421299397945, 0.025834714993834496, -0.003361078444868326, -0.012556808069348335, -0.0060530612245202065, 0.023879429325461388, 0.006150132045149803, 0.007855805568397045, 0.0008892383775673807, 0.017625294625759125, 0.014109942130744457, 0.006476012524217367, 0.010747130028903484, -0.008583837188780308, -0.018901081755757332, 0.004267650656402111, 0.0047114030458033085, -0.021244650706648827, 0.018512798473238945, 0.008826513774693012, 0.005390899255871773, 0.022381765767931938, -0.02361595258116722, -0.012764817103743553, -0.032227523624897, 0.029176725074648857, 0.011419693008065224, -0.003830831963568926, 0.028164414688944817, 0.031201345846056938, 0.0007900007767602801, 0.00042511834180913866, -0.015697743743658066, 0.0021008907351642847, -0.012015985324978828, 0.010726329870522022, -0.007522991392761469, 0.021632933989167213, -0.007585393730551004, -0.013021362014114857, 0.0039001682307571173, -0.020163003355264664, -0.0011960515985265374, -0.018387993797659874, 0.0020072865299880505, 0.017999710515141487, -0.005512238014489412, 0.012327998876571655, -0.010393515229225159, 0.001790610607713461, 0.005831184796988964, -0.035722073167562485, 0.011267152614891529, -0.017805568873882294, 0.004198314622044563, 0.01809678040444851, 0.0008060347754508257, -0.03200564906001091, -0.6327910423278809, -0.018207719549536705, 0.021216915920376778, -0.004645533859729767, 0.02103664167225361, 0.01883174665272236, 0.016668451949954033, -0.0001270804787054658, -0.013451246544718742, 0.008985987864434719, 0.0026971830520778894, 0.02116144634783268, 0.005546906031668186, -0.003848165972158313, -0.019303232431411743, -0.03200564906001091, -0.009422806091606617, 0.008424363099038601, -0.011371157132089138, -0.01353445090353489, -0.023158332332968712, 0.003751095151528716, 0.0075507257133722305, -0.018027445301413536, 0.023602085188031197, -0.010344979353249073, -0.009020655415952206, -0.028732972219586372, 0.006316539365798235, 0.01657138206064701, -0.02351888082921505, 0.037497084587812424, 0.032504867762327194, 0.002497841138392687, 0.041268981993198395, 0.006385875400155783, -0.016280168667435646, 0.02937086671590805, 0.010559922084212303, 0.02744331769645214, -0.053638581186532974, 0.017653027549386024, 0.040714289993047714, -0.002584511414170265, 0.009117726236581802, 0.039216626435518265, 0.006583483889698982, 0.009804156608879566, -0.010448983870446682, 0.011967449449002743, 0.0005325896199792624, 0.01601669006049633, -0.0396326445043087, -0.00362975662574172, 0.020204605534672737, -0.01935870200395584, 0.010587656870484352, -0.0006950966781005263, -0.012036786414682865, 0.009880426339805126, -0.0010591123718768358, -0.015545204281806946, -0.025834714993834496, -0.02404583804309368, 0.009131593629717827, 0.01895655132830143, -0.02118918113410473, 0.01315310038626194, -0.002879190957173705, -0.007162442430853844, 0.004773805849254131, 0.02903805300593376, -0.023726889863610268, 0.0368037223815918, -0.013638455420732498, 0.015725478529930115, -0.009436673484742641, 0.011315688490867615, 0.0033038759138435125, 0.018277054652571678, -0.02719370648264885, -0.021979615092277527, -0.012889622710645199, -0.004305785987526178, 0.018998153507709503, -0.004919412080198526, -0.01865147054195404, -0.029759149998426437, 0.01895655132830143, -0.04531822353601456, 0.016945797950029373, 0.003390546189621091, -0.017264744266867638, -0.01773623190820217, 0.014907309785485268, -0.004298852290958166, -0.03999319300055504, 0.0021771606989204884, -0.0060149263590574265, -0.016820993274450302, 0.026971830055117607, -0.01408914104104042, 0.018596002832055092, -0.002142492448911071, -0.0004944546381011605, -0.0013806595234200358, -0.007522991392761469, 0.015253991819918156, 0.01865147054195404, -0.019760852679610252, 0.005515704397112131, 0.00932573527097702, 0.007068838458508253, -0.03256033733487129, -0.027984140440821648, -0.033031824976205826, 0.022672977298498154, 0.007717133034020662, -0.02235403098165989, -0.028899380937218666, 0.009748687036335468, 0.0017680763266980648, -0.01451902650296688, -0.026195263490080833, 0.018387993797659874, 0.0013945268001407385, -0.005033817142248154, -0.02462826296687126, -0.005283427890390158, -0.0027145170606672764, 0.006073861848562956, 0.004978348035365343, 0.0062368023209273815, -0.02557123638689518, 0.01368699036538601, 0.017403418198227882, 0.01999659650027752, -0.012820286676287651, 0.028192149475216866, -0.007509123999625444, 0.016086027026176453, -0.010663926601409912, 0.005425567273050547, 0.009263332933187485, -0.010386581532657146, -0.040991634130477905, -0.0009187062969431281, 0.00632347259670496, -0.0366927832365036, -0.010358846746385098, -0.008951319381594658, 0.010615391656756401, -0.01241813600063324, 0.020481949672102928, 0.01665458455681801, -0.00778646906837821, -0.01405447255820036, -0.02042648196220398, 0.011211683973670006, 0.005331963300704956, -6.432569080061512e-06, 0.01454676128923893, -0.0034512155689299107, -0.010878869332373142, 0.029759149998426437, 0.005862386431545019, 0.0048466091975569725, -0.006368541624397039, -0.004000706132501364, -0.009083058685064316, 0.015337195247411728, -0.0018859480042010546, -0.011281020008027554, 0.00041970144957304, -0.0040977769531309605, 0.03258807212114334, -0.01966378092765808, 0.00345641584135592, -0.0037996305618435144, 0.009450540877878666, 0.0058831870555877686, -0.008264889940619469, -0.011038342490792274, 0.0037822965532541275, 0.03081306256353855, -0.006597351282835007, 0.004267650656402111, 0.03136775270104408, -0.00018742475367616862, -0.0071277739480137825, -0.010039899498224258, 0.02912125550210476, -0.008216354064643383, 0.0054221004247665405, -0.008320358581840992, -0.011766374111175537, 0.018277054652571678, 0.008472898975014687, 0.0078003364615142345, -0.009270266629755497, 0.04043694585561752, -0.005047684535384178, 0.028344688937067986, -0.014463556930422783, 0.02250657044351101, -0.022035084664821625, 0.008646239526569843, -0.019317099824547768, 0.04431977868080139, -0.009485209360718727, 0.012196259573101997, -0.012660812586545944, -0.00169787323102355, 0.004811940714716911, -0.0003832998627331108, -0.005893587600439787, 0.012106122449040413, 0.014532893896102905, -0.006326939444988966, 0.0052764941938221455, -0.006007992662489414, 0.0034460152965039015, 0.005377031862735748, 0.004579664207994938, 8.325775706907734e-05, -0.0062368023209273815, -0.004683668725192547, -0.0005928255850449204, 0.015240124426782131, 0.00866704061627388, -0.0197885874658823, -0.005144755356013775, 0.022395633161067963, 0.009582280181348324, 0.00554343918338418, -0.033087294548749924, 0.0293986015021801, -0.002430238062515855, 0.01733408123254776, -0.01898428611457348, -0.013097631745040417, 0.0069093648344278336, 0.01198825053870678, 0.027859335765242577, 0.0396881103515625, 0.0010660459520295262, 0.016210833564400673, 0.027401715517044067, -0.0033160096500068903, 0.01361072063446045, -0.004153246060013771, -0.0015158654423430562, -0.00728031387552619, 0.036249030381441116, 0.02392103150486946, -0.017625294625759125, 0.018110647797584534, 0.007377385161817074, 0.011156214401125908, 0.03411347046494484, 0.02134172059595585, 0.00505461823195219, -0.0013667922466993332, -0.017528222873806953, 0.01999659650027752, 0.021632933989167213, -0.022534305229783058, -0.006292271427810192, -0.017874903976917267, -0.01220319326967001, -0.014865707606077194, -0.02566830813884735, 0.013451246544718742, -0.0023401009384542704, 0.024891739711165428, 0.0037996305618435144, -0.0012055853148922324, -0.0006205600802786648, 0.003792696865275502, 0.015462000854313374, -0.0063408068381249905, -0.03782989829778671, 0.016848726198077202, 0.009651616215705872, 0.0005256560398265719, -0.0020090199541300535, 0.0009187062969431281, 0.002856656676158309, -0.010878869332373142, 0.04093616455793381, 0.030979469418525696, 0.012764817103743553, -0.012896556407213211, 0.012660812586545944, -0.009402005933225155, 0.010816466994583607, -0.00778646906837821, -0.01806904561817646, 0.0010218441020697355, -0.007467522285878658, 0.006625085603445768, -0.01018550619482994, -0.007509123999625444, -0.0025325091555714607, 0.037441615015268326, -0.011801042594015598, -0.006375474855303764, -0.013250171206891537, -0.02055128663778305, -0.03905021771788597, 0.004444458521902561, -0.008465965278446674, -0.03211658447980881, 0.012660812586545944, 0.0027803867124021053, -0.0047044698148965836, -0.02676382102072239, -0.022839386016130447, 0.017902638763189316, -0.0015852017095312476, -0.02903805300593376, -0.023421810939908028, -0.03580527752637863, 0.013340309262275696, 0.13578826189041138, 0.017139939591288567, -0.009942828677594662, 0.0035916215274482965, -0.0012939891312271357, -0.0007150308229029179, -0.007183243054896593, -0.007890474051237106, -0.012931224890053272, -0.005858919583261013, -0.0021338253282010555, -0.0027613190468400717, -0.004964480642229319, -0.0015435998793691397, 0.007932075299322605, 0.02326926961541176, 0.0055261049419641495, -0.014297150075435638, -0.003227605950087309, -0.005390899255871773, -0.0047807395458221436, -0.026514209806919098, -0.0009880426805466413, 0.022187624126672745, 0.007633929140865803, -0.005474102683365345, 0.04207328334450722, 0.00859077088534832, -0.02186867594718933, -0.021383322775363922, 0.007737933658063412, -0.010684727691113949, 0.0091731958091259, 0.0068712299689650536, -0.0023661020677536726, -0.016377240419387817, -0.00895825307816267, 0.02161906659603119, 0.04465259239077568, -0.018179984763264656, 0.03000876121222973, 0.009166262112557888, -0.006306138820946217, -0.009041456505656242, 0.004090843256562948, 0.001315656816586852, -0.006528014782816172, 0.030119698494672775, 0.018124515190720558, 0.01094820536673069, 0.013860330916941166, 0.001918882830068469, 0.020384879782795906, -0.01416541077196598, -0.009138527326285839, -0.0009031056542880833, -0.03267127647995949, -0.00720404414460063, -0.04162953048944473, 0.023407943546772003, -0.022243093699216843, 0.0021563596092164516, 0.0030854663345962763, -0.027706794440746307, -0.005259160418063402, -0.05266787111759186, -0.03311502933502197, -0.02774839662015438, -0.0030577320139855146, -0.042184218764305115, -0.0007774335681460798, 0.008549168705940247, -0.013652321882545948, 0.01512918621301651, 0.019317099824547768, 0.03330916911363602, 0.026569679379463196, -0.00802221242338419, 0.012841087765991688, 0.04137991741299629, -0.0008151351939886808, -0.011274086311459541, 0.003518818411976099, -0.030480248853564262, -0.009887360036373138, 0.005286894738674164, -0.0016476043965667486, -0.014935044571757317, -0.012043719179928303, -0.005931722465902567, -0.009471341967582703, 0.010920471511781216, 0.013569118455052376, -0.02321380190551281, 0.02027394063770771, 0.030147433280944824, -0.021078241989016533, 0.009408939629793167, -0.019525108858942986, 0.015253991819918156, 0.004187914077192545, -0.03400253504514694, 0.0005564240273088217, -0.023532748222351074, -0.0041081770323216915, -0.0058797202073037624, -0.003643623786047101, 0.003140935441479087, -0.04823034629225731, -0.023449545726180077, 0.023158332332968712, -0.020065931603312492, -0.02336634136736393, -0.023879429325461388, 0.00702723627910018, 0.013832597061991692, -0.0029294597916305065, 0.00603226013481617, -0.016987400129437447, -0.007446721196174622, 0.001750742201693356, -0.021480392664670944, 0.03111814334988594, 0.02369915507733822, -0.03899474814534187, 0.026957962661981583, -0.0006500280578620732, -0.024725332856178284, 0.01819385215640068, 0.0027578521985560656, 0.005335430148988962, -0.013465113937854767, -0.013451246544718742, -0.00949214305728674, -0.013922734186053276, 0.004066575318574905, -0.022894853726029396, 0.012702414765954018, -0.002561977133154869, 0.002662514802068472, -0.010497519746422768, 0.010691661387681961, 0.0009767754236236215, -0.0008576036780141294, -0.02379622682929039, -0.03583301231265068, 0.01241813600063324, 0.00927720032632351, 0.01137809082865715, 0.016099894419312477, -0.011156214401125908, -0.016099894419312477, 0.02450345642864704, -0.004579664207994938, -0.023324739187955856, 0.007522991392761469, 0.0037025597412139177, -0.0026555813383311033, 0.027110502123832703, 0.045429158955812454, 0.02486400678753853, 0.002650381065905094, 0.01557293813675642, 0.008015278726816177, -0.0019310166826471686, 0.01809678040444851, -0.02532162517309189, -0.004382055718451738, 0.0014118609251454473, 0.01941417157649994, 0.00949214305728674, 0.015905752778053284, 0.007016836199909449, -0.00429538544267416, -0.0018200784688815475, 0.007717133034020662, -0.012757883407175541, -0.02906578779220581, -0.0018946151249110699, -0.03330916911363602, 0.001102447509765625, -0.023837829008698463, -0.02496107667684555, -0.002353968331590295, -0.005623175762593746, -0.0071277739480137825, 0.01877627708017826, 0.00362975662574172, -0.0012957225553691387, -0.005127421114593744, 0.02278391644358635, 0.006892030593007803, 0.02655581198632717, 3.147219103993848e-05, -0.0001038961490849033, -0.014976645819842815, -0.030674390494823456, -0.00866704061627388, 0.012404268607497215, 0.009589213877916336, -0.00650028046220541, 0.014463556930422783, -0.00351361813955009, 1.442249686078867e-05, -0.009963629767298698, 0.016515912488102913, 0.013090698048472404, -0.020079798996448517, -0.0024042371660470963, -0.006756824906915426, -0.040353741496801376, -0.02012140117585659, -0.013437380082905293, -0.027706794440746307, 0.03735841065645218, -0.01241813600063324, -0.022562040016055107, 0.0036609580274671316, 0.006555749569088221, -0.0027110502123832703, 0.004274584352970123, -0.0011483829002827406, 0.0455678328871727, 0.019012020900845528, 0.018512798473238945, 0.027665194123983383, 0.010268709622323513, -0.012757883407175541, -0.020024331286549568, -0.006933632306754589, -0.006098129786550999, 0.014491291716694832, 0.03591621667146683, -0.006295738276094198, 0.007356584072113037, 0.01824931986629963, -0.004954080563038588, -0.03733067587018013, -0.01751435548067093, 0.006177866365760565, 0.00374762830324471, -0.0047044698148965836, -0.009506010450422764, -0.005259160418063402, -0.006430943962186575, 0.012307197786867619, -0.002459706040099263, 0.003355878172442317, -0.006885096896439791, -0.019330967217683792, -0.015295593068003654, 0.009408939629793167, 0.006996035110205412, 0.016682319343090057, -0.004045774694532156, 0.008646239526569843, -0.002376502612605691, -0.018304789438843727, 0.0030767994467169046, 0.014366486109793186, -0.030757592990994453, 0.015156920999288559, -0.010587656870484352, 0.01837412640452385, 0.005016482900828123, 0.02296419069170952, -0.019802454859018326, 0.005189823918044567, 0.007661663927137852, 0.028136679902672768, 0.001737741637043655, 0.011093812063336372, 0.03855099529027939, -0.008569969795644283, 0.02012140117585659, 0.0018876814283430576, 0.010546054691076279, -0.0120991887524724, -0.006295738276094198, -0.01867920532822609, 0.019247762858867645, -0.02088410034775734, 0.011648502200841904, -0.0014118609251454473, -0.010913537815213203, -0.01885947957634926, 0.007668597623705864, -0.03852326050400734, -3.2203472073888406e-05, -0.013513649813830853, -0.01862373761832714, -0.00650028046220541, 0.00612586410716176, 0.006722156889736652, 0.017569825053215027, -0.01619696617126465, 0.012757883407175541, -0.017320213839411736, -0.012002117931842804, -0.0005477569648064673, -0.02544643171131611, -0.01033804565668106, -0.029537273570895195, 0.001667538657784462, -0.0031565362587571144, -0.025127483531832695, 0.02587631717324257, 0.005893587600439787, -0.01941417157649994, -0.05019949749112129, 0.026098191738128662, 0.015198522247374058, 0.0004394189454615116, -0.0017039402155205607, -0.014713168144226074, -0.0026919827796518803, 0.004628199618309736, -0.01132955588400364, 0.004642067011445761, 0.013846464455127716, -0.015448133461177349, -0.0049228789284825325, 0.0029675946570932865, 0.0013893266441300511, 0.03170056641101837, 0.008985987864434719, 0.025626705959439278, 0.001552267000079155, 0.016945797950029373, -0.018457328900694847, 0.0015644008526578546, 0.010622325353324413, -0.009769488126039505, -0.001624203403480351, -0.024239979684352875, -0.010067634284496307, -0.014588362537324429, 0.029343131929636, 0.003498017555102706, -0.004420190583914518, -0.002038487931713462, 0.01286188792437315, 0.012896556407213211, 0.010573789477348328, -0.021203048527240753, -0.012071453966200352, -0.03441855311393738, -0.03652637451887131, -0.032449398189783096, -0.009637748822569847, -0.011190882883965969, 7.247812754940242e-05, 0.012640012428164482, -0.03877287358045578, -0.016086027026176453, -0.008285691030323505, -0.056522972881793976, -0.019830189645290375, -0.01641884259879589, 0.017625294625759125, -0.0024250380229204893, 0.008424363099038601, 0.01231413148343563, 0.002041954779997468, 0.022922588512301445, 0.04967254400253296, -0.016710054129362106, -0.015087584033608437, 0.010788732208311558, -0.011267152614891529, 0.013478981330990791, 0.0003306475991848856, -0.036554109305143356, -0.012196259573101997, -0.011537563987076283, -0.003848165972158313, 0.01278561819344759, -0.005789583083242178, -0.015975089743733406, 0.0017221409361809492, -0.007061904761940241, 0.03283768519759178, -0.003837765660136938, 0.019580578431487083, 0.015905752778053284, -0.012757883407175541, -0.017722364515066147, 0.007640862837433815, -0.00938813854008913, -0.019497374072670937, 0.006964833941310644, 0.007855805568397045, -0.03028610721230507, 0.002374769188463688, -0.029537273570895195, 0.008271823637187481, 0.0014109942130744457, 0.0213139858096838, 0.02045421488583088, -0.01885947957634926, -0.005019949749112129, 0.03325369954109192, -0.00395910395309329, -0.007183243054896593, 0.0025966453831642866, 0.003270941087976098, -0.025155218318104744, -0.029204459860920906, 0.021355587989091873, -0.03161736577749252, -0.0030109297949820757, -0.02544643171131611, -0.012432003393769264, -0.019497374072670937, 0.015725478529930115, -0.005338896997272968, -0.0013520583743229508, 0.015115318819880486, 0.010081501677632332, -0.01969151571393013, -0.024170642718672752, 0.015115318819880486, -0.0020332876592874527, 0.020523551851511, -0.011336488649249077, -0.005966390948742628, -0.0053076958283782005, -0.002541176276281476, 0.002690249355509877, 0.027055034413933754, -0.026417139917612076, -0.0032570739276707172, 0.01212692353874445, -0.0065522827208042145, 0.02501654624938965, 0.008202487602829933, 0.21821528673171997, 0.006597351282835007, -0.024156775325536728, 0.02159133180975914, -0.008729442954063416, 0.025280024856328964, 0.0352228544652462, 0.021702269092202187, 0.008140084333717823, 0.031894709914922714, 0.0014361286303028464, -0.011294887401163578, 0.002875724108889699, 0.004125511273741722, -0.01180797629058361, -0.03236619755625725, -0.029897823929786682, -0.01751435548067093, 0.010351913049817085, -0.012133857235312462, -0.009714019484817982, 0.005519171245396137, 0.013894999399781227, -0.020204605534672737, 0.041296716779470444, 0.0176114272326231, -0.016515912488102913, 0.021327853202819824, 0.006195200607180595, 0.004146312363445759, -0.004336987156420946, 0.014713168144226074, 0.011322622187435627, 0.029343131929636, 0.004534595645964146, -0.02468373067677021, -0.025210687890648842, 0.008445164188742638, -0.0013173901243135333, 0.01981632225215435, -0.035694338381290436, -0.022950323298573494, -0.036249030381441116, -0.006670154631137848, -0.01022710744291544, 0.020592888817191124, 0.001134515623562038, -0.016030557453632355, -0.007453654892742634, 0.028677504509687424, -0.023005792871117592, -0.0016094694146886468, 0.012383467517793179, 0.021813208237290382, -0.034196674823760986, 0.0065522827208042145, 0.02511361613869667, 0.003914035391062498, -0.05411006882786751, 0.007266446948051453, -0.007862739264965057, 0.03053571656346321, -0.016918063163757324, 0.05660617724061012, 0.010379647836089134, 0.010157771408557892, 0.0035742875188589096, 0.013451246544718742, 0.01938643679022789, -0.02060675621032715, 0.01368699036538601, 0.01408914104104042, 0.021951880306005478, 0.0061293309554457664, -0.016404975205659866, -0.014241681434214115, 0.03111814334988594, 0.016585249453783035, 0.026847025379538536, 0.00608772924169898, -0.004655934404581785, 0.02640327252447605, -0.007342716678977013, 0.04079749435186386, -0.011211683973670006, -0.018387993797659874, 0.008812647312879562, -0.0012376534286886454, 0.007328849285840988, -0.01809678040444851, 0.00612586410716176, -0.03280995041131973, -0.01849893108010292, -0.01246667094528675, -0.005536505486816168, 0.022215358912944794, 0.005401299800723791, 0.011801042594015598, -0.015794815495610237, 0.003390546189621091, -0.043626416474580765, 0.03647090494632721, -0.00041471788426861167, 0.005623175762593746, -0.046843621879816055, 0.025488032028079033, 0.0017325413646176457, -0.0003234972828067839, 0.005616242066025734, -0.0011787174735218287, -0.008320358581840992, -0.022617509588599205, -0.003706026589497924, -0.007592327427119017, 0.005512238014489412, 0.0012809885665774345, 0.004572730511426926, -0.03724747523665428, 0.016793258488178253, 0.02364368736743927, -0.01241813600063324, -0.008625438436865807, -0.01050445344299078, 0.031007204204797745, 0.010331111960113049, -0.02612592652440071, -0.014588362537324429, -0.017320213839411736, 0.011350356042385101, -0.02790093794465065, 0.011260218918323517, -0.022492703050374985, 0.021577464416623116, -0.019857922568917274, 0.0027526521589607, 0.022894853726029396, 0.010989807546138763, 0.0029675946570932865, 0.0068400283344089985, -0.02802574262022972, -0.00040193399763666093, -0.005137821659445763, 0.036914657801389694, -0.017070602625608444, 0.01426941528916359, -0.027027299627661705, 0.0033870793413370848, -0.011232484132051468, -0.007370451465249062, -0.01862373761832714, -0.024420253932476044, 0.0018495464464649558, 0.008389695547521114, 0.00960308127105236, 0.03763575851917267, -0.019774720072746277, 0.019303232431411743, -0.017139939591288567, 0.023449545726180077, 0.0030785328708589077, -0.027998007833957672, 0.020537419244647026, 0.006850428879261017, -0.012640012428164482, -0.02909352257847786, 0.006039193831384182, -0.1788322478532791, 0.03838459029793739, 0.019525108858942986, -0.03552793338894844, 0.03170056641101837, -0.007391252089291811, 0.020870232954621315, 0.00183394574560225, -0.043931495398283005, 0.017500488087534904, 0.017015134915709496, 0.007391252089291811, -0.03236619755625725, -0.03472363203763962, 0.0227561816573143, -0.0010781798046082258, -0.014491291716694832, 0.017042867839336395, 0.022797783836722374, 0.01387419831007719, 0.010428182780742645, 0.012071453966200352, 0.010663926601409912, 0.013513649813830853, 0.011142347007989883, -0.011357289738953114, -0.012716282159090042, -0.0038620333652943373, -0.0032016048207879066, -0.006597351282835007, -0.025404829531908035, 0.0037580288480967283, 0.03023063763976097, 0.00816088542342186, 0.019122958183288574, 0.00601145951077342, -0.008535301312804222, 0.004759938456118107, -0.0037822965532541275, 0.01573934592306614, 0.007959810085594654, 0.02777613140642643, 0.01058072317391634, 0.005966390948742628, -0.004805007483810186, 0.014103008434176445, 0.018596002832055092, -0.004645533859729767, 0.013513649813830853, -0.021785473451018333, -0.0076547302305698395, -0.033031824976205826, 0.04063108563423157, -0.005279961042106152, 0.011412759311497211, 0.00306293205358088, 0.010643125511705875, 0.038162712007761, 0.008583837188780308, -0.02045421488583088, 0.015087584033608437, -0.04002092778682709, -0.00012773051275871694, -0.012702414765954018, 0.02397650107741356, -0.005023416597396135, -0.013770193792879581, 0.0048084743320941925, -0.014782504178583622, 0.027887070551514626, -0.012667746283113956, -0.0010149104055017233, 0.006548815872520208, -0.03142322227358818, 0.02851109579205513, 0.008875049650669098, -0.0191368255764246, 0.024337049573659897, 0.014879574999213219, 0.0018218118930235505, -0.015018247999250889, 0.014186211861670017, -0.01198825053870678, -0.00805688090622425, -0.007682464551180601, -0.005127421114593744, 0.0018460795981809497, -0.003255340503528714, 0.014283282682299614, 0.002083556493744254, 0.018124515190720558, -0.03902248293161392, 0.014491291716694832, -0.01619696617126465, 0.006881630048155785, 0.0003042131138499826, 0.018970418721437454, -0.006937099155038595, -0.00837582815438509, -0.006337339989840984, -0.009811090305447578, -0.0030265306122601032, -0.0032154719810932875, 0.011447426863014698, 0.027789998799562454, -0.004028440453112125, 0.015406531281769276, 0.035416994243860245, 0.015032115392386913, -0.018207719549536705, -0.009824956767261028, 0.011828777380287647, 0.018082913011312485, 0.02670835144817829, -0.004714869894087315, 0.018207719549536705, -0.003910568542778492, -0.00042685173684731126, 0.014851841144263744, -0.011703971773386002, 0.061237841844558716, 0.01614149659872055, 0.016515912488102913, -0.003955637104809284, -0.034862302243709564, -0.01626630127429962, -0.08470125496387482, 0.0047807395458221436, 0.0005516571109183133, -0.015253991819918156, 0.005453302059322596, 0.0029675946570932865, 0.019067488610744476, -5.183973553357646e-05, -0.006961367093026638, 0.008202487602829933, 0.0013572585303336382, -0.01657138206064701, 0.002879190957173705, -0.0025671774055808783, -0.00013076397590339184, -0.01451902650296688, -0.019428038969635963, -0.009180129505693913, 0.0033229433465749025, 0.012764817103743553, -0.005019949749112129, -0.008257956244051456, -0.000316780322464183, -0.012196259573101997, 0.016030557453632355, -0.021688401699066162, -0.01895655132830143, 0.009547611698508263, 0.024434121325612068, 0.020717693492770195, 0.017971975728869438, -0.010053766891360283, -0.004284984897822142, -0.019025888293981552, -0.015309460461139679, -0.007564593106508255, -0.008535301312804222, -0.004895144607871771, 0.015794815495610237, -0.025099748745560646, 0.018457328900694847, 0.011502896435558796, 0.009346536360681057, -0.0242538470774889, 0.00529036158695817, -0.012029852718114853, -0.005137821659445763, 0.02082863263785839, 0.012549874372780323, -0.021397190168499947, -0.028843911364674568, -0.0003085466451011598, 0.012986693531274796, -0.005363164935261011, 0.02876070700585842, 0.03114587627351284, 0.013950468972325325, 0.04437524825334549, -0.028871646150946617, -0.017847169190645218, -0.007696331944316626, -0.008777978830039501, -0.010296444408595562, 0.0002478773531038314, 0.024697598069906235, -0.009457474574446678, -0.005515704397112131, -0.016973532736301422, 0.004447925370186567, -0.022978058084845543, -0.005415166728198528, 0.021022774279117584, -0.01928936503827572, 0.00370949343778193, -0.04634439945220947, 0.007141641341149807, -0.011385024525225163, -0.0064101433381438255, -0.0032622739672660828, -0.0059871915727853775, -0.012362666428089142, -0.021216915920376778, 0.006555749569088221, -0.00039110021316446364, 0.020953437313437462, 0.003830831963568926, 0.008861182257533073, 0.008750244043767452, -0.012230928055942059, -0.028372423723340034, 0.006919765379279852, 0.021730003878474236, -0.0013771927915513515, -0.004971414338797331, -0.02673608623445034, -0.014505159109830856, -0.03697012737393379, -0.015919620171189308, 0.005692512262612581, 0.014907309785485268, -0.012716282159090042, -0.001680539222434163, -0.08547782152891159, 0.03328143432736397, -0.01586415059864521, -0.00529036158695817, -0.0048466091975569725, -0.022035084664821625, 0.011738639324903488, -0.026112059131264687, -0.004649000708013773, 0.02141105756163597, -0.02161906659603119, 0.01763916015625, -0.013194702565670013, 0.02174387127161026, 0.005761848762631416, -0.018387993797659874, 0.030674390494823456, -0.010130036622285843, -0.00042403495172038674, -0.0015852017095312476, 0.007925141602754593, 0.007377385161817074, 0.028732972219586372, 0.009270266629755497, 0.008604638278484344, 0.02526615746319294, -0.017777834087610245, 0.001440462190657854, -0.01665458455681801, -0.003848165972158313, 0.01632177084684372, -0.029897823929786682, -0.0198717899620533, 0.01702900044620037, -0.00483967550098896, -0.017292479053139687, -0.021147578954696655, 0.019857922568917274, 0.013867264613509178, -0.01159303355962038, -0.0249333418905735, -0.015656141564249992, 0.008500633761286736, -0.010955139063298702, 0.010039899498224258, 0.010254842229187489, 0.008382761850953102, -0.01451902650296688, 0.015073716640472412, 0.009984430857002735, 0.0022551638539880514, 0.008417429402470589, -0.004912478383630514, -0.021632933989167213, -0.0007258646655827761, -0.01736181601881981, 0.043598681688308716, -0.010296444408595562, -0.013853397220373154, -0.004184447228908539, 0.011461294256150723, 0.008992921561002731, 0.004538062494248152, -0.0006829628255218267, 0.0024666397366672754, -0.0056613110937178135, 0.012480538338422775, 0.006184800062328577, 0.018304789438843727, -0.036581844091415405, -0.016959665343165398, -0.003139202017337084, 0.0072317784652113914, 0.0249888114631176, 0.00997056346386671, 0.008556102402508259, 0.013957401737570763, 0.010130036622285843, -0.010282577015459538, 0.02296419069170952, 0.001977818552404642, -0.02995329163968563, 0.0006894630496390164, -0.0010634459322318435, 0.012404268607497215, 0.0061605325900018215, -0.04046468064188957, -0.015462000854313374, -0.014213946647942066, 0.009360403753817081, -0.01619696617126465, -0.002707583364099264, 0.002152892993763089, -0.003127068281173706, 0.003130535129457712, -0.014740902930498123, -0.01809678040444851, 0.013929667882621288, -0.005553839728236198, 0.031007204204797745, 0.016099894419312477, 0.013305640779435635, 0.0031582696828991175, -0.005127421114593744, -0.024295447394251823, 0.01662684977054596, -0.01568387635052204, -0.022062817588448524, -0.015032115392386913, -0.01028951071202755, 0.0010140436934307218, 0.0019050155533477664, 0.014338752254843712, 0.01730634644627571, -0.01478250417858</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Which clients are employed by a company similar to Stevens Valley School?</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>SELECT employer.name, client.ID, client.Client_ID, client.Person_Org, client.Name, client.SSN, address.Address, address.City,  address.State, address.Zip  FROM client INNER JOIN address ON client.Address_ID = address.ID INNER JOIN employer ON client.Employer_ID = employer.ID WHERE employer.Name LIKE '%Stevens Valley School%'</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>[0.012511341832578182, -0.01192118413746357, -0.008130289614200592, -0.02228713035583496, -0.009991021826863289, 0.038547709584236145, -0.01653829962015152, 0.0019405771745368838, 0.00014536971866618842, -0.018718412145972252, -0.023356357589364052, 0.0032233023084700108, 0.004353280644863844, -0.0023276512511074543, 0.0016793456161394715, -0.004988567903637886, 0.007873397320508957, -0.0275360606610775, 0.007547074928879738, 0.0008826328557915986, -0.010845014825463295, 0.029493996873497963, 0.003912398125976324, -0.019523803144693375, -0.004183176439255476, -0.008199719712138176, -0.001698439009487629, -0.005592611618340015, 0.003252810100093484, 0.016121719032526016, 0.03538168594241142, -0.011004704050719738, -0.02121790312230587, -0.0036867496091872454, 0.0005272364360280335, 0.003731879172846675, 0.011948956176638603, 0.006765983998775482, 0.018024109303951263, 0.012900152243673801, 0.0022946717217564583, -0.021148473024368286, -0.0033569554798305035, -0.015816224738955498, -0.014746998436748981, -0.015330213122069836, 0.0006400606944225729, 0.005957120563834906, -0.023675736039876938, 0.020468056201934814, 0.032410070300102234, 0.006765983998775482, -0.01735757850110531, -0.016940996050834656, 0.005314890295267105, 0.011386571452021599, 0.0051343715749681, -0.004492141306400299, -0.013073727488517761, -0.01910722255706787, 0.0012757820077240467, 0.003717993153259158, -0.0149275166913867, 0.003940170165151358, -0.011386571452021599, -0.0031642864923924208, -0.020495828241109848, 0.003235452575609088, -0.005512766540050507, 0.006342459004372358, 0.027994301170110703, 0.005391263868659735, -0.011900355108082294, -0.006141111254692078, 0.019232196733355522, -0.013649999164044857, -0.00040464854100719094, -0.023356357589364052, 0.007064534351229668, 0.0018867687322199345, -0.0071860370226204395, -0.03982522711157799, -0.03465961292386055, 0.011261596344411373, 0.013608341105282307, -0.023259153589606285, 0.005887690465897322, 0.006418832112103701, -0.018565665930509567, 0.0062278988771140575, 0.016816021874547005, 0.027119480073451996, 0.00705411983653903, 0.01920442469418049, -0.01795467920601368, 0.011837868019938469, 0.0043984102085232735, 0.02649460732936859, 0.019273854792118073, -0.023425787687301636, -0.006085566710680723, 0.030438248068094254, -0.023786824196577072, -0.013018183410167694, -0.03282665088772774, -0.0003829515480902046, -0.010761698707938194, -0.013198702596127987, 0.0011959371622651815, -0.02607802487909794, -0.030466020107269287, -0.014580365270376205, 0.00721380952745676, -0.01520523801445961, -0.006866657640784979, -0.004453954286873341, 0.02907741442322731, 0.007172151003032923, 0.016760477796196938, -0.017968565225601196, 0.02792487107217312, 0.011456001549959183, 0.02212049625813961, -0.028827466070652008, 0.028938554227352142, 0.003290996653959155, -0.01782970316708088, -0.002732082735747099, -0.018648982048034668, -0.012705747038125992, 0.007547074928879738, 0.010046565905213356, 0.01110190711915493, -0.021717801690101624, -0.01705208420753479, -0.011018590070307255, 0.016982654109597206, 0.02181500382721424, -0.019662663340568542, -0.003046254860237241, 0.010539521463215351, 0.016052287071943283, 0.006984689272940159, 0.017496438696980476, -0.011289368383586407, 0.022023294121026993, 0.015663478523492813, 0.027244454249739647, -0.010796413756906986, -0.00878293439745903, -0.0008075613295659423, -0.010004907846450806, -0.0018433748045936227, -0.023522989824414253, -0.010039622895419598, -0.012969582341611385, 0.004422710742801428, 0.0092967189848423, -0.027286112308502197, -0.018760070204734802, -0.04040843993425369, 0.022814800962805748, 9.606334788259119e-05, -0.0018451105570420623, 0.010921387933194637, 0.014483163133263588, 0.001799980876967311, -0.007477644365280867, 0.01011599600315094, -0.017815817147493362, -0.024328380823135376, 0.009074541740119457, -0.026189113035798073, 0.005099656525999308, 0.005832145921885967, -0.018024109303951263, 0.007199923507869244, 0.004953852854669094, 0.003700635628774762, -0.03715910390019417, 0.018607323989272118, 0.019870955497026443, -0.0026105795986950397, 0.04321342706680298, -0.007720650639384985, 0.0030549336224794388, -0.0037804804742336273, 0.0006938691949471831, -0.0040200152434408665, -0.007547074928879738, 0.039575278759002686, 0.01243496872484684, -0.0058182599022984505, -0.013094556517899036, -0.6412028074264526, -0.01774638704955578, -0.012636316940188408, 0.00882459245622158, 0.03604821860790253, 0.03507619351148605, 0.023772938176989555, 0.007137435954064131, -0.014871972613036633, 0.0013243831926956773, 0.015024719759821892, 0.013393106870353222, -0.011393514461815357, -0.004755976144224405, 0.00020894184126518667, -0.027633264660835266, -0.007727593649178743, 0.011976729147136211, 0.010081280954182148, -0.007831739261746407, -0.01400409359484911, 0.0229397751390934, -0.013781916350126266, -0.005700228735804558, 0.04804577678442001, 0.024328380823135376, -0.021287333220243454, -0.01576068066060543, 0.0029421094805002213, 0.0011594862444326282, -0.026702897623181343, 0.025244861841201782, 0.011483773589134216, 0.026008594781160355, 0.04399104416370392, 0.018287943676114082, -0.020454170182347298, 0.032187893986701965, -0.005328776314854622, 0.03793672099709511, -0.03774231672286987, 0.0012801213888451457, 0.021828889846801758, 0.002808456076309085, -0.00865101721137762, 0.039158694446086884, 0.009824388660490513, -0.004082502331584692, -0.008338580839335918, -0.015191351994872093, 0.0253420639783144, 0.00565857021138072, -0.019259968772530556, 9.129001409746706e-05, 0.035409457981586456, -0.02298143319785595, 0.0040477872826159, -0.003992242738604546, -0.01516357995569706, 0.019579347223043442, -0.004992039408534765, 0.008165004663169384, -0.005717586260288954, -0.017232602462172508, -0.018968360498547554, 0.006665309891104698, -0.011615690775215626, -0.003940170165151358, 0.0016724026063457131, -0.015871768817305565, 0.030854830518364906, 0.0182185135781765, -0.004169290419667959, 0.02203718014061451, 0.0012966110371053219, 0.014170726761221886, -0.010692267678678036, -0.0077484226785600185, -0.0013200438115745783, 0.02039862610399723, -0.018287943676114082, -0.026647353544831276, -0.004405353218317032, -0.0006708703585900366, -0.0033656342420727015, 0.0006383249419741333, -0.022023294121026993, -0.016177263110876083, 0.01803799532353878, -0.024453354999423027, 0.010386774316430092, 0.02039862610399723, -0.0010431904811412096, -0.045296333730220795, 0.002614051103591919, 0.020370854064822197, -0.009893819689750671, 0.00425260653719306, 0.011011647060513496, -0.023078635334968567, -0.001996121369302273, 0.008769048377871513, -0.009435579180717468, -0.0038290817756205797, -0.0040477872826159, 0.011476830579340458, -0.0057314722798764706, 0.009137028828263283, 0.019509917125105858, -0.026355745270848274, 0.022259358316659927, -0.022064952179789543, -0.021620599552989006, -0.008005314506590366, 0.005481522995978594, -0.03879765793681145, 0.00429426459595561, -0.012983468361198902, -0.02203718014061451, -0.013698600232601166, -0.0011386570986360312, -0.02259262278676033, 0.004186647944152355, 6.856243271613494e-05, -0.0010431904811412096, 0.003731879172846675, -0.01067143864929676, -0.026508493348956108, -6.113122071838006e-05, -0.0019128050189465284, -0.006575050298124552, -0.011810095980763435, 0.021273447200655937, -0.013851347379386425, -0.0002913903445005417, 0.01196284219622612, 0.0033274476882070303, -0.011858697049319744, -0.0015352778136730194, -0.03402085229754448, -0.00019321154104545712, -0.0015890862559899688, -0.0022599566727876663, -0.007956713438034058, -0.003077498637139797, 0.003933227155357599, -0.021939978003501892, 0.007755365688353777, -0.01657995767891407, -0.026689011603593826, -0.004443539772182703, -0.013177872635424137, -0.010122939012944698, -0.0016081795329228044, -0.003379520494490862, 0.0008691807161085308, -0.009359206072986126, -0.018954474478960037, 0.01363611314445734, -0.009845217689871788, 0.008859307505190372, 0.012816835194826126, -0.014899744652211666, -0.020495828241109848, -0.0028188705909997225, -0.005353076849132776, 0.02392568439245224, 0.00174530444201082, 0.012955696322023869, -0.005905047990381718, 0.04001963138580322, -0.0031694937497377396, 0.025050455704331398, 0.01885727234184742, 0.011969785206019878, 0.026897301897406578, -0.023606305941939354, 0.023078635334968567, -0.02169002965092659, -0.0008800291689112782, 0.002223505638539791, 0.006800699047744274, -0.005290589760988951, 0.016593843698501587, 0.034937333315610886, 0.004221362993121147, 0.007734536658972502, 0.02439781092107296, -0.017801931127905846, 0.0014337359461933374, 0.007970599457621574, 0.023953458294272423, -0.00882459245622158, -0.007651220075786114, 0.019232196733355522, 0.001799980876967311, 0.019037790596485138, 0.025911392644047737, 0.018926702439785004, 0.011761494912207127, 0.028799694031476974, -3.601697244448587e-05, 0.014538707211613655, -0.0017678693402558565, 0.011094964109361172, -0.041380465030670166, -0.008442725986242294, -0.03415971249341965, 0.02370350807905197, 0.02052360028028488, 0.009206458926200867, -0.010650609619915485, -0.015663478523492813, -0.011990615166723728, -0.006318158470094204, 0.004151932429522276, -0.009477237239480019, 0.008845421485602856, 0.01516357995569706, -0.004863593261688948, 0.0024387396406382322, -0.00541209289804101, 0.030049439519643784, -0.003624262288212776, 0.00734572671353817, -0.009199515916407108, -0.004526856355369091, 0.0024786621797829866, 0.008345523849129677, 0.008796820417046547, -0.0002939939731732011, 0.007998371496796608, 0.017774159088730812, -0.0022165626287460327, 0.007005518302321434, -0.0022044123616069555, 0.012032273225486279, -0.00994242075830698, 0.0208707507699728, -0.010095166973769665, -0.011247710324823856, 0.004044315777719021, 0.010942216962575912, -0.012178076431155205, 0.04329674318432808, 0.010365945287048817, 0.012171133421361446, 0.012205848470330238, -0.011254653334617615, 0.03679806366562843, -0.013032069429755211, 0.018107425421476364, 0.00489830831065774, -0.0006526448996737599, 0.029521768912672997, -0.0020846452098339796, 0.022259358316659927, 0.01058812253177166, 0.00709924940019846, 0.02246764861047268, -0.01103941909968853, -0.0024665119126439095, 0.00425260653719306, -0.03274333477020264, 0.024633875116705894, 0.007727593649178743, -0.02495325356721878, -0.01889893040060997, 0.006668781396001577, -0.019273854792118073, 0.0031070064287632704, 0.006710439454764128, 0.014038808643817902, 0.004471312277019024, 0.009095370769500732, 0.005103128030896187, 0.0028483786154538393, 0.0003723200352396816, -0.007692878600209951, 0.014385960064828396, -0.0027928343042731285, -0.033743131905794144, 0.021509509533643723, -0.006443133112043142, 0.006457019131630659, 0.02250930666923523, -0.0006752097979187965, -0.0005255006835795939, -0.027647150680422783, 0.02916073054075241, 0.009463351219892502, 0.0009607419488020241, -0.023856254294514656, 0.021537283435463905, -0.004204005468636751, 0.005512766540050507, -0.0014181140577420592, -0.014871972613036633, -0.003756179939955473, 0.0034836658742278814, 0.01170595083385706, 0.017107628285884857, 0.010615894570946693, 0.018621210008859634, 0.044046588242053986, -0.008199719712138176, -0.006967331748455763, -0.022925889119505882, -0.023606305941939354, -0.029882805421948433, 0.018246285617351532, -0.0026574451476335526, -0.013483365997672081, 0.0006795491790398955, 0.011615690775215626, -0.015816224738955498, -0.012080874294042587, -0.003473251359537244, 0.04238026216626167, 0.0007776194834150374, -0.01469145342707634, -0.02220381423830986, -0.025661442428827286, -0.00012909698125440627, 0.12897375226020813, 0.033520955592393875, -0.024286722764372826, 0.003264960367232561, 0.02495325356721878, -0.004596286453306675, -0.02924404665827751, -0.012441911734640598, 0.0017045141430571675, -0.005196858663111925, -0.005932820029556751, -0.0228564590215683, -0.016552185639739037, -0.00360690476372838, 0.006922202184796333, 0.02177334576845169, -0.0030983276665210724, -0.01906556263566017, -0.006436189636588097, -0.018801728263497353, -0.02560589835047722, -0.002108945744112134, 0.014441505074501038, 0.016871565952897072, 0.00822749175131321, 0.01641332544386387, 0.03749236837029457, 0.04746256023645401, 0.00469348905608058, -0.022953661158680916, 0.0026244658511132, 0.01594119891524315, -0.014510935172438622, 0.017551982775330544, -0.013177872635424137, 0.014663681387901306, -0.02169002965092659, -0.003382991999387741, 0.030132755637168884, 0.009185629896819592, 0.04065839201211929, 0.018662868067622185, -0.0029542597476392984, -0.014031865634024143, 0.01552461739629507, 0.0023102934937924147, 0.0011612219968810678, 0.009435579180717468, -0.00016967032570391893, -0.004658774007111788, 0.003082705894485116, -0.009581383317708969, 0.01614949107170105, -0.02809150330722332, -0.003506230656057596, -0.0004942570230923593, -0.0064813196659088135, 0.009095370769500732, -0.009400864131748676, -0.018315715715289116, -0.05854363739490509, -0.01351113896816969, -0.004662245512008667, -0.011761494912207127, 0.0010536049958318472, -0.009053712710738182, -0.0048948368057608604, -0.014219327829778194, 0.006835414096713066, -0.016121719032526016, -0.0053391908295452595, 0.009845217689871788, -0.034131940454244614, -0.010171541012823582, 0.04282461479306221, 0.01211558934301138, 0.009324491024017334, -0.006661838386207819, -0.010900558903813362, 0.029410680755972862, -0.010949159972369671, -0.015413529239594936, 0.011948956176638603, -0.011074135079979897, 0.001554371090605855, 0.0046900175511837006, -0.024939367547631264, 0.011157451197504997, -0.0028067203238606453, 0.00508924201130867, 0.0035340029280632734, 0.008470498025417328, -0.017343692481517792, -0.051267340779304504, 0.010726982727646828, 0.0027112537063658237, 0.007547074928879738, 0.01988484151661396, -0.0004755976260639727, -0.013261189684271812, 0.015052491798996925, -0.02675844170153141, 0.01086584385484457, -0.019523803144693375, 0.010969989001750946, -0.012219734489917755, -0.011094964109361172, -0.0013408728409558535, -0.03224343806505203, 0.005634269677102566, 0.04118606075644493, -0.011699007824063301, 0.005478051491081715, 0.026702897623181343, 0.003096591914072633, 0.017038198187947273, -0.004068616311997175, 0.018621210008859634, 0.009629984386265278, -0.0032094160560518503, 0.04685157537460327, -0.012643259949982166, 0.025022683665156364, 0.001639423193410039, -0.025619784370064735, -0.001354758976958692, 0.0252587478607893, -0.03490956127643585, 0.01544130127876997, -0.0038985118735581636, -0.022689824923872948, 0.02891078218817711, -0.007324897684156895, -0.0014007565332576632, -0.041852593421936035, -0.030743742361664772, -0.018787842243909836, 0.01764918491244316, 0.007036761846393347, -0.015746794641017914, 0.0053044757805764675, 0.020759662613272667, -0.0005849503795616329, -0.01984318345785141, -0.011282425373792648, -0.029132958501577377, -0.011546260677278042, -0.0021419250406324863, 0.003603433258831501, 0.0003202473162673414, -0.015774566680192947, -0.0006526448996737599, 0.01937105692923069, 0.00865101721137762, -0.0058668614365160465, -0.029049642384052277, -0.013337562792003155, 0.016246693208813667, 0.02868860401213169, 0.02632797323167324, 0.017815817147493362, 0.004408824723213911, 0.009532781317830086, -0.021273447200655937, 0.005262817721813917, 0.01224056351929903, -0.016691047698259354, -0.017107628285884857, 0.011914241127669811, 0.0034541580826044083, 0.015663478523492813, -0.00605779467150569, 0.02452278509736061, 0.001982235349714756, 0.005092713516205549, 0.015108035877346992, 0.01898224651813507, -0.02478662133216858, -0.0115532036870718, -0.05887690559029579, 0.0028987154364585876, -0.014316529966890812, -0.005863389931619167, 0.024508899077773094, -0.022967547178268433, -0.018787842243909836, 0.025050455704331398, -0.009886876679956913, -0.01535798516124487, -0.01649664156138897, 0.020690232515335083, -0.016816021874547005, 0.022453762590885162, -0.003638148307800293, 0.02749440260231495, -0.004769862163811922, -0.010872786864638329, -0.034298572689294815, -0.0060196081176400185, 0.005363491363823414, 0.0022373918909579515, 0.004356752149760723, 0.019857069477438927, -0.003150400472804904, -0.015788452699780464, 0.0013773237587884068, -0.014608137309551239, -0.008831535466015339, -0.011150508187711239, 0.0043636951595544815, 0.005668984726071358, -0.01705208420753479, -0.016302237287163734, 0.005047583486884832, 0.020801320672035217, 0.003908926621079445, -0.029993893578648567, -0.0007359613082371652, -0.010810299776494503, -0.01842680387198925, 0.01290709525346756, -0.029271818697452545, 0.029882805421948433, 0.020384740084409714, 0.038853202015161514, 0.025703100487589836, 0.005728000774979591, -0.0017687372164800763, -0.002692160429432988, -0.0030688196420669556, 0.01941271498799324, 0.014802542515099049, 0.02611968293786049, -0.020426398143172264, -0.002206148114055395, 0.023995116353034973, -0.0024474184028804302, -0.009275889955461025, -0.01524689607322216, 0.026480721309781075, 0.010657552629709244, -0.008456612005829811, -0.009324491024017334, 0.0042977361008524895, -0.028424769639968872, 0.016260579228401184, 0.0045754574239254, -0.00322677381336689, 0.008831535466015339, 0.0028518501203507185, -0.00642230361700058, 0.01118522323668003, -0.002664388157427311, 0.022967547178268433, 0.010407603345811367, 0.018357373774051666, 0.004731675609946251, -0.005436393432319164, 0.024078432470560074, 0.019121108576655388, -0.007887283340096474, 0.040047403424978256, -0.019121108576655388, -0.001418981933966279, 0.000273164885584265, 0.020648574456572533, -0.011164394207298756, 0.008574643172323704, -0.009741072542965412, 0.025966936722397804, -0.007602619007229805, 0.004169290419667959, 0.012691861018538475, -0.020370854064822197, 0.004054730292409658, -0.0024370038881897926, 0.0013860026374459267, -0.011886469088494778, 0.0025515640154480934, 0.005023282952606678, 0.04201922565698624, -0.0072693536058068275, 0.0007233770447783172, -0.001498826895840466, 0.012837664224207401, -0.010053508915007114, 0.0038811543490737677, -0.018648982048034668, -0.005172558128833771, -0.022412104532122612, -0.0182185135781765, -0.015385757200419903, 0.014094353653490543, 0.005599554628133774, 0.003960999194532633, -0.007769251707941294, 0.014219327829778194, 0.01834348775446415, -0.044907525181770325, 0.007116606924682856, -0.017024312168359756, 0.03032715991139412, -0.04771250858902931, 0.027119480073451996, -0.008289978839457035, -0.016899337992072105, 0.021245675161480904, 0.0050684125162661076, -0.0255086962133646, -0.059210170060396194, 0.0065889363177120686, 0.014316529966890812, -0.0006513430853374302, -0.004981624893844128, 0.0015873505035415292, -0.0081788906827569, -0.003464572597295046, -0.007290182635188103, -0.023481331765651703, 0.001808659639209509, -0.01980152539908886, -0.011504602618515491, -0.02232878841459751, -0.011178280226886272, 0.016732705757021904, -0.015996742993593216, -0.0031017991714179516, -0.0320490300655365, -0.011108850128948689, -0.034631840884685516, -0.014677567407488823, 0.008671846240758896, -0.015469073317945004, -0.02400900237262249, -0.02082909271121025, -0.0021662258077412844, -0.010345116257667542, -0.0025342062581330538, 0.004755976144224405, -0.02181500382721424, 0.015857882797718048, 0.014774770475924015, 0.03143804520368576, 0.03349318355321884, -0.029105186462402344, -0.023634077981114388, -0.003777008969336748, -0.043879956007003784, -0.014483163133263588, -0.0016446304507553577, -0.005099656525999308, 0.01544130127876997, 0.0017522474518045783, -0.02246764861047268, -0.01688545197248459, -0.005436393432319164, -0.04449094459414482, 0.0029369022231549025, 0.006370231043547392, 0.016302237287163734, 0.022870345041155815, 0.03638148307800293, 0.0015170522965490818, -0.008470498025417328, -0.010289572179317474, 0.010942216962575912, -0.02486993744969368, 0.01898224651813507, -0.01159486174583435, -0.015663478523492813, 0.019509917125105858, -0.0026539736427366734, -0.022134384140372276, 0.005922405514866114, 0.02121790312230587, -0.015927312895655632, 0.011254653334617615, -0.021190131083130836, -0.02328692562878132, -0.0015899541322141886, 0.024147862568497658, 0.0010874522849917412, -0.007790080737322569, 0.014719226397573948, -0.009907705709338188, -0.02185666188597679, -0.012289165519177914, 0.013295904733240604, -0.013531967997550964, -0.015094149857759476, -0.000588855822570622, -0.0035287956707179546, -0.012900152243673801, 0.0127543481066823, 0.011136622168123722, 0.019162766635417938, -0.006571578793227673, 0.014233213849365711, 0.01031040120869875, -0.011081078089773655, -0.0013617019867524505, 0.008630187250673771, 0.006727796979248524, -0.010345116257667542, 0.010254857130348682, -0.00582173140719533, -0.03104923479259014, -0.027175024151802063, -0.008963453583419323, -0.021870547905564308, 0.0015621819766238332, -0.004061673302203417, 0.0008418424986302853, -0.0016767419874668121, -0.0033343906980007887, -0.0011586183682084084, -0.0015257310587912798, -0.001186390407383442, 0.024286722764372826, -0.03354872763156891, -0.005051054991781712, 0.007005518302321434, -0.01544130127876997, 0.024925481528043747, -0.003409028286114335, -0.02289811708033085, -0.009949363768100739, -0.01400409359484911, -0.01099776104092598, 0.0026539736427366734, -0.02478662133216858, -0.02349521778523922, 0.00012399819388519973, 0.01524689607322216, 9.13442563614808e-05, -0.013490309938788414, 0.21140141785144806, 0.03682583570480347, -0.006286914460361004, 0.02702227793633938, 0.005582197103649378, 0.00758178997784853, 0.0371035598218441, 0.011692064814269543, -0.01834348775446415, 0.025453152135014534, 0.0013573626056313515, -0.010296515189111233, 0.0024890766944736242, 0.003134778467938304, 0.008206662721931934, -0.03738128021359444, -0.029605085030198097, -0.011268539354205132, -0.019037790596485138, 0.022662052884697914, 0.009789673611521721, 0.018787842243909836, 0.01752421073615551, -0.020176447927951813, 0.02160671353340149, 0.03049379214644432, -0.02899409830570221, 0.02757771871984005, 0.025675328448414803, 0.03199348598718643, -0.005925877019762993, 0.017288148403167725, 0.015857882797718048, 0.004044315777719021, -0.0037284076679497957, -0.017329806461930275, -0.011622633785009384, -0.005596083123236895, 0.016760477796196938, 0.03104923479259014, -0.005120485555380583, -0.024370038881897926, -0.03793672099709511, -0.0035687179770320654, -0.02482827939093113, -0.0159828569740057, -0.01914888061583042, -0.002614051103591919, 0.0056655132211744785, 0.012608544901013374, -0.02663346752524376, 0.00858852919191122, 0.011685121804475784, 0.03329877555370331, -0.0029837675392627716, -0.0014181140577420592, 0.006672252900898457, 0.010699210688471794, -0.042852386832237244, -0.013448650948703289, -0.016052287071943283, 0.016593843698501587, 0.0038811543490737677, 0.03602044656872749, 0.028633059933781624, -0.016677161678671837, 0.003219830570742488, 0.021676143631339073, 0.01262937393039465, -0.0069430312141776085, 0.014996946789324284, 0.020606916397809982, 0.02105127088725567, 0.007644277065992355, -0.024064546450972557, -0.026966731995344162, 0.00774147966876626, 0.039408646523952484, -0.0027338184881955385, 0.03088260255753994, -0.03127141296863556, 0.014066580682992935, -0.02224547229707241, 0.030993690714240074, 0.0008965188753791153, -0.009442522190511227, 0.011657348833978176, -0.021537283435463905, -0.012247506529092789, -0.00034606672124937177, 0.0013790595112368464, -0.006373702548444271, -0.013615284115076065, -0.020884636789560318, 0.012337766587734222, 0.027730466797947884, 0.00681805657222867, 0.025966936722397804, 0.006064737681299448, 0.005762715823948383, -0.02907741442322731, 0.06026551127433777, -0.005238517187535763, 0.027438858523964882, -0.01594119891524315, 0.005891161970794201, 0.013434764929115772, 0.018607323989272118, -0.010976932011544704, -0.0057835448533296585, -0.007769251707941294, -0.02220381423830986, -0.004801106173545122, -0.015774566680192947, 0.0049955109134316444, -0.006856243126094341, 0.004631001967936754, -0.02509211376309395, 0.02388402633368969, 0.003553096204996109, 0.015594047494232655, 0.002058608690276742, -0.005054526496678591, 0.016760477796196938, 0.01696876809000969, -0.004884422291070223, 0.00501633994281292, -0.01752421073615551, 0.0023623663000762463, -0.0052176876924932, 0.007755365688353777, 0.0007715443498454988, 0.02380071021616459, -0.02757771871984005, -0.0032163590658456087, -0.005974478088319302, -0.004172761924564838, -0.007276296615600586, 0.0047073750756680965, -0.012247506529092789, 0.023161951452493668, 0.0022755784448236227, 0.028202593326568604, 0.005505823530256748, 0.0026713311672210693, -0.02289811708033085, 0.010969989001750946, -0.004835821222513914, -0.009268946945667267, -0.021148473024368286, -0.008213605731725693, -0.026466835290193558, -0.010164598003029823, -0.01641332544386387, 0.027883213013410568, -0.008019200526177883, -0.007984485477209091, -0.03377090394496918, -0.004269964061677456, -0.002134982030838728, -0.047990232706069946, 0.03066042624413967, 0.030132755637168884, -0.02177334576845169, -0.03815889731049538, -0.007887283340096474, -0.17951901257038116, 0.01885727234184742, 0.009609155356884003, -0.006838885601609945, 0.02503656968474388, 0.005686342716217041, 0.022745370864868164, -0.015038605779409409, -0.03707578778266907, 0.011844811029732227, 0.011615690775215626, -0.004322037100791931, -0.017079856246709824, -0.008317750878632069, -0.002997653791680932, 0.002758119022473693, -0.0003443309396971017, -0.009289775975048542, 0.010511749424040318, 0.0004703903687186539, 0.025411494076251984, -0.006772927008569241, -0.011574032716453075, 0.004433125257492065, 0.009352263063192368, 0.013761087320744991, -0.025397608056664467, 0.00762344803661108, -0.002537677763029933, -0.012796006165444851, 0.002723403973504901, 0.025230975821614265, -0.007644277065992355, -0.019621005281805992, 0.008033087477087975, -0.024939367547631264, -0.0007168679730966687, -0.024383924901485443, 0.005790487863123417, 0.016552185639739037, 0.016010629013180733, 0.010143768042325974, 0.010289572179317474, 0.0076581635512411594, 0.006439661141484976, -0.004755976144224405, 0.026300201192498207, 0.00031655881321057677, 0.02134287729859352, -0.027938757091760635, 0.0066167088225483894, -0.041241604834795, 0.0022408633958548307, 0.008130289614200592, -0.016954882070422173, 0.007172151003032923, 0.013615284115076065, 0.013990207575261593, -0.008040030486881733, -0.000234978215303272, -0.020468056201934814, -0.031549133360385895, 0.010324287228286266, 0.0076303910464048386, -0.024425582960247993, -0.033187687397003174, -0.007935884408652782, -0.01782970316708088, -0.027772124856710434, 0.011518488638103008, 0.006509091705083847, -0.021828889846801758, 0.013754144310951233, -0.02212049625813961, 0.012740462087094784, 0.012178076431155205, 0.007123549934476614, 0.018440689891576767, -0.0003065782075282186, 0.003794366493821144, -0.012462740764021873, 0.043879956007003784, -0.015427415259182453, 0.004752504639327526, -0.01984318345785141, 0.01937105692923069, 0.011303254403173923, -0.0010917916661128402, 0.0318823978304863, 0.0007546207052655518, 0.011823982000350952, -0.042463578283786774, 0.002315500983968377, -0.022620394825935364, -0.00036407518200576305, 0.008894022554159164, 0.018648982048034668, -0.008456612005829811, 0.010963045991957188, -0.0025359420105814934, -0.00013549759751185775, -0.030771514400839806, -0.006804170552641153, 0.0023259154986590147, 0.02710559405386448, -0.010227085091173649, -0.006783341523259878, 0.04210254177451134, 0.018496235832571983, -0.02259262278676033, -0.01910722255706787, 0.0033274476882070303, 0.0161078330129385, -0.009685528464615345, -0.016566071659326553, 0.024578331038355827, -0.00942863617092371, -0.011303254403173923, 0.025841962546110153, 0.005276703741401434, 0.06743071973323822, 0.024453354999423027, 0.0006378910038620234, -0.012997354380786419, -0.0006687006680294871, 0.015705136582255363, -0.07498473674058914, 0.001482337131164968, 0.009373092092573643, -0.009088427759706974, -0.004565042909234762, 0.044296540319919586, 0.013205645605921745, 0.037992265075445175, -0.008366352878510952, 0.03471515700221062, 0.013941606506705284, -0.022148270159959793, 0.007998371496796608, -0.007262410596013069, -0.0038186670280992985, -0.022023294121026993, -0.001164693501777947, -0.016635501757264137, -0.027563832700252533, 0.022023294121026993, 0.003171229502186179, 0.008067802526056767, -0.008567700162529945, 0.0001568691077409312, -0.0025463567581027746, 0.028272023424506187, -0.027758238837122917, 0.012073931284248829, 0.02530040591955185, 0.018149083480238914, 0.032187893986701965, -0.011310197412967682, 0.012622430920600891, 0.013115385547280312, 0.00794282741844654, 0.004613643977791071, -0.07115218043327332, -0.030688198283314705, 0.03499287739396095, -0.025369836017489433, 0.0011473358608782291, 0.01050480641424656, -0.0020308366511017084, -0.03496510535478592, -0.0030688196420669556, -0.016940996050834656, -0.021828889846801758, 0.01178926695138216, 0.02507822774350643, -0.0025862790644168854, -0.01705208420753479, -0.007588732987642288, 0.006661838386207819, -0.012740462087094784, 0.016330009326338768, 0.031549133360385895, -0.006595879793167114, 0.037603456526994705, -0.020801320672035217, 0.011206052266061306, 0.003981828223913908, -0.0018138668965548277, -0.0009572704439051449, 0.00014244062185753137, 0.027091708034276962, -0.01539964322000742, -0.01123382430523634, -0.007151321973651648, -0.0029369022231549025, -0.012747405096888542, -0.007158264983445406, 0.008484384045004845, -0.03557609021663666, 0.025883620604872704, -0.02693895995616913, 0.011261596344411373, -0.005550953559577465, -0.0163577813655138, -0.017621412873268127, -0.03010498359799385, -0.02010701783001423, -0.012268335558474064, 0.002528999000787735, -0.014816428534686565, -0.006585464812815189, 0.006130696274340153, -0.005915462505072355, 0.013434764929115772, -0.0012471419759094715, -0.024286722764372826, 0.03504842147231102, 0.011740665882825851, 0.012525227852165699, -0.007324897684156895, -0.013774973340332508, -0.010706153698265553, -0.025592012330889702, -0.00013159213995095342, -0.015774566680192947, 0.0251754317432642, -0.0047247326001524925, -0.013525024987757206, -0.06759735196828842, 0.022398218512535095, -0.0158995408564806, -0.017774159088730812, 0.007727593649178743, -0.008657960221171379, 0.022009408101439476, -0.031854625791311264, -0.013629170134663582, 0.003832553280517459, -0.03396530821919441, 0.019857069477438927, -0.008519099093973637, 0.01988484151661396, -0.013101499527692795, -0.012546056881546974, 0.021801117807626724, -0.036353711038827896, 0.029743945226073265, 0.030771514400839806, 0.006047380156815052, -0.030354931950569153, 0.024300608783960342, -0.0073040686547756195, 0.007179094012826681, 0.0158995408564806, -0.017704728990793228, 0.01769084297120571, -0.019662663340568542, -0.025147657841444016, 0.010470091365277767, -0.026564037427306175, -0.008116403594613075, 0.022967547178268433, -0.008331636898219585, -0.006814585067331791, 0.005137843079864979, 0.02435615286231041, 0.014788656495511532, 0.017163172364234924, -0.03177130967378616, -0.027036163955926895, 0.006849300116300583, -0.02289811708033085, -0.022828686982393265, 0.011692064814269543, -0.004512970335781574, 0.00014612911036238074, 0.006113338749855757, 0.016691047698259354, 0.012782120145857334, -0.006141111254692078, -0.006620180327445269, -0.024619989097118378, -0.004422710742801428, -0.008630187250673771, -0.007192980032414198, -0.019995929673314095, 0.005793959368020296, 0.008498270064592361, 0.014156840741634369, 0.009782730601727962, 0.021759459748864174, 0.011497659608721733, 0.01606617495417595, 0.02005147375166416, -0.002537677763029933, 0.007720650639384985, 0.018996132537722588, 0.007491530384868383, -0.02237044647336006, 0.005502352025359869, 0.019732095301151276, 0.018621210008859634, -0.008352466858923435, -0.0036902211140841246, 0.014316529966890812, 0.014233213849365711, -0.012400253675878048, 0.03110477887094021, -0.009074541740119457, -0.004377581179141998, -0.025453152135014534, 0.004186647944152355, 0.011372685432434082, 0.004197062458842993, -0.0320490300655365, -0.006526449229568243, 0.0037631229497492313, 0.013018183410167694, -0.004221362993121147, 0.019315512850880623, -0.009949363768100739, -0.027688808739185333, -0.008220548741519451, 0.002541149500757456, -0.03365981578826904, -0.006606294307857752, -0.006995103787630796, 0.02066246047616005, 0.013851347379386425, 0.010969989001750946, -0.0032962041441351175, -0.017718615010380745, -0.0319657139480114, 0.014844200573861599, -0.006252199411392212, -0.006457019131630659, -0.008470498025417328, 0.007151321973651648, 0.022092724218964577, -0.013920777477324009, 0.00886</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Which clients are employed by Stevens Valley School? Include Employer name, client name, client id, and their complete address</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SELECT client.Name, client.ID, employer.Name, address.Address, address.City, address.State, address.Zip FROM client INNER JOIN employer ON client.Employer_ID = employer.ID INNER JOIN address ON client.Address_ID = address.ID WHERE employer.Name = 'Stevens Valley School';</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>[0.012723113410174847, 0.01613204926252365, -0.002328544622287154, -0.01813177950680256, -0.0155952088534832, 0.04493352770805359, -0.008146550506353378, -0.012065484188497066, -0.020064404234290123, -0.022708341479301453, -0.010307332500815392, 0.0060897814109921455, -0.011280355975031853, 0.01131390780210495, -0.019795984029769897, -0.009481940418481827, 0.005418731365352869, -0.033230412751436234, 0.016776258125901222, -0.009663124568760395, -0.009387994185090065, 0.013078770600259304, 0.011850748211145401, -0.0025416030548512936, -0.005435507278889418, -0.013696136884391308, -0.00011659498704830185, -0.012166141532361507, -0.002120519056916237, 0.00711313309147954, 0.0015576755395159125, -0.017098361626267433, -0.007488921284675598, -0.03843776136636734, -0.010199964977800846, 0.011293776333332062, -8.781321957940236e-05, 0.011340750381350517, 0.017621781677007675, 0.011998379603028297, 0.021929923444986343, -0.016118628904223442, -0.011441407725214958, -0.0005104176234453917, -0.003195876954123378, -0.006529319565743208, -0.005589848849922419, -0.015970997512340546, -0.03935039043426514, 0.013810215517878532, 0.02447991445660591, -0.003566632280126214, -0.010542199946939945, -0.02348676137626171, 0.011280355975031853, 0.004945640917867422, -0.00655951676890254, 0.004388669040054083, -0.02515096589922905, -0.01725941337645054, 0.00012372489436529577, 0.0015652248403057456, -0.008609575219452381, -0.002300024963915348, -0.011434697546064854, -0.007670104969292879, -0.004603405017405748, 0.011112593114376068, -0.0037075530271977186, 0.011448117904365063, 0.03951144218444824, 0.0077976044267416, -0.003616961184889078, 0.00868339091539383, -0.006260899361222982, -0.021151505410671234, 0.002107098000124097, -0.024251757189631462, 0.011542065069079399, 0.008421680890023708, -0.012105747126042843, -0.025768332183361053, -0.03143199533224106, 0.023540444672107697, 0.026533329859375954, -0.00790497288107872, 0.0033904816955327988, -0.0023469985462725163, -0.018534408882260323, -0.0030012724455446005, 0.0143336346372962, 0.015554945915937424, -0.017192307859659195, 0.012884166091680527, -0.015165736898779869, 0.013769952580332756, 0.01415916159749031, 0.01613204926252365, 0.018816251307725906, -0.02164808288216591, 0.001157561782747507, 0.02131255716085434, -0.016440732404589653, -0.017326518893241882, -0.026318592950701714, 0.004657089244574308, -0.01197824813425541, -0.02217150293290615, -9.908476931741461e-05, -0.021822554990649223, -0.025285175070166588, 0.004036367405205965, 0.003744460642337799, -0.009696677327156067, 0.012817060574889183, 0.007690236438065767, 0.022641237825155258, 0.002221176400780678, 0.01197824813425541, -0.014830212108790874, 0.02128571644425392, 0.017044678330421448, 0.02172860875725746, -0.022037291899323463, 0.018749145790934563, 0.004499392118304968, -0.014024951495230198, -0.012112458236515522, 0.002966042375192046, -0.0010342563036829233, -0.01735336147248745, 0.01487047504633665, 0.01032746396958828, -0.01801099069416523, -0.02065492793917656, -0.019245723262429237, 0.008643127977848053, 0.027217799797654152, -0.026278330013155937, -0.015259684063494205, 0.005928729195147753, 0.027043327689170837, 0.016105206683278084, 0.01634678617119789, -0.00022039808391127735, 0.01097167283296585, 0.027754640206694603, 0.02955305576324463, 0.007186948787420988, -0.013072059489786625, -0.01733993925154209, 0.0033233766444027424, 0.0022379527799785137, -0.015648892149329185, -0.007931814529001713, 0.0057878089137375355, 0.018588094040751457, 0.01197824813425541, -0.015970997512340546, -0.032344624400138855, -0.03467987850308418, 0.030009370297193527, 0.019943615421652794, -0.02294992096722126, 0.012568771839141846, 0.018977303057909012, -0.028720952570438385, -0.03347199037671089, 0.008005630224943161, -0.00013620224490296096, -0.015232841484248638, 0.001649106154218316, -0.027486220002174377, 0.012454693205654621, 3.3211748814210296e-05, -0.006750766187906265, 0.0010250293416902423, -0.007394974119961262, -0.00422761682420969, -0.033901460468769073, 0.01372968964278698, 0.00046889641089364886, -0.011850748211145401, 0.03580724447965622, -0.011354170739650726, -0.007743920665234327, 0.0007893228903412819, 0.0014259818708524108, 0.013823635876178741, -0.006304517388343811, 0.04592668265104294, 0.023204918950796127, 0.005576428025960922, -0.0029777856543660164, -0.6321830749511719, -0.023540444672107697, -0.006817871239036322, -0.020708613097667694, 0.021003874018788338, 0.02383570745587349, 0.02524491213262081, 0.015729419887065887, -0.007287606131285429, 0.017957305535674095, -0.012266799807548523, 0.041229330003261566, -0.012152721174061298, 0.00559655949473381, 0.006878265645354986, -0.026425961405038834, -0.010877725668251514, 0.01236074697226286, 0.003368672449141741, -0.005006035324186087, -0.010911277495324612, 0.02756674587726593, -0.002308413153514266, 0.009763781912624836, 0.04028986021876335, 0.027942534536123276, -0.007019186392426491, -0.0233928132802248, -0.0019091381691396236, 0.011864169500768185, -0.01725941337645054, 0.02317807823419571, -0.0034273893106728792, 0.016319943591952324, 0.034545671194791794, 0.016964152455329895, -0.023084130138158798, 0.041900381445884705, -0.007616420742124319, 0.040370386093854904, -0.018722303211688995, -0.03065357729792595, 0.008851153776049614, -0.013823635876178741, -0.004197419621050358, 0.02963358163833618, 0.00939470436424017, 0.006374977994710207, -0.0064085302874445915, -0.006492411717772484, 0.018843092024326324, -0.017058098688721657, -0.028801478445529938, 0.0005523582804016769, 0.029069898650050163, -0.033230412751436234, -0.0024912741500884295, -0.002437590155750513, 0.0006819548434577882, 0.009146415628492832, -0.007663394324481487, 0.01877598837018013, -0.01911151222884655, -0.016870204359292984, -0.024533599615097046, 0.014534949325025082, -0.0039759729988873005, -0.012756666168570518, 0.02065492793917656, -0.012944560497999191, 0.018400199711322784, 0.02437254786491394, 0.011521933600306511, 0.022533869370818138, 0.011797063983976841, 0.0014159161364659667, -0.0015006362227723002, -0.0030516013503074646, -0.005888466257601976, 0.009132994338870049, 0.0008509756880812347, -0.015769682824611664, -0.013957845978438854, -0.011126014403998852, -0.010636147111654282, 0.006311228033155203, -0.027271484956145287, -0.02250702679157257, 0.00708629097789526, -0.02351360209286213, 0.02152729406952858, 0.010548911057412624, 0.01615889184176922, -0.025983067229390144, -0.007012475747615099, 0.014508107677102089, 0.014065214432775974, -0.004006170202046633, 0.008321023546159267, -0.027419114485383034, -0.017715727910399437, 0.00025164385442622006, 0.002088644076138735, 0.015528104268014431, 0.007623131386935711, 0.010065754875540733, -0.02845253236591816, 0.010233516804873943, 0.0031757454853504896, -0.014977842569351196, 0.015581788495182991, -0.008260629139840603, -0.02810358628630638, 0.00010181091056438163, -0.02735201083123684, -0.038276709616184235, 0.011280355975031853, 0.015447578392922878, -0.020842822268605232, 0.003120383946225047, 0.028479374945163727, 0.003533079754561186, 0.021809134632349014, -0.02328544482588768, 0.007663394324481487, 0.016064943745732307, -0.000575006240978837, -0.030814629048109055, 0.004334984812885523, 0.002300024963915348, 0.005230837035924196, -0.01427995041012764, 0.03269357234239578, -0.014065214432775974, -0.00939470436424017, -0.007864709943532944, 0.020292561501264572, -0.011998379603028297, -0.015877049416303635, -0.02976779080927372, 0.002308413153514266, 0.015031526796519756, -0.004855048842728138, -0.00678431848064065, -0.005432152189314365, -0.010938120074570179, -0.007656684145331383, -0.007348001003265381, -0.016172312200069427, -0.011186408810317516, -0.011025356128811836, -0.0066433981992304325, 0.008267339318990707, 0.011454829014837742, 0.006009255535900593, 0.0012825449230149388, -0.003908867947757244, -0.02175545133650303, 0.004865114577114582, -0.017487570643424988, 0.0057710325345396996, 0.01648099534213543, -0.01042812131345272, -0.02217150293290615, -0.004435642622411251, -0.00928733590990305, 0.02810358628630638, -0.002935845172032714, 0.0053046527318656445, -0.0048047201707959175, 0.03612934798002243, 0.0004684769955929369, -0.004006170202046633, 0.011515223421156406, 0.005126824136823416, 0.032666727900505066, -0.03019726276397705, 0.006683661136776209, -0.01988993026316166, -0.015152315609157085, 0.009676544927060604, 0.0059253741055727005, -0.006421951577067375, 0.019245723262429237, 0.02515096589922905, 0.006884976290166378, 0.0033049227204173803, 0.012897586449980736, -0.013957845978438854, -0.025728069245815277, -0.0009361151605844498, 0.005730769596993923, 0.007488921284675598, -0.012944560497999191, 0.025312017649412155, 0.020722033455967903, 0.01405179314315319, 0.01214601006358862, 0.020480455830693245, 0.024345705285668373, 0.02909674122929573, -0.003303245175629854, 0.010770357213914394, 0.012072195298969746, 0.0377667099237442, -0.03167357295751572, -0.0018068029312416911, -0.019192038103938103, 0.02547306939959526, 0.02164808288216591, 0.006368267349898815, -0.025419386103749275, -0.018507568165659904, -0.011079040355980396, -0.014548370614647865, 0.005677085369825363, -0.005019456148147583, 0.02019861340522766, -0.011669564992189407, -0.0032965345308184624, 0.010361016727983952, -0.011495091952383518, 0.04117564484477043, -0.00977049209177494, 0.0026842011138796806, 0.006415240932255983, 0.01147496048361063, 0.025567015632987022, 0.010548911057412624, 0.005120113957673311, -0.010964961722493172, 0.005448928568512201, 0.02657359279692173, 0.00395248644053936, 0.003888736478984356, 0.011119303293526173, 0.015340209938585758, -0.013756531290709972, 0.028613584116101265, -0.016306523233652115, -0.013219690881669521, 0.006848068442195654, 0.013521663844585419, -0.006750766187906265, 0.03274725377559662, 0.025338860228657722, 0.011005224660038948, 0.018185462802648544, -0.00835457630455494, 0.04074617475271225, -0.0018437106627970934, 0.018427040427923203, -0.008374707773327827, 0.00524090277031064, 0.013434426859021187, 0.006556161679327488, 0.02207755483686924, 0.013152586296200752, 0.022574132308363914, 0.01580994576215744, -0.007361421827226877, -0.008428392000496387, 0.0018789408495649695, -0.01648099534213543, 0.028291480615735054, 0.019285986199975014, -0.03151252120733261, -0.008502207696437836, 0.011615880765020847, -0.024734914302825928, 0.003274725517258048, 0.007636552676558495, 0.007824446074664593, 0.016521258279681206, 0.019849667325615883, 0.009528914466500282, -0.015984417870640755, 0.005472415126860142, 0.008716943673789501, 0.011991668492555618, -0.019245723262429237, -0.006848068442195654, -0.0006966341170482337, 0.0143336346372962, 0.010897857137024403, 0.01724599301815033, 0.003590119071304798, 0.008763916790485382, -0.029177267104387283, 0.015568367205560207, 0.01329350657761097, -0.004046433139592409, -0.025432806462049484, 0.014696002006530762, 0.00028603518148884177, 8.398613863391802e-05, 0.00972351897507906, -0.03298883140087128, -0.0005297103198245168, 0.014951000921428204, -0.0035397903993725777, 0.01218627393245697, 0.023003604263067245, 0.021782292053103447, 0.05467717722058296, -0.013139165006577969, -0.006663529668003321, -0.017286255955696106, -0.011360881850123405, -0.01756809651851654, 0.015957575291395187, 0.016172312200069427, -0.01766204461455345, -0.0010879402980208397, 0.03591461107134819, -0.014964422211050987, -0.015877049416303635, -0.00845523364841938, 0.042678799480199814, -0.013850478455424309, -0.027097010985016823, -0.04818141087889671, -0.028613584116101265, 0.011783643625676632, 0.07558710873126984, 0.029069898650050163, -0.01230035163462162, 0.007978787645697594, 0.018937040120363235, -0.0036840662360191345, -0.035297244787216187, -0.00022081748466007411, -0.0070460280403494835, -0.020077824592590332, 0.002467787591740489, -0.032022520899772644, -0.017648622393608093, -0.009851018898189068, 0.012957981787621975, 0.009267204441130161, 0.010924698784947395, -0.021607819944620132, -0.005841492675244808, -0.013702847063541412, -0.031002523377537727, 0.0023168011102825403, -0.00023277057334780693, 0.0063816881738603115, 0.01614546962082386, 0.023352550342679024, 0.023862548172473907, 0.02987515926361084, 0.01866861991584301, -0.024184653535485268, 0.011991668492555618, 0.033552516251802444, -0.00846194475889206, 0.024251757189631462, -0.00939470436424017, 0.04088038578629494, -0.012179562821984291, 0.0026959446258842945, 0.019916772842407227, 0.012971402145922184, 0.030438842251896858, 0.009629571810364723, -0.008602865040302277, -0.019084671512246132, 0.029150424525141716, 0.0064890566281974316, 0.007307737600058317, 0.004710773006081581, 0.0028972597792744637, -0.0020114732906222343, 0.011602459475398064, -0.004079985897988081, 0.031593047082424164, -0.038384076207876205, -0.019272563979029655, -0.0015299946535378695, -0.0028335098177194595, 0.008066024631261826, -0.02239965833723545, -0.03019726276397705, -0.04152459278702736, -0.005405310075730085, 0.006898397114127874, -0.011864169500768185, -0.007891551591455936, -0.006958791520446539, -0.0014972810167819262, 0.0062172808684408665, 0.003590119071304798, 0.001441080472432077, 0.009622861631214619, 0.028640426695346832, -0.02603675238788128, 0.012018511071801186, 0.03688092529773712, 0.015165736898779869, 0.027164116501808167, -0.003303245175629854, 0.00015559978783130646, 0.01131390780210495, -0.0031975547317415476, -0.015675734728574753, 0.013541795313358307, -0.0023671300150454044, -0.012595614418387413, 0.010924698784947395, -0.019178617745637894, 0.007663394324481487, -0.005713993217796087, 0.017621781677007675, -0.011105882935225964, -0.004207485355436802, -0.01582336612045765, -0.03062673658132553, -0.0028267994057387114, 0.002940878039225936, -0.0032176862005144358, 0.0023570642806589603, -0.011414566077291965, -0.0006223991513252258, 0.018265988677740097, -0.020722033455967903, 0.002456044079735875, -0.0025751555804163218, 0.017286255955696106, -0.013058639131486416, -0.007093001622706652, -0.007549315690994263, -0.02406386472284794, 0.009193388745188713, 0.02634543552994728, -0.01791704259812832, 0.005576428025960922, 0.006378333084285259, -0.000502448936458677, 0.008240497671067715, -0.00999864935874939, 0.005885111168026924, 0.00802576169371605, 0.010978383012115955, 0.01799756847321987, -0.009374572895467281, 0.029902001842856407, 0.01660178415477276, -0.028801478445529938, 0.008757206611335278, 0.0178096741437912, -0.02834516391158104, 0.020292561501264572, 0.002244663191959262, -0.016011260449886322, 0.02362097054719925, -0.009535624645650387, 0.003724329173564911, -0.019165197387337685, -0.01978256367146969, -0.017957305535674095, 0.018051253631711006, 0.0003132966230623424, -0.01582336612045765, -0.01988993026316166, 0.018198885023593903, -0.010126149281859398, 0.0008237142465077341, 0.00450610276311636, -0.031002523377537727, 0.002221176400780678, -0.015514682978391647, 0.018749145790934563, 0.018614934757351875, -0.020010720938444138, 0.011011935770511627, 0.015460998751223087, 0.02241308055818081, -0.005388534162193537, -0.009267204441130161, -0.017876779660582542, 0.03392830491065979, 0.023218341171741486, 0.012716403231024742, 0.014749685302376747, 0.012038642540574074, 0.017178887501358986, -0.038679338991642, -0.0005045459256507456, 0.007871420122683048, -0.02109782211482525, -0.020695190876722336, -0.003761237021535635, -0.01236074697226286, 0.02481544017791748, -0.007059449329972267, 0.018641777336597443, -0.004975838121026754, 0.004798009525984526, 0.0025751555804163218, 0.0057710325345396996, 0.005542875733226538, -0.011823906563222408, -0.057817693799734116, 0.0042678797617554665, -0.013320348225533962, -0.010978383012115955, 0.041121963411569595, -0.03663934767246246, -0.009280625730752945, 0.010683121159672737, -0.028694111853837967, -0.011716538108885288, -0.026533329859375954, 0.01197824813425541, -0.02591596357524395, 0.027727797627449036, -0.0058985319919884205, -0.0028502861969172955, -0.0077372100204229355, -0.005056363996118307, -0.039940912276506424, -0.011434697546064854, 0.02019861340522766, 0.013877320103347301, 0.010179833509027958, 0.02600990980863571, -0.0008639772422611713, -0.020480455830693245, 0.006522608920931816, 0.016427312046289444, 0.0022044002544134855, -0.009575887583196163, -0.01005233358591795, 0.012119168415665627, -0.006703792605549097, -0.005351626314222813, -0.0007234761142171919, 0.009508782997727394, -0.01481679081916809, -0.01932624913752079, 0.013528374023735523, -0.019742300733923912, -0.024976491928100586, 0.0035532114561647177, -0.03484093025326729, 0.010548911057412624, 0.024439651519060135, 0.03953828290104866, 0.030143579468131065, -0.0064253066666424274, -0.014548370614647865, 0.007743920665234327, -0.011615880765020847, 0.016199154779314995, 0.019957035779953003, 0.023312287405133247, -0.013863898813724518, -0.02284255251288414, 0.04536300152540207, -0.00044750666711479425, -0.004331629723310471, -0.0033149884548038244, 0.028506217524409294, 0.03712250292301178, 0.0009109507664106786, -0.017742570489645004, 0.00824720785021782, -0.025432806462049484, 0.014360476285219193, -0.0035196589305996895, 0.007938524708151817, -0.00708629097789526, 0.006539385300129652, -0.019581247121095657, -0.006844712886959314, -0.025956226512789726, 0.022426500916481018, 0.017970727756619453, -0.00325459404848516, -0.014628896489739418, 0.005247613415122032, 0.02307070977985859, 0.005036232527345419, -0.02120518870651722, 0.02831832319498062, -0.011434697546064854, -0.000204670344828628, -0.012763376347720623, 0.03280093893408775, -0.01801099069416523, -0.002117163734510541, 0.01868204027414322, 0.028801478445529938, -0.017219150438904762, -0.015997840091586113, 0.01669573225080967, -0.009025626815855503, -0.0008329412085004151, 0.012266799807548523, 0.0009923155885189772, -0.014239687472581863, -0.016561521217226982, -0.0035297246649861336, 0.030841471627354622, 0.00868339091539383, -0.00024011018103919923, -0.02351360209286213, 0.009401414543390274, -0.02733858861029148, -0.007334579713642597, -0.009783913381397724, -0.006421951577067375, -0.02351360209286213, -0.03161989152431488, 0.0009143060306087136, 0.007616420742124319, 0.00354314548894763, 0.011810485273599625, 0.0015367051819339395, -0.00256844493560493, 0.025325438007712364, -0.042651958763599396, 0.006992344278842211, -0.006445438135415316, 0.026224646717309952, -0.05148297920823097, 0.011401144787669182, -0.012978113256394863, -0.03229093924164772, -0.006458858959376812, 0.016293101012706757, -0.04042407125234604, -0.04340353235602379, 0.014534949325025082, 0.018051253631711006, -0.01399810891598463, -0.004948996007442474, -0.027298325672745705, -0.018078094348311424, 0.0004240199050400406, 0.0001700693101156503, -0.025567015632987022, 0.009213520213961601, -0.015219421125948429, -0.019500721246004105, -0.018359936773777008, -0.017219150438904762, 0.0070997122675180435, -0.012642587535083294, 0.022372817620635033, -0.01323982235044241, -0.006156886462122202, -0.02141992561519146, -0.012971402145922184, 0.009636281989514828, -0.020359667018055916, -0.0010845850920304656, -0.006737344898283482, -0.016387049108743668, -0.012884166091680527, 0.010669699870049953, -0.0032176862005144358, -0.02316465601325035, -0.004680575802922249, 0.0018940394511446357, 0.04149775207042694, 0.030224105343222618, -0.013810215517878532, -0.028828321024775505, -0.0038719603326171637, -0.032881464809179306, -0.03231778368353844, -0.012447983026504517, -0.0028704176656901836, 0.011334039270877838, 0.011669564992189407, -0.01527310535311699, -0.014548370614647865, -0.022439921274781227, -0.042007748037576675, -0.005344915669411421, 0.02151387184858322, 0.01583678647875786, 0.013615611009299755, 0.03956512734293938, -0.0007905811653472483, -0.0085626021027565, -0.005703927483409643, 0.03645145148038864, -0.015622051432728767, 0.011743380688130856, 0.0002967300533782691, -0.020681770518422127, 0.007623131386935711, 0.0009059178992174566, -0.01692388951778412, -0.010320753790438175, 0.0008841087692417204, -0.0031606468837708235, -0.0011139435227960348, -0.013078770600259304, -0.02712385356426239, 0.0006333037163130939, 0.0238491278141737, -0.008703522384166718, -0.017299676313996315, 0.018359936773777008, -0.009347730316221714, -0.006442083045840263, -0.018158622086048126, 0.0017078230157494545, -0.009522203356027603, -0.011609170585870743, -0.005224126391112804, 0.0010158023796975613, -0.018400199711322784, 0.01703125610947609, 0.012434561736881733, 0.013387453742325306, -0.013608899898827076, 0.0020332823041826487, 0.010012070648372173, 0.0056334673427045345, -0.015863629058003426, 0.0316467322409153, 0.0017497636144980788, 0.011743380688130856, 0.026439381763339043, 0.014011530205607414, -0.028372006490826607, -0.002942555584013462, -0.016776258125901222, -0.01240772008895874, 0.001143301953561604, -0.005730769596993923, -0.00259528704918921, -0.012468114495277405, -0.0025416030548512936, -0.014467844739556313, -0.0012624133378267288, -0.0028351875953376293, 0.008052603341639042, -0.013702847063541412, -0.015783103182911873, -0.01691046729683876, -0.025513332337141037, 0.007482211105525494, 0.0003189585986547172, -0.01669573225080967, -0.020601244643330574, -0.016762835904955864, -0.0004663799481932074, 0.015179158188402653, -0.03263988718390465, -0.007220501080155373, 0.01136759202927351, 0.0025432805996388197, 0.0002271085832035169, -0.02217150293290615, 0.214950829744339, 0.009743650443851948, -0.0007872259011492133, 0.01790362223982811, 0.002283248584717512, 0.010045623406767845, 0.037068817764520645, 0.008529049344360828, 0.003070055041462183, 0.01646757498383522, -0.0030398578383028507, -0.009159836918115616, 0.0006106557557359338, 0.010226806625723839, 0.021003874018788338, -0.03250567615032196, -0.03688092529773712, -0.01470942236483097, -0.031995680183172226, 0.009300757199525833, 0.006022676359862089, 0.026157541200518608, 0.011542065069079399, -0.03744460642337799, 0.02545964904129505, 0.014696002006530762, -0.009153125807642937, 0.044987212866544724, 0.030143579468131065, 0.032908305525779724, -0.02238623797893524, 0.01015299092978239, 0.015742840245366096, -0.00428130105137825, -0.0029811409767717123, -0.007643262855708599, 0.005871690344065428, -0.010146280750632286, 0.012743244878947735, 0.049711406230926514, 0.0059522162191569805, -0.031995680183172226, -0.03988723084330559, -0.02614411897957325, -0.01010601781308651, -0.011119303293526173, -0.007153396029025316, -0.003090186743065715, -0.019192038103938103, 0.017836516723036766, -0.03194199502468109, -0.003593474393710494, 0.004375247750431299, 0.009461808949708939, 0.001773250405676663, 0.010407989844679832, 0.008414970710873604, 0.023419655859470367, -0.03269357234239578, -0.008166681975126266, 0.00650583254173398, 0.024023599922657013, -0.006284385919570923, 0.029392004013061523, 0.026748064905405045, -0.01225337851792574, 0.00557307293638587, 0.01005233358591795, 0.02120518870651722, -0.02042677067220211, 0.027311747893691063, 0.013535084202885628, 0.023459918797016144, 0.016078365966677666, -0.03642461076378822, -0.03097568266093731, 0.012085615657269955, 0.023137815296649933, -5.4365558753488585e-05, 0.034223563969135284, -0.03961880877614021, -0.003700842382386327, -0.014615475200116634, 0.0007779989391565323, -0.010354306548833847, -0.013837057165801525, 0.019728878512978554, -0.01218627393245697, -0.00927391555160284, 0.013226401060819626, -0.009267204441130161, 0.00038040164508856833, -0.006119978614151478, -0.014830212108790874, 0.018386777490377426, 0.03569987788796425, 0.011555486358702183, 0.02813042886555195, 0.01027377974241972, 0.012508377432823181, -0.020037561655044556, 0.07021870464086533, 0.00262212916277349, 0.014588633552193642, -0.022265449166297913, -0.00582471676170826, 0.014306792058050632, 0.009609440341591835, -0.021218610927462578, -0.010803909972310066, -0.006690371315926313, -0.025499911978840828, -0.006884976290166378, -0.011099171824753284, 0.0023268668446689844, -0.0003850150969810784, 0.00582136120647192, -0.03161989152431488, 0.01658836379647255, 0.009032336995005608, 0.01877598837018013, -0.010797199793159962, 0.0006387560279108584, 0.025083860382437706, 0.02183597721159458, -0.00045044251601211727, -0.008931679651141167, -0.0188833549618721, -0.0015534814447164536, -0.010119438171386719, 0.014360476285219193, 0.00977049209177494, 0.019312826916575432, -0.025540174916386604, -0.00999864935874939, -0.005609980318695307, 0.003209298010915518, 0.00949536170810461, -0.0006882459856569767, -0.01733993925154209, 0.01657494157552719, -0.00516373198479414, 0.021701766178011894, 0.00620386004447937, -0.016400469467043877, -0.020708613097667694, -0.0077640521340072155, -0.010797199793159962, 0.003264659782871604, -0.03427724912762642, -0.022654658183455467, -0.028962530195713043, -0.016400469467043877, -0.012213115580379963, 0.03680039942264557, -0.012286931276321411, -0.01065627858042717, -0.03280093893408775, -0.010072465054690838, -0.006193794310092926, -0.035404615104198456, 0.0327204130589962, 0.020037561655044556, -0.02767411433160305, -0.04973824694752693, 0.006160241551697254, -0.17082256078720093, 0.0064789908938109875, 0.01405179314315319, -0.018869934603571892, 0.01119311898946762, -0.008294181898236275, 0.006730634719133377, -0.01053548976778984, -0.05258350074291229, 0.02273518405854702, 0.015098631381988525, -0.007817735895514488, -0.021715188398957253, -0.004982548300176859, -0.002420814009383321, -0.012011799961328506, -0.005284521263092756, -0.012642587535083294, 0.02548648975789547, 0.01415916159749031, 0.028828321024775505, -0.006170307751744986, -0.012005089782178402, -0.00894510094076395, -0.007093001622706652, 0.018467305228114128, -0.023124393075704575, 0.014441002160310745, -0.015662314370274544, -0.012011799961328506, -0.012239957228302956, 0.02909674122929573, 0.001132397330366075, -0.010448252782225609, 0.006059584207832813, -0.023808864876627922, -0.001465406152419746, -0.010508648119866848, 0.001641556853428483, 0.02195676602423191, 0.012293641455471516, 0.012045352719724178, 0.008529049344360828, 0.00392564432695508, 0.005911953281611204, -0.0022094331216067076, 0.02128571644425392, 0.022238606587052345, 0.019702037796378136, -0.036505136638879776, 0.013421006500720978, -0.04753720387816429, 0.016199154779314995, 0.010119438171386719, -0.011132724583148956, 0.020359667018055916, 0.02131255716085434, 0.012984823435544968, -0.011427986435592175, 0.0011533676879480481, -0.017715727910399437, -0.034250408411026, 0.000980572309345007, -0.012280220165848732, -0.020252298563718796, -0.010770357213914394, -0.007475500460714102, -0.018910197541117668, -0.010569042526185513, 0.017729148268699646, -0.009797334671020508, -0.03548514097929001, 0.01427995041012764, -0.029392004013061523, 0.020359667018055916, -0.01098509319126606, -0.00021599431056529284, 0.008884705603122711, -0.006646753288805485, -0.0017212440725415945, -0.023459918797016144, 0.03435777500271797, -0.00488524604588747, 0.006331359501928091, -0.01318613812327385, 0.009924833662807941, 0.010824041441082954, 0.006707147695124149, 0.04960403963923454, 0.008710232563316822, 0.0031774232629686594, -0.04796667397022247, 0.020936770364642143, -0.014038372784852982, 0.005784453824162483, 0.004690641537308693, 0.036934610456228256, 0.0002742918150033802, 0.010716672986745834, 0.0027429182082414627, 0.0064789908938109875, -0.038491446524858475, -0.012823771685361862, 0.019017565995454788, 0.03438461571931839, -0.011461539193987846, -0.011501802131533623, 0.04018249362707138, 0.03170041739940643, -0.005942150484770536, -0.02799621783196926, 0.016749415546655655, 0.00845523364841938, -0.00028666428988799453, -0.00358340865932405, 0.012602324597537518, -0.03897460177540779, -0.027862008661031723, 0.01202522125095129, 0.022587552666664124, 0.04700036346912384, 0.02909674122929573, 0.008831022307276726, 0.0010493549052625895, 0.005885111168026924, 0.0044759055599570274, -0.07311764359474182, -0.007287606131285429, 0.00873036403208971, -0.005895176902413368, 0.008032471872866154, 0.04445037245750427, 0.0012422818690538406, 0.04581931605935097, 0.010736804455518723, 0.037068817764520645, -0.010374438017606735, -0.006740700453519821, 0.00425445893779397, -0.006210570689290762, -0.006187083665281534, -0.018413620069622993, -0.017407044768333435, -0.019178617745637894, -0.017098361626267433, 0.030250947922468185, -0.013132454827427864, -0.009971807710826397, 0.009837597608566284, 0.0018252568552270532, -0.01615889184176922, 0.02054755948483944, -0.020050983875989914, 0.012038642540574074, 0.023352550342679024, 0.014360476285219193, 0.025003334507346153, -0.008750495500862598, 0.006723924074321985, 0.021701766178011894, 0.005549585912376642, 0.01005233358591795, -0.06570924818515778, -0.023097550496459007, 0.023110972717404366, -0.023325707763433456, -0.004438997711986303, 0.00428130105137825, 0.010085886344313622, -0.027486220002174377, -0.0009218553313985467, 0.0030281145591288805, -0.017433887347579002, 0.024654388427734375, 0.027862008661031723, -0.014481265097856522, -0.02810358628630638, -0.0025130833964794874, -0.012763376347720623, -0.015152315609157085, 0.010421411134302616, 0.016668889671564102, -0.012756666168570518, 0.024412810802459717, -0.026184381917119026, 0.005653598811477423, 0.012414430268108845, -0.007515763398259878, 0.004925509449094534, -0.005099982488900423, 0.022668078541755676, -0.018413620069622993, -0.021473608911037445, -0.005405310075730085, 0.014347055926918983, -0.014494686387479305, -0.00043114981963299215, 0.012441272847354412, -0.04031670093536377, 0.017286255955696106, -0.036961451172828674, -0.01042812131345272, -0.02184939756989479, -0.005764321889728308, -0.016105206683278084, -0.02294992096722126, -0.00526774488389492, -0.015125473961234093, -0.025956226512789726, -0.00823378749191761, 0.0021758805960416794, 0.015608630143105984, -0.010662989690899849, 0.0011961471755057573, -0.011682985350489616, -0.02802306041121483, 0.035001982003450394, 0.014749685302376747, 0.01582336612045765, -0.017044678330421448, -0.008367997594177723, -0.02405044250190258, -0.037713028490543365, -0.00229163677431643, -0.0072808959521353245, 0.012729824520647526, 0.0006395948003046215, 0.0010325786424800754, -0.07655341923236847, 0.01009930670261383, -0.01932624913752079, -0.022493606433272362, -0.0036639347672462463, 0.002776470733806491, 0.02536570094525814, -0.025728069245815277, -0.011340750381350517, 0.022788867354393005, -0.01571599766612053, 0.01114614587277174, -0.0031858112197369337, 0.03148568049073219, -0.016333363950252533, -0.009481940418481827, 0.02963358163833618, -0.02284255251288414, 0.0026808460243046284, 0.024130968376994133, -0.006978922989219427, -0.021473608911037445, 0.008502207696437836, -0.010032202117145061, 0.007032607216387987, 0.03314988315105438, -0.020144930109381676, 0.010891146026551723, -0.01334047969430685, -0.013085480779409409, 0.01580994576215744, -0.022896235808730125, 0.005713993217796087, 0.04098775237798691, -0.012219825759530067, 0.010850883089005947, 0.0256878063082695, 0.025983067229390144, 0.01715204492211342, -0.021809134632349014, -0.02692253887653351, -0.013246532529592514, 0.005576428025960922, -0.016964152455329895, -0.016950730234384537, 0.012045352719724178, -0.01214601006358862, -0.011374302208423615, 0.008663259446620941, 0.020359667018055916, 0.021795714274048805, -0.00895852129906416, -0.006791029125452042, -0.015246262773871422, 0.0032915016636252403, -0.02799621783196926, -0.0022564067039638758, -0.011877590790390968, 0.011186408810317516, -0.008609575219452381, 0.05094613879919052, -0.0031774232629686594, 0.037954606115818024, 0.002773115411400795, 0.025083860382437706, 0.008005630224943161, -0.007394974119961262, 0.008482076227664948, 0.0005762644577771425, 0.008314313367009163, -0.026667539030313492, -0.015528104268014431, 0.007267474662512541, 0.008857863955199718, 0.020279139280319214, 0.010783778503537178, 0.015232841484248638, 0.02657359279692173, -0.004428931977599859, 0.02052071876823902, 0.02527175471186638, 0.013031796552240849, -0.017111781984567642, 0.014360476285219193, 0.010132859461009502, 0.01527310535311699, -0.045872997492551804, 0.003918933682143688, 0.004603405017405748, 0.00807944592088461, -0.024627545848488808, 0.028157271444797516, -0.02183597721159458, -0.019916772842407227, -0.0015677412739023566, 0.013984688557684422, -0.019916772842407227, 0.0016533001326024532, 0.020735453814268112, 0.0038216314278542995, -0.006569582503288984, 0.02053413912653923, -0.0025265044532716274, -0.01680309884250164, -0.03030463121831417, 0.015447578392922878, -0.024627545848488808, -0.018520988523960114, -0.010844172909855843, 0.02219834364950657, -0.007717078551650047, -0.00861628632992506, 0.010850883089005947, 0.016387049108743668, -0.006173662841320038, 0.001405850</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>